<commit_message>
Add a class for CDS locus
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -19,31 +19,32 @@
     <sheet name="Transcript species types" sheetId="10" r:id="rId10"/>
     <sheet name="Exon loci" sheetId="11" r:id="rId11"/>
     <sheet name="Protein species types" sheetId="12" r:id="rId12"/>
-    <sheet name="Complex species types" sheetId="13" r:id="rId13"/>
-    <sheet name="Concentrations" sheetId="14" r:id="rId14"/>
-    <sheet name="Observables" sheetId="15" r:id="rId15"/>
-    <sheet name="Reactions" sheetId="16" r:id="rId16"/>
-    <sheet name="Rate laws" sheetId="17" r:id="rId17"/>
-    <sheet name="Parameters" sheetId="18" r:id="rId18"/>
-    <sheet name="Properties" sheetId="19" r:id="rId19"/>
-    <sheet name="References" sheetId="20" r:id="rId20"/>
+    <sheet name="CDS loci" sheetId="21" r:id="rId13"/>
+    <sheet name="Complex species types" sheetId="13" r:id="rId14"/>
+    <sheet name="Concentrations" sheetId="14" r:id="rId15"/>
+    <sheet name="Observables" sheetId="15" r:id="rId16"/>
+    <sheet name="Reactions" sheetId="16" r:id="rId17"/>
+    <sheet name="Rate laws" sheetId="17" r:id="rId18"/>
+    <sheet name="Parameters" sheetId="18" r:id="rId19"/>
+    <sheet name="Properties" sheetId="19" r:id="rId20"/>
+    <sheet name="References" sheetId="20" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">Cell!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12">'Complex species types'!$A$1:$J$221</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13">'Complex species types'!$A$1:$J$221</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Gene loci'!$B$1:$H$1064</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8">'pre-RNA species types'!$A$1:$G$915</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11">'Protein species types'!$A$1:$F$719</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16">'Rate laws'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15">Reactions!$A$1:$F$220</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11">'Protein species types'!$A$1:$G$719</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17">'Rate laws'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16">Reactions!$A$1:$F$220</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6">'Regulatory element loci'!$A$1:$H$776</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">'Regulatory module'!$A$1:$C$849</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">'Gene loci'!$I$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="8">'pre-RNA species types'!$A$1:$G$915</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="11">'Protein species types'!$A$1:$F$719</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="11">'Protein species types'!$A$1:$G$719</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="6">'Regulatory element loci'!$A$1:$H$776</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="7">'Regulatory module'!$A$1:$C$849</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
@@ -82,7 +83,7 @@
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="471">
   <si>
     <t>Id</t>
   </si>
@@ -1493,6 +1494,18 @@
   </si>
   <si>
     <t>Ploidy</t>
+  </si>
+  <si>
+    <t>CDS_ENSP00000234111</t>
+  </si>
+  <si>
+    <t>CDS_ENSP00000385333</t>
+  </si>
+  <si>
+    <t>CDS_ENSP00000390691</t>
+  </si>
+  <si>
+    <t>Coding Region</t>
   </si>
 </sst>
 </file>
@@ -2130,14 +2143,14 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="1"/>
-    <col min="2" max="2" width="43.42578125" style="2"/>
-    <col min="3" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="21.5546875" style="1"/>
+    <col min="2" max="2" width="43.44140625" style="2"/>
+    <col min="3" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2145,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2153,7 +2166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2161,7 +2174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2169,25 +2182,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2195,7 +2208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -2212,22 +2225,22 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125"/>
-    <col min="2" max="2" width="11.7109375"/>
-    <col min="3" max="4" width="8.5703125"/>
-    <col min="5" max="5" width="7.42578125"/>
-    <col min="6" max="6" width="10.42578125"/>
-    <col min="7" max="7" width="10.7109375"/>
-    <col min="8" max="8" width="19.85546875"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="16.44140625"/>
+    <col min="2" max="2" width="11.6640625"/>
+    <col min="3" max="4" width="8.5546875"/>
+    <col min="5" max="5" width="7.44140625"/>
+    <col min="6" max="6" width="10.44140625"/>
+    <col min="7" max="7" width="10.6640625"/>
+    <col min="8" max="8" width="19.88671875"/>
+    <col min="9" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2254,7 +2267,7 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>291</v>
       </c>
@@ -2268,7 +2281,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -2282,7 +2295,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>297</v>
       </c>
@@ -2296,7 +2309,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>300</v>
       </c>
@@ -2320,24 +2333,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMG21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125"/>
-    <col min="2" max="2" width="12.7109375"/>
-    <col min="3" max="3" width="8.5703125"/>
+    <col min="1" max="1" width="16.44140625"/>
+    <col min="2" max="2" width="12.6640625"/>
+    <col min="3" max="3" width="8.5546875"/>
     <col min="4" max="4" width="10"/>
-    <col min="5" max="5" width="10.140625"/>
-    <col min="6" max="6" width="10.42578125"/>
-    <col min="7" max="7" width="10.7109375"/>
-    <col min="8" max="8" width="19.85546875"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="5" max="5" width="10.109375"/>
+    <col min="6" max="6" width="10.44140625"/>
+    <col min="7" max="7" width="10.6640625"/>
+    <col min="8" max="8" width="19.88671875"/>
+    <col min="9" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1021" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1021" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2364,7 +2377,7 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>303</v>
       </c>
@@ -2383,7 +2396,7 @@
       <c r="AMF2" s="33"/>
       <c r="AMG2" s="33"/>
     </row>
-    <row r="3" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>305</v>
       </c>
@@ -2402,7 +2415,7 @@
       <c r="AMF3" s="33"/>
       <c r="AMG3" s="33"/>
     </row>
-    <row r="4" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>307</v>
       </c>
@@ -2421,7 +2434,7 @@
       <c r="AMF4" s="33"/>
       <c r="AMG4" s="33"/>
     </row>
-    <row r="5" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>309</v>
       </c>
@@ -2440,7 +2453,7 @@
       <c r="AMF5" s="33"/>
       <c r="AMG5" s="33"/>
     </row>
-    <row r="6" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>311</v>
       </c>
@@ -2459,7 +2472,7 @@
       <c r="AMF6" s="33"/>
       <c r="AMG6" s="33"/>
     </row>
-    <row r="7" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>313</v>
       </c>
@@ -2478,7 +2491,7 @@
       <c r="AMF7" s="33"/>
       <c r="AMG7" s="33"/>
     </row>
-    <row r="8" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>315</v>
       </c>
@@ -2497,7 +2510,7 @@
       <c r="AMF8" s="33"/>
       <c r="AMG8" s="33"/>
     </row>
-    <row r="9" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>317</v>
       </c>
@@ -2516,7 +2529,7 @@
       <c r="AMF9" s="33"/>
       <c r="AMG9" s="33"/>
     </row>
-    <row r="10" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>319</v>
       </c>
@@ -2535,7 +2548,7 @@
       <c r="AMF10" s="33"/>
       <c r="AMG10" s="33"/>
     </row>
-    <row r="11" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>321</v>
       </c>
@@ -2554,7 +2567,7 @@
       <c r="AMF11" s="33"/>
       <c r="AMG11" s="33"/>
     </row>
-    <row r="12" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>323</v>
       </c>
@@ -2573,7 +2586,7 @@
       <c r="AMF12" s="33"/>
       <c r="AMG12" s="33"/>
     </row>
-    <row r="13" spans="1:1021" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1021" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>325</v>
       </c>
@@ -2590,7 +2603,7 @@
         <v>10448121</v>
       </c>
     </row>
-    <row r="14" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>327</v>
       </c>
@@ -2607,7 +2620,7 @@
         <v>10440601</v>
       </c>
     </row>
-    <row r="15" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>329</v>
       </c>
@@ -2624,7 +2637,7 @@
         <v>10447474</v>
       </c>
     </row>
-    <row r="16" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>331</v>
       </c>
@@ -2641,7 +2654,7 @@
         <v>10444544</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>333</v>
       </c>
@@ -2658,7 +2671,7 @@
         <v>10447628</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>335</v>
       </c>
@@ -2675,7 +2688,7 @@
         <v>10444095</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>337</v>
       </c>
@@ -2692,7 +2705,7 @@
         <v>10444474</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>339</v>
       </c>
@@ -2709,7 +2722,7 @@
         <v>10444931</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>341</v>
       </c>
@@ -2734,27 +2747,28 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMF4"/>
+  <dimension ref="A1:AMG4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="13"/>
-    <col min="2" max="2" width="33.85546875" style="13"/>
-    <col min="3" max="3" width="16.42578125" style="14"/>
-    <col min="4" max="4" width="16.42578125" style="11"/>
-    <col min="5" max="5" width="10.42578125" style="2"/>
-    <col min="6" max="6" width="40.28515625" style="13"/>
-    <col min="7" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="19.85546875" style="2"/>
-    <col min="9" max="1020" width="9.140625" style="2"/>
-    <col min="1023" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="20.33203125" style="13"/>
+    <col min="2" max="2" width="33.88671875" style="13"/>
+    <col min="3" max="3" width="16.44140625" style="14"/>
+    <col min="4" max="4" width="16.44140625" style="11"/>
+    <col min="5" max="5" width="25.5546875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="2"/>
+    <col min="7" max="7" width="40.33203125" style="13"/>
+    <col min="8" max="8" width="9.109375" style="2"/>
+    <col min="9" max="9" width="19.88671875" style="2"/>
+    <col min="10" max="1021" width="9.109375" style="2"/>
+    <col min="1024" max="1026" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2768,19 +2782,22 @@
         <v>344</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>346</v>
       </c>
@@ -2793,8 +2810,11 @@
       <c r="D2" s="11" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>349</v>
       </c>
@@ -2807,8 +2827,11 @@
       <c r="D3" s="11" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>350</v>
       </c>
@@ -2821,9 +2844,12 @@
       <c r="D4" s="11" t="s">
         <v>297</v>
       </c>
+      <c r="E4" s="13" t="s">
+        <v>469</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F719"/>
+  <autoFilter ref="A1:G719"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
@@ -2835,30 +2861,122 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="32">
+        <v>10439999</v>
+      </c>
+      <c r="E2" s="34">
+        <v>10448100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="34">
+        <v>10440600</v>
+      </c>
+      <c r="E3" s="34">
+        <v>10447000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="34">
+        <v>10444500</v>
+      </c>
+      <c r="E4" s="34">
+        <v>10447601</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMH5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" style="2"/>
+    <col min="1" max="1" width="38.6640625" style="2"/>
     <col min="2" max="2" width="46" style="35"/>
-    <col min="3" max="3" width="32.85546875" style="2"/>
+    <col min="3" max="3" width="32.88671875" style="2"/>
     <col min="4" max="4" width="45" style="36"/>
-    <col min="5" max="5" width="29.28515625" style="36"/>
-    <col min="6" max="6" width="16.42578125" style="11"/>
-    <col min="7" max="8" width="8.42578125" style="2"/>
-    <col min="9" max="9" width="13.42578125" style="2"/>
-    <col min="10" max="10" width="37.28515625" style="2"/>
-    <col min="11" max="11" width="13.42578125" style="2"/>
-    <col min="12" max="12" width="19.85546875" style="2"/>
-    <col min="13" max="1022" width="8.42578125" style="2"/>
-    <col min="1023" max="1025" width="8.42578125"/>
+    <col min="5" max="5" width="29.33203125" style="36"/>
+    <col min="6" max="6" width="16.44140625" style="11"/>
+    <col min="7" max="8" width="8.44140625" style="2"/>
+    <col min="9" max="9" width="13.44140625" style="2"/>
+    <col min="10" max="10" width="37.33203125" style="2"/>
+    <col min="11" max="11" width="13.44140625" style="2"/>
+    <col min="12" max="12" width="19.88671875" style="2"/>
+    <col min="13" max="1022" width="8.44140625" style="2"/>
+    <col min="1023" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>352</v>
       </c>
@@ -2896,7 +3014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>359</v>
       </c>
@@ -2921,7 +3039,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>365</v>
       </c>
@@ -2943,7 +3061,7 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>367</v>
       </c>
@@ -2965,7 +3083,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>369</v>
       </c>
@@ -2994,7 +3112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK12"/>
   <sheetViews>
@@ -3005,18 +3123,18 @@
       <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="39"/>
-    <col min="2" max="2" width="8.5703125" style="39"/>
-    <col min="3" max="3" width="11.5703125" style="39"/>
-    <col min="4" max="4" width="10.42578125" style="39"/>
-    <col min="5" max="5" width="10.7109375" style="39"/>
-    <col min="6" max="6" width="19.85546875" style="39"/>
-    <col min="7" max="1025" width="8.5703125" style="39"/>
+    <col min="1" max="1" width="19.44140625" style="39"/>
+    <col min="2" max="2" width="8.5546875" style="39"/>
+    <col min="3" max="3" width="11.5546875" style="39"/>
+    <col min="4" max="4" width="10.44140625" style="39"/>
+    <col min="5" max="5" width="10.6640625" style="39"/>
+    <col min="6" max="6" width="19.88671875" style="39"/>
+    <col min="7" max="1025" width="8.5546875" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="40" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="40" customFormat="1" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>372</v>
       </c>
@@ -3036,7 +3154,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>375</v>
       </c>
@@ -3050,7 +3168,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
         <v>378</v>
       </c>
@@ -3064,7 +3182,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>381</v>
       </c>
@@ -3075,7 +3193,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
         <v>383</v>
       </c>
@@ -3086,7 +3204,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
         <v>384</v>
       </c>
@@ -3097,7 +3215,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
         <v>385</v>
       </c>
@@ -3108,7 +3226,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
         <v>386</v>
       </c>
@@ -3119,7 +3237,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="39" t="s">
         <v>387</v>
       </c>
@@ -3130,7 +3248,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="41" t="s">
         <v>388</v>
       </c>
@@ -3141,7 +3259,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="41" t="s">
         <v>389</v>
       </c>
@@ -3152,7 +3270,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
         <v>390</v>
       </c>
@@ -3169,7 +3287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -3177,17 +3295,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16"/>
-    <col min="4" max="4" width="15.42578125"/>
+    <col min="4" max="4" width="15.44140625"/>
     <col min="5" max="5" width="14"/>
-    <col min="6" max="6" width="10.5703125"/>
-    <col min="7" max="7" width="11.140625"/>
-    <col min="8" max="8" width="20.5703125"/>
+    <col min="6" max="6" width="10.5546875"/>
+    <col min="7" max="7" width="11.109375"/>
+    <col min="8" max="8" width="20.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3213,7 +3331,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>393</v>
       </c>
@@ -3231,7 +3349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMH8"/>
   <sheetViews>
@@ -3239,19 +3357,19 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="2"/>
-    <col min="2" max="2" width="23.42578125" style="2"/>
-    <col min="3" max="3" width="17.7109375" style="2"/>
-    <col min="4" max="4" width="18.7109375" style="2"/>
-    <col min="5" max="5" width="12.7109375" style="2"/>
-    <col min="6" max="6" width="14.7109375" style="2"/>
-    <col min="7" max="1022" width="37.28515625" style="2"/>
-    <col min="1023" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="18.6640625" style="2"/>
+    <col min="2" max="2" width="23.44140625" style="2"/>
+    <col min="3" max="3" width="17.6640625" style="2"/>
+    <col min="4" max="4" width="18.6640625" style="2"/>
+    <col min="5" max="5" width="12.6640625" style="2"/>
+    <col min="6" max="6" width="14.6640625" style="2"/>
+    <col min="7" max="1022" width="37.33203125" style="2"/>
+    <col min="1023" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3277,7 +3395,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>398</v>
       </c>
@@ -3294,7 +3412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>402</v>
       </c>
@@ -3311,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>405</v>
       </c>
@@ -3328,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>408</v>
       </c>
@@ -3345,7 +3463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -3362,7 +3480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>412</v>
       </c>
@@ -3379,7 +3497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>415</v>
       </c>
@@ -3407,7 +3525,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
@@ -3418,20 +3536,20 @@
       <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="42"/>
-    <col min="2" max="2" width="10.7109375" style="42"/>
-    <col min="3" max="3" width="10.42578125" style="42"/>
+    <col min="1" max="1" width="20.33203125" style="42"/>
+    <col min="2" max="2" width="10.6640625" style="42"/>
+    <col min="3" max="3" width="10.44140625" style="42"/>
     <col min="4" max="4" width="11" style="42"/>
-    <col min="5" max="5" width="6.5703125" style="42"/>
-    <col min="6" max="6" width="28.7109375" style="42"/>
+    <col min="5" max="5" width="6.5546875" style="42"/>
+    <col min="6" max="6" width="28.6640625" style="42"/>
     <col min="7" max="7" width="11" style="42"/>
     <col min="8" max="8" width="20" style="42"/>
-    <col min="9" max="1025" width="8.7109375" style="42"/>
+    <col min="9" max="1025" width="8.6640625" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
         <v>416</v>
       </c>
@@ -3457,7 +3575,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
         <v>398</v>
       </c>
@@ -3472,7 +3590,7 @@
       <c r="F2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
         <v>402</v>
       </c>
@@ -3489,7 +3607,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>405</v>
       </c>
@@ -3510,7 +3628,7 @@
       </c>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>408</v>
       </c>
@@ -3525,7 +3643,7 @@
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
         <v>37</v>
       </c>
@@ -3540,7 +3658,7 @@
       </c>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="42" t="s">
         <v>37</v>
       </c>
@@ -3552,7 +3670,7 @@
       </c>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="42" t="s">
         <v>412</v>
       </c>
@@ -3566,7 +3684,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="42" t="s">
         <v>415</v>
       </c>
@@ -3587,22 +3705,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="8.5703125"/>
-    <col min="6" max="6" width="10.5703125"/>
-    <col min="7" max="7" width="11.140625"/>
-    <col min="8" max="8" width="20.5703125"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="1" max="5" width="8.5546875"/>
+    <col min="6" max="6" width="10.5546875"/>
+    <col min="7" max="7" width="11.109375"/>
+    <col min="8" max="8" width="20.5546875"/>
+    <col min="9" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3628,7 +3746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>437</v>
       </c>
@@ -3648,7 +3766,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>441</v>
       </c>
@@ -3668,7 +3786,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>444</v>
       </c>
@@ -3688,7 +3806,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>446</v>
       </c>
@@ -3711,114 +3829,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375"/>
-    <col min="2" max="2" width="15.5703125"/>
-    <col min="4" max="4" width="13.140625"/>
-    <col min="5" max="5" width="10.5703125"/>
-    <col min="6" max="6" width="11.140625"/>
-    <col min="7" max="7" width="19.85546875"/>
-    <col min="1021" max="1025" width="8.7109375"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>448</v>
-      </c>
-      <c r="B2" t="s">
-        <v>449</v>
-      </c>
-      <c r="C2" s="46">
-        <v>3.0000000000000001E-12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>451</v>
-      </c>
-      <c r="B3" t="s">
-        <v>452</v>
-      </c>
-      <c r="C3" s="46">
-        <v>10000000</v>
-      </c>
-      <c r="D3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>454</v>
-      </c>
-      <c r="B4" t="s">
-        <v>455</v>
-      </c>
-      <c r="C4">
-        <v>0.7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>457</v>
-      </c>
-      <c r="B5" t="s">
-        <v>458</v>
-      </c>
-      <c r="C5">
-        <v>71280</v>
-      </c>
-      <c r="D5" t="s">
-        <v>459</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -3833,14 +3843,14 @@
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="6"/>
-    <col min="2" max="2" width="51.140625" style="2"/>
-    <col min="3" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="16.44140625" style="6"/>
+    <col min="2" max="2" width="51.109375" style="2"/>
+    <col min="3" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3848,7 +3858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -3856,7 +3866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
@@ -3864,7 +3874,7 @@
         <v>9606</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -3878,20 +3888,128 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625"/>
+    <col min="2" max="2" width="15.5546875"/>
+    <col min="4" max="4" width="13.109375"/>
+    <col min="5" max="5" width="10.5546875"/>
+    <col min="6" max="6" width="11.109375"/>
+    <col min="7" max="7" width="19.88671875"/>
+    <col min="1021" max="1025" width="8.6640625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2" s="46">
+        <v>3.0000000000000001E-12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C3" s="46">
+        <v>10000000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>454</v>
+      </c>
+      <c r="B4" t="s">
+        <v>455</v>
+      </c>
+      <c r="C4">
+        <v>0.7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B5" t="s">
+        <v>458</v>
+      </c>
+      <c r="C5">
+        <v>71280</v>
+      </c>
+      <c r="D5" t="s">
+        <v>459</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="18.5703125"/>
-    <col min="3" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="8.5546875"/>
+    <col min="2" max="2" width="18.5546875"/>
+    <col min="3" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>460</v>
       </c>
@@ -3899,7 +4017,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>364</v>
       </c>
@@ -3907,7 +4025,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>380</v>
       </c>
@@ -3915,7 +4033,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>464</v>
       </c>
@@ -3937,19 +4055,19 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="16.140625" style="2"/>
-    <col min="3" max="3" width="17.7109375" style="2"/>
-    <col min="4" max="4" width="11.28515625" style="2"/>
-    <col min="5" max="5" width="11.140625" style="2"/>
-    <col min="6" max="6" width="20.5703125" style="2"/>
-    <col min="7" max="1020" width="9.140625" style="2"/>
-    <col min="1024" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="9.109375" style="7"/>
+    <col min="2" max="2" width="16.109375" style="2"/>
+    <col min="3" max="3" width="17.6640625" style="2"/>
+    <col min="4" max="4" width="11.33203125" style="2"/>
+    <col min="5" max="5" width="11.109375" style="2"/>
+    <col min="6" max="6" width="20.5546875" style="2"/>
+    <col min="7" max="1020" width="9.109375" style="2"/>
+    <col min="1024" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3969,7 +4087,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -3986,7 +4104,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -3998,7 +4116,7 @@
       </c>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -4012,7 +4130,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
@@ -4038,19 +4156,19 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="9"/>
-    <col min="2" max="2" width="39.42578125" style="9"/>
-    <col min="3" max="3" width="13.7109375" style="2"/>
-    <col min="4" max="4" width="10.7109375" style="2"/>
+    <col min="1" max="1" width="23.88671875" style="9"/>
+    <col min="2" max="2" width="39.44140625" style="9"/>
+    <col min="3" max="3" width="13.6640625" style="2"/>
+    <col min="4" max="4" width="10.6640625" style="2"/>
     <col min="5" max="5" width="55" style="9"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="19.85546875" style="2"/>
-    <col min="8" max="1022" width="9.140625" style="2"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="7" max="7" width="19.88671875" style="2"/>
+    <col min="8" max="1022" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4073,7 +4191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -4081,7 +4199,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -4092,7 +4210,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4100,7 +4218,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -4108,7 +4226,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>40</v>
       </c>
@@ -4119,7 +4237,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>43</v>
       </c>
@@ -4130,7 +4248,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>46</v>
       </c>
@@ -4141,7 +4259,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>49</v>
       </c>
@@ -4166,24 +4284,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="7"/>
+    <col min="1" max="1" width="14.109375" style="7"/>
     <col min="2" max="2" width="13" style="11"/>
-    <col min="3" max="4" width="11.7109375" style="2"/>
-    <col min="5" max="5" width="22.140625" style="2"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="8" width="13.42578125" style="2"/>
-    <col min="9" max="9" width="13.42578125"/>
-    <col min="10" max="10" width="19.85546875"/>
-    <col min="11" max="12" width="13.42578125"/>
+    <col min="3" max="4" width="11.6640625" style="2"/>
+    <col min="5" max="5" width="22.109375" style="2"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="7" max="8" width="13.44140625" style="2"/>
+    <col min="9" max="9" width="13.44140625"/>
+    <col min="10" max="10" width="19.88671875"/>
+    <col min="11" max="12" width="13.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4215,7 +4333,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>56</v>
       </c>
@@ -4234,7 +4352,7 @@
       </c>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>57</v>
       </c>
@@ -4251,7 +4369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>58</v>
       </c>
@@ -4268,7 +4386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>59</v>
       </c>
@@ -4285,7 +4403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>60</v>
       </c>
@@ -4302,7 +4420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>61</v>
       </c>
@@ -4319,7 +4437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>62</v>
       </c>
@@ -4336,7 +4454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>63</v>
       </c>
@@ -4353,7 +4471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>64</v>
       </c>
@@ -4370,7 +4488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>65</v>
       </c>
@@ -4387,7 +4505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>66</v>
       </c>
@@ -4404,7 +4522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>67</v>
       </c>
@@ -4421,7 +4539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>68</v>
       </c>
@@ -4438,7 +4556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>69</v>
       </c>
@@ -4455,7 +4573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>70</v>
       </c>
@@ -4472,7 +4590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>71</v>
       </c>
@@ -4489,7 +4607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>72</v>
       </c>
@@ -4506,7 +4624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>73</v>
       </c>
@@ -4523,7 +4641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>74</v>
       </c>
@@ -4540,7 +4658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>75</v>
       </c>
@@ -4557,7 +4675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>76</v>
       </c>
@@ -4574,7 +4692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>77</v>
       </c>
@@ -4591,7 +4709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>78</v>
       </c>
@@ -4608,7 +4726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>79</v>
       </c>
@@ -4625,7 +4743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>80</v>
       </c>
@@ -4660,19 +4778,19 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="11"/>
-    <col min="2" max="2" width="16.42578125" style="11"/>
-    <col min="3" max="3" width="42.42578125" style="13"/>
-    <col min="4" max="6" width="13.42578125" style="14"/>
-    <col min="7" max="8" width="13.42578125" style="11"/>
-    <col min="9" max="9" width="16.42578125" style="15"/>
-    <col min="10" max="1023" width="32.5703125" style="2"/>
-    <col min="1024" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="17.44140625" style="11"/>
+    <col min="2" max="2" width="16.44140625" style="11"/>
+    <col min="3" max="3" width="42.44140625" style="13"/>
+    <col min="4" max="6" width="13.44140625" style="14"/>
+    <col min="7" max="8" width="13.44140625" style="11"/>
+    <col min="9" max="9" width="16.44140625" style="15"/>
+    <col min="10" max="1023" width="32.5546875" style="2"/>
+    <col min="1024" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1023" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4713,7 +4831,7 @@
       <c r="AMH1" s="2"/>
       <c r="AMI1" s="2"/>
     </row>
-    <row r="2" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>87</v>
       </c>
@@ -4739,7 +4857,7 @@
         <v>20651511</v>
       </c>
     </row>
-    <row r="3" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>92</v>
       </c>
@@ -4765,7 +4883,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="4" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>96</v>
       </c>
@@ -4791,7 +4909,7 @@
         <v>69387254</v>
       </c>
     </row>
-    <row r="5" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>99</v>
       </c>
@@ -4817,7 +4935,7 @@
         <v>40574685</v>
       </c>
     </row>
-    <row r="6" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>102</v>
       </c>
@@ -4843,7 +4961,7 @@
         <v>112649530</v>
       </c>
     </row>
-    <row r="7" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>105</v>
       </c>
@@ -4869,7 +4987,7 @@
         <v>83605875</v>
       </c>
     </row>
-    <row r="8" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>108</v>
       </c>
@@ -4895,7 +5013,7 @@
         <v>127899195</v>
       </c>
     </row>
-    <row r="9" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>111</v>
       </c>
@@ -4921,7 +5039,7 @@
         <v>160421711</v>
       </c>
     </row>
-    <row r="10" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>114</v>
       </c>
@@ -4947,7 +5065,7 @@
         <v>152129619</v>
       </c>
     </row>
-    <row r="11" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>117</v>
       </c>
@@ -4973,7 +5091,7 @@
         <v>56051604</v>
       </c>
     </row>
-    <row r="12" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>120</v>
       </c>
@@ -4999,7 +5117,7 @@
         <v>18084998</v>
       </c>
     </row>
-    <row r="13" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>123</v>
       </c>
@@ -5025,7 +5143,7 @@
         <v>19967258</v>
       </c>
     </row>
-    <row r="14" spans="1:1023" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>126</v>
       </c>
@@ -5051,7 +5169,7 @@
         <v>136423761</v>
       </c>
     </row>
-    <row r="15" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>129</v>
       </c>
@@ -5077,7 +5195,7 @@
         <v>7787981</v>
       </c>
     </row>
-    <row r="16" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>132</v>
       </c>
@@ -5103,7 +5221,7 @@
         <v>133421307</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>135</v>
       </c>
@@ -5129,7 +5247,7 @@
         <v>13732346</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>138</v>
       </c>
@@ -5155,7 +5273,7 @@
         <v>114450279</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>141</v>
       </c>
@@ -5181,7 +5299,7 @@
         <v>77065580</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>144</v>
       </c>
@@ -5207,7 +5325,7 @@
         <v>113359493</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>147</v>
       </c>
@@ -5233,7 +5351,7 @@
         <v>52476628</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>150</v>
       </c>
@@ -5259,7 +5377,7 @@
         <v>103057462</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>153</v>
       </c>
@@ -5285,7 +5403,7 @@
         <v>65578352</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>156</v>
       </c>
@@ -5311,7 +5429,7 @@
         <v>101251932</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>159</v>
       </c>
@@ -5337,7 +5455,7 @@
         <v>89155846</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>162</v>
       </c>
@@ -5363,7 +5481,7 @@
         <v>49223225</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>165</v>
       </c>
@@ -5389,7 +5507,7 @@
         <v>50988121</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>168</v>
       </c>
@@ -5415,7 +5533,7 @@
         <v>41440717</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>171</v>
       </c>
@@ -5441,7 +5559,7 @@
         <v>47784686</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>174</v>
       </c>
@@ -5467,7 +5585,7 @@
         <v>13638940</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>177</v>
       </c>
@@ -5493,7 +5611,7 @@
         <v>44652233</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>180</v>
       </c>
@@ -5519,7 +5637,7 @@
         <v>31668931</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>183</v>
       </c>
@@ -5545,7 +5663,7 @@
         <v>20859417</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>186</v>
       </c>
@@ -5571,7 +5689,7 @@
         <v>38738299</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>189</v>
       </c>
@@ -5597,7 +5715,7 @@
         <v>119605895</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>192</v>
       </c>
@@ -5623,7 +5741,7 @@
         <v>23005465</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>195</v>
       </c>
@@ -5668,26 +5786,26 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="16.42578125" style="11"/>
+    <col min="1" max="3" width="16.44140625" style="11"/>
     <col min="4" max="4" width="22" style="11"/>
-    <col min="5" max="5" width="13.7109375" style="11"/>
-    <col min="6" max="6" width="25.140625" style="11"/>
-    <col min="7" max="7" width="13.42578125" style="11"/>
-    <col min="8" max="8" width="23.28515625" style="11"/>
-    <col min="9" max="9" width="25.140625" style="2"/>
-    <col min="10" max="10" width="19.85546875"/>
-    <col min="11" max="11" width="9.140625" style="14"/>
-    <col min="12" max="12" width="10.42578125" style="14"/>
-    <col min="13" max="13" width="10.7109375" style="14"/>
-    <col min="14" max="15" width="9.140625" style="11"/>
-    <col min="16" max="16" width="22.85546875" style="14"/>
-    <col min="17" max="1012" width="9.140625" style="11"/>
-    <col min="1013" max="1021" width="9.140625" style="2"/>
+    <col min="5" max="5" width="13.6640625" style="11"/>
+    <col min="6" max="6" width="25.109375" style="11"/>
+    <col min="7" max="7" width="13.44140625" style="11"/>
+    <col min="8" max="8" width="23.33203125" style="11"/>
+    <col min="9" max="9" width="25.109375" style="2"/>
+    <col min="10" max="10" width="19.88671875"/>
+    <col min="11" max="11" width="9.109375" style="14"/>
+    <col min="12" max="12" width="10.44140625" style="14"/>
+    <col min="13" max="13" width="10.6640625" style="14"/>
+    <col min="14" max="15" width="9.109375" style="11"/>
+    <col min="16" max="16" width="22.88671875" style="14"/>
+    <col min="17" max="1012" width="9.109375" style="11"/>
+    <col min="1013" max="1021" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1021" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1021" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -5734,7 +5852,7 @@
       <c r="AMF1" s="1"/>
       <c r="AMG1" s="1"/>
     </row>
-    <row r="2" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>199</v>
       </c>
@@ -5761,7 +5879,7 @@
       <c r="N2" s="22"/>
       <c r="O2" s="22"/>
     </row>
-    <row r="3" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>203</v>
       </c>
@@ -5788,7 +5906,7 @@
       <c r="N3" s="22"/>
       <c r="O3" s="22"/>
     </row>
-    <row r="4" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>206</v>
       </c>
@@ -5815,7 +5933,7 @@
       <c r="N4" s="22"/>
       <c r="O4" s="22"/>
     </row>
-    <row r="5" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>210</v>
       </c>
@@ -5842,7 +5960,7 @@
       <c r="N5" s="22"/>
       <c r="O5" s="22"/>
     </row>
-    <row r="6" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>214</v>
       </c>
@@ -5869,7 +5987,7 @@
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
     </row>
-    <row r="7" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>217</v>
       </c>
@@ -5896,7 +6014,7 @@
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
     </row>
-    <row r="8" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>219</v>
       </c>
@@ -5923,7 +6041,7 @@
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
     </row>
-    <row r="9" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>222</v>
       </c>
@@ -5950,7 +6068,7 @@
       <c r="N9" s="22"/>
       <c r="O9" s="22"/>
     </row>
-    <row r="10" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>224</v>
       </c>
@@ -5977,7 +6095,7 @@
       <c r="N10" s="22"/>
       <c r="O10" s="22"/>
     </row>
-    <row r="11" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>226</v>
       </c>
@@ -6004,7 +6122,7 @@
       <c r="N11" s="22"/>
       <c r="O11" s="22"/>
     </row>
-    <row r="12" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>228</v>
       </c>
@@ -6031,7 +6149,7 @@
       <c r="N12" s="22"/>
       <c r="O12" s="22"/>
     </row>
-    <row r="13" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>230</v>
       </c>
@@ -6058,7 +6176,7 @@
       <c r="N13" s="22"/>
       <c r="O13" s="22"/>
     </row>
-    <row r="14" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>232</v>
       </c>
@@ -6085,7 +6203,7 @@
       <c r="N14" s="22"/>
       <c r="O14" s="22"/>
     </row>
-    <row r="15" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>234</v>
       </c>
@@ -6112,7 +6230,7 @@
       <c r="N15" s="22"/>
       <c r="O15" s="22"/>
     </row>
-    <row r="16" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>237</v>
       </c>
@@ -6139,7 +6257,7 @@
       <c r="N16" s="22"/>
       <c r="O16" s="22"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>239</v>
       </c>
@@ -6166,7 +6284,7 @@
       <c r="N17" s="22"/>
       <c r="O17" s="22"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>241</v>
       </c>
@@ -6193,7 +6311,7 @@
       <c r="N18" s="22"/>
       <c r="O18" s="22"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>243</v>
       </c>
@@ -6220,7 +6338,7 @@
       <c r="N19" s="22"/>
       <c r="O19" s="22"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>245</v>
       </c>
@@ -6247,7 +6365,7 @@
       <c r="N20" s="22"/>
       <c r="O20" s="22"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>247</v>
       </c>
@@ -6274,7 +6392,7 @@
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>249</v>
       </c>
@@ -6301,7 +6419,7 @@
       <c r="N22" s="22"/>
       <c r="O22" s="22"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>251</v>
       </c>
@@ -6328,7 +6446,7 @@
       <c r="N23" s="22"/>
       <c r="O23" s="22"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>253</v>
       </c>
@@ -6355,7 +6473,7 @@
       <c r="N24" s="22"/>
       <c r="O24" s="22"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>255</v>
       </c>
@@ -6382,7 +6500,7 @@
       <c r="N25" s="22"/>
       <c r="O25" s="22"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>257</v>
       </c>
@@ -6409,7 +6527,7 @@
       <c r="N26" s="22"/>
       <c r="O26" s="22"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>259</v>
       </c>
@@ -6436,7 +6554,7 @@
       <c r="N27" s="22"/>
       <c r="O27" s="22"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>261</v>
       </c>
@@ -6463,7 +6581,7 @@
       <c r="N28" s="22"/>
       <c r="O28" s="22"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>263</v>
       </c>
@@ -6490,7 +6608,7 @@
       <c r="N29" s="22"/>
       <c r="O29" s="22"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>265</v>
       </c>
@@ -6517,7 +6635,7 @@
       <c r="N30" s="22"/>
       <c r="O30" s="22"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>267</v>
       </c>
@@ -6544,7 +6662,7 @@
       <c r="N31" s="22"/>
       <c r="O31" s="22"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>269</v>
       </c>
@@ -6571,7 +6689,7 @@
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>271</v>
       </c>
@@ -6598,7 +6716,7 @@
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>273</v>
       </c>
@@ -6625,7 +6743,7 @@
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>275</v>
       </c>
@@ -6652,7 +6770,7 @@
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>277</v>
       </c>
@@ -6679,7 +6797,7 @@
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>279</v>
       </c>
@@ -6725,21 +6843,21 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="11"/>
-    <col min="2" max="2" width="50.5703125" style="11"/>
-    <col min="3" max="3" width="22.85546875" style="15"/>
-    <col min="4" max="4" width="13.42578125" style="23"/>
-    <col min="5" max="5" width="19.85546875" style="14"/>
-    <col min="6" max="6" width="10.7109375" style="14"/>
-    <col min="7" max="8" width="9.140625" style="11"/>
-    <col min="9" max="1016" width="9.140625" style="23"/>
-    <col min="1017" max="1019" width="8.42578125"/>
-    <col min="1020" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="17.44140625" style="11"/>
+    <col min="2" max="2" width="50.5546875" style="11"/>
+    <col min="3" max="3" width="22.88671875" style="15"/>
+    <col min="4" max="4" width="13.44140625" style="23"/>
+    <col min="5" max="5" width="19.88671875" style="14"/>
+    <col min="6" max="6" width="10.6640625" style="14"/>
+    <col min="7" max="8" width="9.109375" style="11"/>
+    <col min="9" max="1016" width="9.109375" style="23"/>
+    <col min="1017" max="1019" width="8.44140625"/>
+    <col min="1020" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>281</v>
       </c>
@@ -6757,7 +6875,7 @@
       </c>
       <c r="F1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>92</v>
       </c>
@@ -6768,7 +6886,7 @@
       <c r="H2" s="22"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>108</v>
       </c>
@@ -6798,23 +6916,23 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="14"/>
-    <col min="2" max="2" width="21.140625" style="14"/>
-    <col min="3" max="3" width="10.7109375" style="14"/>
-    <col min="4" max="4" width="22.85546875" style="15"/>
-    <col min="5" max="5" width="10.7109375"/>
-    <col min="6" max="6" width="13.42578125"/>
-    <col min="7" max="7" width="13.42578125" style="11"/>
-    <col min="8" max="8" width="13.42578125" style="25"/>
-    <col min="9" max="9" width="10.7109375" style="22"/>
-    <col min="10" max="10" width="19.85546875" style="11"/>
-    <col min="11" max="11" width="13.42578125" style="11"/>
-    <col min="12" max="1021" width="9.140625" style="2"/>
+    <col min="1" max="1" width="19.5546875" style="14"/>
+    <col min="2" max="2" width="21.109375" style="14"/>
+    <col min="3" max="3" width="10.6640625" style="14"/>
+    <col min="4" max="4" width="22.88671875" style="15"/>
+    <col min="5" max="5" width="10.6640625"/>
+    <col min="6" max="6" width="13.44140625"/>
+    <col min="7" max="7" width="13.44140625" style="11"/>
+    <col min="8" max="8" width="13.44140625" style="25"/>
+    <col min="9" max="9" width="10.6640625" style="22"/>
+    <col min="10" max="10" width="19.88671875" style="11"/>
+    <col min="11" max="11" width="13.44140625" style="11"/>
+    <col min="12" max="1021" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -6847,7 +6965,7 @@
       </c>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>285</v>
       </c>
@@ -6873,7 +6991,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>287</v>
       </c>

</xml_diff>

<commit_message>
Add attributes to regulatory elements
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -38,32 +38,32 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="11">'Protein species types'!$A$1:$G$719</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17">'Rate laws'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16">Reactions!$A$1:$F$220</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6">'Regulatory element loci'!$A$1:$H$776</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6">'Regulatory element loci'!$A$1:$K$776</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">'Regulatory module'!$A$1:$C$849</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">'Gene loci'!$I$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="8">'pre-RNA species types'!$A$1:$G$915</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="11">'Protein species types'!$A$1:$G$719</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="6">'Regulatory element loci'!$A$1:$H$776</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'Regulatory element loci'!$A$1:$K$776</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="7">'Regulatory module'!$A$1:$C$849</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="5">'Gene loci'!$B$1:$H$1064</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="8">'pre-RNA species types'!$A$1:$G$915</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Regulatory element loci'!$A$1:$H$776</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Regulatory element loci'!$A$1:$K$776</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="7">'Regulatory module'!$A$1:$C$849</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Gene loci'!$I$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="8">'pre-RNA species types'!$A$1:$G$915</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Regulatory element loci'!$A$1:$H$776</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Regulatory element loci'!$A$1:$K$776</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="7">'Regulatory module'!$A$1:$C$849</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">'Gene loci'!$B$1:$H$1064</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="8">'pre-RNA species types'!$A$1:$G$849</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Regulatory element loci'!$A$2:$P$849</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Regulatory element loci'!$A$2:$S$849</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">'Gene loci'!$I$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="475">
   <si>
     <t>Id</t>
   </si>
@@ -1506,6 +1506,18 @@
   </si>
   <si>
     <t>Coding Region</t>
+  </si>
+  <si>
+    <t>Bound End</t>
+  </si>
+  <si>
+    <t>Bound Start</t>
+  </si>
+  <si>
+    <t>Motif Features</t>
+  </si>
+  <si>
+    <t>ENSP00000234111, ENSP00000390691</t>
   </si>
 </sst>
 </file>
@@ -2143,14 +2155,14 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="1"/>
-    <col min="2" max="2" width="43.44140625" style="2"/>
-    <col min="3" max="1025" width="8.44140625"/>
+    <col min="1" max="1" width="21.5703125" style="1"/>
+    <col min="2" max="2" width="43.42578125" style="2"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2158,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2166,7 +2178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2174,7 +2186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2182,25 +2194,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2208,7 +2220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -2228,19 +2240,19 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625"/>
-    <col min="2" max="2" width="11.6640625"/>
-    <col min="3" max="4" width="8.5546875"/>
-    <col min="5" max="5" width="7.44140625"/>
-    <col min="6" max="6" width="10.44140625"/>
-    <col min="7" max="7" width="10.6640625"/>
-    <col min="8" max="8" width="19.88671875"/>
-    <col min="9" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="16.42578125"/>
+    <col min="2" max="2" width="11.7109375"/>
+    <col min="3" max="4" width="8.5703125"/>
+    <col min="5" max="5" width="7.42578125"/>
+    <col min="6" max="6" width="10.42578125"/>
+    <col min="7" max="7" width="10.7109375"/>
+    <col min="8" max="8" width="19.85546875"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2267,7 +2279,7 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>291</v>
       </c>
@@ -2281,7 +2293,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -2295,7 +2307,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>297</v>
       </c>
@@ -2309,7 +2321,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>300</v>
       </c>
@@ -2337,20 +2349,20 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625"/>
-    <col min="2" max="2" width="12.6640625"/>
-    <col min="3" max="3" width="8.5546875"/>
+    <col min="1" max="1" width="16.42578125"/>
+    <col min="2" max="2" width="12.7109375"/>
+    <col min="3" max="3" width="8.5703125"/>
     <col min="4" max="4" width="10"/>
-    <col min="5" max="5" width="10.109375"/>
-    <col min="6" max="6" width="10.44140625"/>
-    <col min="7" max="7" width="10.6640625"/>
-    <col min="8" max="8" width="19.88671875"/>
-    <col min="9" max="1025" width="8.5546875"/>
+    <col min="5" max="5" width="10.140625"/>
+    <col min="6" max="6" width="10.42578125"/>
+    <col min="7" max="7" width="10.7109375"/>
+    <col min="8" max="8" width="19.85546875"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1021" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1021" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2377,7 +2389,7 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>303</v>
       </c>
@@ -2396,7 +2408,7 @@
       <c r="AMF2" s="33"/>
       <c r="AMG2" s="33"/>
     </row>
-    <row r="3" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>305</v>
       </c>
@@ -2415,7 +2427,7 @@
       <c r="AMF3" s="33"/>
       <c r="AMG3" s="33"/>
     </row>
-    <row r="4" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>307</v>
       </c>
@@ -2434,7 +2446,7 @@
       <c r="AMF4" s="33"/>
       <c r="AMG4" s="33"/>
     </row>
-    <row r="5" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>309</v>
       </c>
@@ -2453,7 +2465,7 @@
       <c r="AMF5" s="33"/>
       <c r="AMG5" s="33"/>
     </row>
-    <row r="6" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>311</v>
       </c>
@@ -2472,7 +2484,7 @@
       <c r="AMF6" s="33"/>
       <c r="AMG6" s="33"/>
     </row>
-    <row r="7" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>313</v>
       </c>
@@ -2491,7 +2503,7 @@
       <c r="AMF7" s="33"/>
       <c r="AMG7" s="33"/>
     </row>
-    <row r="8" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>315</v>
       </c>
@@ -2510,7 +2522,7 @@
       <c r="AMF8" s="33"/>
       <c r="AMG8" s="33"/>
     </row>
-    <row r="9" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>317</v>
       </c>
@@ -2529,7 +2541,7 @@
       <c r="AMF9" s="33"/>
       <c r="AMG9" s="33"/>
     </row>
-    <row r="10" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>319</v>
       </c>
@@ -2548,7 +2560,7 @@
       <c r="AMF10" s="33"/>
       <c r="AMG10" s="33"/>
     </row>
-    <row r="11" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>321</v>
       </c>
@@ -2567,7 +2579,7 @@
       <c r="AMF11" s="33"/>
       <c r="AMG11" s="33"/>
     </row>
-    <row r="12" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>323</v>
       </c>
@@ -2586,7 +2598,7 @@
       <c r="AMF12" s="33"/>
       <c r="AMG12" s="33"/>
     </row>
-    <row r="13" spans="1:1021" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1021" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>325</v>
       </c>
@@ -2603,7 +2615,7 @@
         <v>10448121</v>
       </c>
     </row>
-    <row r="14" spans="1:1021" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1021" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>327</v>
       </c>
@@ -2620,7 +2632,7 @@
         <v>10440601</v>
       </c>
     </row>
-    <row r="15" spans="1:1021" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1021" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>329</v>
       </c>
@@ -2637,7 +2649,7 @@
         <v>10447474</v>
       </c>
     </row>
-    <row r="16" spans="1:1021" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1021" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>331</v>
       </c>
@@ -2654,7 +2666,7 @@
         <v>10444544</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>333</v>
       </c>
@@ -2671,7 +2683,7 @@
         <v>10447628</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>335</v>
       </c>
@@ -2688,7 +2700,7 @@
         <v>10444095</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>337</v>
       </c>
@@ -2705,7 +2717,7 @@
         <v>10444474</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>339</v>
       </c>
@@ -2722,7 +2734,7 @@
         <v>10444931</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>341</v>
       </c>
@@ -2749,26 +2761,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="13"/>
-    <col min="2" max="2" width="33.88671875" style="13"/>
-    <col min="3" max="3" width="16.44140625" style="14"/>
-    <col min="4" max="4" width="16.44140625" style="11"/>
-    <col min="5" max="5" width="25.5546875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="2"/>
-    <col min="7" max="7" width="40.33203125" style="13"/>
-    <col min="8" max="8" width="9.109375" style="2"/>
-    <col min="9" max="9" width="19.88671875" style="2"/>
-    <col min="10" max="1021" width="9.109375" style="2"/>
-    <col min="1024" max="1026" width="8.6640625"/>
+    <col min="1" max="1" width="20.28515625" style="13"/>
+    <col min="2" max="2" width="33.85546875" style="13"/>
+    <col min="3" max="3" width="16.42578125" style="14"/>
+    <col min="4" max="4" width="16.42578125" style="11"/>
+    <col min="5" max="5" width="25.5703125" style="30" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="2"/>
+    <col min="7" max="7" width="40.28515625" style="13"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="19.85546875" style="2"/>
+    <col min="10" max="1021" width="9.140625" style="2"/>
+    <col min="1024" max="1026" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2797,7 +2809,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>346</v>
       </c>
@@ -2814,7 +2826,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>349</v>
       </c>
@@ -2831,7 +2843,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>350</v>
       </c>
@@ -2867,18 +2879,18 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2904,7 +2916,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>467</v>
       </c>
@@ -2918,7 +2930,7 @@
         <v>10448100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>468</v>
       </c>
@@ -2932,7 +2944,7 @@
         <v>10447000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>469</v>
       </c>
@@ -2959,24 +2971,24 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" style="2"/>
+    <col min="1" max="1" width="38.7109375" style="2"/>
     <col min="2" max="2" width="46" style="35"/>
-    <col min="3" max="3" width="32.88671875" style="2"/>
+    <col min="3" max="3" width="32.85546875" style="2"/>
     <col min="4" max="4" width="45" style="36"/>
-    <col min="5" max="5" width="29.33203125" style="36"/>
-    <col min="6" max="6" width="16.44140625" style="11"/>
-    <col min="7" max="8" width="8.44140625" style="2"/>
-    <col min="9" max="9" width="13.44140625" style="2"/>
-    <col min="10" max="10" width="37.33203125" style="2"/>
-    <col min="11" max="11" width="13.44140625" style="2"/>
-    <col min="12" max="12" width="19.88671875" style="2"/>
-    <col min="13" max="1022" width="8.44140625" style="2"/>
-    <col min="1023" max="1025" width="8.44140625"/>
+    <col min="5" max="5" width="29.28515625" style="36"/>
+    <col min="6" max="6" width="16.42578125" style="11"/>
+    <col min="7" max="8" width="8.42578125" style="2"/>
+    <col min="9" max="9" width="13.42578125" style="2"/>
+    <col min="10" max="10" width="37.28515625" style="2"/>
+    <col min="11" max="11" width="13.42578125" style="2"/>
+    <col min="12" max="12" width="19.85546875" style="2"/>
+    <col min="13" max="1022" width="8.42578125" style="2"/>
+    <col min="1023" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>352</v>
       </c>
@@ -3014,7 +3026,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>359</v>
       </c>
@@ -3039,7 +3051,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>365</v>
       </c>
@@ -3061,7 +3073,7 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>367</v>
       </c>
@@ -3083,7 +3095,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>369</v>
       </c>
@@ -3123,18 +3135,18 @@
       <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" style="39"/>
-    <col min="2" max="2" width="8.5546875" style="39"/>
-    <col min="3" max="3" width="11.5546875" style="39"/>
-    <col min="4" max="4" width="10.44140625" style="39"/>
-    <col min="5" max="5" width="10.6640625" style="39"/>
-    <col min="6" max="6" width="19.88671875" style="39"/>
-    <col min="7" max="1025" width="8.5546875" style="39"/>
+    <col min="1" max="1" width="19.42578125" style="39"/>
+    <col min="2" max="2" width="8.5703125" style="39"/>
+    <col min="3" max="3" width="11.5703125" style="39"/>
+    <col min="4" max="4" width="10.42578125" style="39"/>
+    <col min="5" max="5" width="10.7109375" style="39"/>
+    <col min="6" max="6" width="19.85546875" style="39"/>
+    <col min="7" max="1025" width="8.5703125" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="40" customFormat="1" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="40" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>372</v>
       </c>
@@ -3154,7 +3166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>375</v>
       </c>
@@ -3168,7 +3180,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>378</v>
       </c>
@@ -3182,7 +3194,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>381</v>
       </c>
@@ -3193,7 +3205,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
         <v>383</v>
       </c>
@@ -3204,7 +3216,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>384</v>
       </c>
@@ -3215,7 +3227,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
         <v>385</v>
       </c>
@@ -3226,7 +3238,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
         <v>386</v>
       </c>
@@ -3237,7 +3249,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
         <v>387</v>
       </c>
@@ -3248,7 +3260,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>388</v>
       </c>
@@ -3259,7 +3271,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>389</v>
       </c>
@@ -3270,7 +3282,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>390</v>
       </c>
@@ -3295,17 +3307,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16"/>
-    <col min="4" max="4" width="15.44140625"/>
+    <col min="4" max="4" width="15.42578125"/>
     <col min="5" max="5" width="14"/>
-    <col min="6" max="6" width="10.5546875"/>
-    <col min="7" max="7" width="11.109375"/>
-    <col min="8" max="8" width="20.5546875"/>
+    <col min="6" max="6" width="10.5703125"/>
+    <col min="7" max="7" width="11.140625"/>
+    <col min="8" max="8" width="20.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3331,7 +3343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>393</v>
       </c>
@@ -3357,19 +3369,19 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="2"/>
-    <col min="2" max="2" width="23.44140625" style="2"/>
-    <col min="3" max="3" width="17.6640625" style="2"/>
-    <col min="4" max="4" width="18.6640625" style="2"/>
-    <col min="5" max="5" width="12.6640625" style="2"/>
-    <col min="6" max="6" width="14.6640625" style="2"/>
-    <col min="7" max="1022" width="37.33203125" style="2"/>
-    <col min="1023" max="1025" width="8.44140625"/>
+    <col min="1" max="1" width="18.7109375" style="2"/>
+    <col min="2" max="2" width="23.42578125" style="2"/>
+    <col min="3" max="3" width="17.7109375" style="2"/>
+    <col min="4" max="4" width="18.7109375" style="2"/>
+    <col min="5" max="5" width="12.7109375" style="2"/>
+    <col min="6" max="6" width="14.7109375" style="2"/>
+    <col min="7" max="1022" width="37.28515625" style="2"/>
+    <col min="1023" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3395,7 +3407,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>398</v>
       </c>
@@ -3412,7 +3424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>402</v>
       </c>
@@ -3429,7 +3441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>405</v>
       </c>
@@ -3446,7 +3458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>408</v>
       </c>
@@ -3463,7 +3475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -3480,7 +3492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>412</v>
       </c>
@@ -3497,7 +3509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>415</v>
       </c>
@@ -3536,20 +3548,20 @@
       <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="42"/>
-    <col min="2" max="2" width="10.6640625" style="42"/>
-    <col min="3" max="3" width="10.44140625" style="42"/>
+    <col min="1" max="1" width="20.28515625" style="42"/>
+    <col min="2" max="2" width="10.7109375" style="42"/>
+    <col min="3" max="3" width="10.42578125" style="42"/>
     <col min="4" max="4" width="11" style="42"/>
-    <col min="5" max="5" width="6.5546875" style="42"/>
-    <col min="6" max="6" width="28.6640625" style="42"/>
+    <col min="5" max="5" width="6.5703125" style="42"/>
+    <col min="6" max="6" width="28.7109375" style="42"/>
     <col min="7" max="7" width="11" style="42"/>
     <col min="8" max="8" width="20" style="42"/>
-    <col min="9" max="1025" width="8.6640625" style="42"/>
+    <col min="9" max="1025" width="8.7109375" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>416</v>
       </c>
@@ -3575,7 +3587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>398</v>
       </c>
@@ -3590,7 +3602,7 @@
       <c r="F2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>402</v>
       </c>
@@ -3607,7 +3619,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>405</v>
       </c>
@@ -3628,7 +3640,7 @@
       </c>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
         <v>408</v>
       </c>
@@ -3643,7 +3655,7 @@
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>37</v>
       </c>
@@ -3658,7 +3670,7 @@
       </c>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>37</v>
       </c>
@@ -3670,7 +3682,7 @@
       </c>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>412</v>
       </c>
@@ -3684,7 +3696,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
         <v>415</v>
       </c>
@@ -3711,16 +3723,16 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="8.5546875"/>
-    <col min="6" max="6" width="10.5546875"/>
-    <col min="7" max="7" width="11.109375"/>
-    <col min="8" max="8" width="20.5546875"/>
-    <col min="9" max="1025" width="8.5546875"/>
+    <col min="1" max="5" width="8.5703125"/>
+    <col min="6" max="6" width="10.5703125"/>
+    <col min="7" max="7" width="11.140625"/>
+    <col min="8" max="8" width="20.5703125"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3746,7 +3758,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>437</v>
       </c>
@@ -3766,7 +3778,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>441</v>
       </c>
@@ -3786,7 +3798,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>444</v>
       </c>
@@ -3806,7 +3818,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>446</v>
       </c>
@@ -3843,14 +3855,14 @@
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="6"/>
-    <col min="2" max="2" width="51.109375" style="2"/>
-    <col min="3" max="1025" width="8.44140625"/>
+    <col min="1" max="1" width="16.42578125" style="6"/>
+    <col min="2" max="2" width="51.140625" style="2"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3858,7 +3870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -3866,7 +3878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
@@ -3874,7 +3886,7 @@
         <v>9606</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -3894,18 +3906,18 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625"/>
-    <col min="2" max="2" width="15.5546875"/>
-    <col min="4" max="4" width="13.109375"/>
-    <col min="5" max="5" width="10.5546875"/>
-    <col min="6" max="6" width="11.109375"/>
-    <col min="7" max="7" width="19.88671875"/>
-    <col min="1021" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="17.7109375"/>
+    <col min="2" max="2" width="15.5703125"/>
+    <col min="4" max="4" width="13.140625"/>
+    <col min="5" max="5" width="10.5703125"/>
+    <col min="6" max="6" width="11.140625"/>
+    <col min="7" max="7" width="19.85546875"/>
+    <col min="1021" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>352</v>
       </c>
@@ -3928,7 +3940,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>448</v>
       </c>
@@ -3942,7 +3954,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>451</v>
       </c>
@@ -3956,7 +3968,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>454</v>
       </c>
@@ -3970,7 +3982,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>457</v>
       </c>
@@ -4002,14 +4014,14 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875"/>
-    <col min="2" max="2" width="18.5546875"/>
-    <col min="3" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="18.5703125"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>460</v>
       </c>
@@ -4017,7 +4029,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>364</v>
       </c>
@@ -4025,7 +4037,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>380</v>
       </c>
@@ -4033,7 +4045,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>464</v>
       </c>
@@ -4055,19 +4067,19 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="7"/>
-    <col min="2" max="2" width="16.109375" style="2"/>
-    <col min="3" max="3" width="17.6640625" style="2"/>
-    <col min="4" max="4" width="11.33203125" style="2"/>
-    <col min="5" max="5" width="11.109375" style="2"/>
-    <col min="6" max="6" width="20.5546875" style="2"/>
-    <col min="7" max="1020" width="9.109375" style="2"/>
-    <col min="1024" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="16.140625" style="2"/>
+    <col min="3" max="3" width="17.7109375" style="2"/>
+    <col min="4" max="4" width="11.28515625" style="2"/>
+    <col min="5" max="5" width="11.140625" style="2"/>
+    <col min="6" max="6" width="20.5703125" style="2"/>
+    <col min="7" max="1020" width="9.140625" style="2"/>
+    <col min="1024" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4087,7 +4099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -4104,7 +4116,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -4116,7 +4128,7 @@
       </c>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -4130,7 +4142,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
@@ -4156,19 +4168,19 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="9"/>
-    <col min="2" max="2" width="39.44140625" style="9"/>
-    <col min="3" max="3" width="13.6640625" style="2"/>
-    <col min="4" max="4" width="10.6640625" style="2"/>
+    <col min="1" max="1" width="23.85546875" style="9"/>
+    <col min="2" max="2" width="39.42578125" style="9"/>
+    <col min="3" max="3" width="13.7109375" style="2"/>
+    <col min="4" max="4" width="10.7109375" style="2"/>
     <col min="5" max="5" width="55" style="9"/>
-    <col min="6" max="6" width="9.109375" style="2"/>
-    <col min="7" max="7" width="19.88671875" style="2"/>
-    <col min="8" max="1022" width="9.109375" style="2"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="19.85546875" style="2"/>
+    <col min="8" max="1022" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4191,7 +4203,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -4199,7 +4211,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -4210,7 +4222,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4218,7 +4230,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -4226,7 +4238,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>40</v>
       </c>
@@ -4237,7 +4249,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>43</v>
       </c>
@@ -4248,7 +4260,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>46</v>
       </c>
@@ -4259,7 +4271,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>49</v>
       </c>
@@ -4288,20 +4300,20 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" style="7"/>
+    <col min="1" max="1" width="14.140625" style="7"/>
     <col min="2" max="2" width="13" style="11"/>
-    <col min="3" max="4" width="11.6640625" style="2"/>
-    <col min="5" max="5" width="22.109375" style="2"/>
-    <col min="6" max="6" width="9.109375" style="2"/>
-    <col min="7" max="8" width="13.44140625" style="2"/>
-    <col min="9" max="9" width="13.44140625"/>
-    <col min="10" max="10" width="19.88671875"/>
-    <col min="11" max="12" width="13.44140625"/>
+    <col min="3" max="4" width="11.7109375" style="2"/>
+    <col min="5" max="5" width="22.140625" style="2"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="8" width="13.42578125" style="2"/>
+    <col min="9" max="9" width="13.42578125"/>
+    <col min="10" max="10" width="19.85546875"/>
+    <col min="11" max="12" width="13.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4333,7 +4345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>56</v>
       </c>
@@ -4352,7 +4364,7 @@
       </c>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>57</v>
       </c>
@@ -4369,7 +4381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>58</v>
       </c>
@@ -4386,7 +4398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>59</v>
       </c>
@@ -4403,7 +4415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>60</v>
       </c>
@@ -4420,7 +4432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>61</v>
       </c>
@@ -4437,7 +4449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>62</v>
       </c>
@@ -4454,7 +4466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>63</v>
       </c>
@@ -4471,7 +4483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>64</v>
       </c>
@@ -4488,7 +4500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>65</v>
       </c>
@@ -4505,7 +4517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>66</v>
       </c>
@@ -4522,7 +4534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>67</v>
       </c>
@@ -4539,7 +4551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>68</v>
       </c>
@@ -4556,7 +4568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>69</v>
       </c>
@@ -4573,7 +4585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>70</v>
       </c>
@@ -4590,7 +4602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>71</v>
       </c>
@@ -4607,7 +4619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>72</v>
       </c>
@@ -4624,7 +4636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>73</v>
       </c>
@@ -4641,7 +4653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>74</v>
       </c>
@@ -4658,7 +4670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>75</v>
       </c>
@@ -4675,7 +4687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>76</v>
       </c>
@@ -4692,7 +4704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>77</v>
       </c>
@@ -4709,7 +4721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>78</v>
       </c>
@@ -4726,7 +4738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>79</v>
       </c>
@@ -4743,7 +4755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>80</v>
       </c>
@@ -4778,19 +4790,19 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="11"/>
-    <col min="2" max="2" width="16.44140625" style="11"/>
-    <col min="3" max="3" width="42.44140625" style="13"/>
-    <col min="4" max="6" width="13.44140625" style="14"/>
-    <col min="7" max="8" width="13.44140625" style="11"/>
-    <col min="9" max="9" width="16.44140625" style="15"/>
-    <col min="10" max="1023" width="32.5546875" style="2"/>
-    <col min="1024" max="1025" width="8.44140625"/>
+    <col min="1" max="1" width="17.42578125" style="11"/>
+    <col min="2" max="2" width="16.42578125" style="11"/>
+    <col min="3" max="3" width="42.42578125" style="13"/>
+    <col min="4" max="6" width="13.42578125" style="14"/>
+    <col min="7" max="8" width="13.42578125" style="11"/>
+    <col min="9" max="9" width="16.42578125" style="15"/>
+    <col min="10" max="1023" width="32.5703125" style="2"/>
+    <col min="1024" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1023" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4831,7 +4843,7 @@
       <c r="AMH1" s="2"/>
       <c r="AMI1" s="2"/>
     </row>
-    <row r="2" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>87</v>
       </c>
@@ -4857,7 +4869,7 @@
         <v>20651511</v>
       </c>
     </row>
-    <row r="3" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>92</v>
       </c>
@@ -4883,7 +4895,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="4" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>96</v>
       </c>
@@ -4909,7 +4921,7 @@
         <v>69387254</v>
       </c>
     </row>
-    <row r="5" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>99</v>
       </c>
@@ -4935,7 +4947,7 @@
         <v>40574685</v>
       </c>
     </row>
-    <row r="6" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>102</v>
       </c>
@@ -4961,7 +4973,7 @@
         <v>112649530</v>
       </c>
     </row>
-    <row r="7" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>105</v>
       </c>
@@ -4987,7 +4999,7 @@
         <v>83605875</v>
       </c>
     </row>
-    <row r="8" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>108</v>
       </c>
@@ -5013,7 +5025,7 @@
         <v>127899195</v>
       </c>
     </row>
-    <row r="9" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>111</v>
       </c>
@@ -5039,7 +5051,7 @@
         <v>160421711</v>
       </c>
     </row>
-    <row r="10" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>114</v>
       </c>
@@ -5065,7 +5077,7 @@
         <v>152129619</v>
       </c>
     </row>
-    <row r="11" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>117</v>
       </c>
@@ -5091,7 +5103,7 @@
         <v>56051604</v>
       </c>
     </row>
-    <row r="12" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>120</v>
       </c>
@@ -5117,7 +5129,7 @@
         <v>18084998</v>
       </c>
     </row>
-    <row r="13" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>123</v>
       </c>
@@ -5143,7 +5155,7 @@
         <v>19967258</v>
       </c>
     </row>
-    <row r="14" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1023" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>126</v>
       </c>
@@ -5169,7 +5181,7 @@
         <v>136423761</v>
       </c>
     </row>
-    <row r="15" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>129</v>
       </c>
@@ -5195,7 +5207,7 @@
         <v>7787981</v>
       </c>
     </row>
-    <row r="16" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>132</v>
       </c>
@@ -5221,7 +5233,7 @@
         <v>133421307</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>135</v>
       </c>
@@ -5247,7 +5259,7 @@
         <v>13732346</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>138</v>
       </c>
@@ -5273,7 +5285,7 @@
         <v>114450279</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>141</v>
       </c>
@@ -5299,7 +5311,7 @@
         <v>77065580</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>144</v>
       </c>
@@ -5325,7 +5337,7 @@
         <v>113359493</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>147</v>
       </c>
@@ -5351,7 +5363,7 @@
         <v>52476628</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>150</v>
       </c>
@@ -5377,7 +5389,7 @@
         <v>103057462</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>153</v>
       </c>
@@ -5403,7 +5415,7 @@
         <v>65578352</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>156</v>
       </c>
@@ -5429,7 +5441,7 @@
         <v>101251932</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>159</v>
       </c>
@@ -5455,7 +5467,7 @@
         <v>89155846</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>162</v>
       </c>
@@ -5481,7 +5493,7 @@
         <v>49223225</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>165</v>
       </c>
@@ -5507,7 +5519,7 @@
         <v>50988121</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>168</v>
       </c>
@@ -5533,7 +5545,7 @@
         <v>41440717</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>171</v>
       </c>
@@ -5559,7 +5571,7 @@
         <v>47784686</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>174</v>
       </c>
@@ -5585,7 +5597,7 @@
         <v>13638940</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>177</v>
       </c>
@@ -5611,7 +5623,7 @@
         <v>44652233</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>180</v>
       </c>
@@ -5637,7 +5649,7 @@
         <v>31668931</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>183</v>
       </c>
@@ -5663,7 +5675,7 @@
         <v>20859417</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>186</v>
       </c>
@@ -5689,7 +5701,7 @@
         <v>38738299</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>189</v>
       </c>
@@ -5715,7 +5727,7 @@
         <v>119605895</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>192</v>
       </c>
@@ -5741,7 +5753,7 @@
         <v>23005465</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>195</v>
       </c>
@@ -5780,32 +5792,35 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMG37"/>
+  <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="16.44140625" style="11"/>
+    <col min="1" max="3" width="16.42578125" style="11"/>
     <col min="4" max="4" width="22" style="11"/>
-    <col min="5" max="5" width="13.6640625" style="11"/>
-    <col min="6" max="6" width="25.109375" style="11"/>
-    <col min="7" max="7" width="13.44140625" style="11"/>
-    <col min="8" max="8" width="23.33203125" style="11"/>
-    <col min="9" max="9" width="25.109375" style="2"/>
-    <col min="10" max="10" width="19.88671875"/>
-    <col min="11" max="11" width="9.109375" style="14"/>
-    <col min="12" max="12" width="10.44140625" style="14"/>
-    <col min="13" max="13" width="10.6640625" style="14"/>
-    <col min="14" max="15" width="9.109375" style="11"/>
-    <col min="16" max="16" width="22.88671875" style="14"/>
-    <col min="17" max="1012" width="9.109375" style="11"/>
-    <col min="1013" max="1021" width="9.109375" style="2"/>
+    <col min="5" max="5" width="13.7109375" style="11"/>
+    <col min="6" max="6" width="25.140625" style="11"/>
+    <col min="7" max="7" width="13.42578125" style="11"/>
+    <col min="8" max="8" width="16.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="30" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" style="11"/>
+    <col min="12" max="12" width="25.140625" style="2"/>
+    <col min="13" max="13" width="19.85546875"/>
+    <col min="14" max="14" width="9.140625" style="14"/>
+    <col min="15" max="15" width="10.42578125" style="14"/>
+    <col min="16" max="16" width="10.7109375" style="14"/>
+    <col min="17" max="18" width="9.140625" style="11"/>
+    <col min="19" max="19" width="22.85546875" style="14"/>
+    <col min="20" max="1015" width="9.140625" style="11"/>
+    <col min="1016" max="1024" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1021" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1024" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -5827,32 +5842,41 @@
       <c r="G1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
       <c r="P1" s="20"/>
-      <c r="ALY1" s="1"/>
-      <c r="ALZ1" s="1"/>
-      <c r="AMA1" s="1"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="20"/>
       <c r="AMB1" s="1"/>
       <c r="AMC1" s="1"/>
       <c r="AMD1" s="1"/>
       <c r="AME1" s="1"/>
       <c r="AMF1" s="1"/>
       <c r="AMG1" s="1"/>
-    </row>
-    <row r="2" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="AMH1" s="1"/>
+      <c r="AMI1" s="1"/>
+      <c r="AMJ1" s="1"/>
+    </row>
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>199</v>
       </c>
@@ -5874,12 +5898,18 @@
       <c r="G2" s="11">
         <v>203895200</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="5"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-    </row>
-    <row r="3" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H2" s="30">
+        <v>203893820</v>
+      </c>
+      <c r="I2" s="30">
+        <v>203895200</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="5"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+    </row>
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>203</v>
       </c>
@@ -5901,12 +5931,18 @@
       <c r="G3" s="11">
         <v>20605200</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="5"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-    </row>
-    <row r="4" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H3" s="30">
+        <v>20602802</v>
+      </c>
+      <c r="I3" s="30">
+        <v>20605200</v>
+      </c>
+      <c r="K3" s="14"/>
+      <c r="L3" s="5"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+    </row>
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>206</v>
       </c>
@@ -5928,12 +5964,18 @@
       <c r="G4" s="11">
         <v>45648411</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="5"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-    </row>
-    <row r="5" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H4" s="30">
+        <v>45648015</v>
+      </c>
+      <c r="I4" s="30">
+        <v>45648411</v>
+      </c>
+      <c r="K4" s="14"/>
+      <c r="L4" s="5"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+    </row>
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>210</v>
       </c>
@@ -5955,12 +5997,18 @@
       <c r="G5" s="11">
         <v>85414201</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="5"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-    </row>
-    <row r="6" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H5" s="30">
+        <v>85413000</v>
+      </c>
+      <c r="I5" s="30">
+        <v>85414201</v>
+      </c>
+      <c r="K5" s="14"/>
+      <c r="L5" s="5"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+    </row>
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>214</v>
       </c>
@@ -5982,12 +6030,18 @@
       <c r="G6" s="11">
         <v>39878600</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="5"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-    </row>
-    <row r="7" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H6" s="30">
+        <v>39877210</v>
+      </c>
+      <c r="I6" s="30">
+        <v>39878600</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="5"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+    </row>
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>217</v>
       </c>
@@ -6009,12 +6063,18 @@
       <c r="G7" s="11">
         <v>185318582</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="5"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-    </row>
-    <row r="8" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H7" s="30">
+        <v>185316402</v>
+      </c>
+      <c r="I7" s="30">
+        <v>185318582</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="5"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+    </row>
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>219</v>
       </c>
@@ -6036,12 +6096,18 @@
       <c r="G8" s="11">
         <v>53863800</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="5"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-    </row>
-    <row r="9" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H8" s="30">
+        <v>53862600</v>
+      </c>
+      <c r="I8" s="30">
+        <v>53863800</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="L8" s="5"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>222</v>
       </c>
@@ -6063,12 +6129,18 @@
       <c r="G9" s="11">
         <v>118837001</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="5"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-    </row>
-    <row r="10" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H9" s="30">
+        <v>118834600</v>
+      </c>
+      <c r="I9" s="30">
+        <v>118837001</v>
+      </c>
+      <c r="K9" s="14"/>
+      <c r="L9" s="5"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+    </row>
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>224</v>
       </c>
@@ -6090,12 +6162,18 @@
       <c r="G10" s="11">
         <v>141851600</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="5"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-    </row>
-    <row r="11" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H10" s="30">
+        <v>141848202</v>
+      </c>
+      <c r="I10" s="30">
+        <v>141851600</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="5"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+    </row>
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>226</v>
       </c>
@@ -6117,12 +6195,18 @@
       <c r="G11" s="11">
         <v>2991401</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="5"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-    </row>
-    <row r="12" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H11" s="30">
+        <v>2988400</v>
+      </c>
+      <c r="I11" s="30">
+        <v>2991400</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="5"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+    </row>
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>228</v>
       </c>
@@ -6144,12 +6228,18 @@
       <c r="G12" s="11">
         <v>43971001</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="5"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-    </row>
-    <row r="13" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H12" s="30">
+        <v>43970600</v>
+      </c>
+      <c r="I12" s="30">
+        <v>43971001</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="5"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+    </row>
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>230</v>
       </c>
@@ -6171,12 +6261,18 @@
       <c r="G13" s="11">
         <v>893236</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="5"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-    </row>
-    <row r="14" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H13" s="30">
+        <v>890483</v>
+      </c>
+      <c r="I13" s="30">
+        <v>893236</v>
+      </c>
+      <c r="K13" s="14"/>
+      <c r="L13" s="5"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+    </row>
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>232</v>
       </c>
@@ -6198,12 +6294,18 @@
       <c r="G14" s="11">
         <v>116112801</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="5"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-    </row>
-    <row r="15" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H14" s="30">
+        <v>116112401</v>
+      </c>
+      <c r="I14" s="30">
+        <v>116112801</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="5"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+    </row>
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>234</v>
       </c>
@@ -6225,12 +6327,21 @@
       <c r="G15" s="11">
         <v>72121926</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="5"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-    </row>
-    <row r="16" spans="1:1021" x14ac:dyDescent="0.3">
+      <c r="H15" s="30">
+        <v>72121544</v>
+      </c>
+      <c r="I15" s="30">
+        <v>72121926</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="5"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+    </row>
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>237</v>
       </c>
@@ -6252,12 +6363,18 @@
       <c r="G16" s="11">
         <v>22702000</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="5"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H16" s="30">
+        <v>22700001</v>
+      </c>
+      <c r="I16" s="30">
+        <v>22702000</v>
+      </c>
+      <c r="K16" s="14"/>
+      <c r="L16" s="5"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>239</v>
       </c>
@@ -6279,12 +6396,18 @@
       <c r="G17" s="11">
         <v>46023801</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="5"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H17" s="30">
+        <v>46022400</v>
+      </c>
+      <c r="I17" s="30">
+        <v>46023801</v>
+      </c>
+      <c r="K17" s="14"/>
+      <c r="L17" s="5"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>241</v>
       </c>
@@ -6306,12 +6429,18 @@
       <c r="G18" s="11">
         <v>132187000</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="5"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H18" s="30">
+        <v>132186801</v>
+      </c>
+      <c r="I18" s="30">
+        <v>132187000</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="L18" s="5"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+    </row>
+    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>243</v>
       </c>
@@ -6333,12 +6462,21 @@
       <c r="G19" s="11">
         <v>102368872</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="5"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H19" s="30">
+        <v>102368448</v>
+      </c>
+      <c r="I19" s="30">
+        <v>102368872</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="K19" s="14"/>
+      <c r="L19" s="5"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>245</v>
       </c>
@@ -6360,12 +6498,18 @@
       <c r="G20" s="11">
         <v>101940201</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="5"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H20" s="30">
+        <v>101939801</v>
+      </c>
+      <c r="I20" s="30">
+        <v>101940201</v>
+      </c>
+      <c r="K20" s="14"/>
+      <c r="L20" s="5"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>247</v>
       </c>
@@ -6387,12 +6531,18 @@
       <c r="G21" s="11">
         <v>99985401</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="5"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H21" s="30">
+        <v>99984000</v>
+      </c>
+      <c r="I21" s="30">
+        <v>99985401</v>
+      </c>
+      <c r="K21" s="14"/>
+      <c r="L21" s="5"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>249</v>
       </c>
@@ -6414,12 +6564,18 @@
       <c r="G22" s="11">
         <v>52849993</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="5"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H22" s="30">
+        <v>52849669</v>
+      </c>
+      <c r="I22" s="30">
+        <v>52849993</v>
+      </c>
+      <c r="K22" s="14"/>
+      <c r="L22" s="5"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>251</v>
       </c>
@@ -6441,12 +6597,18 @@
       <c r="G23" s="11">
         <v>23579130</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="5"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H23" s="30">
+        <v>23578503</v>
+      </c>
+      <c r="I23" s="30">
+        <v>23579130</v>
+      </c>
+      <c r="K23" s="14"/>
+      <c r="L23" s="5"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>253</v>
       </c>
@@ -6468,12 +6630,18 @@
       <c r="G24" s="11">
         <v>90215000</v>
       </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="5"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H24" s="30">
+        <v>90214601</v>
+      </c>
+      <c r="I24" s="30">
+        <v>90215000</v>
+      </c>
+      <c r="K24" s="14"/>
+      <c r="L24" s="5"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>255</v>
       </c>
@@ -6495,12 +6663,18 @@
       <c r="G25" s="11">
         <v>47720200</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="5"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H25" s="30">
+        <v>47716801</v>
+      </c>
+      <c r="I25" s="30">
+        <v>47720200</v>
+      </c>
+      <c r="K25" s="14"/>
+      <c r="L25" s="5"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>257</v>
       </c>
@@ -6522,12 +6696,18 @@
       <c r="G26" s="11">
         <v>50369600</v>
       </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="5"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H26" s="30">
+        <v>50368000</v>
+      </c>
+      <c r="I26" s="30">
+        <v>50369600</v>
+      </c>
+      <c r="K26" s="14"/>
+      <c r="L26" s="5"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>259</v>
       </c>
@@ -6549,12 +6729,18 @@
       <c r="G27" s="11">
         <v>18650600</v>
       </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="5"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H27" s="30">
+        <v>18650001</v>
+      </c>
+      <c r="I27" s="30">
+        <v>18650600</v>
+      </c>
+      <c r="K27" s="14"/>
+      <c r="L27" s="5"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>261</v>
       </c>
@@ -6576,12 +6762,18 @@
       <c r="G28" s="11">
         <v>33756401</v>
       </c>
-      <c r="H28" s="14"/>
-      <c r="I28" s="5"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H28" s="30">
+        <v>33756200</v>
+      </c>
+      <c r="I28" s="30">
+        <v>33756401</v>
+      </c>
+      <c r="K28" s="14"/>
+      <c r="L28" s="5"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>263</v>
       </c>
@@ -6603,12 +6795,18 @@
       <c r="G29" s="11">
         <v>58328001</v>
       </c>
-      <c r="H29" s="14"/>
-      <c r="I29" s="5"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H29" s="30">
+        <v>58326200</v>
+      </c>
+      <c r="I29" s="30">
+        <v>58328001</v>
+      </c>
+      <c r="K29" s="14"/>
+      <c r="L29" s="5"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>265</v>
       </c>
@@ -6630,12 +6828,18 @@
       <c r="G30" s="11">
         <v>50118213</v>
       </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="5"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H30" s="30">
+        <v>50117624</v>
+      </c>
+      <c r="I30" s="30">
+        <v>50118213</v>
+      </c>
+      <c r="K30" s="14"/>
+      <c r="L30" s="5"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>267</v>
       </c>
@@ -6657,12 +6861,18 @@
       <c r="G31" s="11">
         <v>62961734</v>
       </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="5"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H31" s="30">
+        <v>62960832</v>
+      </c>
+      <c r="I31" s="30">
+        <v>62961734</v>
+      </c>
+      <c r="K31" s="14"/>
+      <c r="L31" s="5"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="22"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>269</v>
       </c>
@@ -6684,12 +6894,18 @@
       <c r="G32" s="11">
         <v>57964896</v>
       </c>
-      <c r="H32" s="14"/>
-      <c r="I32" s="5"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H32" s="30">
+        <v>57964075</v>
+      </c>
+      <c r="I32" s="30">
+        <v>57964896</v>
+      </c>
+      <c r="K32" s="14"/>
+      <c r="L32" s="5"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>271</v>
       </c>
@@ -6711,12 +6927,18 @@
       <c r="G33" s="11">
         <v>36711020</v>
       </c>
-      <c r="H33" s="14"/>
-      <c r="I33" s="5"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H33" s="30">
+        <v>36710048</v>
+      </c>
+      <c r="I33" s="30">
+        <v>36711020</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="5"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>273</v>
       </c>
@@ -6738,12 +6960,18 @@
       <c r="G34" s="11">
         <v>43346796</v>
       </c>
-      <c r="H34" s="14"/>
-      <c r="I34" s="5"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H34" s="30">
+        <v>43346380</v>
+      </c>
+      <c r="I34" s="30">
+        <v>43346796</v>
+      </c>
+      <c r="K34" s="14"/>
+      <c r="L34" s="5"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>275</v>
       </c>
@@ -6765,12 +6993,18 @@
       <c r="G35" s="11">
         <v>30592601</v>
       </c>
-      <c r="H35" s="14"/>
-      <c r="I35" s="5"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H35" s="30">
+        <v>30591000</v>
+      </c>
+      <c r="I35" s="30">
+        <v>30592601</v>
+      </c>
+      <c r="K35" s="14"/>
+      <c r="L35" s="5"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>277</v>
       </c>
@@ -6792,12 +7026,18 @@
       <c r="G36" s="11">
         <v>135326600</v>
       </c>
-      <c r="H36" s="14"/>
-      <c r="I36" s="5"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H36" s="30">
+        <v>135326401</v>
+      </c>
+      <c r="I36" s="30">
+        <v>135326600</v>
+      </c>
+      <c r="K36" s="14"/>
+      <c r="L36" s="5"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>279</v>
       </c>
@@ -6819,13 +7059,19 @@
       <c r="G37" s="11">
         <v>14200</v>
       </c>
-      <c r="H37" s="14"/>
-      <c r="I37" s="5"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
+      <c r="H37" s="30">
+        <v>13401</v>
+      </c>
+      <c r="I37" s="30">
+        <v>14200</v>
+      </c>
+      <c r="K37" s="14"/>
+      <c r="L37" s="5"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H776"/>
+  <autoFilter ref="A1:K776"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
@@ -6843,21 +7089,21 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="11"/>
-    <col min="2" max="2" width="50.5546875" style="11"/>
-    <col min="3" max="3" width="22.88671875" style="15"/>
-    <col min="4" max="4" width="13.44140625" style="23"/>
-    <col min="5" max="5" width="19.88671875" style="14"/>
-    <col min="6" max="6" width="10.6640625" style="14"/>
-    <col min="7" max="8" width="9.109375" style="11"/>
-    <col min="9" max="1016" width="9.109375" style="23"/>
-    <col min="1017" max="1019" width="8.44140625"/>
-    <col min="1020" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="17.42578125" style="11"/>
+    <col min="2" max="2" width="50.5703125" style="11"/>
+    <col min="3" max="3" width="22.85546875" style="15"/>
+    <col min="4" max="4" width="13.42578125" style="23"/>
+    <col min="5" max="5" width="19.85546875" style="14"/>
+    <col min="6" max="6" width="10.7109375" style="14"/>
+    <col min="7" max="8" width="9.140625" style="11"/>
+    <col min="9" max="1016" width="9.140625" style="23"/>
+    <col min="1017" max="1019" width="8.42578125"/>
+    <col min="1020" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>281</v>
       </c>
@@ -6875,7 +7121,7 @@
       </c>
       <c r="F1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>92</v>
       </c>
@@ -6886,7 +7132,7 @@
       <c r="H2" s="22"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>108</v>
       </c>
@@ -6916,23 +7162,23 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" style="14"/>
-    <col min="2" max="2" width="21.109375" style="14"/>
-    <col min="3" max="3" width="10.6640625" style="14"/>
-    <col min="4" max="4" width="22.88671875" style="15"/>
-    <col min="5" max="5" width="10.6640625"/>
-    <col min="6" max="6" width="13.44140625"/>
-    <col min="7" max="7" width="13.44140625" style="11"/>
-    <col min="8" max="8" width="13.44140625" style="25"/>
-    <col min="9" max="9" width="10.6640625" style="22"/>
-    <col min="10" max="10" width="19.88671875" style="11"/>
-    <col min="11" max="11" width="13.44140625" style="11"/>
-    <col min="12" max="1021" width="9.109375" style="2"/>
+    <col min="1" max="1" width="19.5703125" style="14"/>
+    <col min="2" max="2" width="21.140625" style="14"/>
+    <col min="3" max="3" width="10.7109375" style="14"/>
+    <col min="4" max="4" width="22.85546875" style="15"/>
+    <col min="5" max="5" width="10.7109375"/>
+    <col min="6" max="6" width="13.42578125"/>
+    <col min="7" max="7" width="13.42578125" style="11"/>
+    <col min="8" max="8" width="13.42578125" style="25"/>
+    <col min="9" max="9" width="10.7109375" style="22"/>
+    <col min="10" max="10" width="19.85546875" style="11"/>
+    <col min="11" max="11" width="13.42578125" style="11"/>
+    <col min="12" max="1021" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -6965,7 +7211,7 @@
       </c>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>285</v>
       </c>
@@ -6991,7 +7237,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>287</v>
       </c>

</xml_diff>

<commit_message>
Change CDS attribute to match annotation format
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="478">
   <si>
     <t>Id</t>
   </si>
@@ -1493,18 +1493,6 @@
     <t>Ploidy</t>
   </si>
   <si>
-    <t>CDS_ENSP00000234111</t>
-  </si>
-  <si>
-    <t>CDS_ENSP00000385333</t>
-  </si>
-  <si>
-    <t>CDS_ENSP00000390691</t>
-  </si>
-  <si>
-    <t>Coding Region</t>
-  </si>
-  <si>
     <t>Bound End</t>
   </si>
   <si>
@@ -1518,6 +1506,27 @@
   </si>
   <si>
     <t>Sequence Path</t>
+  </si>
+  <si>
+    <t>Exon</t>
+  </si>
+  <si>
+    <t>cds_1</t>
+  </si>
+  <si>
+    <t>cds_2</t>
+  </si>
+  <si>
+    <t>cds_3</t>
+  </si>
+  <si>
+    <t>cds_4</t>
+  </si>
+  <si>
+    <t>cds_1, cds_2</t>
+  </si>
+  <si>
+    <t>Coding Regions</t>
   </si>
 </sst>
 </file>
@@ -2236,8 +2245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2345,8 +2354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMG21"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2400,10 +2409,10 @@
         <v>303</v>
       </c>
       <c r="D2" s="32">
+        <v>10439968</v>
+      </c>
+      <c r="E2" s="32">
         <v>10440868</v>
-      </c>
-      <c r="E2" s="32">
-        <v>10439968</v>
       </c>
       <c r="AMF2" s="33"/>
       <c r="AMG2" s="33"/>
@@ -2419,10 +2428,10 @@
         <v>305</v>
       </c>
       <c r="D3" s="32">
+        <v>10441509</v>
+      </c>
+      <c r="E3" s="32">
         <v>10441723</v>
-      </c>
-      <c r="E3" s="32">
-        <v>10441509</v>
       </c>
       <c r="AMF3" s="33"/>
       <c r="AMG3" s="33"/>
@@ -2438,10 +2447,10 @@
         <v>307</v>
       </c>
       <c r="D4" s="32">
+        <v>10441817</v>
+      </c>
+      <c r="E4" s="32">
         <v>10441929</v>
-      </c>
-      <c r="E4" s="32">
-        <v>10441817</v>
       </c>
       <c r="AMF4" s="33"/>
       <c r="AMG4" s="33"/>
@@ -2457,10 +2466,10 @@
         <v>309</v>
       </c>
       <c r="D5" s="32">
+        <v>10442012</v>
+      </c>
+      <c r="E5" s="32">
         <v>10442174</v>
-      </c>
-      <c r="E5" s="32">
-        <v>10442012</v>
       </c>
       <c r="AMF5" s="33"/>
       <c r="AMG5" s="33"/>
@@ -2476,10 +2485,10 @@
         <v>311</v>
       </c>
       <c r="D6" s="32">
+        <v>10443230</v>
+      </c>
+      <c r="E6" s="32">
         <v>10443313</v>
-      </c>
-      <c r="E6" s="32">
-        <v>10443230</v>
       </c>
       <c r="AMF6" s="33"/>
       <c r="AMG6" s="33"/>
@@ -2495,10 +2504,10 @@
         <v>313</v>
       </c>
       <c r="D7" s="32">
+        <v>10443490</v>
+      </c>
+      <c r="E7" s="32">
         <v>10443571</v>
-      </c>
-      <c r="E7" s="32">
-        <v>10443490</v>
       </c>
       <c r="AMF7" s="33"/>
       <c r="AMG7" s="33"/>
@@ -2514,10 +2523,10 @@
         <v>315</v>
       </c>
       <c r="D8" s="32">
+        <v>10443702</v>
+      </c>
+      <c r="E8" s="32">
         <v>10443836</v>
-      </c>
-      <c r="E8" s="32">
-        <v>10443702</v>
       </c>
       <c r="AMF8" s="33"/>
       <c r="AMG8" s="33"/>
@@ -2533,10 +2542,10 @@
         <v>317</v>
       </c>
       <c r="D9" s="32">
+        <v>10444095</v>
+      </c>
+      <c r="E9" s="32">
         <v>10444267</v>
-      </c>
-      <c r="E9" s="32">
-        <v>10444095</v>
       </c>
       <c r="AMF9" s="33"/>
       <c r="AMG9" s="33"/>
@@ -2552,10 +2561,10 @@
         <v>319</v>
       </c>
       <c r="D10" s="32">
+        <v>10444474</v>
+      </c>
+      <c r="E10" s="32">
         <v>10444647</v>
-      </c>
-      <c r="E10" s="32">
-        <v>10444474</v>
       </c>
       <c r="AMF10" s="33"/>
       <c r="AMG10" s="33"/>
@@ -2571,10 +2580,10 @@
         <v>321</v>
       </c>
       <c r="D11" s="32">
+        <v>10444931</v>
+      </c>
+      <c r="E11" s="32">
         <v>10445049</v>
-      </c>
-      <c r="E11" s="32">
-        <v>10444931</v>
       </c>
       <c r="AMF11" s="33"/>
       <c r="AMG11" s="33"/>
@@ -2590,10 +2599,10 @@
         <v>323</v>
       </c>
       <c r="D12" s="32">
+        <v>10445155</v>
+      </c>
+      <c r="E12" s="32">
         <v>10445264</v>
-      </c>
-      <c r="E12" s="32">
-        <v>10445155</v>
       </c>
       <c r="AMF12" s="33"/>
       <c r="AMG12" s="33"/>
@@ -2609,10 +2618,10 @@
         <v>325</v>
       </c>
       <c r="D13" s="34">
+        <v>10448121</v>
+      </c>
+      <c r="E13" s="34">
         <v>10448504</v>
-      </c>
-      <c r="E13" s="34">
-        <v>10448121</v>
       </c>
     </row>
     <row r="14" spans="1:1021" x14ac:dyDescent="0.3">
@@ -2626,10 +2635,10 @@
         <v>327</v>
       </c>
       <c r="D14" s="34">
+        <v>10440601</v>
+      </c>
+      <c r="E14" s="34">
         <v>10440868</v>
-      </c>
-      <c r="E14" s="34">
-        <v>10440601</v>
       </c>
     </row>
     <row r="15" spans="1:1021" x14ac:dyDescent="0.3">
@@ -2643,10 +2652,10 @@
         <v>329</v>
       </c>
       <c r="D15" s="34">
+        <v>10447474</v>
+      </c>
+      <c r="E15" s="34">
         <v>10447780</v>
-      </c>
-      <c r="E15" s="34">
-        <v>10447474</v>
       </c>
     </row>
     <row r="16" spans="1:1021" x14ac:dyDescent="0.3">
@@ -2660,10 +2669,10 @@
         <v>331</v>
       </c>
       <c r="D16" s="34">
+        <v>10444544</v>
+      </c>
+      <c r="E16" s="34">
         <v>10444647</v>
-      </c>
-      <c r="E16" s="34">
-        <v>10444544</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2677,10 +2686,10 @@
         <v>333</v>
       </c>
       <c r="D17" s="34">
+        <v>10447628</v>
+      </c>
+      <c r="E17" s="34">
         <v>10447788</v>
-      </c>
-      <c r="E17" s="34">
-        <v>10447628</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -2694,10 +2703,10 @@
         <v>335</v>
       </c>
       <c r="D18" s="34">
+        <v>10444095</v>
+      </c>
+      <c r="E18" s="34">
         <v>10444267</v>
-      </c>
-      <c r="E18" s="34">
-        <v>10444095</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -2711,10 +2720,10 @@
         <v>337</v>
       </c>
       <c r="D19" s="34">
+        <v>10444474</v>
+      </c>
+      <c r="E19" s="34">
         <v>10444547</v>
-      </c>
-      <c r="E19" s="34">
-        <v>10444474</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -2728,10 +2737,10 @@
         <v>339</v>
       </c>
       <c r="D20" s="34">
+        <v>10444931</v>
+      </c>
+      <c r="E20" s="34">
         <v>10445049</v>
-      </c>
-      <c r="E20" s="34">
-        <v>10444931</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2745,10 +2754,10 @@
         <v>341</v>
       </c>
       <c r="D21" s="34">
+        <v>10448121</v>
+      </c>
+      <c r="E21" s="34">
         <v>10448309</v>
-      </c>
-      <c r="E21" s="34">
-        <v>10448121</v>
       </c>
     </row>
   </sheetData>
@@ -2761,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMG4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2794,7 +2803,7 @@
         <v>343</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>344</v>
@@ -2823,7 +2832,7 @@
         <v>290</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>466</v>
+        <v>476</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2840,7 +2849,7 @@
         <v>293</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2857,7 +2866,7 @@
         <v>296</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -2873,24 +2882,25 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.88671875" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2900,62 +2910,91 @@
       <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="18" t="s">
+        <v>471</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="32">
-        <v>10439999</v>
-      </c>
-      <c r="E2" s="34">
-        <v>10448100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D2" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="32">
+        <v>10440000</v>
+      </c>
+      <c r="F2" s="32">
+        <v>10440868</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="34">
-        <v>10440600</v>
-      </c>
-      <c r="E3" s="34">
-        <v>10447000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="32">
+        <v>10441509</v>
+      </c>
+      <c r="F3" s="32">
+        <v>10441723</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="34">
-        <v>10444500</v>
-      </c>
-      <c r="E4" s="34">
-        <v>10447601</v>
+        <v>56</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="E4" s="32">
+        <v>10444931</v>
+      </c>
+      <c r="F4" s="32">
+        <v>10445049</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>475</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="E5" s="32">
+        <v>10445155</v>
+      </c>
+      <c r="F5" s="32">
+        <v>10445264</v>
       </c>
     </row>
   </sheetData>
@@ -4321,7 +4360,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>52</v>
@@ -5843,13 +5882,13 @@
         <v>85</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="K1" s="18" t="s">
         <v>11</v>
@@ -6469,7 +6508,7 @@
         <v>102368872</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="K19" s="14"/>
       <c r="L19" s="5"/>

</xml_diff>

<commit_message>
Add attributes to RegulatoryModule class to cover available data
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -38,32 +38,32 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="11">'Protein species types'!$A$1:$G$719</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17">'Rate laws'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16">Reactions!$A$1:$F$220</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6">'Regulatory element loci'!$A$1:$K$776</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7">'Regulatory module'!$A$1:$C$849</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6">'Regulatory element loci'!$A$1:$L$776</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7">'Regulatory module'!$A$1:$H$849</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">'Gene loci'!$I$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="8">'pre-RNA species types'!$A$1:$G$915</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="11">'Protein species types'!$A$1:$G$719</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="6">'Regulatory element loci'!$A$1:$K$776</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="7">'Regulatory module'!$A$1:$C$849</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'Regulatory element loci'!$A$1:$L$776</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="7">'Regulatory module'!$A$1:$H$849</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="5">'Gene loci'!$B$1:$H$1064</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="8">'pre-RNA species types'!$A$1:$G$915</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Regulatory element loci'!$A$1:$K$776</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="7">'Regulatory module'!$A$1:$C$849</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Regulatory element loci'!$A$1:$L$776</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="7">'Regulatory module'!$A$1:$H$849</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Gene loci'!$I$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="8">'pre-RNA species types'!$A$1:$G$915</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Regulatory element loci'!$A$1:$K$776</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="7">'Regulatory module'!$A$1:$C$849</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Regulatory element loci'!$A$1:$L$776</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="7">'Regulatory module'!$A$1:$H$849</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">'Gene loci'!$B$1:$H$1064</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="8">'pre-RNA species types'!$A$1:$G$849</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Regulatory element loci'!$A$2:$S$849</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Regulatory element loci'!$A$2:$T$849</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">'Gene loci'!$I$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="490">
   <si>
     <t>Id</t>
   </si>
@@ -938,12 +938,6 @@
     <t>Gene</t>
   </si>
   <si>
-    <t>Regulatory Elements</t>
-  </si>
-  <si>
-    <t>ENSR00000309980, ENSR00000172399</t>
-  </si>
-  <si>
     <t>Double stranded</t>
   </si>
   <si>
@@ -1527,6 +1521,48 @@
   </si>
   <si>
     <t>Coding Regions</t>
+  </si>
+  <si>
+    <t>Regulatory Element</t>
+  </si>
+  <si>
+    <t>Binding factor</t>
+  </si>
+  <si>
+    <t>proximal</t>
+  </si>
+  <si>
+    <t>distal</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>rm1</t>
+  </si>
+  <si>
+    <t>rm2</t>
+  </si>
+  <si>
+    <t>rm3</t>
+  </si>
+  <si>
+    <t>rm4</t>
+  </si>
+  <si>
+    <t>reg_mod_1</t>
+  </si>
+  <si>
+    <t>reg_mod_2</t>
+  </si>
+  <si>
+    <t>reg_mod_3</t>
+  </si>
+  <si>
+    <t>reg_mod_4</t>
   </si>
 </sst>
 </file>
@@ -2164,14 +2200,14 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="1"/>
-    <col min="2" max="2" width="43.44140625" style="2"/>
-    <col min="3" max="1025" width="8.44140625"/>
+    <col min="1" max="1" width="21.5703125" style="1"/>
+    <col min="2" max="2" width="43.42578125" style="2"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2179,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2187,7 +2223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2195,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2203,25 +2239,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2229,7 +2265,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -2249,19 +2285,19 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625"/>
-    <col min="2" max="2" width="11.6640625"/>
-    <col min="3" max="4" width="8.5546875"/>
-    <col min="5" max="5" width="7.44140625"/>
-    <col min="6" max="6" width="10.44140625"/>
-    <col min="7" max="7" width="10.6640625"/>
-    <col min="8" max="8" width="19.88671875"/>
-    <col min="9" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="16.42578125"/>
+    <col min="2" max="2" width="11.7109375"/>
+    <col min="3" max="4" width="8.5703125"/>
+    <col min="5" max="5" width="7.42578125"/>
+    <col min="6" max="6" width="10.42578125"/>
+    <col min="7" max="7" width="10.7109375"/>
+    <col min="8" max="8" width="19.85546875"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2269,10 +2305,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>30</v>
@@ -2288,60 +2324,60 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D2" t="s">
         <v>290</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>291</v>
       </c>
-      <c r="C2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D3" t="s">
         <v>293</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>294</v>
       </c>
-      <c r="C3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" t="s">
         <v>296</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>297</v>
       </c>
-      <c r="C4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D5" t="s">
         <v>299</v>
-      </c>
-      <c r="B5" t="s">
-        <v>300</v>
-      </c>
-      <c r="C5" t="s">
-        <v>284</v>
-      </c>
-      <c r="D5" t="s">
-        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2358,20 +2394,20 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625"/>
-    <col min="2" max="2" width="12.6640625"/>
-    <col min="3" max="3" width="8.5546875"/>
+    <col min="1" max="1" width="16.42578125"/>
+    <col min="2" max="2" width="12.7109375"/>
+    <col min="3" max="3" width="8.5703125"/>
     <col min="4" max="4" width="10"/>
-    <col min="5" max="5" width="10.109375"/>
-    <col min="6" max="6" width="10.44140625"/>
-    <col min="7" max="7" width="10.6640625"/>
-    <col min="8" max="8" width="19.88671875"/>
-    <col min="9" max="1025" width="8.5546875"/>
+    <col min="5" max="5" width="10.140625"/>
+    <col min="6" max="6" width="10.42578125"/>
+    <col min="7" max="7" width="10.7109375"/>
+    <col min="8" max="8" width="19.85546875"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1021" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1021" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2398,15 +2434,15 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D2" s="32">
         <v>10439968</v>
@@ -2417,15 +2453,15 @@
       <c r="AMF2" s="33"/>
       <c r="AMG2" s="33"/>
     </row>
-    <row r="3" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D3" s="32">
         <v>10441509</v>
@@ -2436,15 +2472,15 @@
       <c r="AMF3" s="33"/>
       <c r="AMG3" s="33"/>
     </row>
-    <row r="4" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D4" s="32">
         <v>10441817</v>
@@ -2455,15 +2491,15 @@
       <c r="AMF4" s="33"/>
       <c r="AMG4" s="33"/>
     </row>
-    <row r="5" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D5" s="32">
         <v>10442012</v>
@@ -2474,15 +2510,15 @@
       <c r="AMF5" s="33"/>
       <c r="AMG5" s="33"/>
     </row>
-    <row r="6" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D6" s="32">
         <v>10443230</v>
@@ -2493,15 +2529,15 @@
       <c r="AMF6" s="33"/>
       <c r="AMG6" s="33"/>
     </row>
-    <row r="7" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D7" s="32">
         <v>10443490</v>
@@ -2512,15 +2548,15 @@
       <c r="AMF7" s="33"/>
       <c r="AMG7" s="33"/>
     </row>
-    <row r="8" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D8" s="32">
         <v>10443702</v>
@@ -2531,15 +2567,15 @@
       <c r="AMF8" s="33"/>
       <c r="AMG8" s="33"/>
     </row>
-    <row r="9" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D9" s="32">
         <v>10444095</v>
@@ -2550,15 +2586,15 @@
       <c r="AMF9" s="33"/>
       <c r="AMG9" s="33"/>
     </row>
-    <row r="10" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D10" s="32">
         <v>10444474</v>
@@ -2569,15 +2605,15 @@
       <c r="AMF10" s="33"/>
       <c r="AMG10" s="33"/>
     </row>
-    <row r="11" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D11" s="32">
         <v>10444931</v>
@@ -2588,15 +2624,15 @@
       <c r="AMF11" s="33"/>
       <c r="AMG11" s="33"/>
     </row>
-    <row r="12" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D12" s="32">
         <v>10445155</v>
@@ -2607,15 +2643,15 @@
       <c r="AMF12" s="33"/>
       <c r="AMG12" s="33"/>
     </row>
-    <row r="13" spans="1:1021" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1021" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B13" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D13" s="34">
         <v>10448121</v>
@@ -2624,15 +2660,15 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="14" spans="1:1021" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1021" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B14" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D14" s="34">
         <v>10440601</v>
@@ -2641,15 +2677,15 @@
         <v>10440868</v>
       </c>
     </row>
-    <row r="15" spans="1:1021" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1021" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B15" t="s">
         <v>56</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D15" s="34">
         <v>10447474</v>
@@ -2658,15 +2694,15 @@
         <v>10447780</v>
       </c>
     </row>
-    <row r="16" spans="1:1021" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1021" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B16" t="s">
         <v>56</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D16" s="34">
         <v>10444544</v>
@@ -2675,15 +2711,15 @@
         <v>10444647</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B17" t="s">
         <v>56</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D17" s="34">
         <v>10447628</v>
@@ -2692,15 +2728,15 @@
         <v>10447788</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B18" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D18" s="34">
         <v>10444095</v>
@@ -2709,15 +2745,15 @@
         <v>10444267</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B19" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D19" s="34">
         <v>10444474</v>
@@ -2726,15 +2762,15 @@
         <v>10444547</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D20" s="34">
         <v>10444931</v>
@@ -2743,15 +2779,15 @@
         <v>10445049</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B21" t="s">
         <v>56</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D21" s="34">
         <v>10448121</v>
@@ -2770,26 +2806,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="13"/>
-    <col min="2" max="2" width="33.88671875" style="13"/>
-    <col min="3" max="3" width="16.44140625" style="14"/>
-    <col min="4" max="4" width="16.44140625" style="11"/>
-    <col min="5" max="5" width="25.5546875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="2"/>
-    <col min="7" max="7" width="40.33203125" style="13"/>
-    <col min="8" max="8" width="9.109375" style="2"/>
-    <col min="9" max="9" width="19.88671875" style="2"/>
-    <col min="10" max="1021" width="9.109375" style="2"/>
-    <col min="1024" max="1026" width="8.6640625"/>
+    <col min="1" max="1" width="20.28515625" style="13"/>
+    <col min="2" max="2" width="33.85546875" style="13"/>
+    <col min="3" max="3" width="16.42578125" style="14"/>
+    <col min="4" max="4" width="16.42578125" style="11"/>
+    <col min="5" max="5" width="25.5703125" style="30" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="2"/>
+    <col min="7" max="7" width="40.28515625" style="13"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="19.85546875" style="2"/>
+    <col min="10" max="1021" width="9.140625" style="2"/>
+    <col min="1024" max="1026" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2797,16 +2833,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>342</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>477</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>344</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>11</v>
@@ -2818,55 +2854,55 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="D2" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="B3" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="B4" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>347</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="E3" s="13" t="s">
+      <c r="D4" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>472</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -2888,19 +2924,19 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2911,7 +2947,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>84</v>
@@ -2929,15 +2965,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E2" s="32">
         <v>10440000</v>
@@ -2946,15 +2982,15 @@
         <v>10440868</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B3" t="s">
         <v>56</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E3" s="32">
         <v>10441509</v>
@@ -2963,15 +2999,15 @@
         <v>10441723</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E4" s="32">
         <v>10444931</v>
@@ -2980,15 +3016,15 @@
         <v>10445049</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E5" s="32">
         <v>10445155</v>
@@ -3010,47 +3046,47 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" style="2"/>
+    <col min="1" max="1" width="38.7109375" style="2"/>
     <col min="2" max="2" width="46" style="35"/>
-    <col min="3" max="3" width="32.88671875" style="2"/>
+    <col min="3" max="3" width="32.85546875" style="2"/>
     <col min="4" max="4" width="45" style="36"/>
-    <col min="5" max="5" width="29.33203125" style="36"/>
-    <col min="6" max="6" width="16.44140625" style="11"/>
-    <col min="7" max="8" width="8.44140625" style="2"/>
-    <col min="9" max="9" width="13.44140625" style="2"/>
-    <col min="10" max="10" width="37.33203125" style="2"/>
-    <col min="11" max="11" width="13.44140625" style="2"/>
-    <col min="12" max="12" width="19.88671875" style="2"/>
-    <col min="13" max="1022" width="8.44140625" style="2"/>
-    <col min="1023" max="1025" width="8.44140625"/>
+    <col min="5" max="5" width="29.28515625" style="36"/>
+    <col min="6" max="6" width="16.42578125" style="11"/>
+    <col min="7" max="8" width="8.42578125" style="2"/>
+    <col min="9" max="9" width="13.42578125" style="2"/>
+    <col min="10" max="10" width="37.28515625" style="2"/>
+    <col min="11" max="11" width="13.42578125" style="2"/>
+    <col min="12" max="12" width="19.85546875" style="2"/>
+    <col min="13" max="1022" width="8.42578125" style="2"/>
+    <col min="1023" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>352</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>353</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="G1" s="37" t="s">
         <v>354</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="H1" s="37" t="s">
         <v>355</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>356</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>357</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>54</v>
@@ -3065,21 +3101,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>358</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="D2" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="E2" s="36" t="s">
         <v>360</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>361</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>362</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="13"/>
@@ -3087,24 +3123,24 @@
       <c r="I2" s="11"/>
       <c r="J2" s="13"/>
       <c r="K2" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="D3" s="36" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="E3" s="36" t="s">
         <v>360</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>365</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>362</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="13"/>
@@ -3112,21 +3148,21 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C4" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>365</v>
+      </c>
+      <c r="E4" s="36" t="s">
         <v>360</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>367</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>362</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="13"/>
@@ -3134,21 +3170,21 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>367</v>
+      </c>
+      <c r="E5" s="36" t="s">
         <v>368</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>369</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>370</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="13"/>
@@ -3174,26 +3210,26 @@
       <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" style="39"/>
-    <col min="2" max="2" width="8.5546875" style="39"/>
-    <col min="3" max="3" width="11.5546875" style="39"/>
-    <col min="4" max="4" width="10.44140625" style="39"/>
-    <col min="5" max="5" width="10.6640625" style="39"/>
-    <col min="6" max="6" width="19.88671875" style="39"/>
-    <col min="7" max="1025" width="8.5546875" style="39"/>
+    <col min="1" max="1" width="19.42578125" style="39"/>
+    <col min="2" max="2" width="8.5703125" style="39"/>
+    <col min="3" max="3" width="11.5703125" style="39"/>
+    <col min="4" max="4" width="10.42578125" style="39"/>
+    <col min="5" max="5" width="10.7109375" style="39"/>
+    <col min="6" max="6" width="19.85546875" style="39"/>
+    <col min="7" max="1025" width="8.5703125" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="40" customFormat="1" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="40" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>369</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>371</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>372</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>373</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>11</v>
@@ -3205,131 +3241,131 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B2" s="39">
         <v>1</v>
       </c>
       <c r="C2" s="39" t="s">
+        <v>373</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
         <v>375</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
-        <v>377</v>
       </c>
       <c r="B3" s="39">
         <v>1</v>
       </c>
       <c r="C3" s="39" t="s">
+        <v>376</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
         <v>378</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
-        <v>380</v>
       </c>
       <c r="B4" s="39">
         <v>1</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B5" s="39">
         <v>1</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B6" s="39">
         <v>0.25</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B7" s="39">
         <v>0.25</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B8" s="39">
         <v>0.25</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B9" s="39">
         <v>0.25</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B10" s="39">
         <v>0.5</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B11" s="39">
         <v>0.5</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B12" s="39">
         <v>0.5</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -3346,17 +3382,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16"/>
-    <col min="4" max="4" width="15.44140625"/>
+    <col min="4" max="4" width="15.42578125"/>
     <col min="5" max="5" width="14"/>
-    <col min="6" max="6" width="10.5546875"/>
-    <col min="7" max="7" width="11.109375"/>
-    <col min="8" max="8" width="20.5546875"/>
+    <col min="6" max="6" width="10.5703125"/>
+    <col min="7" max="7" width="11.140625"/>
+    <col min="8" max="8" width="20.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3364,13 +3400,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>11</v>
@@ -3382,12 +3418,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -3408,19 +3444,19 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="2"/>
-    <col min="2" max="2" width="23.44140625" style="2"/>
-    <col min="3" max="3" width="17.6640625" style="2"/>
-    <col min="4" max="4" width="18.6640625" style="2"/>
-    <col min="5" max="5" width="12.6640625" style="2"/>
-    <col min="6" max="6" width="14.6640625" style="2"/>
-    <col min="7" max="1022" width="37.33203125" style="2"/>
-    <col min="1023" max="1025" width="8.44140625"/>
+    <col min="1" max="1" width="18.7109375" style="2"/>
+    <col min="2" max="2" width="23.42578125" style="2"/>
+    <col min="3" max="3" width="17.7109375" style="2"/>
+    <col min="4" max="4" width="18.7109375" style="2"/>
+    <col min="5" max="5" width="12.7109375" style="2"/>
+    <col min="6" max="6" width="14.7109375" style="2"/>
+    <col min="7" max="1022" width="37.28515625" style="2"/>
+    <col min="1023" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3428,13 +3464,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>393</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>394</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>395</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>396</v>
       </c>
       <c r="F1" s="37" t="s">
         <v>11</v>
@@ -3446,75 +3482,75 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>398</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>403</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>406</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>409</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -3522,44 +3558,44 @@
         <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>413</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -3587,34 +3623,34 @@
       <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="42"/>
-    <col min="2" max="2" width="10.6640625" style="42"/>
-    <col min="3" max="3" width="10.44140625" style="42"/>
+    <col min="1" max="1" width="20.28515625" style="42"/>
+    <col min="2" max="2" width="10.7109375" style="42"/>
+    <col min="3" max="3" width="10.42578125" style="42"/>
     <col min="4" max="4" width="11" style="42"/>
-    <col min="5" max="5" width="6.5546875" style="42"/>
-    <col min="6" max="6" width="28.6640625" style="42"/>
+    <col min="5" max="5" width="6.5703125" style="42"/>
+    <col min="6" max="6" width="28.7109375" style="42"/>
     <col min="7" max="7" width="11" style="42"/>
     <col min="8" max="8" width="20" style="42"/>
-    <col min="9" max="1025" width="8.6640625" style="42"/>
+    <col min="9" max="1025" width="8.7109375" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>414</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>415</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>416</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>417</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>418</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>419</v>
       </c>
       <c r="F1" s="43" t="s">
         <v>11</v>
@@ -3626,47 +3662,47 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B3" s="42" t="s">
+        <v>418</v>
+      </c>
+      <c r="C3" s="42" t="s">
         <v>420</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>422</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3" s="42" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D4" s="42">
         <v>1</v>
@@ -3675,78 +3711,78 @@
         <v>2</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="42" t="s">
+        <v>427</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>428</v>
+      </c>
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>409</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>418</v>
+      </c>
+      <c r="C8" s="45" t="s">
         <v>429</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="H8" s="45" t="s">
         <v>430</v>
       </c>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
-        <v>411</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>420</v>
-      </c>
-      <c r="C8" s="45" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>418</v>
+      </c>
+      <c r="C9" s="45" t="s">
         <v>431</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H9" s="45" t="s">
         <v>432</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
-        <v>414</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>420</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>433</v>
-      </c>
-      <c r="H9" s="45" t="s">
-        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -3762,16 +3798,16 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="8.5546875"/>
-    <col min="6" max="6" width="10.5546875"/>
-    <col min="7" max="7" width="11.109375"/>
-    <col min="8" max="8" width="20.5546875"/>
-    <col min="9" max="1025" width="8.5546875"/>
+    <col min="1" max="5" width="8.5703125"/>
+    <col min="6" max="6" width="10.5703125"/>
+    <col min="7" max="7" width="11.140625"/>
+    <col min="8" max="8" width="20.5703125"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3779,13 +3815,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F1" s="37" t="s">
         <v>11</v>
@@ -3797,12 +3833,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C2">
         <v>20.5</v>
@@ -3811,18 +3847,18 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E2" t="s">
+        <v>436</v>
+      </c>
+      <c r="H2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>438</v>
       </c>
-      <c r="H2" t="s">
+      <c r="B3" t="s">
         <v>439</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>440</v>
-      </c>
-      <c r="B3" t="s">
-        <v>441</v>
       </c>
       <c r="C3">
         <v>1.35</v>
@@ -3831,18 +3867,18 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="E3" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B4" t="s">
         <v>442</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>443</v>
-      </c>
-      <c r="B4" t="s">
-        <v>444</v>
       </c>
       <c r="C4">
         <v>0.46</v>
@@ -3851,18 +3887,18 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="E4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H4" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C5">
         <v>1.2</v>
@@ -3871,10 +3907,10 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="E5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -3894,14 +3930,14 @@
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="6"/>
-    <col min="2" max="2" width="51.109375" style="2"/>
-    <col min="3" max="1025" width="8.44140625"/>
+    <col min="1" max="1" width="16.42578125" style="6"/>
+    <col min="2" max="2" width="51.140625" style="2"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3909,7 +3945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -3917,7 +3953,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
@@ -3925,7 +3961,7 @@
         <v>9606</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -3945,29 +3981,29 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625"/>
-    <col min="2" max="2" width="15.5546875"/>
-    <col min="4" max="4" width="13.109375"/>
-    <col min="5" max="5" width="10.5546875"/>
-    <col min="6" max="6" width="11.109375"/>
-    <col min="7" max="7" width="19.88671875"/>
-    <col min="1021" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="17.7109375"/>
+    <col min="2" max="2" width="15.5703125"/>
+    <col min="4" max="4" width="13.140625"/>
+    <col min="5" max="5" width="10.5703125"/>
+    <col min="6" max="6" width="11.140625"/>
+    <col min="7" max="7" width="19.85546875"/>
+    <col min="1021" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>11</v>
@@ -3979,60 +4015,60 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C2" s="46">
         <v>3.0000000000000001E-12</v>
       </c>
       <c r="D2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B3" t="s">
         <v>449</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>450</v>
-      </c>
-      <c r="B3" t="s">
-        <v>451</v>
       </c>
       <c r="C3" s="46">
         <v>10000000</v>
       </c>
       <c r="D3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4" t="s">
         <v>452</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>453</v>
-      </c>
-      <c r="B4" t="s">
-        <v>454</v>
       </c>
       <c r="C4">
         <v>0.7</v>
       </c>
       <c r="D4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>454</v>
+      </c>
+      <c r="B5" t="s">
         <v>455</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>456</v>
-      </c>
-      <c r="B5" t="s">
-        <v>457</v>
       </c>
       <c r="C5">
         <v>71280</v>
       </c>
       <c r="D5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -4053,43 +4089,43 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875"/>
-    <col min="2" max="2" width="18.5546875"/>
-    <col min="3" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="18.5703125"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2" t="s">
         <v>459</v>
       </c>
-      <c r="B1" s="8" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B3" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>363</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>379</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>462</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>463</v>
-      </c>
-      <c r="B4" t="s">
-        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -4106,19 +4142,19 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="7"/>
-    <col min="2" max="2" width="16.109375" style="2"/>
-    <col min="3" max="3" width="17.6640625" style="2"/>
-    <col min="4" max="4" width="11.33203125" style="2"/>
-    <col min="5" max="5" width="11.109375" style="2"/>
-    <col min="6" max="6" width="20.5546875" style="2"/>
-    <col min="7" max="1020" width="9.109375" style="2"/>
-    <col min="1024" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="16.140625" style="2"/>
+    <col min="3" max="3" width="17.7109375" style="2"/>
+    <col min="4" max="4" width="11.28515625" style="2"/>
+    <col min="5" max="5" width="11.140625" style="2"/>
+    <col min="6" max="6" width="20.5703125" style="2"/>
+    <col min="7" max="1020" width="9.140625" style="2"/>
+    <col min="1024" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4138,7 +4174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -4155,7 +4191,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -4167,7 +4203,7 @@
       </c>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -4181,7 +4217,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
@@ -4207,19 +4243,19 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="9"/>
-    <col min="2" max="2" width="39.44140625" style="9"/>
-    <col min="3" max="3" width="13.6640625" style="2"/>
-    <col min="4" max="4" width="10.6640625" style="2"/>
+    <col min="1" max="1" width="23.85546875" style="9"/>
+    <col min="2" max="2" width="39.42578125" style="9"/>
+    <col min="3" max="3" width="13.7109375" style="2"/>
+    <col min="4" max="4" width="10.7109375" style="2"/>
     <col min="5" max="5" width="55" style="9"/>
-    <col min="6" max="6" width="9.109375" style="2"/>
-    <col min="7" max="7" width="19.88671875" style="2"/>
-    <col min="8" max="1022" width="9.109375" style="2"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="19.85546875" style="2"/>
+    <col min="8" max="1022" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4242,7 +4278,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -4250,7 +4286,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -4261,7 +4297,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4269,7 +4305,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -4277,7 +4313,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>40</v>
       </c>
@@ -4288,7 +4324,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>43</v>
       </c>
@@ -4299,7 +4335,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>46</v>
       </c>
@@ -4310,7 +4346,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>49</v>
       </c>
@@ -4339,20 +4375,20 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" style="7"/>
+    <col min="1" max="1" width="14.140625" style="7"/>
     <col min="2" max="2" width="13" style="11"/>
-    <col min="3" max="4" width="11.6640625" style="2"/>
-    <col min="5" max="5" width="22.109375" style="2"/>
-    <col min="6" max="6" width="9.109375" style="2"/>
-    <col min="7" max="8" width="13.44140625" style="2"/>
-    <col min="9" max="9" width="13.44140625"/>
-    <col min="10" max="10" width="19.88671875"/>
-    <col min="11" max="12" width="13.44140625"/>
+    <col min="3" max="4" width="11.7109375" style="2"/>
+    <col min="5" max="5" width="22.140625" style="2"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="8" width="13.42578125" style="2"/>
+    <col min="9" max="9" width="13.42578125"/>
+    <col min="10" max="10" width="19.85546875"/>
+    <col min="11" max="12" width="13.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4360,7 +4396,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>52</v>
@@ -4369,7 +4405,7 @@
         <v>53</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>54</v>
@@ -4384,7 +4420,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
@@ -4403,7 +4439,7 @@
       </c>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>56</v>
       </c>
@@ -4420,7 +4456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>57</v>
       </c>
@@ -4437,7 +4473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>58</v>
       </c>
@@ -4454,7 +4490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>59</v>
       </c>
@@ -4471,7 +4507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>60</v>
       </c>
@@ -4488,7 +4524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>61</v>
       </c>
@@ -4505,7 +4541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>62</v>
       </c>
@@ -4522,7 +4558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>63</v>
       </c>
@@ -4539,7 +4575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>64</v>
       </c>
@@ -4556,7 +4592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>65</v>
       </c>
@@ -4573,7 +4609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>66</v>
       </c>
@@ -4590,7 +4626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>67</v>
       </c>
@@ -4607,7 +4643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>68</v>
       </c>
@@ -4624,7 +4660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>69</v>
       </c>
@@ -4641,7 +4677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>70</v>
       </c>
@@ -4658,7 +4694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>71</v>
       </c>
@@ -4675,7 +4711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>72</v>
       </c>
@@ -4692,7 +4728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>73</v>
       </c>
@@ -4709,7 +4745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>74</v>
       </c>
@@ -4726,7 +4762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>75</v>
       </c>
@@ -4743,7 +4779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>76</v>
       </c>
@@ -4760,7 +4796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>77</v>
       </c>
@@ -4777,7 +4813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>78</v>
       </c>
@@ -4794,7 +4830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>79</v>
       </c>
@@ -4826,22 +4862,22 @@
   <dimension ref="A1:AMI37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="11"/>
-    <col min="2" max="2" width="16.44140625" style="11"/>
-    <col min="3" max="3" width="42.44140625" style="13"/>
-    <col min="4" max="6" width="13.44140625" style="14"/>
-    <col min="7" max="8" width="13.44140625" style="11"/>
-    <col min="9" max="9" width="16.44140625" style="15"/>
-    <col min="10" max="1023" width="32.5546875" style="2"/>
-    <col min="1024" max="1025" width="8.44140625"/>
+    <col min="1" max="1" width="17.42578125" style="11"/>
+    <col min="2" max="2" width="16.42578125" style="11"/>
+    <col min="3" max="3" width="42.42578125" style="13"/>
+    <col min="4" max="6" width="13.42578125" style="14"/>
+    <col min="7" max="8" width="13.42578125" style="11"/>
+    <col min="9" max="9" width="16.42578125" style="15"/>
+    <col min="10" max="1023" width="32.5703125" style="2"/>
+    <col min="1024" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1023" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4882,7 +4918,7 @@
       <c r="AMH1" s="2"/>
       <c r="AMI1" s="2"/>
     </row>
-    <row r="2" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>86</v>
       </c>
@@ -4908,7 +4944,7 @@
         <v>20651511</v>
       </c>
     </row>
-    <row r="3" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>91</v>
       </c>
@@ -4934,7 +4970,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="4" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>95</v>
       </c>
@@ -4960,7 +4996,7 @@
         <v>69387254</v>
       </c>
     </row>
-    <row r="5" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>98</v>
       </c>
@@ -4986,7 +5022,7 @@
         <v>40574685</v>
       </c>
     </row>
-    <row r="6" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>101</v>
       </c>
@@ -5012,7 +5048,7 @@
         <v>112649530</v>
       </c>
     </row>
-    <row r="7" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>104</v>
       </c>
@@ -5038,7 +5074,7 @@
         <v>83605875</v>
       </c>
     </row>
-    <row r="8" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>107</v>
       </c>
@@ -5064,7 +5100,7 @@
         <v>127899195</v>
       </c>
     </row>
-    <row r="9" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>110</v>
       </c>
@@ -5090,7 +5126,7 @@
         <v>160421711</v>
       </c>
     </row>
-    <row r="10" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>113</v>
       </c>
@@ -5116,7 +5152,7 @@
         <v>152129619</v>
       </c>
     </row>
-    <row r="11" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>116</v>
       </c>
@@ -5142,7 +5178,7 @@
         <v>56051604</v>
       </c>
     </row>
-    <row r="12" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>119</v>
       </c>
@@ -5168,7 +5204,7 @@
         <v>18084998</v>
       </c>
     </row>
-    <row r="13" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>122</v>
       </c>
@@ -5194,7 +5230,7 @@
         <v>19967258</v>
       </c>
     </row>
-    <row r="14" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>125</v>
       </c>
@@ -5220,7 +5256,7 @@
         <v>136423761</v>
       </c>
     </row>
-    <row r="15" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>128</v>
       </c>
@@ -5246,7 +5282,7 @@
         <v>7787981</v>
       </c>
     </row>
-    <row r="16" spans="1:1023" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>131</v>
       </c>
@@ -5272,7 +5308,7 @@
         <v>133421307</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>134</v>
       </c>
@@ -5298,7 +5334,7 @@
         <v>13732346</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>137</v>
       </c>
@@ -5324,7 +5360,7 @@
         <v>114450279</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>140</v>
       </c>
@@ -5350,7 +5386,7 @@
         <v>77065580</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>143</v>
       </c>
@@ -5376,7 +5412,7 @@
         <v>113359493</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>146</v>
       </c>
@@ -5402,7 +5438,7 @@
         <v>52476628</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>149</v>
       </c>
@@ -5428,7 +5464,7 @@
         <v>103057462</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>152</v>
       </c>
@@ -5454,7 +5490,7 @@
         <v>65578352</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>155</v>
       </c>
@@ -5480,7 +5516,7 @@
         <v>101251932</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>158</v>
       </c>
@@ -5506,7 +5542,7 @@
         <v>89155846</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>161</v>
       </c>
@@ -5532,7 +5568,7 @@
         <v>49223225</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>164</v>
       </c>
@@ -5558,7 +5594,7 @@
         <v>50988121</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>167</v>
       </c>
@@ -5584,7 +5620,7 @@
         <v>41440717</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>170</v>
       </c>
@@ -5610,7 +5646,7 @@
         <v>47784686</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>173</v>
       </c>
@@ -5636,7 +5672,7 @@
         <v>13638940</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>176</v>
       </c>
@@ -5662,7 +5698,7 @@
         <v>44652233</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>179</v>
       </c>
@@ -5688,7 +5724,7 @@
         <v>31668931</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>182</v>
       </c>
@@ -5714,7 +5750,7 @@
         <v>20859417</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>185</v>
       </c>
@@ -5740,7 +5776,7 @@
         <v>38738299</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>188</v>
       </c>
@@ -5766,7 +5802,7 @@
         <v>119605895</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>191</v>
       </c>
@@ -5792,7 +5828,7 @@
         <v>23005465</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>194</v>
       </c>
@@ -5831,35 +5867,36 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ37"/>
+  <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="16.44140625" style="11"/>
+    <col min="1" max="3" width="16.42578125" style="11"/>
     <col min="4" max="4" width="22" style="11"/>
-    <col min="5" max="5" width="13.6640625" style="11"/>
-    <col min="6" max="6" width="25.109375" style="11"/>
-    <col min="7" max="7" width="13.44140625" style="11"/>
-    <col min="8" max="8" width="16.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" style="30" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" style="11"/>
-    <col min="12" max="12" width="25.109375" style="2"/>
-    <col min="13" max="13" width="19.88671875"/>
-    <col min="14" max="14" width="9.109375" style="14"/>
-    <col min="15" max="15" width="10.44140625" style="14"/>
-    <col min="16" max="16" width="10.6640625" style="14"/>
-    <col min="17" max="18" width="9.109375" style="11"/>
-    <col min="19" max="19" width="22.88671875" style="14"/>
-    <col min="20" max="1015" width="9.109375" style="11"/>
-    <col min="1016" max="1024" width="9.109375" style="2"/>
+    <col min="5" max="5" width="13.7109375" style="11"/>
+    <col min="6" max="6" width="9.140625" style="30"/>
+    <col min="7" max="7" width="25.140625" style="11"/>
+    <col min="8" max="8" width="13.42578125" style="11"/>
+    <col min="9" max="9" width="16.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="30" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" style="11"/>
+    <col min="13" max="13" width="25.140625" style="2"/>
+    <col min="14" max="14" width="19.85546875"/>
+    <col min="15" max="15" width="9.140625" style="14"/>
+    <col min="16" max="16" width="10.42578125" style="14"/>
+    <col min="17" max="17" width="10.7109375" style="14"/>
+    <col min="18" max="19" width="9.140625" style="11"/>
+    <col min="20" max="20" width="22.85546875" style="14"/>
+    <col min="21" max="1016" width="9.140625" style="11"/>
+    <col min="1017" max="1025" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1025" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -5876,36 +5913,38 @@
         <v>197</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>467</v>
-      </c>
       <c r="I1" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="20"/>
       <c r="O1" s="20"/>
       <c r="P1" s="20"/>
-      <c r="Q1" s="21"/>
+      <c r="Q1" s="20"/>
       <c r="R1" s="21"/>
-      <c r="S1" s="20"/>
-      <c r="AMB1" s="1"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="20"/>
       <c r="AMC1" s="1"/>
       <c r="AMD1" s="1"/>
       <c r="AME1" s="1"/>
@@ -5914,8 +5953,9 @@
       <c r="AMH1" s="1"/>
       <c r="AMI1" s="1"/>
       <c r="AMJ1" s="1"/>
-    </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="AMK1" s="1"/>
+    </row>
+    <row r="2" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>198</v>
       </c>
@@ -5931,24 +5971,27 @@
       <c r="E2" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="11">
         <v>203893801</v>
       </c>
-      <c r="G2" s="11">
+      <c r="H2" s="11">
         <v>203895200</v>
       </c>
-      <c r="H2" s="30">
+      <c r="I2" s="30">
         <v>203893820</v>
       </c>
-      <c r="I2" s="30">
+      <c r="J2" s="30">
         <v>203895200</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="5"/>
-      <c r="Q2" s="22"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="5"/>
       <c r="R2" s="22"/>
-    </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S2" s="22"/>
+    </row>
+    <row r="3" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>202</v>
       </c>
@@ -5964,24 +6007,27 @@
       <c r="E3" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="11">
         <v>20602802</v>
       </c>
-      <c r="G3" s="11">
+      <c r="H3" s="11">
         <v>20605200</v>
       </c>
-      <c r="H3" s="30">
+      <c r="I3" s="30">
         <v>20602802</v>
       </c>
-      <c r="I3" s="30">
+      <c r="J3" s="30">
         <v>20605200</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="5"/>
-      <c r="Q3" s="22"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="5"/>
       <c r="R3" s="22"/>
-    </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S3" s="22"/>
+    </row>
+    <row r="4" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>205</v>
       </c>
@@ -5997,24 +6043,27 @@
       <c r="E4" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="11">
         <v>45648015</v>
       </c>
-      <c r="G4" s="11">
+      <c r="H4" s="11">
         <v>45648411</v>
       </c>
-      <c r="H4" s="30">
+      <c r="I4" s="30">
         <v>45648015</v>
       </c>
-      <c r="I4" s="30">
+      <c r="J4" s="30">
         <v>45648411</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="5"/>
-      <c r="Q4" s="22"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="5"/>
       <c r="R4" s="22"/>
-    </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S4" s="22"/>
+    </row>
+    <row r="5" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>209</v>
       </c>
@@ -6030,24 +6079,27 @@
       <c r="E5" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="11">
         <v>85413000</v>
       </c>
-      <c r="G5" s="11">
+      <c r="H5" s="11">
         <v>85414201</v>
       </c>
-      <c r="H5" s="30">
+      <c r="I5" s="30">
         <v>85413000</v>
       </c>
-      <c r="I5" s="30">
+      <c r="J5" s="30">
         <v>85414201</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="5"/>
-      <c r="Q5" s="22"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="5"/>
       <c r="R5" s="22"/>
-    </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S5" s="22"/>
+    </row>
+    <row r="6" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>213</v>
       </c>
@@ -6063,24 +6115,27 @@
       <c r="E6" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="11">
         <v>39877201</v>
       </c>
-      <c r="G6" s="11">
+      <c r="H6" s="11">
         <v>39878600</v>
       </c>
-      <c r="H6" s="30">
+      <c r="I6" s="30">
         <v>39877210</v>
       </c>
-      <c r="I6" s="30">
+      <c r="J6" s="30">
         <v>39878600</v>
       </c>
-      <c r="K6" s="14"/>
-      <c r="L6" s="5"/>
-      <c r="Q6" s="22"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="5"/>
       <c r="R6" s="22"/>
-    </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S6" s="22"/>
+    </row>
+    <row r="7" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>216</v>
       </c>
@@ -6096,24 +6151,27 @@
       <c r="E7" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="11">
         <v>185316402</v>
       </c>
-      <c r="G7" s="11">
+      <c r="H7" s="11">
         <v>185318582</v>
       </c>
-      <c r="H7" s="30">
+      <c r="I7" s="30">
         <v>185316402</v>
       </c>
-      <c r="I7" s="30">
+      <c r="J7" s="30">
         <v>185318582</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="5"/>
-      <c r="Q7" s="22"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="5"/>
       <c r="R7" s="22"/>
-    </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S7" s="22"/>
+    </row>
+    <row r="8" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>218</v>
       </c>
@@ -6129,24 +6187,27 @@
       <c r="E8" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="11">
         <v>53862600</v>
       </c>
-      <c r="G8" s="11">
+      <c r="H8" s="11">
         <v>53863800</v>
       </c>
-      <c r="H8" s="30">
+      <c r="I8" s="30">
         <v>53862600</v>
       </c>
-      <c r="I8" s="30">
+      <c r="J8" s="30">
         <v>53863800</v>
       </c>
-      <c r="K8" s="14"/>
-      <c r="L8" s="5"/>
-      <c r="Q8" s="22"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="5"/>
       <c r="R8" s="22"/>
-    </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S8" s="22"/>
+    </row>
+    <row r="9" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>221</v>
       </c>
@@ -6162,24 +6223,27 @@
       <c r="E9" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="11">
         <v>118834600</v>
       </c>
-      <c r="G9" s="11">
+      <c r="H9" s="11">
         <v>118837001</v>
       </c>
-      <c r="H9" s="30">
+      <c r="I9" s="30">
         <v>118834600</v>
       </c>
-      <c r="I9" s="30">
+      <c r="J9" s="30">
         <v>118837001</v>
       </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="5"/>
-      <c r="Q9" s="22"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="5"/>
       <c r="R9" s="22"/>
-    </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S9" s="22"/>
+    </row>
+    <row r="10" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>223</v>
       </c>
@@ -6195,24 +6259,27 @@
       <c r="E10" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="11">
         <v>141848202</v>
       </c>
-      <c r="G10" s="11">
+      <c r="H10" s="11">
         <v>141851600</v>
       </c>
-      <c r="H10" s="30">
+      <c r="I10" s="30">
         <v>141848202</v>
       </c>
-      <c r="I10" s="30">
+      <c r="J10" s="30">
         <v>141851600</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="5"/>
-      <c r="Q10" s="22"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="5"/>
       <c r="R10" s="22"/>
-    </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S10" s="22"/>
+    </row>
+    <row r="11" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>225</v>
       </c>
@@ -6228,24 +6295,27 @@
       <c r="E11" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="11">
         <v>2988400</v>
       </c>
-      <c r="G11" s="11">
+      <c r="H11" s="11">
         <v>2991401</v>
       </c>
-      <c r="H11" s="30">
+      <c r="I11" s="30">
         <v>2988400</v>
       </c>
-      <c r="I11" s="30">
+      <c r="J11" s="30">
         <v>2991400</v>
       </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="5"/>
-      <c r="Q11" s="22"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="5"/>
       <c r="R11" s="22"/>
-    </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S11" s="22"/>
+    </row>
+    <row r="12" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>227</v>
       </c>
@@ -6261,24 +6331,27 @@
       <c r="E12" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="11">
         <v>43970600</v>
       </c>
-      <c r="G12" s="11">
+      <c r="H12" s="11">
         <v>43971001</v>
       </c>
-      <c r="H12" s="30">
+      <c r="I12" s="30">
         <v>43970600</v>
       </c>
-      <c r="I12" s="30">
+      <c r="J12" s="30">
         <v>43971001</v>
       </c>
-      <c r="K12" s="14"/>
-      <c r="L12" s="5"/>
-      <c r="Q12" s="22"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="5"/>
       <c r="R12" s="22"/>
-    </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S12" s="22"/>
+    </row>
+    <row r="13" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>229</v>
       </c>
@@ -6294,24 +6367,27 @@
       <c r="E13" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" s="11">
         <v>890483</v>
       </c>
-      <c r="G13" s="11">
+      <c r="H13" s="11">
         <v>893236</v>
       </c>
-      <c r="H13" s="30">
+      <c r="I13" s="30">
         <v>890483</v>
       </c>
-      <c r="I13" s="30">
+      <c r="J13" s="30">
         <v>893236</v>
       </c>
-      <c r="K13" s="14"/>
-      <c r="L13" s="5"/>
-      <c r="Q13" s="22"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="5"/>
       <c r="R13" s="22"/>
-    </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S13" s="22"/>
+    </row>
+    <row r="14" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>231</v>
       </c>
@@ -6327,24 +6403,27 @@
       <c r="E14" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="11">
         <v>116112401</v>
       </c>
-      <c r="G14" s="11">
+      <c r="H14" s="11">
         <v>116112801</v>
       </c>
-      <c r="H14" s="30">
+      <c r="I14" s="30">
         <v>116112401</v>
       </c>
-      <c r="I14" s="30">
+      <c r="J14" s="30">
         <v>116112801</v>
       </c>
-      <c r="K14" s="14"/>
-      <c r="L14" s="5"/>
-      <c r="Q14" s="22"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="5"/>
       <c r="R14" s="22"/>
-    </row>
-    <row r="15" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S14" s="22"/>
+    </row>
+    <row r="15" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>233</v>
       </c>
@@ -6360,27 +6439,30 @@
       <c r="E15" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="11">
         <v>72121544</v>
       </c>
-      <c r="G15" s="11">
+      <c r="H15" s="11">
         <v>72121926</v>
       </c>
-      <c r="H15" s="30">
+      <c r="I15" s="30">
         <v>72121544</v>
       </c>
-      <c r="I15" s="30">
+      <c r="J15" s="30">
         <v>72121926</v>
       </c>
-      <c r="J15" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="K15" s="14"/>
-      <c r="L15" s="5"/>
-      <c r="Q15" s="22"/>
+      <c r="K15" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="L15" s="14"/>
+      <c r="M15" s="5"/>
       <c r="R15" s="22"/>
-    </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.3">
+      <c r="S15" s="22"/>
+    </row>
+    <row r="16" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>236</v>
       </c>
@@ -6396,24 +6478,27 @@
       <c r="E16" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="11">
         <v>22700001</v>
       </c>
-      <c r="G16" s="11">
+      <c r="H16" s="11">
         <v>22702000</v>
       </c>
-      <c r="H16" s="30">
+      <c r="I16" s="30">
         <v>22700001</v>
       </c>
-      <c r="I16" s="30">
+      <c r="J16" s="30">
         <v>22702000</v>
       </c>
-      <c r="K16" s="14"/>
-      <c r="L16" s="5"/>
-      <c r="Q16" s="22"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="5"/>
       <c r="R16" s="22"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S16" s="22"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>238</v>
       </c>
@@ -6429,24 +6514,27 @@
       <c r="E17" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="11">
         <v>46022400</v>
       </c>
-      <c r="G17" s="11">
+      <c r="H17" s="11">
         <v>46023801</v>
       </c>
-      <c r="H17" s="30">
+      <c r="I17" s="30">
         <v>46022400</v>
       </c>
-      <c r="I17" s="30">
+      <c r="J17" s="30">
         <v>46023801</v>
       </c>
-      <c r="K17" s="14"/>
-      <c r="L17" s="5"/>
-      <c r="Q17" s="22"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="5"/>
       <c r="R17" s="22"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S17" s="22"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>240</v>
       </c>
@@ -6462,24 +6550,27 @@
       <c r="E18" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="11">
         <v>132186801</v>
       </c>
-      <c r="G18" s="11">
+      <c r="H18" s="11">
         <v>132187000</v>
       </c>
-      <c r="H18" s="30">
+      <c r="I18" s="30">
         <v>132186801</v>
       </c>
-      <c r="I18" s="30">
+      <c r="J18" s="30">
         <v>132187000</v>
       </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="5"/>
-      <c r="Q18" s="22"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="5"/>
       <c r="R18" s="22"/>
-    </row>
-    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S18" s="22"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>242</v>
       </c>
@@ -6495,27 +6586,30 @@
       <c r="E19" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="11">
         <v>102368448</v>
       </c>
-      <c r="G19" s="11">
+      <c r="H19" s="11">
         <v>102368872</v>
       </c>
-      <c r="H19" s="30">
+      <c r="I19" s="30">
         <v>102368448</v>
       </c>
-      <c r="I19" s="30">
+      <c r="J19" s="30">
         <v>102368872</v>
       </c>
-      <c r="J19" s="13" t="s">
-        <v>469</v>
-      </c>
-      <c r="K19" s="14"/>
-      <c r="L19" s="5"/>
-      <c r="Q19" s="22"/>
+      <c r="K19" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="L19" s="14"/>
+      <c r="M19" s="5"/>
       <c r="R19" s="22"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S19" s="22"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>244</v>
       </c>
@@ -6531,24 +6625,27 @@
       <c r="E20" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="11">
         <v>101939801</v>
       </c>
-      <c r="G20" s="11">
+      <c r="H20" s="11">
         <v>101940201</v>
       </c>
-      <c r="H20" s="30">
+      <c r="I20" s="30">
         <v>101939801</v>
       </c>
-      <c r="I20" s="30">
+      <c r="J20" s="30">
         <v>101940201</v>
       </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="5"/>
-      <c r="Q20" s="22"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="5"/>
       <c r="R20" s="22"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S20" s="22"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>246</v>
       </c>
@@ -6564,24 +6661,27 @@
       <c r="E21" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="11">
         <v>99984000</v>
       </c>
-      <c r="G21" s="11">
+      <c r="H21" s="11">
         <v>99985401</v>
       </c>
-      <c r="H21" s="30">
+      <c r="I21" s="30">
         <v>99984000</v>
       </c>
-      <c r="I21" s="30">
+      <c r="J21" s="30">
         <v>99985401</v>
       </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="5"/>
-      <c r="Q21" s="22"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="5"/>
       <c r="R21" s="22"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S21" s="22"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>248</v>
       </c>
@@ -6597,24 +6697,27 @@
       <c r="E22" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="11">
         <v>52849669</v>
       </c>
-      <c r="G22" s="11">
+      <c r="H22" s="11">
         <v>52849993</v>
       </c>
-      <c r="H22" s="30">
+      <c r="I22" s="30">
         <v>52849669</v>
       </c>
-      <c r="I22" s="30">
+      <c r="J22" s="30">
         <v>52849993</v>
       </c>
-      <c r="K22" s="14"/>
-      <c r="L22" s="5"/>
-      <c r="Q22" s="22"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="5"/>
       <c r="R22" s="22"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S22" s="22"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>250</v>
       </c>
@@ -6630,24 +6733,27 @@
       <c r="E23" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="11">
         <v>23578503</v>
       </c>
-      <c r="G23" s="11">
+      <c r="H23" s="11">
         <v>23579130</v>
       </c>
-      <c r="H23" s="30">
+      <c r="I23" s="30">
         <v>23578503</v>
       </c>
-      <c r="I23" s="30">
+      <c r="J23" s="30">
         <v>23579130</v>
       </c>
-      <c r="K23" s="14"/>
-      <c r="L23" s="5"/>
-      <c r="Q23" s="22"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="5"/>
       <c r="R23" s="22"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S23" s="22"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>252</v>
       </c>
@@ -6663,24 +6769,27 @@
       <c r="E24" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="11">
         <v>90214601</v>
       </c>
-      <c r="G24" s="11">
+      <c r="H24" s="11">
         <v>90215000</v>
       </c>
-      <c r="H24" s="30">
+      <c r="I24" s="30">
         <v>90214601</v>
       </c>
-      <c r="I24" s="30">
+      <c r="J24" s="30">
         <v>90215000</v>
       </c>
-      <c r="K24" s="14"/>
-      <c r="L24" s="5"/>
-      <c r="Q24" s="22"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="5"/>
       <c r="R24" s="22"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S24" s="22"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>254</v>
       </c>
@@ -6696,24 +6805,27 @@
       <c r="E25" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" s="11">
         <v>47716801</v>
       </c>
-      <c r="G25" s="11">
+      <c r="H25" s="11">
         <v>47720200</v>
       </c>
-      <c r="H25" s="30">
+      <c r="I25" s="30">
         <v>47716801</v>
       </c>
-      <c r="I25" s="30">
+      <c r="J25" s="30">
         <v>47720200</v>
       </c>
-      <c r="K25" s="14"/>
-      <c r="L25" s="5"/>
-      <c r="Q25" s="22"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="5"/>
       <c r="R25" s="22"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S25" s="22"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>256</v>
       </c>
@@ -6729,24 +6841,27 @@
       <c r="E26" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="11">
         <v>50368000</v>
       </c>
-      <c r="G26" s="11">
+      <c r="H26" s="11">
         <v>50369600</v>
       </c>
-      <c r="H26" s="30">
+      <c r="I26" s="30">
         <v>50368000</v>
       </c>
-      <c r="I26" s="30">
+      <c r="J26" s="30">
         <v>50369600</v>
       </c>
-      <c r="K26" s="14"/>
-      <c r="L26" s="5"/>
-      <c r="Q26" s="22"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="5"/>
       <c r="R26" s="22"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S26" s="22"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>258</v>
       </c>
@@ -6762,24 +6877,27 @@
       <c r="E27" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" s="11">
         <v>18650001</v>
       </c>
-      <c r="G27" s="11">
+      <c r="H27" s="11">
         <v>18650600</v>
       </c>
-      <c r="H27" s="30">
+      <c r="I27" s="30">
         <v>18650001</v>
       </c>
-      <c r="I27" s="30">
+      <c r="J27" s="30">
         <v>18650600</v>
       </c>
-      <c r="K27" s="14"/>
-      <c r="L27" s="5"/>
-      <c r="Q27" s="22"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="5"/>
       <c r="R27" s="22"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S27" s="22"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>260</v>
       </c>
@@ -6795,24 +6913,27 @@
       <c r="E28" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="11">
         <v>33756200</v>
       </c>
-      <c r="G28" s="11">
+      <c r="H28" s="11">
         <v>33756401</v>
       </c>
-      <c r="H28" s="30">
+      <c r="I28" s="30">
         <v>33756200</v>
       </c>
-      <c r="I28" s="30">
+      <c r="J28" s="30">
         <v>33756401</v>
       </c>
-      <c r="K28" s="14"/>
-      <c r="L28" s="5"/>
-      <c r="Q28" s="22"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="5"/>
       <c r="R28" s="22"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S28" s="22"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>262</v>
       </c>
@@ -6828,24 +6949,27 @@
       <c r="E29" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="11">
         <v>58326200</v>
       </c>
-      <c r="G29" s="11">
+      <c r="H29" s="11">
         <v>58328001</v>
       </c>
-      <c r="H29" s="30">
+      <c r="I29" s="30">
         <v>58326200</v>
       </c>
-      <c r="I29" s="30">
+      <c r="J29" s="30">
         <v>58328001</v>
       </c>
-      <c r="K29" s="14"/>
-      <c r="L29" s="5"/>
-      <c r="Q29" s="22"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="5"/>
       <c r="R29" s="22"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S29" s="22"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>264</v>
       </c>
@@ -6861,24 +6985,27 @@
       <c r="E30" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="11">
         <v>50117624</v>
       </c>
-      <c r="G30" s="11">
+      <c r="H30" s="11">
         <v>50118213</v>
       </c>
-      <c r="H30" s="30">
+      <c r="I30" s="30">
         <v>50117624</v>
       </c>
-      <c r="I30" s="30">
+      <c r="J30" s="30">
         <v>50118213</v>
       </c>
-      <c r="K30" s="14"/>
-      <c r="L30" s="5"/>
-      <c r="Q30" s="22"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="5"/>
       <c r="R30" s="22"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S30" s="22"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>266</v>
       </c>
@@ -6894,24 +7021,27 @@
       <c r="E31" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="11">
         <v>62960832</v>
       </c>
-      <c r="G31" s="11">
+      <c r="H31" s="11">
         <v>62961734</v>
       </c>
-      <c r="H31" s="30">
+      <c r="I31" s="30">
         <v>62960832</v>
       </c>
-      <c r="I31" s="30">
+      <c r="J31" s="30">
         <v>62961734</v>
       </c>
-      <c r="K31" s="14"/>
-      <c r="L31" s="5"/>
-      <c r="Q31" s="22"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="5"/>
       <c r="R31" s="22"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S31" s="22"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>268</v>
       </c>
@@ -6927,24 +7057,27 @@
       <c r="E32" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" s="11">
         <v>57964075</v>
       </c>
-      <c r="G32" s="11">
+      <c r="H32" s="11">
         <v>57964896</v>
       </c>
-      <c r="H32" s="30">
+      <c r="I32" s="30">
         <v>57964075</v>
       </c>
-      <c r="I32" s="30">
+      <c r="J32" s="30">
         <v>57964896</v>
       </c>
-      <c r="K32" s="14"/>
-      <c r="L32" s="5"/>
-      <c r="Q32" s="22"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="5"/>
       <c r="R32" s="22"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S32" s="22"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>270</v>
       </c>
@@ -6960,24 +7093,27 @@
       <c r="E33" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" s="11">
         <v>36710048</v>
       </c>
-      <c r="G33" s="11">
+      <c r="H33" s="11">
         <v>36711020</v>
       </c>
-      <c r="H33" s="30">
+      <c r="I33" s="30">
         <v>36710048</v>
       </c>
-      <c r="I33" s="30">
+      <c r="J33" s="30">
         <v>36711020</v>
       </c>
-      <c r="K33" s="14"/>
-      <c r="L33" s="5"/>
-      <c r="Q33" s="22"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="5"/>
       <c r="R33" s="22"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S33" s="22"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>272</v>
       </c>
@@ -6993,24 +7129,27 @@
       <c r="E34" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34" s="11">
         <v>43346380</v>
       </c>
-      <c r="G34" s="11">
+      <c r="H34" s="11">
         <v>43346796</v>
       </c>
-      <c r="H34" s="30">
+      <c r="I34" s="30">
         <v>43346380</v>
       </c>
-      <c r="I34" s="30">
+      <c r="J34" s="30">
         <v>43346796</v>
       </c>
-      <c r="K34" s="14"/>
-      <c r="L34" s="5"/>
-      <c r="Q34" s="22"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="5"/>
       <c r="R34" s="22"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S34" s="22"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>274</v>
       </c>
@@ -7026,24 +7165,27 @@
       <c r="E35" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" s="11">
         <v>30591000</v>
       </c>
-      <c r="G35" s="11">
+      <c r="H35" s="11">
         <v>30592601</v>
       </c>
-      <c r="H35" s="30">
+      <c r="I35" s="30">
         <v>30591000</v>
       </c>
-      <c r="I35" s="30">
+      <c r="J35" s="30">
         <v>30592601</v>
       </c>
-      <c r="K35" s="14"/>
-      <c r="L35" s="5"/>
-      <c r="Q35" s="22"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="5"/>
       <c r="R35" s="22"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S35" s="22"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>276</v>
       </c>
@@ -7059,24 +7201,27 @@
       <c r="E36" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="11">
         <v>135326401</v>
       </c>
-      <c r="G36" s="11">
+      <c r="H36" s="11">
         <v>135326600</v>
       </c>
-      <c r="H36" s="30">
+      <c r="I36" s="30">
         <v>135326401</v>
       </c>
-      <c r="I36" s="30">
+      <c r="J36" s="30">
         <v>135326600</v>
       </c>
-      <c r="K36" s="14"/>
-      <c r="L36" s="5"/>
-      <c r="Q36" s="22"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="5"/>
       <c r="R36" s="22"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S36" s="22"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>278</v>
       </c>
@@ -7092,25 +7237,28 @@
       <c r="E37" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G37" s="11">
         <v>13401</v>
       </c>
-      <c r="G37" s="11">
+      <c r="H37" s="11">
         <v>14200</v>
       </c>
-      <c r="H37" s="30">
+      <c r="I37" s="30">
         <v>13401</v>
       </c>
-      <c r="I37" s="30">
+      <c r="J37" s="30">
         <v>14200</v>
       </c>
-      <c r="K37" s="14"/>
-      <c r="L37" s="5"/>
-      <c r="Q37" s="22"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="5"/>
       <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K776"/>
+  <autoFilter ref="A1:L776"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
@@ -7122,68 +7270,160 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMB3"/>
+  <dimension ref="A1:AMG5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="11"/>
-    <col min="2" max="2" width="50.5546875" style="11"/>
-    <col min="3" max="3" width="22.88671875" style="15"/>
-    <col min="4" max="4" width="13.44140625" style="23"/>
-    <col min="5" max="5" width="19.88671875" style="14"/>
-    <col min="6" max="6" width="10.6640625" style="14"/>
-    <col min="7" max="8" width="9.109375" style="11"/>
-    <col min="9" max="1016" width="9.109375" style="23"/>
-    <col min="1017" max="1019" width="8.44140625"/>
-    <col min="1020" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="9.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="30" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" style="11"/>
+    <col min="5" max="5" width="18.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" style="15"/>
+    <col min="9" max="9" width="13.42578125" style="23"/>
+    <col min="10" max="10" width="19.85546875" style="14"/>
+    <col min="11" max="11" width="10.7109375" style="14"/>
+    <col min="12" max="13" width="9.140625" style="11"/>
+    <col min="14" max="1021" width="9.140625" style="23"/>
+    <col min="1022" max="1024" width="8.42578125"/>
+    <col min="1025" max="1030" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>486</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="22"/>
+      <c r="F2" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>487</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="11"/>
+      <c r="D3" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>481</v>
+      </c>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>488</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>479</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>489</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>479</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>480</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C849"/>
+  <autoFilter ref="A1:H849"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
@@ -7201,23 +7441,23 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" style="14"/>
-    <col min="2" max="2" width="21.109375" style="14"/>
-    <col min="3" max="3" width="10.6640625" style="14"/>
-    <col min="4" max="4" width="22.88671875" style="15"/>
-    <col min="5" max="5" width="10.6640625"/>
-    <col min="6" max="6" width="13.44140625"/>
-    <col min="7" max="7" width="13.44140625" style="11"/>
-    <col min="8" max="8" width="13.44140625" style="25"/>
-    <col min="9" max="9" width="10.6640625" style="22"/>
-    <col min="10" max="10" width="19.88671875" style="11"/>
-    <col min="11" max="11" width="13.44140625" style="11"/>
-    <col min="12" max="1021" width="9.109375" style="2"/>
+    <col min="1" max="1" width="19.5703125" style="14"/>
+    <col min="2" max="2" width="21.140625" style="14"/>
+    <col min="3" max="3" width="10.7109375" style="14"/>
+    <col min="4" max="4" width="22.85546875" style="15"/>
+    <col min="5" max="5" width="10.7109375"/>
+    <col min="6" max="6" width="13.42578125"/>
+    <col min="7" max="7" width="13.42578125" style="11"/>
+    <col min="8" max="8" width="13.42578125" style="25"/>
+    <col min="9" max="9" width="10.7109375" style="22"/>
+    <col min="10" max="10" width="19.85546875" style="11"/>
+    <col min="11" max="11" width="13.42578125" style="11"/>
+    <col min="12" max="1021" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -7234,7 +7474,7 @@
         <v>52</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>30</v>
@@ -7250,12 +7490,12 @@
       </c>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>89</v>
@@ -7276,12 +7516,12 @@
       <c r="J2" s="22"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Modify Observable to allow flexible expression
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="2070" yWindow="705" windowWidth="16380" windowHeight="8175" tabRatio="993" firstSheet="8" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="492">
   <si>
     <t>Id</t>
   </si>
@@ -1259,12 +1259,6 @@
     <t>ENSP00000390691[c]</t>
   </si>
   <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>Observables</t>
-  </si>
-  <si>
     <t>obs_isoenzyme1</t>
   </si>
   <si>
@@ -1563,6 +1557,18 @@
   </si>
   <si>
     <t>reg_mod_4</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>Complex_3[c]</t>
+  </si>
+  <si>
+    <t>Complex_2[c]</t>
+  </si>
+  <si>
+    <t>Complex_1[c]</t>
   </si>
 </sst>
 </file>
@@ -2839,7 +2845,7 @@
         <v>341</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>342</v>
@@ -2868,7 +2874,7 @@
         <v>288</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2885,7 +2891,7 @@
         <v>291</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2902,7 +2908,7 @@
         <v>294</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -2947,7 +2953,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>84</v>
@@ -2967,7 +2973,7 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
@@ -2984,7 +2990,7 @@
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B3" t="s">
         <v>56</v>
@@ -3001,7 +3007,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
@@ -3018,7 +3024,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
@@ -3043,7 +3049,7 @@
   <dimension ref="A1:AMH5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3201,13 +3207,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK12"/>
+  <dimension ref="A1:AMK15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3368,6 +3374,39 @@
         <v>373</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
+        <v>491</v>
+      </c>
+      <c r="B13" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
+        <v>490</v>
+      </c>
+      <c r="B14" s="39">
+        <v>0.36</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
+        <v>489</v>
+      </c>
+      <c r="B15" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>373</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3376,23 +3415,22 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16"/>
-    <col min="4" max="4" width="15.42578125"/>
-    <col min="5" max="5" width="14"/>
-    <col min="6" max="6" width="10.5703125"/>
-    <col min="7" max="7" width="11.140625"/>
-    <col min="8" max="8" width="20.5703125"/>
+    <col min="3" max="3" width="15.42578125"/>
+    <col min="5" max="5" width="10.5703125"/>
+    <col min="6" max="6" width="11.140625"/>
+    <col min="7" max="7" width="20.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3400,30 +3438,30 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>388</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="C2" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>390</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>391</v>
+      <c r="D2" s="13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3464,13 +3502,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>391</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>392</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>393</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>394</v>
       </c>
       <c r="F1" s="37" t="s">
         <v>11</v>
@@ -3484,16 +3522,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>398</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -3501,16 +3539,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>401</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -3518,16 +3556,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>404</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -3535,16 +3573,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>407</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -3558,10 +3596,10 @@
         <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
@@ -3569,16 +3607,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>411</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -3586,16 +3624,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -3638,19 +3676,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>412</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>413</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>414</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>415</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>416</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>417</v>
       </c>
       <c r="F1" s="43" t="s">
         <v>11</v>
@@ -3664,13 +3702,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D2"/>
       <c r="E2"/>
@@ -3679,30 +3717,30 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B3" s="42" t="s">
+        <v>416</v>
+      </c>
+      <c r="C3" s="42" t="s">
         <v>418</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>420</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3" s="42" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D4" s="42">
         <v>1</v>
@@ -3711,22 +3749,22 @@
         <v>2</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H5"/>
     </row>
@@ -3735,13 +3773,13 @@
         <v>37</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H6"/>
     </row>
@@ -3750,39 +3788,39 @@
         <v>37</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H8" s="45" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H9" s="45" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3818,7 +3856,7 @@
         <v>370</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>371</v>
@@ -3835,10 +3873,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C2">
         <v>20.5</v>
@@ -3847,18 +3885,18 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B3" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C3">
         <v>1.35</v>
@@ -3867,18 +3905,18 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="E3" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H3" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C4">
         <v>0.46</v>
@@ -3890,15 +3928,15 @@
         <v>373</v>
       </c>
       <c r="H4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C5">
         <v>1.2</v>
@@ -3910,7 +3948,7 @@
         <v>373</v>
       </c>
       <c r="H5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -4017,58 +4055,58 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C2" s="46">
         <v>3.0000000000000001E-12</v>
       </c>
       <c r="D2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C3" s="46">
         <v>10000000</v>
       </c>
       <c r="D3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C4">
         <v>0.7</v>
       </c>
       <c r="D4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C5">
         <v>71280</v>
       </c>
       <c r="D5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4098,10 +4136,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4109,7 +4147,7 @@
         <v>361</v>
       </c>
       <c r="B2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4117,15 +4155,15 @@
         <v>377</v>
       </c>
       <c r="B3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -4396,7 +4434,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>52</v>
@@ -4405,7 +4443,7 @@
         <v>53</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>54</v>
@@ -5922,13 +5960,13 @@
         <v>85</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>464</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>466</v>
       </c>
       <c r="L1" s="18" t="s">
         <v>11</v>
@@ -6602,7 +6640,7 @@
         <v>102368872</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="L19" s="14"/>
       <c r="M19" s="5"/>
@@ -7272,7 +7310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -7306,16 +7344,16 @@
         <v>280</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>82</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>11</v>
@@ -7330,10 +7368,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>91</v>
@@ -7343,10 +7381,10 @@
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22" t="s">
+        <v>476</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>478</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>480</v>
       </c>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
@@ -7354,10 +7392,10 @@
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>107</v>
@@ -7367,10 +7405,10 @@
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
@@ -7378,10 +7416,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C4" s="30" t="s">
         <v>107</v>
@@ -7393,18 +7431,18 @@
         <v>347</v>
       </c>
       <c r="F4" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="G4" s="30" t="s">
         <v>479</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C5" s="30" t="s">
         <v>104</v>
@@ -7416,10 +7454,10 @@
         <v>347</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify rate law equation to allow flexible expression
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="705" windowWidth="16380" windowHeight="8175" tabRatio="993" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="1020" yWindow="672" windowWidth="16380" windowHeight="8172" tabRatio="993" firstSheet="10" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="500">
   <si>
     <t>Id</t>
   </si>
@@ -1334,24 +1334,9 @@
     <t>Direction</t>
   </si>
   <si>
-    <t>Equation</t>
-  </si>
-  <si>
-    <t>K cat</t>
-  </si>
-  <si>
-    <t>K m</t>
-  </si>
-  <si>
     <t>forward</t>
   </si>
   <si>
-    <t>""</t>
-  </si>
-  <si>
-    <t>"2"</t>
-  </si>
-  <si>
     <t>Order 2, same, MA kinetics</t>
   </si>
   <si>
@@ -1569,6 +1554,45 @@
   </si>
   <si>
     <t>Complex_1[c]</t>
+  </si>
+  <si>
+    <t>kdeg</t>
+  </si>
+  <si>
+    <t>degradation constant</t>
+  </si>
+  <si>
+    <t>M s^-1</t>
+  </si>
+  <si>
+    <t>Complex_4[c]</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>O2_degradation_forward</t>
+  </si>
+  <si>
+    <t>O2_synthesis_forward</t>
+  </si>
+  <si>
+    <t>Oxygen_ionization_forward</t>
+  </si>
+  <si>
+    <t>Oxygen_deionization_forward</t>
+  </si>
+  <si>
+    <t>Ozone_forward</t>
+  </si>
+  <si>
+    <t>Ozone_backward</t>
+  </si>
+  <si>
+    <t>ORNDC_isoenzyme1_forward</t>
+  </si>
+  <si>
+    <t>ORNDC_isoenzyme2_forward</t>
   </si>
 </sst>
 </file>
@@ -1709,7 +1733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1827,6 +1851,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -2206,14 +2231,14 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="1"/>
-    <col min="2" max="2" width="43.42578125" style="2"/>
-    <col min="3" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="21.5546875" style="1"/>
+    <col min="2" max="2" width="43.44140625" style="2"/>
+    <col min="3" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2221,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2229,7 +2254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2237,7 +2262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2245,25 +2270,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2271,7 +2296,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -2291,19 +2316,19 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125"/>
-    <col min="2" max="2" width="11.7109375"/>
-    <col min="3" max="4" width="8.5703125"/>
-    <col min="5" max="5" width="7.42578125"/>
-    <col min="6" max="6" width="10.42578125"/>
-    <col min="7" max="7" width="10.7109375"/>
-    <col min="8" max="8" width="19.85546875"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="16.44140625"/>
+    <col min="2" max="2" width="11.6640625"/>
+    <col min="3" max="4" width="8.5546875"/>
+    <col min="5" max="5" width="7.44140625"/>
+    <col min="6" max="6" width="10.44140625"/>
+    <col min="7" max="7" width="10.6640625"/>
+    <col min="8" max="8" width="19.88671875"/>
+    <col min="9" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2330,7 +2355,7 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>288</v>
       </c>
@@ -2344,7 +2369,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>291</v>
       </c>
@@ -2358,7 +2383,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -2372,7 +2397,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>297</v>
       </c>
@@ -2400,20 +2425,20 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125"/>
-    <col min="2" max="2" width="12.7109375"/>
-    <col min="3" max="3" width="8.5703125"/>
+    <col min="1" max="1" width="16.44140625"/>
+    <col min="2" max="2" width="12.6640625"/>
+    <col min="3" max="3" width="8.5546875"/>
     <col min="4" max="4" width="10"/>
-    <col min="5" max="5" width="10.140625"/>
-    <col min="6" max="6" width="10.42578125"/>
-    <col min="7" max="7" width="10.7109375"/>
-    <col min="8" max="8" width="19.85546875"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="5" max="5" width="10.109375"/>
+    <col min="6" max="6" width="10.44140625"/>
+    <col min="7" max="7" width="10.6640625"/>
+    <col min="8" max="8" width="19.88671875"/>
+    <col min="9" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1021" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1021" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2440,7 +2465,7 @@
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>300</v>
       </c>
@@ -2459,7 +2484,7 @@
       <c r="AMF2" s="33"/>
       <c r="AMG2" s="33"/>
     </row>
-    <row r="3" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>302</v>
       </c>
@@ -2478,7 +2503,7 @@
       <c r="AMF3" s="33"/>
       <c r="AMG3" s="33"/>
     </row>
-    <row r="4" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>304</v>
       </c>
@@ -2497,7 +2522,7 @@
       <c r="AMF4" s="33"/>
       <c r="AMG4" s="33"/>
     </row>
-    <row r="5" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>306</v>
       </c>
@@ -2516,7 +2541,7 @@
       <c r="AMF5" s="33"/>
       <c r="AMG5" s="33"/>
     </row>
-    <row r="6" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>308</v>
       </c>
@@ -2535,7 +2560,7 @@
       <c r="AMF6" s="33"/>
       <c r="AMG6" s="33"/>
     </row>
-    <row r="7" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>310</v>
       </c>
@@ -2554,7 +2579,7 @@
       <c r="AMF7" s="33"/>
       <c r="AMG7" s="33"/>
     </row>
-    <row r="8" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>312</v>
       </c>
@@ -2573,7 +2598,7 @@
       <c r="AMF8" s="33"/>
       <c r="AMG8" s="33"/>
     </row>
-    <row r="9" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>314</v>
       </c>
@@ -2592,7 +2617,7 @@
       <c r="AMF9" s="33"/>
       <c r="AMG9" s="33"/>
     </row>
-    <row r="10" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>316</v>
       </c>
@@ -2611,7 +2636,7 @@
       <c r="AMF10" s="33"/>
       <c r="AMG10" s="33"/>
     </row>
-    <row r="11" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>318</v>
       </c>
@@ -2630,7 +2655,7 @@
       <c r="AMF11" s="33"/>
       <c r="AMG11" s="33"/>
     </row>
-    <row r="12" spans="1:1021" s="30" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1021" s="30" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>320</v>
       </c>
@@ -2649,7 +2674,7 @@
       <c r="AMF12" s="33"/>
       <c r="AMG12" s="33"/>
     </row>
-    <row r="13" spans="1:1021" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1021" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>322</v>
       </c>
@@ -2666,7 +2691,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="14" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>324</v>
       </c>
@@ -2683,7 +2708,7 @@
         <v>10440868</v>
       </c>
     </row>
-    <row r="15" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>326</v>
       </c>
@@ -2700,7 +2725,7 @@
         <v>10447780</v>
       </c>
     </row>
-    <row r="16" spans="1:1021" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1021" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>328</v>
       </c>
@@ -2717,7 +2742,7 @@
         <v>10444647</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>330</v>
       </c>
@@ -2734,7 +2759,7 @@
         <v>10447788</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>332</v>
       </c>
@@ -2751,7 +2776,7 @@
         <v>10444267</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>334</v>
       </c>
@@ -2768,7 +2793,7 @@
         <v>10444547</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>336</v>
       </c>
@@ -2785,7 +2810,7 @@
         <v>10445049</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>338</v>
       </c>
@@ -2816,22 +2841,22 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="13"/>
-    <col min="2" max="2" width="33.85546875" style="13"/>
-    <col min="3" max="3" width="16.42578125" style="14"/>
-    <col min="4" max="4" width="16.42578125" style="11"/>
-    <col min="5" max="5" width="25.5703125" style="30" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="2"/>
-    <col min="7" max="7" width="40.28515625" style="13"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="19.85546875" style="2"/>
-    <col min="10" max="1021" width="9.140625" style="2"/>
-    <col min="1024" max="1026" width="8.7109375"/>
+    <col min="1" max="1" width="20.33203125" style="13"/>
+    <col min="2" max="2" width="33.88671875" style="13"/>
+    <col min="3" max="3" width="16.44140625" style="14"/>
+    <col min="4" max="4" width="16.44140625" style="11"/>
+    <col min="5" max="5" width="25.5546875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="2"/>
+    <col min="7" max="7" width="40.33203125" style="13"/>
+    <col min="8" max="8" width="9.109375" style="2"/>
+    <col min="9" max="9" width="19.88671875" style="2"/>
+    <col min="10" max="1021" width="9.109375" style="2"/>
+    <col min="1024" max="1026" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2845,7 +2870,7 @@
         <v>341</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>342</v>
@@ -2860,7 +2885,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>343</v>
       </c>
@@ -2874,10 +2899,10 @@
         <v>288</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>346</v>
       </c>
@@ -2891,10 +2916,10 @@
         <v>291</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>347</v>
       </c>
@@ -2908,7 +2933,7 @@
         <v>294</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -2930,19 +2955,19 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2953,7 +2978,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>84</v>
@@ -2971,9 +2996,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
@@ -2988,9 +3013,9 @@
         <v>10440868</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B3" t="s">
         <v>56</v>
@@ -3005,9 +3030,9 @@
         <v>10441723</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
@@ -3022,9 +3047,9 @@
         <v>10445049</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
@@ -3052,24 +3077,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" style="2"/>
+    <col min="1" max="1" width="38.6640625" style="2"/>
     <col min="2" max="2" width="46" style="35"/>
-    <col min="3" max="3" width="32.85546875" style="2"/>
+    <col min="3" max="3" width="32.88671875" style="2"/>
     <col min="4" max="4" width="45" style="36"/>
-    <col min="5" max="5" width="29.28515625" style="36"/>
-    <col min="6" max="6" width="16.42578125" style="11"/>
-    <col min="7" max="8" width="8.42578125" style="2"/>
-    <col min="9" max="9" width="13.42578125" style="2"/>
-    <col min="10" max="10" width="37.28515625" style="2"/>
-    <col min="11" max="11" width="13.42578125" style="2"/>
-    <col min="12" max="12" width="19.85546875" style="2"/>
-    <col min="13" max="1022" width="8.42578125" style="2"/>
-    <col min="1023" max="1025" width="8.42578125"/>
+    <col min="5" max="5" width="29.33203125" style="36"/>
+    <col min="6" max="6" width="16.44140625" style="11"/>
+    <col min="7" max="8" width="8.44140625" style="2"/>
+    <col min="9" max="9" width="13.44140625" style="2"/>
+    <col min="10" max="10" width="37.33203125" style="2"/>
+    <col min="11" max="11" width="13.44140625" style="2"/>
+    <col min="12" max="12" width="19.88671875" style="2"/>
+    <col min="13" max="1022" width="8.44140625" style="2"/>
+    <col min="1023" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>349</v>
       </c>
@@ -3107,7 +3132,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>356</v>
       </c>
@@ -3132,7 +3157,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>362</v>
       </c>
@@ -3154,7 +3179,7 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>364</v>
       </c>
@@ -3176,7 +3201,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>366</v>
       </c>
@@ -3207,27 +3232,27 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK15"/>
+  <dimension ref="A1:AMK16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="39"/>
-    <col min="2" max="2" width="8.5703125" style="39"/>
-    <col min="3" max="3" width="11.5703125" style="39"/>
-    <col min="4" max="4" width="10.42578125" style="39"/>
-    <col min="5" max="5" width="10.7109375" style="39"/>
-    <col min="6" max="6" width="19.85546875" style="39"/>
-    <col min="7" max="1025" width="8.5703125" style="39"/>
+    <col min="1" max="1" width="19.44140625" style="39"/>
+    <col min="2" max="2" width="8.5546875" style="39"/>
+    <col min="3" max="3" width="11.5546875" style="39"/>
+    <col min="4" max="4" width="10.44140625" style="39"/>
+    <col min="5" max="5" width="10.6640625" style="39"/>
+    <col min="6" max="6" width="19.88671875" style="39"/>
+    <col min="7" max="1025" width="8.5546875" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="40" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="40" customFormat="1" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>369</v>
       </c>
@@ -3247,7 +3272,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>372</v>
       </c>
@@ -3261,7 +3286,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
         <v>375</v>
       </c>
@@ -3275,7 +3300,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>378</v>
       </c>
@@ -3286,7 +3311,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
         <v>380</v>
       </c>
@@ -3297,7 +3322,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
         <v>381</v>
       </c>
@@ -3308,7 +3333,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
         <v>382</v>
       </c>
@@ -3319,7 +3344,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
         <v>383</v>
       </c>
@@ -3330,7 +3355,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="39" t="s">
         <v>384</v>
       </c>
@@ -3341,7 +3366,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="41" t="s">
         <v>385</v>
       </c>
@@ -3352,7 +3377,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="41" t="s">
         <v>386</v>
       </c>
@@ -3363,7 +3388,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
         <v>387</v>
       </c>
@@ -3374,9 +3399,9 @@
         <v>373</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="39" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="B13" s="39">
         <v>0.1</v>
@@ -3385,9 +3410,9 @@
         <v>373</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="39" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="B14" s="39">
         <v>0.36</v>
@@ -3396,14 +3421,25 @@
         <v>373</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="39" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B15" s="39">
         <v>0.5</v>
       </c>
       <c r="C15" s="39" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="39" t="s">
+        <v>490</v>
+      </c>
+      <c r="B16" s="39">
+        <v>0.25</v>
+      </c>
+      <c r="C16" s="39" t="s">
         <v>373</v>
       </c>
     </row>
@@ -3417,20 +3453,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16"/>
-    <col min="3" max="3" width="15.42578125"/>
-    <col min="5" max="5" width="10.5703125"/>
-    <col min="6" max="6" width="11.140625"/>
-    <col min="7" max="7" width="20.5703125"/>
+    <col min="3" max="3" width="15.44140625"/>
+    <col min="5" max="5" width="10.5546875"/>
+    <col min="6" max="6" width="11.109375"/>
+    <col min="7" max="7" width="20.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3438,7 +3474,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>371</v>
@@ -3453,7 +3489,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>388</v>
       </c>
@@ -3482,19 +3518,19 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="2"/>
-    <col min="2" max="2" width="23.42578125" style="2"/>
-    <col min="3" max="3" width="17.7109375" style="2"/>
-    <col min="4" max="4" width="18.7109375" style="2"/>
-    <col min="5" max="5" width="12.7109375" style="2"/>
-    <col min="6" max="6" width="14.7109375" style="2"/>
-    <col min="7" max="1022" width="37.28515625" style="2"/>
-    <col min="1023" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="18.6640625" style="2"/>
+    <col min="2" max="2" width="23.44140625" style="2"/>
+    <col min="3" max="3" width="17.6640625" style="2"/>
+    <col min="4" max="4" width="18.6640625" style="2"/>
+    <col min="5" max="5" width="12.6640625" style="2"/>
+    <col min="6" max="6" width="14.6640625" style="2"/>
+    <col min="7" max="1022" width="37.33203125" style="2"/>
+    <col min="1023" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3520,7 +3556,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>393</v>
       </c>
@@ -3537,7 +3573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>397</v>
       </c>
@@ -3554,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>400</v>
       </c>
@@ -3571,7 +3607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>403</v>
       </c>
@@ -3588,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -3605,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>407</v>
       </c>
@@ -3622,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>410</v>
       </c>
@@ -3654,41 +3690,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="42"/>
-    <col min="2" max="2" width="10.7109375" style="42"/>
-    <col min="3" max="3" width="10.42578125" style="42"/>
-    <col min="4" max="4" width="11" style="42"/>
-    <col min="5" max="5" width="6.5703125" style="42"/>
-    <col min="6" max="6" width="28.7109375" style="42"/>
+    <col min="1" max="1" width="20.33203125" style="42"/>
+    <col min="2" max="2" width="18.21875" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="42"/>
+    <col min="4" max="4" width="10.44140625" style="42"/>
+    <col min="5" max="5" width="11" style="42"/>
+    <col min="6" max="6" width="28.6640625" style="42"/>
     <col min="7" max="7" width="11" style="42"/>
     <col min="8" max="8" width="20" style="42"/>
-    <col min="9" max="1025" width="8.7109375" style="42"/>
+    <col min="9" max="1025" width="8.6640625" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>411</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="C1" s="43" t="s">
         <v>412</v>
       </c>
-      <c r="C1" s="43" t="s">
-        <v>413</v>
-      </c>
       <c r="D1" s="43" t="s">
-        <v>414</v>
+        <v>483</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>415</v>
+        <v>371</v>
       </c>
       <c r="F1" s="43" t="s">
         <v>11</v>
@@ -3700,127 +3736,165 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="45" t="s">
+        <v>492</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>393</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>416</v>
-      </c>
       <c r="C2" s="42" t="s">
-        <v>417</v>
-      </c>
-      <c r="D2"/>
-      <c r="E2"/>
+        <v>413</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>487</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="F2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
+        <v>493</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>397</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="C3" s="42" t="s">
+        <v>413</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>491</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>414</v>
+      </c>
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="45" t="s">
+        <v>494</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>400</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>413</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>415</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="42" t="s">
         <v>416</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="45" t="s">
+        <v>495</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>403</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>413</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>487</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>417</v>
+      </c>
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
+        <v>496</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>413</v>
+      </c>
+      <c r="D6" s="42" t="s">
         <v>418</v>
       </c>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3" s="42" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="42" t="s">
         <v>419</v>
       </c>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
-        <v>400</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>416</v>
-      </c>
-      <c r="C4" s="42" t="s">
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
+        <v>497</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="42" t="s">
         <v>420</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D7" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="E4" s="42">
-        <v>2</v>
-      </c>
-      <c r="F4" s="42" t="s">
-        <v>421</v>
-      </c>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
-        <v>403</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>416</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>417</v>
-      </c>
-      <c r="F5" s="42" t="s">
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
+        <v>498</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>407</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>413</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>422</v>
       </c>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>416</v>
-      </c>
-      <c r="C6" s="42" t="s">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="45" t="s">
         <v>423</v>
       </c>
-      <c r="F6" s="42" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="45" t="s">
+        <v>499</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>410</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>413</v>
+      </c>
+      <c r="D9" s="45" t="s">
         <v>424</v>
       </c>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="42" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="45" t="s">
         <v>425</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>426</v>
-      </c>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
-        <v>407</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>416</v>
-      </c>
-      <c r="C8" s="45" t="s">
-        <v>427</v>
-      </c>
-      <c r="H8" s="45" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
-        <v>410</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>416</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>429</v>
-      </c>
-      <c r="H9" s="45" t="s">
-        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3832,20 +3906,22 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="8.5703125"/>
-    <col min="6" max="6" width="10.5703125"/>
-    <col min="7" max="7" width="11.140625"/>
-    <col min="8" max="8" width="20.5703125"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="1" max="5" width="8.5546875"/>
+    <col min="6" max="6" width="10.5546875"/>
+    <col min="7" max="7" width="11.109375"/>
+    <col min="8" max="8" width="20.5546875"/>
+    <col min="9" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3856,7 +3932,7 @@
         <v>370</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>371</v>
@@ -3871,12 +3947,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B2" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="C2">
         <v>20.5</v>
@@ -3885,18 +3961,18 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E2" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="H2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B3" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C3">
         <v>1.35</v>
@@ -3905,18 +3981,18 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="E3" t="s">
+        <v>429</v>
+      </c>
+      <c r="H3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>434</v>
       </c>
-      <c r="H3" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>439</v>
-      </c>
       <c r="B4" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C4">
         <v>0.46</v>
@@ -3928,15 +4004,15 @@
         <v>373</v>
       </c>
       <c r="H4" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C5">
         <v>1.2</v>
@@ -3948,7 +4024,24 @@
         <v>373</v>
       </c>
       <c r="H5" t="s">
-        <v>438</v>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>487</v>
+      </c>
+      <c r="B6" t="s">
+        <v>488</v>
+      </c>
+      <c r="C6">
+        <v>2.1</v>
+      </c>
+      <c r="D6">
+        <v>1E-3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -3968,14 +4061,14 @@
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="6"/>
-    <col min="2" max="2" width="51.140625" style="2"/>
-    <col min="3" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="16.44140625" style="6"/>
+    <col min="2" max="2" width="51.109375" style="2"/>
+    <col min="3" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3983,7 +4076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -3991,7 +4084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
@@ -3999,7 +4092,7 @@
         <v>9606</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -4019,18 +4112,18 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375"/>
-    <col min="2" max="2" width="15.5703125"/>
-    <col min="4" max="4" width="13.140625"/>
-    <col min="5" max="5" width="10.5703125"/>
-    <col min="6" max="6" width="11.140625"/>
-    <col min="7" max="7" width="19.85546875"/>
-    <col min="1021" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="17.6640625"/>
+    <col min="2" max="2" width="15.5546875"/>
+    <col min="4" max="4" width="13.109375"/>
+    <col min="5" max="5" width="10.5546875"/>
+    <col min="6" max="6" width="11.109375"/>
+    <col min="7" max="7" width="19.88671875"/>
+    <col min="1021" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>349</v>
       </c>
@@ -4053,60 +4146,60 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B2" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="C2" s="46">
         <v>3.0000000000000001E-12</v>
       </c>
       <c r="D2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B3" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="C3" s="46">
         <v>10000000</v>
       </c>
       <c r="D3" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B4" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C4">
         <v>0.7</v>
       </c>
       <c r="D4" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="B5" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="C5">
         <v>71280</v>
       </c>
       <c r="D5" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -4127,43 +4220,43 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="18.5703125"/>
-    <col min="3" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="8.5546875"/>
+    <col min="2" max="2" width="18.5546875"/>
+    <col min="3" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>361</v>
       </c>
       <c r="B2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>377</v>
       </c>
       <c r="B3" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B4" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -4180,19 +4273,19 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="16.140625" style="2"/>
-    <col min="3" max="3" width="17.7109375" style="2"/>
-    <col min="4" max="4" width="11.28515625" style="2"/>
-    <col min="5" max="5" width="11.140625" style="2"/>
-    <col min="6" max="6" width="20.5703125" style="2"/>
-    <col min="7" max="1020" width="9.140625" style="2"/>
-    <col min="1024" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="9.109375" style="7"/>
+    <col min="2" max="2" width="16.109375" style="2"/>
+    <col min="3" max="3" width="17.6640625" style="2"/>
+    <col min="4" max="4" width="11.33203125" style="2"/>
+    <col min="5" max="5" width="11.109375" style="2"/>
+    <col min="6" max="6" width="20.5546875" style="2"/>
+    <col min="7" max="1020" width="9.109375" style="2"/>
+    <col min="1024" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4212,7 +4305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -4229,7 +4322,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -4241,7 +4334,7 @@
       </c>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -4255,7 +4348,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
@@ -4281,19 +4374,19 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="9"/>
-    <col min="2" max="2" width="39.42578125" style="9"/>
-    <col min="3" max="3" width="13.7109375" style="2"/>
-    <col min="4" max="4" width="10.7109375" style="2"/>
+    <col min="1" max="1" width="23.88671875" style="9"/>
+    <col min="2" max="2" width="39.44140625" style="9"/>
+    <col min="3" max="3" width="13.6640625" style="2"/>
+    <col min="4" max="4" width="10.6640625" style="2"/>
     <col min="5" max="5" width="55" style="9"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="19.85546875" style="2"/>
-    <col min="8" max="1022" width="9.140625" style="2"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="7" max="7" width="19.88671875" style="2"/>
+    <col min="8" max="1022" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4316,7 +4409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -4324,7 +4417,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -4335,7 +4428,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4343,7 +4436,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -4351,7 +4444,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>40</v>
       </c>
@@ -4362,7 +4455,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>43</v>
       </c>
@@ -4373,7 +4466,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>46</v>
       </c>
@@ -4384,7 +4477,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>49</v>
       </c>
@@ -4413,20 +4506,20 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="7"/>
+    <col min="1" max="1" width="14.109375" style="7"/>
     <col min="2" max="2" width="13" style="11"/>
-    <col min="3" max="4" width="11.7109375" style="2"/>
-    <col min="5" max="5" width="22.140625" style="2"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="8" width="13.42578125" style="2"/>
-    <col min="9" max="9" width="13.42578125"/>
-    <col min="10" max="10" width="19.85546875"/>
-    <col min="11" max="12" width="13.42578125"/>
+    <col min="3" max="4" width="11.6640625" style="2"/>
+    <col min="5" max="5" width="22.109375" style="2"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="7" max="8" width="13.44140625" style="2"/>
+    <col min="9" max="9" width="13.44140625"/>
+    <col min="10" max="10" width="19.88671875"/>
+    <col min="11" max="12" width="13.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4434,7 +4527,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>52</v>
@@ -4443,7 +4536,7 @@
         <v>53</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>54</v>
@@ -4458,7 +4551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
@@ -4477,7 +4570,7 @@
       </c>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>56</v>
       </c>
@@ -4494,7 +4587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>57</v>
       </c>
@@ -4511,7 +4604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>58</v>
       </c>
@@ -4528,7 +4621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>59</v>
       </c>
@@ -4545,7 +4638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>60</v>
       </c>
@@ -4562,7 +4655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>61</v>
       </c>
@@ -4579,7 +4672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>62</v>
       </c>
@@ -4596,7 +4689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>63</v>
       </c>
@@ -4613,7 +4706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>64</v>
       </c>
@@ -4630,7 +4723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>65</v>
       </c>
@@ -4647,7 +4740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>66</v>
       </c>
@@ -4664,7 +4757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>67</v>
       </c>
@@ -4681,7 +4774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>68</v>
       </c>
@@ -4698,7 +4791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>69</v>
       </c>
@@ -4715,7 +4808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>70</v>
       </c>
@@ -4732,7 +4825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>71</v>
       </c>
@@ -4749,7 +4842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>72</v>
       </c>
@@ -4766,7 +4859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>73</v>
       </c>
@@ -4783,7 +4876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>74</v>
       </c>
@@ -4800,7 +4893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>75</v>
       </c>
@@ -4817,7 +4910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>76</v>
       </c>
@@ -4834,7 +4927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>77</v>
       </c>
@@ -4851,7 +4944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>78</v>
       </c>
@@ -4868,7 +4961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>79</v>
       </c>
@@ -4903,19 +4996,19 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="11"/>
-    <col min="2" max="2" width="16.42578125" style="11"/>
-    <col min="3" max="3" width="42.42578125" style="13"/>
-    <col min="4" max="6" width="13.42578125" style="14"/>
-    <col min="7" max="8" width="13.42578125" style="11"/>
-    <col min="9" max="9" width="16.42578125" style="15"/>
-    <col min="10" max="1023" width="32.5703125" style="2"/>
-    <col min="1024" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="17.44140625" style="11"/>
+    <col min="2" max="2" width="16.44140625" style="11"/>
+    <col min="3" max="3" width="42.44140625" style="13"/>
+    <col min="4" max="6" width="13.44140625" style="14"/>
+    <col min="7" max="8" width="13.44140625" style="11"/>
+    <col min="9" max="9" width="16.44140625" style="15"/>
+    <col min="10" max="1023" width="32.5546875" style="2"/>
+    <col min="1024" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1023" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4956,7 +5049,7 @@
       <c r="AMH1" s="2"/>
       <c r="AMI1" s="2"/>
     </row>
-    <row r="2" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>86</v>
       </c>
@@ -4982,7 +5075,7 @@
         <v>20651511</v>
       </c>
     </row>
-    <row r="3" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>91</v>
       </c>
@@ -5008,7 +5101,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="4" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>95</v>
       </c>
@@ -5034,7 +5127,7 @@
         <v>69387254</v>
       </c>
     </row>
-    <row r="5" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>98</v>
       </c>
@@ -5060,7 +5153,7 @@
         <v>40574685</v>
       </c>
     </row>
-    <row r="6" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>101</v>
       </c>
@@ -5086,7 +5179,7 @@
         <v>112649530</v>
       </c>
     </row>
-    <row r="7" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>104</v>
       </c>
@@ -5112,7 +5205,7 @@
         <v>83605875</v>
       </c>
     </row>
-    <row r="8" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>107</v>
       </c>
@@ -5138,7 +5231,7 @@
         <v>127899195</v>
       </c>
     </row>
-    <row r="9" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>110</v>
       </c>
@@ -5164,7 +5257,7 @@
         <v>160421711</v>
       </c>
     </row>
-    <row r="10" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>113</v>
       </c>
@@ -5190,7 +5283,7 @@
         <v>152129619</v>
       </c>
     </row>
-    <row r="11" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>116</v>
       </c>
@@ -5216,7 +5309,7 @@
         <v>56051604</v>
       </c>
     </row>
-    <row r="12" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>119</v>
       </c>
@@ -5242,7 +5335,7 @@
         <v>18084998</v>
       </c>
     </row>
-    <row r="13" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>122</v>
       </c>
@@ -5268,7 +5361,7 @@
         <v>19967258</v>
       </c>
     </row>
-    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>125</v>
       </c>
@@ -5294,7 +5387,7 @@
         <v>136423761</v>
       </c>
     </row>
-    <row r="15" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>128</v>
       </c>
@@ -5320,7 +5413,7 @@
         <v>7787981</v>
       </c>
     </row>
-    <row r="16" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1023" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>131</v>
       </c>
@@ -5346,7 +5439,7 @@
         <v>133421307</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>134</v>
       </c>
@@ -5372,7 +5465,7 @@
         <v>13732346</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>137</v>
       </c>
@@ -5398,7 +5491,7 @@
         <v>114450279</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>140</v>
       </c>
@@ -5424,7 +5517,7 @@
         <v>77065580</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>143</v>
       </c>
@@ -5450,7 +5543,7 @@
         <v>113359493</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>146</v>
       </c>
@@ -5476,7 +5569,7 @@
         <v>52476628</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>149</v>
       </c>
@@ -5502,7 +5595,7 @@
         <v>103057462</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>152</v>
       </c>
@@ -5528,7 +5621,7 @@
         <v>65578352</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>155</v>
       </c>
@@ -5554,7 +5647,7 @@
         <v>101251932</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>158</v>
       </c>
@@ -5580,7 +5673,7 @@
         <v>89155846</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>161</v>
       </c>
@@ -5606,7 +5699,7 @@
         <v>49223225</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>164</v>
       </c>
@@ -5632,7 +5725,7 @@
         <v>50988121</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>167</v>
       </c>
@@ -5658,7 +5751,7 @@
         <v>41440717</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>170</v>
       </c>
@@ -5684,7 +5777,7 @@
         <v>47784686</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>173</v>
       </c>
@@ -5710,7 +5803,7 @@
         <v>13638940</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>176</v>
       </c>
@@ -5736,7 +5829,7 @@
         <v>44652233</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>179</v>
       </c>
@@ -5762,7 +5855,7 @@
         <v>31668931</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>182</v>
       </c>
@@ -5788,7 +5881,7 @@
         <v>20859417</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>185</v>
       </c>
@@ -5814,7 +5907,7 @@
         <v>38738299</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>188</v>
       </c>
@@ -5840,7 +5933,7 @@
         <v>119605895</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>191</v>
       </c>
@@ -5866,7 +5959,7 @@
         <v>23005465</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>194</v>
       </c>
@@ -5911,30 +6004,30 @@
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="16.42578125" style="11"/>
+    <col min="1" max="3" width="16.44140625" style="11"/>
     <col min="4" max="4" width="22" style="11"/>
-    <col min="5" max="5" width="13.7109375" style="11"/>
-    <col min="6" max="6" width="9.140625" style="30"/>
-    <col min="7" max="7" width="25.140625" style="11"/>
-    <col min="8" max="8" width="13.42578125" style="11"/>
-    <col min="9" max="9" width="16.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="30" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" style="11"/>
-    <col min="13" max="13" width="25.140625" style="2"/>
-    <col min="14" max="14" width="19.85546875"/>
-    <col min="15" max="15" width="9.140625" style="14"/>
-    <col min="16" max="16" width="10.42578125" style="14"/>
-    <col min="17" max="17" width="10.7109375" style="14"/>
-    <col min="18" max="19" width="9.140625" style="11"/>
-    <col min="20" max="20" width="22.85546875" style="14"/>
-    <col min="21" max="1016" width="9.140625" style="11"/>
-    <col min="1017" max="1025" width="9.140625" style="2"/>
+    <col min="5" max="5" width="13.6640625" style="11"/>
+    <col min="6" max="6" width="9.109375" style="30"/>
+    <col min="7" max="7" width="25.109375" style="11"/>
+    <col min="8" max="8" width="13.44140625" style="11"/>
+    <col min="9" max="9" width="16.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" style="30" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" style="11"/>
+    <col min="13" max="13" width="25.109375" style="2"/>
+    <col min="14" max="14" width="19.88671875"/>
+    <col min="15" max="15" width="9.109375" style="14"/>
+    <col min="16" max="16" width="10.44140625" style="14"/>
+    <col min="17" max="17" width="10.6640625" style="14"/>
+    <col min="18" max="19" width="9.109375" style="11"/>
+    <col min="20" max="20" width="22.88671875" style="14"/>
+    <col min="21" max="1016" width="9.109375" style="11"/>
+    <col min="1017" max="1025" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1025" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -5960,13 +6053,13 @@
         <v>85</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="L1" s="18" t="s">
         <v>11</v>
@@ -5993,7 +6086,7 @@
       <c r="AMJ1" s="1"/>
       <c r="AMK1" s="1"/>
     </row>
-    <row r="2" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>198</v>
       </c>
@@ -6029,7 +6122,7 @@
       <c r="R2" s="22"/>
       <c r="S2" s="22"/>
     </row>
-    <row r="3" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>202</v>
       </c>
@@ -6065,7 +6158,7 @@
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
     </row>
-    <row r="4" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>205</v>
       </c>
@@ -6101,7 +6194,7 @@
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
     </row>
-    <row r="5" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>209</v>
       </c>
@@ -6137,7 +6230,7 @@
       <c r="R5" s="22"/>
       <c r="S5" s="22"/>
     </row>
-    <row r="6" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>213</v>
       </c>
@@ -6173,7 +6266,7 @@
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
     </row>
-    <row r="7" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>216</v>
       </c>
@@ -6209,7 +6302,7 @@
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
     </row>
-    <row r="8" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>218</v>
       </c>
@@ -6245,7 +6338,7 @@
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
     </row>
-    <row r="9" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>221</v>
       </c>
@@ -6281,7 +6374,7 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
     </row>
-    <row r="10" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>223</v>
       </c>
@@ -6317,7 +6410,7 @@
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
     </row>
-    <row r="11" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>225</v>
       </c>
@@ -6353,7 +6446,7 @@
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>227</v>
       </c>
@@ -6389,7 +6482,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
     </row>
-    <row r="13" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>229</v>
       </c>
@@ -6425,7 +6518,7 @@
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
     </row>
-    <row r="14" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>231</v>
       </c>
@@ -6461,7 +6554,7 @@
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
     </row>
-    <row r="15" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>233</v>
       </c>
@@ -6500,7 +6593,7 @@
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
     </row>
-    <row r="16" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1025" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>236</v>
       </c>
@@ -6536,7 +6629,7 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>238</v>
       </c>
@@ -6572,7 +6665,7 @@
       <c r="R17" s="22"/>
       <c r="S17" s="22"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>240</v>
       </c>
@@ -6608,7 +6701,7 @@
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>242</v>
       </c>
@@ -6640,14 +6733,14 @@
         <v>102368872</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="L19" s="14"/>
       <c r="M19" s="5"/>
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>244</v>
       </c>
@@ -6683,7 +6776,7 @@
       <c r="R20" s="22"/>
       <c r="S20" s="22"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>246</v>
       </c>
@@ -6719,7 +6812,7 @@
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>248</v>
       </c>
@@ -6755,7 +6848,7 @@
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>250</v>
       </c>
@@ -6791,7 +6884,7 @@
       <c r="R23" s="22"/>
       <c r="S23" s="22"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>252</v>
       </c>
@@ -6827,7 +6920,7 @@
       <c r="R24" s="22"/>
       <c r="S24" s="22"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>254</v>
       </c>
@@ -6863,7 +6956,7 @@
       <c r="R25" s="22"/>
       <c r="S25" s="22"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>256</v>
       </c>
@@ -6899,7 +6992,7 @@
       <c r="R26" s="22"/>
       <c r="S26" s="22"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>258</v>
       </c>
@@ -6935,7 +7028,7 @@
       <c r="R27" s="22"/>
       <c r="S27" s="22"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>260</v>
       </c>
@@ -6971,7 +7064,7 @@
       <c r="R28" s="22"/>
       <c r="S28" s="22"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>262</v>
       </c>
@@ -7007,7 +7100,7 @@
       <c r="R29" s="22"/>
       <c r="S29" s="22"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>264</v>
       </c>
@@ -7043,7 +7136,7 @@
       <c r="R30" s="22"/>
       <c r="S30" s="22"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>266</v>
       </c>
@@ -7079,7 +7172,7 @@
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>268</v>
       </c>
@@ -7115,7 +7208,7 @@
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>270</v>
       </c>
@@ -7151,7 +7244,7 @@
       <c r="R33" s="22"/>
       <c r="S33" s="22"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>272</v>
       </c>
@@ -7187,7 +7280,7 @@
       <c r="R34" s="22"/>
       <c r="S34" s="22"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>274</v>
       </c>
@@ -7223,7 +7316,7 @@
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>276</v>
       </c>
@@ -7259,7 +7352,7 @@
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>278</v>
       </c>
@@ -7314,26 +7407,26 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" style="11"/>
-    <col min="5" max="5" width="18.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5546875" style="11"/>
+    <col min="5" max="5" width="18.44140625" style="30" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" style="15"/>
-    <col min="9" max="9" width="13.42578125" style="23"/>
-    <col min="10" max="10" width="19.85546875" style="14"/>
-    <col min="11" max="11" width="10.7109375" style="14"/>
-    <col min="12" max="13" width="9.140625" style="11"/>
-    <col min="14" max="1021" width="9.140625" style="23"/>
-    <col min="1022" max="1024" width="8.42578125"/>
-    <col min="1025" max="1030" width="8.7109375"/>
+    <col min="7" max="7" width="13.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" style="15"/>
+    <col min="9" max="9" width="13.44140625" style="23"/>
+    <col min="10" max="10" width="19.88671875" style="14"/>
+    <col min="11" max="11" width="10.6640625" style="14"/>
+    <col min="12" max="13" width="9.109375" style="11"/>
+    <col min="14" max="1021" width="9.109375" style="23"/>
+    <col min="1022" max="1024" width="8.44140625"/>
+    <col min="1025" max="1030" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -7344,10 +7437,10 @@
         <v>280</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>82</v>
@@ -7366,12 +7459,12 @@
       </c>
       <c r="K1" s="24"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>91</v>
@@ -7381,21 +7474,21 @@
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>107</v>
@@ -7405,21 +7498,21 @@
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
       <c r="N3" s="11"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C4" s="30" t="s">
         <v>107</v>
@@ -7431,18 +7524,18 @@
         <v>347</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="C5" s="30" t="s">
         <v>104</v>
@@ -7454,10 +7547,10 @@
         <v>347</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -7479,23 +7572,23 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="14"/>
-    <col min="2" max="2" width="21.140625" style="14"/>
-    <col min="3" max="3" width="10.7109375" style="14"/>
-    <col min="4" max="4" width="22.85546875" style="15"/>
-    <col min="5" max="5" width="10.7109375"/>
-    <col min="6" max="6" width="13.42578125"/>
-    <col min="7" max="7" width="13.42578125" style="11"/>
-    <col min="8" max="8" width="13.42578125" style="25"/>
-    <col min="9" max="9" width="10.7109375" style="22"/>
-    <col min="10" max="10" width="19.85546875" style="11"/>
-    <col min="11" max="11" width="13.42578125" style="11"/>
-    <col min="12" max="1021" width="9.140625" style="2"/>
+    <col min="1" max="1" width="19.5546875" style="14"/>
+    <col min="2" max="2" width="21.109375" style="14"/>
+    <col min="3" max="3" width="10.6640625" style="14"/>
+    <col min="4" max="4" width="22.88671875" style="15"/>
+    <col min="5" max="5" width="10.6640625"/>
+    <col min="6" max="6" width="13.44140625"/>
+    <col min="7" max="7" width="13.44140625" style="11"/>
+    <col min="8" max="8" width="13.44140625" style="25"/>
+    <col min="9" max="9" width="10.6640625" style="22"/>
+    <col min="10" max="10" width="19.88671875" style="11"/>
+    <col min="11" max="11" width="13.44140625" style="11"/>
+    <col min="12" max="1021" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="26" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -7528,7 +7621,7 @@
       </c>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>282</v>
       </c>
@@ -7554,7 +7647,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>284</v>
       </c>

</xml_diff>

<commit_message>
Adding ptm locus to eukaryote schema
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10115"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chebaro/WC/wc_kb/tests/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FADA8E-A2BD-0A43-B59A-30CC488912D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6840" tabRatio="993" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="1760" windowWidth="27040" windowHeight="20260" tabRatio="993" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -20,26 +26,27 @@
     <sheet name="Exon loci" sheetId="11" r:id="rId11"/>
     <sheet name="Protein species types" sheetId="12" r:id="rId12"/>
     <sheet name="CDS loci" sheetId="21" r:id="rId13"/>
-    <sheet name="Complex species types" sheetId="13" r:id="rId14"/>
-    <sheet name="Concentrations" sheetId="14" r:id="rId15"/>
-    <sheet name="Observables" sheetId="15" r:id="rId16"/>
-    <sheet name="Reactions" sheetId="16" r:id="rId17"/>
-    <sheet name="Rate laws" sheetId="17" r:id="rId18"/>
-    <sheet name="Parameters" sheetId="18" r:id="rId19"/>
-    <sheet name="Properties" sheetId="19" r:id="rId20"/>
-    <sheet name="References" sheetId="20" r:id="rId21"/>
+    <sheet name="Ptm site" sheetId="22" r:id="rId14"/>
+    <sheet name="Complex species types" sheetId="13" r:id="rId15"/>
+    <sheet name="Concentrations" sheetId="14" r:id="rId16"/>
+    <sheet name="Observables" sheetId="15" r:id="rId17"/>
+    <sheet name="Reactions" sheetId="16" r:id="rId18"/>
+    <sheet name="Rate laws" sheetId="17" r:id="rId19"/>
+    <sheet name="Parameters" sheetId="18" r:id="rId20"/>
+    <sheet name="Properties" sheetId="19" r:id="rId21"/>
+    <sheet name="References" sheetId="20" r:id="rId22"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cell!$A$1:$B$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'Complex species types'!$A$1:$J$221</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Gene loci'!$B$1:$H$1064</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Knowledge base'!$A$1:$B$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cell!$A$1:$B$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Gene loci'!$B$1:$H$1064</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'pre-RNA species types'!$A$1:$G$915</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Protein species types'!$A$1:$G$719</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">'Rate laws'!$A$1:$F$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">Reactions!$A$1:$F$220</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Regulatory element loci'!$A$1:$L$776</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Regulatory module'!$A$1:$H$849</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'pre-RNA species types'!$A$1:$G$915</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Protein species types'!$A$1:$G$719</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Complex species types'!$A$1:$J$221</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Reactions!$A$1:$F$220</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'Rate laws'!$A$1:$F$9</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">'Gene loci'!$I$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Knowledge base'!$A$1:$B$2</definedName>
@@ -88,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="509">
   <si>
     <t>Id</t>
   </si>
@@ -1585,19 +1592,43 @@
   </si>
   <si>
     <t>10.1234/abc234</t>
+  </si>
+  <si>
+    <t>Modified protein</t>
+  </si>
+  <si>
+    <t>Modified residue</t>
+  </si>
+  <si>
+    <t>Abundance ratio</t>
+  </si>
+  <si>
+    <t>s56</t>
+  </si>
+  <si>
+    <t>phosphorylation</t>
+  </si>
+  <si>
+    <t>ENSP00000355428_1</t>
+  </si>
+  <si>
+    <t>ENSP00000355428_2</t>
+  </si>
+  <si>
+    <t>ENSP00000355428_3</t>
+  </si>
+  <si>
+    <t>t73,s77</t>
+  </si>
+  <si>
+    <t>s141</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="31">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1673,150 +1704,31 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1841,194 +1753,8 @@
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2036,251 +1762,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2289,12 +1776,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="35"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="35" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="35" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="35" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2392,59 +1879,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="35" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -2517,6 +1963,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2803,30 +2252,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5583333333333" style="37"/>
-    <col min="2" max="2" width="43.4416666666667" style="8"/>
-    <col min="3" max="1025" width="8.44166666666667"/>
+    <col min="1" max="1" width="21.5" style="37"/>
+    <col min="2" max="2" width="43.5" style="8"/>
+    <col min="3" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:2">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -2834,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" spans="1:2">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
         <v>2</v>
       </c>
@@ -2842,7 +2290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="1:2">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="43" t="s">
         <v>4</v>
       </c>
@@ -2850,7 +2298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
         <v>5</v>
       </c>
@@ -2858,25 +2306,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>9</v>
       </c>
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>10</v>
       </c>
@@ -2884,43 +2332,39 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <autoFilter ref="A1:B9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.4416666666667"/>
-    <col min="2" max="2" width="11.6666666666667"/>
-    <col min="3" max="4" width="8.55833333333333"/>
-    <col min="5" max="5" width="7.44166666666667"/>
-    <col min="6" max="6" width="10.4416666666667"/>
-    <col min="7" max="7" width="10.6666666666667"/>
-    <col min="8" max="8" width="19.8833333333333"/>
-    <col min="9" max="1025" width="8.55833333333333"/>
+    <col min="1" max="1" width="16.5"/>
+    <col min="2" max="2" width="11.6640625"/>
+    <col min="3" max="4" width="8.5"/>
+    <col min="5" max="5" width="7.5"/>
+    <col min="6" max="6" width="10.5"/>
+    <col min="7" max="7" width="10.6640625"/>
+    <col min="8" max="8" width="19.83203125"/>
+    <col min="9" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="23" customFormat="1" ht="12" spans="1:9">
+    <row r="1" spans="1:9" s="23" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -2947,7 +2391,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>311</v>
       </c>
@@ -2961,7 +2405,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>314</v>
       </c>
@@ -2975,7 +2419,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>317</v>
       </c>
@@ -2989,7 +2433,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>320</v>
       </c>
@@ -3004,35 +2448,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMG21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.4416666666667"/>
-    <col min="2" max="2" width="12.6666666666667"/>
-    <col min="3" max="3" width="8.55833333333333"/>
+    <col min="1" max="1" width="16.5"/>
+    <col min="2" max="2" width="12.6640625"/>
+    <col min="3" max="3" width="8.5"/>
     <col min="4" max="4" width="10"/>
-    <col min="5" max="5" width="10.1083333333333"/>
-    <col min="6" max="6" width="10.4416666666667"/>
-    <col min="7" max="7" width="10.6666666666667"/>
-    <col min="8" max="8" width="19.8833333333333"/>
-    <col min="9" max="1025" width="8.55833333333333"/>
+    <col min="5" max="5" width="10.1640625"/>
+    <col min="6" max="6" width="10.5"/>
+    <col min="7" max="7" width="10.6640625"/>
+    <col min="8" max="8" width="19.83203125"/>
+    <col min="9" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="23" customFormat="1" ht="12" spans="1:9">
+    <row r="1" spans="1:1021" s="23" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -3059,7 +2501,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="2" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>323</v>
       </c>
@@ -3078,7 +2520,7 @@
       <c r="AMF2" s="26"/>
       <c r="AMG2" s="26"/>
     </row>
-    <row r="3" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="3" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>325</v>
       </c>
@@ -3097,7 +2539,7 @@
       <c r="AMF3" s="26"/>
       <c r="AMG3" s="26"/>
     </row>
-    <row r="4" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="4" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>327</v>
       </c>
@@ -3116,7 +2558,7 @@
       <c r="AMF4" s="26"/>
       <c r="AMG4" s="26"/>
     </row>
-    <row r="5" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="5" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>329</v>
       </c>
@@ -3135,7 +2577,7 @@
       <c r="AMF5" s="26"/>
       <c r="AMG5" s="26"/>
     </row>
-    <row r="6" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="6" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>331</v>
       </c>
@@ -3154,7 +2596,7 @@
       <c r="AMF6" s="26"/>
       <c r="AMG6" s="26"/>
     </row>
-    <row r="7" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="7" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>333</v>
       </c>
@@ -3173,7 +2615,7 @@
       <c r="AMF7" s="26"/>
       <c r="AMG7" s="26"/>
     </row>
-    <row r="8" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="8" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>335</v>
       </c>
@@ -3192,7 +2634,7 @@
       <c r="AMF8" s="26"/>
       <c r="AMG8" s="26"/>
     </row>
-    <row r="9" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="9" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>337</v>
       </c>
@@ -3211,7 +2653,7 @@
       <c r="AMF9" s="26"/>
       <c r="AMG9" s="26"/>
     </row>
-    <row r="10" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="10" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>339</v>
       </c>
@@ -3230,7 +2672,7 @@
       <c r="AMF10" s="26"/>
       <c r="AMG10" s="26"/>
     </row>
-    <row r="11" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="11" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>341</v>
       </c>
@@ -3249,7 +2691,7 @@
       <c r="AMF11" s="26"/>
       <c r="AMG11" s="26"/>
     </row>
-    <row r="12" s="15" customFormat="1" ht="14.4" customHeight="1" spans="1:1021">
+    <row r="12" spans="1:1021" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>343</v>
       </c>
@@ -3268,7 +2710,7 @@
       <c r="AMF12" s="26"/>
       <c r="AMG12" s="26"/>
     </row>
-    <row r="13" ht="14.4" customHeight="1" spans="1:5">
+    <row r="13" spans="1:1021" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>345</v>
       </c>
@@ -3285,7 +2727,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:1021" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>347</v>
       </c>
@@ -3302,7 +2744,7 @@
         <v>10440868</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:1021" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>349</v>
       </c>
@@ -3319,7 +2761,7 @@
         <v>10447780</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:1021" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>351</v>
       </c>
@@ -3336,7 +2778,7 @@
         <v>10444647</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>353</v>
       </c>
@@ -3353,7 +2795,7 @@
         <v>10447788</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>355</v>
       </c>
@@ -3370,7 +2812,7 @@
         <v>10444267</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>357</v>
       </c>
@@ -3387,7 +2829,7 @@
         <v>10444547</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>359</v>
       </c>
@@ -3404,7 +2846,7 @@
         <v>10445049</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>361</v>
       </c>
@@ -3422,37 +2864,35 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:AMG4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.3333333333333" style="9"/>
-    <col min="2" max="2" width="33.8833333333333" style="9"/>
-    <col min="3" max="3" width="16.4416666666667" style="19"/>
-    <col min="4" max="4" width="16.4416666666667" style="15"/>
-    <col min="5" max="5" width="25.5583333333333" style="15" customWidth="1"/>
-    <col min="6" max="6" width="10.4416666666667" style="8"/>
-    <col min="7" max="7" width="40.3333333333333" style="9"/>
-    <col min="8" max="8" width="9.10833333333333" style="8"/>
-    <col min="9" max="9" width="19.8833333333333" style="8"/>
-    <col min="10" max="1021" width="9.10833333333333" style="8"/>
-    <col min="1024" max="1026" width="8.66666666666667"/>
+    <col min="1" max="1" width="20.33203125" style="9"/>
+    <col min="2" max="2" width="33.83203125" style="9"/>
+    <col min="3" max="3" width="16.5" style="19"/>
+    <col min="4" max="4" width="16.5" style="15"/>
+    <col min="5" max="5" width="25.5" style="15" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="8"/>
+    <col min="7" max="7" width="40.33203125" style="9"/>
+    <col min="8" max="8" width="9.1640625" style="8"/>
+    <col min="9" max="9" width="19.83203125" style="8"/>
+    <col min="10" max="1021" width="9.1640625" style="8"/>
+    <col min="1024" max="1026" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12" spans="1:9">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3481,7 +2921,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>241</v>
       </c>
@@ -3498,8 +2938,8 @@
         <v>369</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="48" t="s">
         <v>370</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -3515,7 +2955,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>300</v>
       </c>
@@ -3533,10 +2973,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G719">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <autoFilter ref="A1:G719" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
@@ -3546,27 +2984,26 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.8833333333333" customWidth="1"/>
-    <col min="2" max="2" width="12.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="17.8833333333333" customWidth="1"/>
-    <col min="5" max="5" width="10.1083333333333" customWidth="1"/>
-    <col min="6" max="6" width="9.88333333333333" customWidth="1"/>
-    <col min="7" max="7" width="10.3333333333333" customWidth="1"/>
-    <col min="8" max="8" width="10.6666666666667" customWidth="1"/>
-    <col min="9" max="9" width="19.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -3595,7 +3032,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" spans="1:6">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>371</v>
       </c>
@@ -3612,7 +3049,7 @@
         <v>10440868</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="1:6">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>375</v>
       </c>
@@ -3629,7 +3066,7 @@
         <v>10441723</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>373</v>
       </c>
@@ -3646,7 +3083,7 @@
         <v>10445049</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>376</v>
       </c>
@@ -3665,37 +3102,142 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0DB845-CD92-6A44-ACBA-7BA9C7C1DD93}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>499</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="47" t="s">
+        <v>504</v>
+      </c>
+      <c r="C2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>503</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>502</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="46"/>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>370</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>503</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>507</v>
+      </c>
+      <c r="F3">
+        <v>0.8</v>
+      </c>
+      <c r="H3" s="46"/>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="47" t="s">
+        <v>506</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>370</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>503</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>508</v>
+      </c>
+      <c r="F4">
+        <v>0.02</v>
+      </c>
+      <c r="H4" s="46"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:AMH5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.6666666666667" style="8"/>
+    <col min="1" max="1" width="38.6640625" style="8"/>
     <col min="2" max="2" width="46" style="13"/>
-    <col min="3" max="3" width="32.8833333333333" style="8"/>
+    <col min="3" max="3" width="32.83203125" style="8"/>
     <col min="4" max="4" width="45" style="14"/>
-    <col min="5" max="5" width="29.3333333333333" style="14"/>
-    <col min="6" max="6" width="16.4416666666667" style="15"/>
-    <col min="7" max="8" width="8.44166666666667" style="8"/>
-    <col min="9" max="9" width="13.4416666666667" style="8"/>
-    <col min="10" max="10" width="37.3333333333333" style="8"/>
-    <col min="11" max="11" width="13.4416666666667" style="8"/>
-    <col min="12" max="12" width="19.8833333333333" style="8"/>
-    <col min="13" max="1022" width="8.44166666666667" style="8"/>
-    <col min="1023" max="1025" width="8.44166666666667"/>
+    <col min="5" max="5" width="29.33203125" style="14"/>
+    <col min="6" max="6" width="16.5" style="15"/>
+    <col min="7" max="8" width="8.5" style="8"/>
+    <col min="9" max="9" width="13.5" style="8"/>
+    <col min="10" max="10" width="37.33203125" style="8"/>
+    <col min="11" max="11" width="13.5" style="8"/>
+    <col min="12" max="12" width="19.83203125" style="8"/>
+    <col min="13" max="1022" width="8.5" style="8"/>
+    <col min="1023" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="15" customHeight="1" spans="1:12">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>377</v>
       </c>
@@ -3733,7 +3275,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" spans="1:11">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>384</v>
       </c>
@@ -3758,7 +3300,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="1:11">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>390</v>
       </c>
@@ -3780,7 +3322,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:11">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>392</v>
       </c>
@@ -3802,7 +3344,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="1:11">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>394</v>
       </c>
@@ -3825,40 +3367,35 @@
       <c r="K5" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J221">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <autoFilter ref="A1:J221" xr:uid="{00000000-0009-0000-0000-00000D000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F16"/>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:AMK16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.4416666666667" style="11"/>
-    <col min="2" max="2" width="8.55833333333333" style="11"/>
-    <col min="3" max="3" width="11.5583333333333" style="11"/>
-    <col min="4" max="4" width="10.4416666666667" style="11"/>
-    <col min="5" max="5" width="10.6666666666667" style="11"/>
-    <col min="6" max="6" width="19.8833333333333" style="11"/>
-    <col min="7" max="1025" width="8.55833333333333" style="11"/>
+    <col min="1" max="1" width="19.5" style="11"/>
+    <col min="2" max="2" width="8.5" style="11"/>
+    <col min="3" max="3" width="11.5" style="11"/>
+    <col min="4" max="4" width="10.5" style="11"/>
+    <col min="5" max="5" width="10.6640625" style="11"/>
+    <col min="6" max="6" width="19.83203125" style="11"/>
+    <col min="7" max="1025" width="8.5" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="1" ht="15.15" customHeight="1" spans="1:6">
+    <row r="1" spans="1:6" s="10" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>397</v>
       </c>
@@ -3878,7 +3415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="15.15" customHeight="1" spans="1:6">
+    <row r="2" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>400</v>
       </c>
@@ -3892,7 +3429,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="3" ht="15.15" customHeight="1" spans="1:5">
+    <row r="3" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>403</v>
       </c>
@@ -3906,7 +3443,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="4" ht="15.15" customHeight="1" spans="1:3">
+    <row r="4" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>406</v>
       </c>
@@ -3917,7 +3454,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="5" ht="15.15" customHeight="1" spans="1:3">
+    <row r="5" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>407</v>
       </c>
@@ -3928,7 +3465,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="6" ht="15.15" customHeight="1" spans="1:3">
+    <row r="6" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>408</v>
       </c>
@@ -3939,7 +3476,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="7" ht="15.15" customHeight="1" spans="1:3">
+    <row r="7" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>409</v>
       </c>
@@ -3950,7 +3487,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="8" ht="15.15" customHeight="1" spans="1:3">
+    <row r="8" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>410</v>
       </c>
@@ -3961,7 +3498,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="9" ht="15.15" customHeight="1" spans="1:3">
+    <row r="9" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>411</v>
       </c>
@@ -3972,7 +3509,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="10" ht="15.15" customHeight="1" spans="1:3">
+    <row r="10" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>412</v>
       </c>
@@ -3983,7 +3520,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="11" ht="15.15" customHeight="1" spans="1:3">
+    <row r="11" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>413</v>
       </c>
@@ -3994,7 +3531,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="12" ht="15.15" customHeight="1" spans="1:3">
+    <row r="12" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>414</v>
       </c>
@@ -4005,7 +3542,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>415</v>
       </c>
@@ -4016,7 +3553,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>416</v>
       </c>
@@ -4027,7 +3564,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>417</v>
       </c>
@@ -4038,7 +3575,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>418</v>
       </c>
@@ -4050,31 +3587,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16"/>
-    <col min="3" max="3" width="15.4416666666667"/>
-    <col min="5" max="5" width="10.5583333333333"/>
-    <col min="6" max="6" width="11.1083333333333"/>
-    <col min="7" max="7" width="20.5583333333333"/>
+    <col min="3" max="3" width="15.5"/>
+    <col min="5" max="5" width="10.5"/>
+    <col min="6" max="6" width="11.1640625"/>
+    <col min="7" max="7" width="20.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12" spans="1:7">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4097,7 +3632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="14.4" customHeight="1" spans="1:4">
+    <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>420</v>
       </c>
@@ -4109,186 +3644,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>
-  <cols>
-    <col min="1" max="1" width="18.6666666666667" style="8"/>
-    <col min="2" max="2" width="23.4416666666667" style="8"/>
-    <col min="3" max="3" width="17.6666666666667" style="8"/>
-    <col min="4" max="4" width="18.6666666666667" style="8"/>
-    <col min="5" max="5" width="12.6666666666667" style="8"/>
-    <col min="6" max="6" width="14.6666666666667" style="8"/>
-    <col min="7" max="1022" width="37.3333333333333" style="8"/>
-    <col min="1023" max="1025" width="8.44166666666667"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>426</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>428</v>
-      </c>
-      <c r="E2" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="8" t="s">
-        <v>429</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>430</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>431</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="E6" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="8" t="s">
-        <v>442</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F220">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
@@ -4298,247 +3654,26 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:AMH8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.3333333333333" style="4"/>
-    <col min="2" max="2" width="18.2166666666667" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.6666666666667" style="4"/>
-    <col min="4" max="4" width="10.4416666666667" style="4"/>
-    <col min="5" max="5" width="11" style="4"/>
-    <col min="6" max="6" width="28.6666666666667" style="4"/>
-    <col min="7" max="7" width="11" style="4"/>
-    <col min="8" max="8" width="20" style="4"/>
-    <col min="9" max="1025" width="8.66666666666667" style="4"/>
+    <col min="1" max="1" width="18.6640625" style="8"/>
+    <col min="2" max="2" width="23.5" style="8"/>
+    <col min="3" max="3" width="17.6640625" style="8"/>
+    <col min="4" max="4" width="18.6640625" style="8"/>
+    <col min="5" max="5" width="12.6640625" style="8"/>
+    <col min="6" max="6" width="14.6640625" style="8"/>
+    <col min="7" max="1022" width="37.33203125" style="8"/>
+    <col min="1023" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:8">
-      <c r="A1" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>446</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2"/>
-      <c r="H2"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>448</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>446</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="6" t="s">
-        <v>455</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="6" t="s">
-        <v>458</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>460</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
-        <v>461</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>445</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
-        <v>464</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>445</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>465</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>466</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F9">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="7"/>
-  <cols>
-    <col min="1" max="5" width="8.55833333333333"/>
-    <col min="6" max="6" width="10.5583333333333"/>
-    <col min="7" max="7" width="11.1083333333333"/>
-    <col min="8" max="8" width="20.5583333333333"/>
-    <col min="9" max="1025" width="8.55833333333333"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4546,13 +3681,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>398</v>
+        <v>422</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>467</v>
+        <v>423</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>399</v>
+        <v>424</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>11</v>
@@ -4564,270 +3699,128 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>468</v>
-      </c>
-      <c r="B2" t="s">
-        <v>469</v>
-      </c>
-      <c r="C2">
-        <v>20.5</v>
-      </c>
-      <c r="D2">
-        <v>0.005</v>
-      </c>
-      <c r="E2" t="s">
-        <v>470</v>
-      </c>
-      <c r="H2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>472</v>
-      </c>
-      <c r="B3" t="s">
-        <v>473</v>
-      </c>
-      <c r="C3">
-        <v>1.35</v>
-      </c>
-      <c r="D3">
-        <v>0.006</v>
-      </c>
-      <c r="E3" t="s">
-        <v>470</v>
-      </c>
-      <c r="H3" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B4" t="s">
-        <v>476</v>
-      </c>
-      <c r="C4">
-        <v>0.46</v>
-      </c>
-      <c r="D4">
-        <v>0.006</v>
-      </c>
-      <c r="E4" t="s">
-        <v>401</v>
-      </c>
-      <c r="H4" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>477</v>
-      </c>
-      <c r="B5" t="s">
-        <v>478</v>
-      </c>
-      <c r="C5">
-        <v>1.2</v>
-      </c>
-      <c r="D5">
-        <v>0.006</v>
-      </c>
-      <c r="E5" t="s">
-        <v>401</v>
-      </c>
-      <c r="H5" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>446</v>
-      </c>
-      <c r="B6" t="s">
-        <v>479</v>
-      </c>
-      <c r="C6">
-        <v>2.1</v>
-      </c>
-      <c r="D6">
-        <v>0.001</v>
-      </c>
-      <c r="E6" t="s">
-        <v>480</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1" width="16.4416666666667" style="42"/>
-    <col min="2" max="2" width="51.1083333333333" style="8"/>
-    <col min="3" max="1025" width="8.44166666666667"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:2">
-      <c r="A1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="8">
-        <v>9606</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B4">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
-  <cols>
-    <col min="1" max="1" width="17.6666666666667"/>
-    <col min="2" max="2" width="15.5583333333333"/>
-    <col min="4" max="4" width="13.1083333333333"/>
-    <col min="5" max="5" width="10.5583333333333"/>
-    <col min="6" max="6" width="11.1083333333333"/>
-    <col min="7" max="7" width="19.8833333333333"/>
-    <col min="1021" max="1025" width="8.66666666666667"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>481</v>
-      </c>
-      <c r="B2" t="s">
-        <v>482</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3e-12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>484</v>
-      </c>
-      <c r="B3" t="s">
-        <v>485</v>
-      </c>
-      <c r="C3" s="2">
-        <v>10000000</v>
-      </c>
-      <c r="D3" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>487</v>
-      </c>
-      <c r="B4" t="s">
-        <v>488</v>
-      </c>
-      <c r="C4">
-        <v>0.7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>490</v>
-      </c>
-      <c r="B5" t="s">
-        <v>491</v>
-      </c>
-      <c r="C5">
-        <v>71280</v>
-      </c>
-      <c r="D5" t="s">
-        <v>492</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <autoFilter ref="A1:F220" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
@@ -4836,23 +3829,548 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:AMK9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" style="4"/>
+    <col min="2" max="2" width="18.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="4"/>
+    <col min="4" max="4" width="10.5" style="4"/>
+    <col min="5" max="5" width="11" style="4"/>
+    <col min="6" max="6" width="28.6640625" style="4"/>
+    <col min="7" max="7" width="11" style="4"/>
+    <col min="8" max="8" width="20" style="4"/>
+    <col min="9" max="1025" width="8.6640625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2"/>
+      <c r="H2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>448</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>466</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F9" xr:uid="{00000000-0009-0000-0000-000011000000}"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" style="42"/>
+    <col min="2" max="2" width="51.1640625" style="8"/>
+    <col min="3" max="1025" width="8.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="8">
+        <v>9606</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="8.5"/>
+    <col min="6" max="6" width="10.5"/>
+    <col min="7" max="7" width="11.1640625"/>
+    <col min="8" max="8" width="20.5"/>
+    <col min="9" max="1025" width="8.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C2">
+        <v>20.5</v>
+      </c>
+      <c r="D2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>470</v>
+      </c>
+      <c r="H2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C3">
+        <v>1.35</v>
+      </c>
+      <c r="D3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>470</v>
+      </c>
+      <c r="H3" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B4" t="s">
+        <v>476</v>
+      </c>
+      <c r="C4">
+        <v>0.46</v>
+      </c>
+      <c r="D4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>401</v>
+      </c>
+      <c r="H4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>477</v>
+      </c>
+      <c r="B5" t="s">
+        <v>478</v>
+      </c>
+      <c r="C5">
+        <v>1.2</v>
+      </c>
+      <c r="D5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>401</v>
+      </c>
+      <c r="H5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>446</v>
+      </c>
+      <c r="B6" t="s">
+        <v>479</v>
+      </c>
+      <c r="C6">
+        <v>2.1</v>
+      </c>
+      <c r="D6">
+        <v>1E-3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>480</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625"/>
+    <col min="2" max="2" width="15.5"/>
+    <col min="4" max="4" width="13.1640625"/>
+    <col min="5" max="5" width="10.5"/>
+    <col min="6" max="6" width="11.1640625"/>
+    <col min="7" max="7" width="19.83203125"/>
+    <col min="1021" max="1025" width="8.6640625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3.0000000000000001E-12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>484</v>
+      </c>
+      <c r="B3" t="s">
+        <v>485</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>487</v>
+      </c>
+      <c r="B4" t="s">
+        <v>488</v>
+      </c>
+      <c r="C4">
+        <v>0.7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>490</v>
+      </c>
+      <c r="B5" t="s">
+        <v>491</v>
+      </c>
+      <c r="C5">
+        <v>71280</v>
+      </c>
+      <c r="D5" t="s">
+        <v>492</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.55833333333333"/>
-    <col min="2" max="2" width="18.5583333333333"/>
-    <col min="3" max="1025" width="8.55833333333333"/>
+    <col min="1" max="1" width="8.5"/>
+    <col min="2" max="2" width="18.5"/>
+    <col min="3" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>493</v>
       </c>
@@ -4860,7 +4378,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>389</v>
       </c>
@@ -4868,7 +4386,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>405</v>
       </c>
@@ -4876,7 +4394,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>497</v>
       </c>
@@ -4885,34 +4403,32 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.10833333333333" style="39"/>
-    <col min="2" max="2" width="16.1083333333333" style="8"/>
-    <col min="3" max="3" width="17.6666666666667" style="8"/>
-    <col min="4" max="4" width="11.3333333333333" style="8"/>
-    <col min="5" max="5" width="11.1083333333333" style="8"/>
-    <col min="6" max="6" width="20.5583333333333" style="8"/>
-    <col min="7" max="1020" width="9.10833333333333" style="8"/>
-    <col min="1024" max="1025" width="8.66666666666667"/>
+    <col min="1" max="1" width="9.1640625" style="39"/>
+    <col min="2" max="2" width="16.1640625" style="8"/>
+    <col min="3" max="3" width="17.6640625" style="8"/>
+    <col min="4" max="4" width="11.33203125" style="8"/>
+    <col min="5" max="5" width="11.1640625" style="8"/>
+    <col min="6" max="6" width="20.5" style="8"/>
+    <col min="7" max="1020" width="9.1640625" style="8"/>
+    <col min="1024" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12" spans="1:6">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4932,7 +4448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
         <v>18</v>
       </c>
@@ -4949,7 +4465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
         <v>22</v>
       </c>
@@ -4961,7 +4477,7 @@
       </c>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
         <v>24</v>
       </c>
@@ -4975,7 +4491,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
         <v>27</v>
       </c>
@@ -4984,7 +4500,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
@@ -4994,27 +4510,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AMH9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.8833333333333" style="41"/>
-    <col min="2" max="2" width="39.4416666666667" style="41"/>
-    <col min="3" max="3" width="13.6666666666667" style="8"/>
-    <col min="4" max="4" width="10.6666666666667" style="8"/>
+    <col min="1" max="1" width="23.83203125" style="41"/>
+    <col min="2" max="2" width="39.5" style="41"/>
+    <col min="3" max="3" width="13.6640625" style="8"/>
+    <col min="4" max="4" width="10.6640625" style="8"/>
     <col min="5" max="5" width="55" style="41"/>
-    <col min="6" max="6" width="9.10833333333333" style="8"/>
-    <col min="7" max="7" width="19.8833333333333" style="8"/>
-    <col min="8" max="1022" width="9.10833333333333" style="8"/>
+    <col min="6" max="6" width="9.1640625" style="8"/>
+    <col min="7" max="7" width="19.83203125" style="8"/>
+    <col min="8" max="1022" width="9.1640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12" spans="1:7">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5037,7 +4552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -5045,7 +4560,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -5056,7 +4571,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -5064,7 +4579,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -5072,7 +4587,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>40</v>
       </c>
@@ -5083,7 +4598,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>43</v>
       </c>
@@ -5094,7 +4609,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>46</v>
       </c>
@@ -5105,7 +4620,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
         <v>49</v>
       </c>
@@ -5117,7 +4632,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
@@ -5127,28 +4642,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1083333333333" style="39"/>
+    <col min="1" max="1" width="14.1640625" style="39"/>
     <col min="2" max="2" width="13" style="15"/>
-    <col min="3" max="4" width="11.6666666666667" style="8"/>
-    <col min="5" max="5" width="22.1083333333333" style="8"/>
-    <col min="6" max="6" width="9.10833333333333" style="8"/>
-    <col min="7" max="8" width="13.4416666666667" style="8"/>
-    <col min="9" max="9" width="13.4416666666667"/>
-    <col min="10" max="10" width="19.8833333333333"/>
-    <col min="11" max="12" width="13.4416666666667"/>
+    <col min="3" max="4" width="11.6640625" style="8"/>
+    <col min="5" max="5" width="22.1640625" style="8"/>
+    <col min="6" max="6" width="9.1640625" style="8"/>
+    <col min="7" max="8" width="13.5" style="8"/>
+    <col min="9" max="9" width="13.5"/>
+    <col min="10" max="10" width="19.83203125"/>
+    <col min="11" max="12" width="13.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5180,7 +4694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
         <v>57</v>
       </c>
@@ -5199,7 +4713,7 @@
       </c>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
         <v>58</v>
       </c>
@@ -5216,7 +4730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
         <v>59</v>
       </c>
@@ -5233,7 +4747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
         <v>60</v>
       </c>
@@ -5250,7 +4764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
         <v>61</v>
       </c>
@@ -5267,7 +4781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
         <v>62</v>
       </c>
@@ -5284,7 +4798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
         <v>63</v>
       </c>
@@ -5301,7 +4815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="s">
         <v>64</v>
       </c>
@@ -5318,7 +4832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="s">
         <v>65</v>
       </c>
@@ -5335,7 +4849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="s">
         <v>66</v>
       </c>
@@ -5352,7 +4866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="39" t="s">
         <v>67</v>
       </c>
@@ -5369,7 +4883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="39" t="s">
         <v>68</v>
       </c>
@@ -5386,7 +4900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="39" t="s">
         <v>69</v>
       </c>
@@ -5403,7 +4917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="39" t="s">
         <v>70</v>
       </c>
@@ -5420,7 +4934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="39" t="s">
         <v>71</v>
       </c>
@@ -5437,7 +4951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="39" t="s">
         <v>72</v>
       </c>
@@ -5454,7 +4968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="s">
         <v>73</v>
       </c>
@@ -5471,7 +4985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="s">
         <v>74</v>
       </c>
@@ -5488,7 +5002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="39" t="s">
         <v>75</v>
       </c>
@@ -5505,7 +5019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="39" t="s">
         <v>76</v>
       </c>
@@ -5522,7 +5036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="39" t="s">
         <v>77</v>
       </c>
@@ -5539,7 +5053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="39" t="s">
         <v>78</v>
       </c>
@@ -5556,7 +5070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="39" t="s">
         <v>79</v>
       </c>
@@ -5573,7 +5087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="39" t="s">
         <v>80</v>
       </c>
@@ -5590,7 +5104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="39" t="s">
         <v>81</v>
       </c>
@@ -5608,7 +5122,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
@@ -5618,27 +5132,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMI37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.4416666666667" style="15"/>
-    <col min="2" max="2" width="16.4416666666667" style="15"/>
-    <col min="3" max="3" width="42.4416666666667" style="9"/>
-    <col min="4" max="6" width="13.4416666666667" style="19"/>
-    <col min="7" max="8" width="13.4416666666667" style="15"/>
-    <col min="9" max="9" width="16.4416666666667" style="27"/>
-    <col min="10" max="1023" width="32.5583333333333" style="8"/>
-    <col min="1024" max="1025" width="8.44166666666667"/>
+    <col min="1" max="1" width="17.5" style="15"/>
+    <col min="2" max="2" width="16.5" style="15"/>
+    <col min="3" max="3" width="42.5" style="9"/>
+    <col min="4" max="6" width="13.5" style="19"/>
+    <col min="7" max="8" width="13.5" style="15"/>
+    <col min="9" max="9" width="16.5" style="27"/>
+    <col min="10" max="1023" width="32.5" style="8"/>
+    <col min="1024" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12" spans="1:1023">
+    <row r="1" spans="1:1023" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5679,7 +5192,7 @@
       <c r="AMH1" s="8"/>
       <c r="AMI1" s="8"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>88</v>
       </c>
@@ -5705,7 +5218,7 @@
         <v>20651511</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>93</v>
       </c>
@@ -5731,7 +5244,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>97</v>
       </c>
@@ -5757,7 +5270,7 @@
         <v>69387254</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>100</v>
       </c>
@@ -5783,7 +5296,7 @@
         <v>40574685</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>103</v>
       </c>
@@ -5809,7 +5322,7 @@
         <v>112649530</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>106</v>
       </c>
@@ -5835,7 +5348,7 @@
         <v>83605875</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>109</v>
       </c>
@@ -5861,7 +5374,7 @@
         <v>127899195</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>112</v>
       </c>
@@ -5887,7 +5400,7 @@
         <v>160421711</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>115</v>
       </c>
@@ -5913,7 +5426,7 @@
         <v>152129619</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>118</v>
       </c>
@@ -5939,7 +5452,7 @@
         <v>56051604</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>121</v>
       </c>
@@ -5965,7 +5478,7 @@
         <v>18084998</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>124</v>
       </c>
@@ -5991,7 +5504,7 @@
         <v>19967258</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" spans="1:8">
+    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>127</v>
       </c>
@@ -6017,7 +5530,7 @@
         <v>136423761</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>130</v>
       </c>
@@ -6043,7 +5556,7 @@
         <v>7787981</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>133</v>
       </c>
@@ -6069,7 +5582,7 @@
         <v>133421307</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>136</v>
       </c>
@@ -6095,7 +5608,7 @@
         <v>13732346</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>139</v>
       </c>
@@ -6121,7 +5634,7 @@
         <v>114450279</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>142</v>
       </c>
@@ -6147,7 +5660,7 @@
         <v>77065580</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>145</v>
       </c>
@@ -6173,7 +5686,7 @@
         <v>113359493</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>148</v>
       </c>
@@ -6199,7 +5712,7 @@
         <v>52476628</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
         <v>151</v>
       </c>
@@ -6225,7 +5738,7 @@
         <v>103057462</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>154</v>
       </c>
@@ -6251,7 +5764,7 @@
         <v>65578352</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>157</v>
       </c>
@@ -6277,7 +5790,7 @@
         <v>101251932</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>160</v>
       </c>
@@ -6303,7 +5816,7 @@
         <v>89155846</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>163</v>
       </c>
@@ -6329,7 +5842,7 @@
         <v>49223225</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>166</v>
       </c>
@@ -6355,7 +5868,7 @@
         <v>50988121</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
         <v>169</v>
       </c>
@@ -6381,7 +5894,7 @@
         <v>41440717</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>172</v>
       </c>
@@ -6407,7 +5920,7 @@
         <v>47784686</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
         <v>175</v>
       </c>
@@ -6433,7 +5946,7 @@
         <v>13638940</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
         <v>178</v>
       </c>
@@ -6459,7 +5972,7 @@
         <v>44652233</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
         <v>181</v>
       </c>
@@ -6485,7 +5998,7 @@
         <v>31668931</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>184</v>
       </c>
@@ -6511,7 +6024,7 @@
         <v>20859417</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
         <v>187</v>
       </c>
@@ -6537,7 +6050,7 @@
         <v>38738299</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>190</v>
       </c>
@@ -6563,7 +6076,7 @@
         <v>119605895</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
         <v>193</v>
       </c>
@@ -6589,7 +6102,7 @@
         <v>23005465</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>196</v>
       </c>
@@ -6616,10 +6129,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:H1064">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <autoFilter ref="B1:H1064" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
@@ -6629,38 +6140,37 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="16.4416666666667" style="15"/>
+    <col min="1" max="3" width="16.5" style="15"/>
     <col min="4" max="4" width="22" style="15"/>
-    <col min="5" max="5" width="13.6666666666667" style="15"/>
-    <col min="6" max="6" width="9.10833333333333" style="15"/>
-    <col min="7" max="7" width="25.1083333333333" style="15"/>
-    <col min="8" max="8" width="13.4416666666667" style="15"/>
-    <col min="9" max="9" width="16.3333333333333" style="15" customWidth="1"/>
-    <col min="10" max="10" width="15.4416666666667" style="15" customWidth="1"/>
-    <col min="11" max="11" width="18.5583333333333" style="15" customWidth="1"/>
-    <col min="12" max="12" width="23.3333333333333" style="15"/>
-    <col min="13" max="13" width="25.1083333333333" style="8"/>
-    <col min="14" max="14" width="19.8833333333333"/>
-    <col min="15" max="15" width="9.10833333333333" style="19"/>
-    <col min="16" max="16" width="10.4416666666667" style="19"/>
-    <col min="17" max="17" width="10.6666666666667" style="19"/>
-    <col min="18" max="19" width="9.10833333333333" style="15"/>
-    <col min="20" max="20" width="22.8833333333333" style="19"/>
-    <col min="21" max="1016" width="9.10833333333333" style="15"/>
-    <col min="1017" max="1025" width="9.10833333333333" style="8"/>
+    <col min="5" max="5" width="13.6640625" style="15"/>
+    <col min="6" max="6" width="9.1640625" style="15"/>
+    <col min="7" max="7" width="25.1640625" style="15"/>
+    <col min="8" max="8" width="13.5" style="15"/>
+    <col min="9" max="9" width="16.33203125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="15" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="15" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" style="15"/>
+    <col min="13" max="13" width="25.1640625" style="8"/>
+    <col min="14" max="14" width="19.83203125"/>
+    <col min="15" max="15" width="9.1640625" style="19"/>
+    <col min="16" max="16" width="10.5" style="19"/>
+    <col min="17" max="17" width="10.6640625" style="19"/>
+    <col min="18" max="19" width="9.1640625" style="15"/>
+    <col min="20" max="20" width="22.83203125" style="19"/>
+    <col min="21" max="1016" width="9.1640625" style="15"/>
+    <col min="1017" max="1025" width="9.1640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12" spans="1:1025">
+    <row r="1" spans="1:1025" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6719,7 +6229,7 @@
       <c r="AMJ1" s="37"/>
       <c r="AMK1" s="37"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>203</v>
       </c>
@@ -6755,7 +6265,7 @@
       <c r="R2" s="18"/>
       <c r="S2" s="18"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>207</v>
       </c>
@@ -6791,7 +6301,7 @@
       <c r="R3" s="18"/>
       <c r="S3" s="18"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>210</v>
       </c>
@@ -6827,7 +6337,7 @@
       <c r="R4" s="18"/>
       <c r="S4" s="18"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>214</v>
       </c>
@@ -6863,7 +6373,7 @@
       <c r="R5" s="18"/>
       <c r="S5" s="18"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>218</v>
       </c>
@@ -6899,7 +6409,7 @@
       <c r="R6" s="18"/>
       <c r="S6" s="18"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>221</v>
       </c>
@@ -6935,7 +6445,7 @@
       <c r="R7" s="18"/>
       <c r="S7" s="18"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>223</v>
       </c>
@@ -6971,7 +6481,7 @@
       <c r="R8" s="18"/>
       <c r="S8" s="18"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>226</v>
       </c>
@@ -7007,7 +6517,7 @@
       <c r="R9" s="18"/>
       <c r="S9" s="18"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>228</v>
       </c>
@@ -7043,7 +6553,7 @@
       <c r="R10" s="18"/>
       <c r="S10" s="18"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>230</v>
       </c>
@@ -7079,7 +6589,7 @@
       <c r="R11" s="18"/>
       <c r="S11" s="18"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>232</v>
       </c>
@@ -7115,7 +6625,7 @@
       <c r="R12" s="18"/>
       <c r="S12" s="18"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>234</v>
       </c>
@@ -7151,7 +6661,7 @@
       <c r="R13" s="18"/>
       <c r="S13" s="18"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>236</v>
       </c>
@@ -7187,7 +6697,7 @@
       <c r="R14" s="18"/>
       <c r="S14" s="18"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>238</v>
       </c>
@@ -7226,7 +6736,7 @@
       <c r="R15" s="18"/>
       <c r="S15" s="18"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>242</v>
       </c>
@@ -7262,7 +6772,7 @@
       <c r="R16" s="18"/>
       <c r="S16" s="18"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>244</v>
       </c>
@@ -7298,7 +6808,7 @@
       <c r="R17" s="18"/>
       <c r="S17" s="18"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>246</v>
       </c>
@@ -7334,7 +6844,7 @@
       <c r="R18" s="18"/>
       <c r="S18" s="18"/>
     </row>
-    <row r="19" ht="15" customHeight="1" spans="1:19">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>248</v>
       </c>
@@ -7373,7 +6883,7 @@
       <c r="R19" s="18"/>
       <c r="S19" s="18"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>251</v>
       </c>
@@ -7409,7 +6919,7 @@
       <c r="R20" s="18"/>
       <c r="S20" s="18"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>253</v>
       </c>
@@ -7445,7 +6955,7 @@
       <c r="R21" s="18"/>
       <c r="S21" s="18"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
         <v>255</v>
       </c>
@@ -7481,7 +6991,7 @@
       <c r="R22" s="18"/>
       <c r="S22" s="18"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>257</v>
       </c>
@@ -7517,7 +7027,7 @@
       <c r="R23" s="18"/>
       <c r="S23" s="18"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>259</v>
       </c>
@@ -7553,7 +7063,7 @@
       <c r="R24" s="18"/>
       <c r="S24" s="18"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>261</v>
       </c>
@@ -7589,7 +7099,7 @@
       <c r="R25" s="18"/>
       <c r="S25" s="18"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>263</v>
       </c>
@@ -7625,7 +7135,7 @@
       <c r="R26" s="18"/>
       <c r="S26" s="18"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>265</v>
       </c>
@@ -7661,7 +7171,7 @@
       <c r="R27" s="18"/>
       <c r="S27" s="18"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
         <v>267</v>
       </c>
@@ -7697,7 +7207,7 @@
       <c r="R28" s="18"/>
       <c r="S28" s="18"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>269</v>
       </c>
@@ -7733,7 +7243,7 @@
       <c r="R29" s="18"/>
       <c r="S29" s="18"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
         <v>271</v>
       </c>
@@ -7769,7 +7279,7 @@
       <c r="R30" s="18"/>
       <c r="S30" s="18"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
         <v>273</v>
       </c>
@@ -7805,7 +7315,7 @@
       <c r="R31" s="18"/>
       <c r="S31" s="18"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
         <v>275</v>
       </c>
@@ -7841,7 +7351,7 @@
       <c r="R32" s="18"/>
       <c r="S32" s="18"/>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>277</v>
       </c>
@@ -7877,7 +7387,7 @@
       <c r="R33" s="18"/>
       <c r="S33" s="18"/>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
         <v>279</v>
       </c>
@@ -7913,7 +7423,7 @@
       <c r="R34" s="18"/>
       <c r="S34" s="18"/>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>281</v>
       </c>
@@ -7949,7 +7459,7 @@
       <c r="R35" s="18"/>
       <c r="S35" s="18"/>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
         <v>283</v>
       </c>
@@ -7985,7 +7495,7 @@
       <c r="R36" s="18"/>
       <c r="S36" s="18"/>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>285</v>
       </c>
@@ -8022,10 +7532,8 @@
       <c r="S37" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L776">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <autoFilter ref="A1:L776" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
@@ -8035,34 +7543,33 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AMG5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.66666666666667" style="15" customWidth="1"/>
-    <col min="2" max="2" width="10.4416666666667" style="15" customWidth="1"/>
-    <col min="3" max="3" width="17.5583333333333" style="15" customWidth="1"/>
-    <col min="4" max="4" width="50.5583333333333" style="15"/>
-    <col min="5" max="5" width="18.4416666666667" style="15" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="15" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="15" customWidth="1"/>
+    <col min="4" max="4" width="50.5" style="15"/>
+    <col min="5" max="5" width="18.5" style="15" customWidth="1"/>
     <col min="6" max="6" width="10" style="15" customWidth="1"/>
-    <col min="7" max="7" width="13.6666666666667" style="15" customWidth="1"/>
-    <col min="8" max="8" width="22.8833333333333" style="27"/>
-    <col min="9" max="9" width="13.4416666666667" style="31"/>
-    <col min="10" max="10" width="19.8833333333333" style="19"/>
-    <col min="11" max="11" width="10.6666666666667" style="19"/>
-    <col min="12" max="13" width="9.10833333333333" style="15"/>
-    <col min="14" max="1021" width="9.10833333333333" style="31"/>
-    <col min="1022" max="1024" width="8.44166666666667"/>
-    <col min="1025" max="1030" width="8.66666666666667"/>
+    <col min="7" max="7" width="13.6640625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" style="27"/>
+    <col min="9" max="9" width="13.5" style="31"/>
+    <col min="10" max="10" width="19.83203125" style="19"/>
+    <col min="11" max="11" width="10.6640625" style="19"/>
+    <col min="12" max="13" width="9.1640625" style="15"/>
+    <col min="14" max="1021" width="9.1640625" style="31"/>
+    <col min="1022" max="1024" width="8.5"/>
+    <col min="1025" max="1030" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12" spans="1:11">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8095,7 +7602,7 @@
       </c>
       <c r="K1" s="32"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>291</v>
       </c>
@@ -8119,7 +7626,7 @@
       <c r="M2" s="18"/>
       <c r="N2" s="15"/>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="1:14">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>295</v>
       </c>
@@ -8143,7 +7650,7 @@
       <c r="M3" s="18"/>
       <c r="N3" s="15"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>298</v>
       </c>
@@ -8166,7 +7673,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>302</v>
       </c>
@@ -8190,10 +7697,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H849">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <autoFilter ref="A1:H849" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
@@ -8203,31 +7708,30 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AMG3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5583333333333" style="19"/>
-    <col min="2" max="2" width="21.1083333333333" style="19"/>
-    <col min="3" max="3" width="10.6666666666667" style="19"/>
-    <col min="4" max="4" width="22.8833333333333" style="27"/>
-    <col min="5" max="5" width="10.6666666666667"/>
-    <col min="6" max="6" width="13.4416666666667"/>
-    <col min="7" max="7" width="13.4416666666667" style="15"/>
-    <col min="8" max="8" width="13.4416666666667" style="28"/>
-    <col min="9" max="9" width="10.6666666666667" style="18"/>
-    <col min="10" max="10" width="19.8833333333333" style="15"/>
-    <col min="11" max="11" width="13.4416666666667" style="15"/>
-    <col min="12" max="1021" width="9.10833333333333" style="8"/>
+    <col min="1" max="1" width="19.5" style="19"/>
+    <col min="2" max="2" width="21.1640625" style="19"/>
+    <col min="3" max="3" width="10.6640625" style="19"/>
+    <col min="4" max="4" width="22.83203125" style="27"/>
+    <col min="5" max="5" width="10.6640625"/>
+    <col min="6" max="6" width="13.5"/>
+    <col min="7" max="7" width="13.5" style="15"/>
+    <col min="8" max="8" width="13.5" style="28"/>
+    <col min="9" max="9" width="10.6640625" style="18"/>
+    <col min="10" max="10" width="19.83203125" style="15"/>
+    <col min="11" max="11" width="13.5" style="15"/>
+    <col min="12" max="1021" width="9.1640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" s="23" customFormat="1" ht="12" spans="1:11">
+    <row r="1" spans="1:11" s="23" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -8260,7 +7764,7 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>305</v>
       </c>
@@ -8280,13 +7784,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="29">
-        <v>649.382685492726</v>
+        <v>649.38268549272595</v>
       </c>
       <c r="H2" s="27"/>
       <c r="J2" s="18"/>
       <c r="K2" s="30"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>307</v>
       </c>
@@ -8313,10 +7817,8 @@
       <c r="K3" s="30"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G915">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <autoFilter ref="A1:G915" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>

</xml_diff>

<commit_message>
adding activity to regulatory module
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chebaro/WC/wc_kb/tests/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD821F7-A720-6F49-8DE4-73F6F00E68C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20295" windowHeight="6780" tabRatio="993" firstSheet="1" activeTab="15"/>
+    <workbookView xWindow="780" yWindow="840" windowWidth="33400" windowHeight="20840" tabRatio="993" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -38,23 +44,23 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'Rate laws'!$A$1:$H$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Reactions!$A$1:$N$220</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Regulatory element'!$A$1:$O$776</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Regulatory module'!$A$1:$J$849</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Regulatory module'!$A$1:$K$849</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="7">Genes!$L$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">KB!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="10">Proteins!$A$1:$H$719</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="4">'Regulatory element'!$A$1:$O$776</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="5">'Regulatory module'!$A$1:$J$849</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">'Regulatory module'!$A$1:$K$849</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="7">Genes!$F$1:$I$1064</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">KB!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="4">'Regulatory element'!$A$1:$O$776</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="5">'Regulatory module'!$A$1:$J$849</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">'Regulatory module'!$A$1:$K$849</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="7">Genes!$L$1</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="0">KB!$A$1:$B$2</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="4">'Regulatory element'!$A$1:$O$776</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Regulatory module'!$A$1:$J$849</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Regulatory module'!$A$1:$K$849</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="1">Cell!$A$1:$B$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="7">Genes!$F$1:$I$1064</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="0">KB!$A$1:$B$2</definedName>
@@ -79,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="493">
   <si>
     <t>Id</t>
   </si>
@@ -1563,8 +1569,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2075,62 +2081,62 @@
   <cellStyles count="58">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="13"/>
-    <cellStyle name="Normal 10 2" xfId="28"/>
-    <cellStyle name="Normal 10 2 2" xfId="52"/>
-    <cellStyle name="Normal 10 3" xfId="41"/>
-    <cellStyle name="Normal 11" xfId="14"/>
-    <cellStyle name="Normal 11 2" xfId="29"/>
-    <cellStyle name="Normal 11 2 2" xfId="53"/>
-    <cellStyle name="Normal 11 3" xfId="42"/>
-    <cellStyle name="Normal 12" xfId="17"/>
-    <cellStyle name="Normal 12 2" xfId="32"/>
-    <cellStyle name="Normal 12 2 2" xfId="55"/>
-    <cellStyle name="Normal 12 3" xfId="44"/>
-    <cellStyle name="Normal 13" xfId="57"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 3 2" xfId="11"/>
-    <cellStyle name="Normal 3 2 2" xfId="26"/>
-    <cellStyle name="Normal 3 3" xfId="15"/>
-    <cellStyle name="Normal 3 3 2" xfId="30"/>
-    <cellStyle name="Normal 3 4" xfId="18"/>
-    <cellStyle name="Normal 3 4 2" xfId="33"/>
-    <cellStyle name="Normal 3 5" xfId="21"/>
-    <cellStyle name="Normal 4" xfId="5"/>
-    <cellStyle name="Normal 5" xfId="6"/>
-    <cellStyle name="Normal 6" xfId="7"/>
-    <cellStyle name="Normal 6 2" xfId="9"/>
-    <cellStyle name="Normal 6 2 2" xfId="24"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="49"/>
-    <cellStyle name="Normal 6 2 3" xfId="38"/>
-    <cellStyle name="Normal 6 3" xfId="12"/>
-    <cellStyle name="Normal 6 3 2" xfId="27"/>
-    <cellStyle name="Normal 6 3 2 2" xfId="51"/>
-    <cellStyle name="Normal 6 3 3" xfId="40"/>
-    <cellStyle name="Normal 6 4" xfId="16"/>
-    <cellStyle name="Normal 6 4 2" xfId="31"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="54"/>
-    <cellStyle name="Normal 6 4 3" xfId="43"/>
-    <cellStyle name="Normal 6 5" xfId="19"/>
-    <cellStyle name="Normal 6 5 2" xfId="34"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="56"/>
-    <cellStyle name="Normal 6 5 3" xfId="45"/>
-    <cellStyle name="Normal 6 6" xfId="22"/>
-    <cellStyle name="Normal 6 6 2" xfId="47"/>
-    <cellStyle name="Normal 6 7" xfId="36"/>
-    <cellStyle name="Normal 7" xfId="2"/>
-    <cellStyle name="Normal 7 2" xfId="20"/>
-    <cellStyle name="Normal 7 2 2" xfId="46"/>
-    <cellStyle name="Normal 7 3" xfId="35"/>
-    <cellStyle name="Normal 8" xfId="8"/>
-    <cellStyle name="Normal 8 2" xfId="23"/>
-    <cellStyle name="Normal 8 2 2" xfId="48"/>
-    <cellStyle name="Normal 8 3" xfId="37"/>
-    <cellStyle name="Normal 9" xfId="10"/>
-    <cellStyle name="Normal 9 2" xfId="25"/>
-    <cellStyle name="Normal 9 2 2" xfId="50"/>
-    <cellStyle name="Normal 9 3" xfId="39"/>
+    <cellStyle name="Normal 10" xfId="13" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 10 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 10 2 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 10 3" xfId="41" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 11" xfId="14" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 11 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 11 2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 11 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 12" xfId="17" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 12 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 12 2 2" xfId="55" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 12 3" xfId="44" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 13" xfId="57" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 3 3" xfId="15" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 3 3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 3 4" xfId="18" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 3 4 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 3 5" xfId="21" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 5" xfId="6" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 6" xfId="7" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 6 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 6 2 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 6 2 3" xfId="38" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 6 3" xfId="12" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 6 3 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 6 3 2 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normal 6 3 3" xfId="40" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normal 6 4" xfId="16" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normal 6 4 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 6 4 3" xfId="43" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 6 5" xfId="19" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 6 5 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 6 5 3" xfId="45" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6 6" xfId="22" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 6 2" xfId="47" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal 6 7" xfId="36" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Normal 7" xfId="2" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Normal 7 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 7 2 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal 7 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 8" xfId="8" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 8 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 8 2 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Normal 8 3" xfId="37" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 9" xfId="10" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Normal 9 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Normal 9 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Normal 9 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2206,6 +2212,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2253,7 +2262,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2286,9 +2295,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2321,6 +2347,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2496,7 +2539,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2506,14 +2549,14 @@
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="25"/>
-    <col min="2" max="2" width="43.42578125" style="4"/>
-    <col min="3" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="21.5" style="25"/>
+    <col min="2" max="2" width="43.5" style="4"/>
+    <col min="3" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -2521,7 +2564,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
@@ -2529,7 +2572,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
@@ -2537,7 +2580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
@@ -2545,25 +2588,25 @@
         <v>425</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>8</v>
       </c>
@@ -2571,7 +2614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>9</v>
       </c>
@@ -2580,33 +2623,33 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9"/>
+  <autoFilter ref="A1:B9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="1023" width="8.42578125"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="1023" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="18" customFormat="1" ht="12.75">
+    <row r="1" spans="1:7" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2629,7 +2672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>285</v>
       </c>
@@ -2643,7 +2686,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>288</v>
       </c>
@@ -2657,7 +2700,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>291</v>
       </c>
@@ -2671,7 +2714,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -2685,10 +2728,10 @@
         <v>296</v>
       </c>
     </row>
-    <row r="19" spans="5:5">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="17"/>
     </row>
-    <row r="20" spans="5:5">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E20" s="17"/>
     </row>
   </sheetData>
@@ -2698,28 +2741,28 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AME15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="5"/>
-    <col min="2" max="2" width="33.85546875" style="5"/>
-    <col min="3" max="3" width="16.42578125" style="12"/>
+    <col min="1" max="1" width="20.33203125" style="5"/>
+    <col min="2" max="2" width="33.83203125" style="5"/>
+    <col min="3" max="3" width="16.5" style="12"/>
     <col min="4" max="4" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="1019" width="9.140625" style="4"/>
-    <col min="1022" max="1024" width="8.7109375"/>
+    <col min="5" max="5" width="25.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="1019" width="9.1640625" style="4"/>
+    <col min="1022" max="1024" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="12.75">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2745,7 +2788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>223</v>
       </c>
@@ -2762,7 +2805,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>303</v>
       </c>
@@ -2779,7 +2822,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>281</v>
       </c>
@@ -2796,24 +2839,24 @@
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F719"/>
+  <autoFilter ref="A1:F719" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -2824,26 +2867,26 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AMD5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="7" customWidth="1"/>
     <col min="3" max="4" width="9" style="38"/>
-    <col min="5" max="5" width="30.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="8" customWidth="1"/>
-    <col min="7" max="9" width="15.7109375" style="4" customWidth="1"/>
-    <col min="10" max="1018" width="8.42578125" style="4"/>
-    <col min="1019" max="1021" width="8.42578125"/>
+    <col min="5" max="5" width="30.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="8" customWidth="1"/>
+    <col min="7" max="9" width="15.6640625" style="4" customWidth="1"/>
+    <col min="10" max="1018" width="8.5" style="4"/>
+    <col min="1019" max="1021" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>317</v>
       </c>
@@ -2872,7 +2915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>320</v>
       </c>
@@ -2892,7 +2935,7 @@
       </c>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>324</v>
       </c>
@@ -2910,7 +2953,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>326</v>
       </c>
@@ -2928,7 +2971,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>328</v>
       </c>
@@ -2947,14 +2990,14 @@
       <c r="I5" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G221"/>
+  <autoFilter ref="A1:G221" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AML16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2964,16 +3007,16 @@
       <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="32" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="6" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" style="6" customWidth="1"/>
-    <col min="5" max="8" width="20.7109375" style="6" customWidth="1"/>
-    <col min="9" max="1026" width="8.42578125" style="6"/>
+    <col min="1" max="1" width="20.6640625" style="32" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="15.6640625" style="6" customWidth="1"/>
+    <col min="5" max="8" width="20.6640625" style="6" customWidth="1"/>
+    <col min="9" max="1026" width="8.5" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="75" customFormat="1" ht="15.2" customHeight="1">
+    <row r="1" spans="1:8" s="75" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
@@ -2999,7 +3042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.2" customHeight="1">
+    <row r="2" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="77" t="s">
         <v>461</v>
       </c>
@@ -3019,7 +3062,7 @@
       <c r="G2" s="37"/>
       <c r="H2" s="37"/>
     </row>
-    <row r="3" spans="1:8" ht="15.2" customHeight="1">
+    <row r="3" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="76" t="s">
         <v>462</v>
       </c>
@@ -3039,7 +3082,7 @@
       </c>
       <c r="H3" s="37"/>
     </row>
-    <row r="4" spans="1:8" ht="15.2" customHeight="1">
+    <row r="4" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="76" t="s">
         <v>463</v>
       </c>
@@ -3057,7 +3100,7 @@
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
     </row>
-    <row r="5" spans="1:8" ht="15.2" customHeight="1">
+    <row r="5" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="76" t="s">
         <v>464</v>
       </c>
@@ -3075,7 +3118,7 @@
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
     </row>
-    <row r="6" spans="1:8" ht="15.2" customHeight="1">
+    <row r="6" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="76" t="s">
         <v>465</v>
       </c>
@@ -3093,7 +3136,7 @@
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:8" ht="15.2" customHeight="1">
+    <row r="7" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="76" t="s">
         <v>466</v>
       </c>
@@ -3111,7 +3154,7 @@
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
     </row>
-    <row r="8" spans="1:8" ht="15.2" customHeight="1">
+    <row r="8" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="76" t="s">
         <v>467</v>
       </c>
@@ -3129,7 +3172,7 @@
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
     </row>
-    <row r="9" spans="1:8" ht="15.2" customHeight="1">
+    <row r="9" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="76" t="s">
         <v>468</v>
       </c>
@@ -3147,7 +3190,7 @@
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
     </row>
-    <row r="10" spans="1:8" ht="15.2" customHeight="1">
+    <row r="10" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="76" t="s">
         <v>469</v>
       </c>
@@ -3165,7 +3208,7 @@
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
     </row>
-    <row r="11" spans="1:8" ht="15.2" customHeight="1">
+    <row r="11" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="76" t="s">
         <v>470</v>
       </c>
@@ -3183,7 +3226,7 @@
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
     </row>
-    <row r="12" spans="1:8" ht="15.2" customHeight="1">
+    <row r="12" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="76" t="s">
         <v>471</v>
       </c>
@@ -3201,7 +3244,7 @@
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="76" t="s">
         <v>472</v>
       </c>
@@ -3219,7 +3262,7 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="76" t="s">
         <v>473</v>
       </c>
@@ -3237,7 +3280,7 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="76" t="s">
         <v>474</v>
       </c>
@@ -3255,7 +3298,7 @@
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="76" t="s">
         <v>475</v>
       </c>
@@ -3280,23 +3323,23 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="36" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="36" customWidth="1"/>
-    <col min="7" max="10" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="36" customWidth="1"/>
+    <col min="7" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="42" customFormat="1">
+    <row r="1" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -3328,7 +3371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
         <v>432</v>
       </c>
@@ -3353,7 +3396,7 @@
       <c r="J2" s="28"/>
       <c r="K2" s="40"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="46" t="s">
         <v>433</v>
       </c>
@@ -3377,7 +3420,7 @@
       <c r="J3" s="28"/>
       <c r="K3" s="40"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
         <v>434</v>
       </c>
@@ -3401,7 +3444,7 @@
       <c r="J4" s="28"/>
       <c r="K4" s="40"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="46" t="s">
         <v>435</v>
       </c>
@@ -3425,7 +3468,7 @@
       <c r="J5" s="28"/>
       <c r="K5" s="40"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C6" s="48"/>
       <c r="D6" s="28"/>
       <c r="E6" s="48"/>
@@ -3435,7 +3478,7 @@
       <c r="J6" s="28"/>
       <c r="K6" s="40"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="28"/>
       <c r="B7" s="48"/>
       <c r="C7" s="48"/>
@@ -3448,7 +3491,7 @@
       <c r="J7" s="28"/>
       <c r="K7" s="40"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="28"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
@@ -3461,7 +3504,7 @@
       <c r="J8" s="28"/>
       <c r="K8" s="40"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="28"/>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
@@ -3479,21 +3522,21 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16"/>
-    <col min="3" max="3" width="15.42578125"/>
-    <col min="6" max="6" width="11.140625"/>
+    <col min="3" max="3" width="15.5"/>
+    <col min="6" max="6" width="11.1640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="12.75">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3516,7 +3559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" customHeight="1">
+    <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>353</v>
       </c>
@@ -3538,24 +3581,24 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" style="41" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="41" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" style="41" customWidth="1"/>
-    <col min="6" max="11" width="15.7109375" style="41" customWidth="1"/>
-    <col min="12" max="14" width="20.7109375" style="41" customWidth="1"/>
-    <col min="15" max="16384" width="18.7109375" style="41"/>
+    <col min="1" max="3" width="20.6640625" style="41" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="41" customWidth="1"/>
+    <col min="6" max="11" width="15.6640625" style="41" customWidth="1"/>
+    <col min="12" max="14" width="20.6640625" style="41" customWidth="1"/>
+    <col min="15" max="16384" width="18.6640625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="51" customFormat="1">
+    <row r="1" spans="1:14" s="51" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
@@ -3599,7 +3642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="50" t="s">
         <v>357</v>
       </c>
@@ -3625,7 +3668,7 @@
       <c r="M2" s="50"/>
       <c r="N2" s="50"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="50" t="s">
         <v>360</v>
       </c>
@@ -3651,7 +3694,7 @@
       <c r="M3" s="50"/>
       <c r="N3" s="50"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="50" t="s">
         <v>363</v>
       </c>
@@ -3677,7 +3720,7 @@
       <c r="M4" s="50"/>
       <c r="N4" s="50"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="50" t="s">
         <v>366</v>
       </c>
@@ -3703,7 +3746,7 @@
       <c r="M5" s="50"/>
       <c r="N5" s="50"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="50" t="s">
         <v>31</v>
       </c>
@@ -3729,7 +3772,7 @@
       <c r="M6" s="50"/>
       <c r="N6" s="50"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="50" t="s">
         <v>370</v>
       </c>
@@ -3755,7 +3798,7 @@
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="50" t="s">
         <v>373</v>
       </c>
@@ -3782,7 +3825,7 @@
       <c r="N8" s="50"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L220"/>
+  <autoFilter ref="A1:L220" xr:uid="{00000000-0009-0000-0000-00000F000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -3793,7 +3836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3803,17 +3846,17 @@
       <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" style="49" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="88" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="49" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="60" customWidth="1"/>
-    <col min="6" max="8" width="20.7109375" style="49" customWidth="1"/>
-    <col min="9" max="1024" width="8.7109375" style="3"/>
+    <col min="1" max="2" width="20.6640625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="88" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="49" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="60" customWidth="1"/>
+    <col min="6" max="8" width="20.6640625" style="49" customWidth="1"/>
+    <col min="9" max="1024" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="59" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:1024" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
         <v>317</v>
       </c>
@@ -4855,7 +4898,7 @@
       <c r="AMI1" s="58"/>
       <c r="AMJ1" s="58"/>
     </row>
-    <row r="2" spans="1:1024">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
         <v>375</v>
       </c>
@@ -4874,7 +4917,7 @@
       <c r="F2" s="41"/>
       <c r="H2" s="41"/>
     </row>
-    <row r="3" spans="1:1024">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
         <v>378</v>
       </c>
@@ -4895,7 +4938,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="4" spans="1:1024">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
         <v>381</v>
       </c>
@@ -4916,7 +4959,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="5" spans="1:1024">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
         <v>384</v>
       </c>
@@ -4937,7 +4980,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="6" spans="1:1024">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
         <v>386</v>
       </c>
@@ -4958,7 +5001,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="7" spans="1:1024">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
         <v>389</v>
       </c>
@@ -4976,7 +5019,7 @@
       </c>
       <c r="F7" s="41"/>
     </row>
-    <row r="8" spans="1:1024">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8" s="49" t="s">
         <v>391</v>
       </c>
@@ -4996,7 +5039,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="1:1024">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" s="49" t="s">
         <v>394</v>
       </c>
@@ -5017,29 +5060,29 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F9"/>
+  <autoFilter ref="A1:F9" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" style="41" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" style="34" customWidth="1"/>
-    <col min="6" max="9" width="20.7109375" style="41" customWidth="1"/>
-    <col min="10" max="1025" width="8.42578125"/>
+    <col min="1" max="3" width="20.6640625" style="41" customWidth="1"/>
+    <col min="4" max="5" width="15.6640625" style="34" customWidth="1"/>
+    <col min="6" max="9" width="20.6640625" style="41" customWidth="1"/>
+    <col min="10" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -5068,7 +5111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>397</v>
       </c>
@@ -5085,7 +5128,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>401</v>
       </c>
@@ -5102,7 +5145,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
         <v>404</v>
       </c>
@@ -5119,7 +5162,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
         <v>406</v>
       </c>
@@ -5136,7 +5179,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
         <v>377</v>
       </c>
@@ -5150,7 +5193,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>410</v>
       </c>
@@ -5164,7 +5207,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>413</v>
       </c>
@@ -5178,7 +5221,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>416</v>
       </c>
@@ -5192,7 +5235,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>419</v>
       </c>
@@ -5206,7 +5249,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -5219,20 +5262,20 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="20.7109375" customWidth="1"/>
-    <col min="1020" max="1024" width="8.7109375"/>
+    <col min="1" max="10" width="20.6640625" customWidth="1"/>
+    <col min="1020" max="1024" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="42" customFormat="1">
+    <row r="1" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
@@ -5275,7 +5318,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5285,14 +5328,14 @@
       <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="64" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="33" customWidth="1"/>
-    <col min="3" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="30.6640625" style="64" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="33" customWidth="1"/>
+    <col min="3" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="44" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:2" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -5300,7 +5343,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
         <v>1</v>
       </c>
@@ -5308,7 +5351,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="64" t="s">
         <v>10</v>
       </c>
@@ -5316,7 +5359,7 @@
         <v>9606</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="64" t="s">
         <v>9</v>
       </c>
@@ -5325,26 +5368,26 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B4"/>
+  <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="20.7109375" customWidth="1"/>
+    <col min="1" max="13" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="67" t="s">
         <v>317</v>
       </c>
@@ -5385,7 +5428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F15" s="42"/>
     </row>
   </sheetData>
@@ -5394,23 +5437,23 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" style="41" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="34" customWidth="1"/>
-    <col min="4" max="12" width="20.7109375" style="41" customWidth="1"/>
-    <col min="13" max="1025" width="8.42578125" style="41"/>
+    <col min="1" max="2" width="20.6640625" style="41" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="34" customWidth="1"/>
+    <col min="4" max="12" width="20.6640625" style="41" customWidth="1"/>
+    <col min="13" max="1025" width="8.5" style="41"/>
     <col min="1026" max="16384" width="9" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
@@ -5448,7 +5491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="41" t="s">
         <v>323</v>
       </c>
@@ -5456,7 +5499,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="41" t="s">
         <v>338</v>
       </c>
@@ -5464,7 +5507,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="41" t="s">
         <v>422</v>
       </c>
@@ -5479,22 +5522,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="26" customWidth="1"/>
-    <col min="2" max="6" width="20.7109375" style="4" customWidth="1"/>
-    <col min="8" max="1020" width="9.140625" style="4"/>
-    <col min="1024" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="20.6640625" style="26" customWidth="1"/>
+    <col min="2" max="6" width="20.6640625" style="4" customWidth="1"/>
+    <col min="8" max="1020" width="9.1640625" style="4"/>
+    <col min="1024" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="12.75">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5514,7 +5557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>14</v>
       </c>
@@ -5531,7 +5574,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
         <v>18</v>
       </c>
@@ -5543,7 +5586,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>20</v>
       </c>
@@ -5557,7 +5600,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>23</v>
       </c>
@@ -5576,24 +5619,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="26" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="9" customWidth="1"/>
-    <col min="3" max="6" width="20.7109375" style="4" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125"/>
+    <col min="1" max="1" width="20.6640625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="9" customWidth="1"/>
+    <col min="3" max="6" width="20.6640625" style="4" customWidth="1"/>
+    <col min="7" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5622,7 +5665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>49</v>
       </c>
@@ -5640,7 +5683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
         <v>50</v>
       </c>
@@ -5657,7 +5700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>51</v>
       </c>
@@ -5674,7 +5717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>52</v>
       </c>
@@ -5691,7 +5734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>53</v>
       </c>
@@ -5708,7 +5751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>54</v>
       </c>
@@ -5725,7 +5768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>55</v>
       </c>
@@ -5742,7 +5785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
         <v>56</v>
       </c>
@@ -5759,7 +5802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>57</v>
       </c>
@@ -5776,7 +5819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
         <v>58</v>
       </c>
@@ -5793,7 +5836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
         <v>59</v>
       </c>
@@ -5810,7 +5853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
         <v>60</v>
       </c>
@@ -5827,7 +5870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
         <v>61</v>
       </c>
@@ -5844,7 +5887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
         <v>62</v>
       </c>
@@ -5861,7 +5904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
         <v>63</v>
       </c>
@@ -5878,7 +5921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
         <v>64</v>
       </c>
@@ -5895,7 +5938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
         <v>65</v>
       </c>
@@ -5912,7 +5955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="26" t="s">
         <v>66</v>
       </c>
@@ -5929,7 +5972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>67</v>
       </c>
@@ -5946,7 +5989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
         <v>68</v>
       </c>
@@ -5963,7 +6006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
         <v>69</v>
       </c>
@@ -5980,7 +6023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
         <v>70</v>
       </c>
@@ -5997,7 +6040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
         <v>71</v>
       </c>
@@ -6014,7 +6057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="26" t="s">
         <v>72</v>
       </c>
@@ -6031,7 +6074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
         <v>489</v>
       </c>
@@ -6059,35 +6102,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="9"/>
-    <col min="2" max="2" width="15.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="39" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="9" customWidth="1"/>
-    <col min="5" max="6" width="15.7109375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="9" customWidth="1"/>
-    <col min="8" max="11" width="15.7109375" style="9" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="9" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" style="9" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" style="12"/>
-    <col min="17" max="17" width="10.7109375" style="12"/>
-    <col min="18" max="19" width="9.140625" style="9"/>
-    <col min="20" max="20" width="22.85546875" style="12"/>
-    <col min="21" max="1016" width="9.140625" style="9"/>
-    <col min="1017" max="1025" width="9.140625" style="4"/>
+    <col min="1" max="1" width="16.5" style="9"/>
+    <col min="2" max="2" width="15.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="9" customWidth="1"/>
+    <col min="5" max="6" width="15.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="9" customWidth="1"/>
+    <col min="8" max="11" width="15.6640625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="10.5" style="12"/>
+    <col min="17" max="17" width="10.6640625" style="12"/>
+    <col min="18" max="19" width="9.1640625" style="9"/>
+    <col min="20" max="20" width="22.83203125" style="12"/>
+    <col min="21" max="1016" width="9.1640625" style="9"/>
+    <col min="1017" max="1025" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="1" customFormat="1" ht="12.75">
+    <row r="1" spans="1:1025" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6148,7 +6191,7 @@
       <c r="AMJ1" s="25"/>
       <c r="AMK1" s="25"/>
     </row>
-    <row r="2" spans="1:1025">
+    <row r="2" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>191</v>
       </c>
@@ -6183,7 +6226,7 @@
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
     </row>
-    <row r="3" spans="1:1025">
+    <row r="3" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>194</v>
       </c>
@@ -6218,7 +6261,7 @@
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
     </row>
-    <row r="4" spans="1:1025">
+    <row r="4" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>196</v>
       </c>
@@ -6253,7 +6296,7 @@
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
     </row>
-    <row r="5" spans="1:1025">
+    <row r="5" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>199</v>
       </c>
@@ -6288,7 +6331,7 @@
       <c r="R5" s="11"/>
       <c r="S5" s="11"/>
     </row>
-    <row r="6" spans="1:1025">
+    <row r="6" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>202</v>
       </c>
@@ -6323,7 +6366,7 @@
       <c r="R6" s="11"/>
       <c r="S6" s="11"/>
     </row>
-    <row r="7" spans="1:1025">
+    <row r="7" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>205</v>
       </c>
@@ -6358,7 +6401,7 @@
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
     </row>
-    <row r="8" spans="1:1025">
+    <row r="8" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>207</v>
       </c>
@@ -6393,7 +6436,7 @@
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
     </row>
-    <row r="9" spans="1:1025">
+    <row r="9" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>209</v>
       </c>
@@ -6428,7 +6471,7 @@
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
     </row>
-    <row r="10" spans="1:1025">
+    <row r="10" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>211</v>
       </c>
@@ -6463,7 +6506,7 @@
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
     </row>
-    <row r="11" spans="1:1025">
+    <row r="11" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>213</v>
       </c>
@@ -6498,7 +6541,7 @@
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
     </row>
-    <row r="12" spans="1:1025">
+    <row r="12" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>215</v>
       </c>
@@ -6533,7 +6576,7 @@
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
     </row>
-    <row r="13" spans="1:1025">
+    <row r="13" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>217</v>
       </c>
@@ -6568,7 +6611,7 @@
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
     </row>
-    <row r="14" spans="1:1025">
+    <row r="14" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>219</v>
       </c>
@@ -6603,7 +6646,7 @@
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
     </row>
-    <row r="15" spans="1:1025">
+    <row r="15" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>221</v>
       </c>
@@ -6641,7 +6684,7 @@
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
     </row>
-    <row r="16" spans="1:1025">
+    <row r="16" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>224</v>
       </c>
@@ -6676,7 +6719,7 @@
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>226</v>
       </c>
@@ -6711,7 +6754,7 @@
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>228</v>
       </c>
@@ -6746,7 +6789,7 @@
       <c r="R18" s="11"/>
       <c r="S18" s="11"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>230</v>
       </c>
@@ -6784,7 +6827,7 @@
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>233</v>
       </c>
@@ -6819,7 +6862,7 @@
       <c r="R20" s="11"/>
       <c r="S20" s="11"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>235</v>
       </c>
@@ -6854,7 +6897,7 @@
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>237</v>
       </c>
@@ -6889,7 +6932,7 @@
       <c r="R22" s="11"/>
       <c r="S22" s="11"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>239</v>
       </c>
@@ -6924,7 +6967,7 @@
       <c r="R23" s="11"/>
       <c r="S23" s="11"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>241</v>
       </c>
@@ -6959,7 +7002,7 @@
       <c r="R24" s="11"/>
       <c r="S24" s="11"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>243</v>
       </c>
@@ -6994,7 +7037,7 @@
       <c r="R25" s="11"/>
       <c r="S25" s="11"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>245</v>
       </c>
@@ -7029,7 +7072,7 @@
       <c r="R26" s="11"/>
       <c r="S26" s="11"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>247</v>
       </c>
@@ -7064,7 +7107,7 @@
       <c r="R27" s="11"/>
       <c r="S27" s="11"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>249</v>
       </c>
@@ -7099,7 +7142,7 @@
       <c r="R28" s="11"/>
       <c r="S28" s="11"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>251</v>
       </c>
@@ -7134,7 +7177,7 @@
       <c r="R29" s="11"/>
       <c r="S29" s="11"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>253</v>
       </c>
@@ -7169,7 +7212,7 @@
       <c r="R30" s="11"/>
       <c r="S30" s="11"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>255</v>
       </c>
@@ -7204,7 +7247,7 @@
       <c r="R31" s="11"/>
       <c r="S31" s="11"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>257</v>
       </c>
@@ -7239,7 +7282,7 @@
       <c r="R32" s="11"/>
       <c r="S32" s="11"/>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>259</v>
       </c>
@@ -7274,7 +7317,7 @@
       <c r="R33" s="11"/>
       <c r="S33" s="11"/>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>261</v>
       </c>
@@ -7309,7 +7352,7 @@
       <c r="R34" s="11"/>
       <c r="S34" s="11"/>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>263</v>
       </c>
@@ -7344,7 +7387,7 @@
       <c r="R35" s="11"/>
       <c r="S35" s="11"/>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>265</v>
       </c>
@@ -7379,7 +7422,7 @@
       <c r="R36" s="11"/>
       <c r="S36" s="11"/>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>267</v>
       </c>
@@ -7415,7 +7458,7 @@
       <c r="S37" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M776"/>
+  <autoFilter ref="A1:M776" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -7426,32 +7469,33 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMF5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AMG5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" style="9"/>
-    <col min="5" max="5" width="18.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="10" style="9" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="9" customWidth="1"/>
-    <col min="8" max="8" width="9" style="12"/>
-    <col min="9" max="9" width="13.42578125" style="20"/>
-    <col min="10" max="10" width="9" style="19"/>
-    <col min="11" max="12" width="9.140625" style="9"/>
-    <col min="13" max="1020" width="9.140625" style="20"/>
-    <col min="1021" max="1023" width="8.42578125"/>
-    <col min="1024" max="1029" width="8.7109375"/>
+    <col min="1" max="1" width="9.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="50.5" style="9"/>
+    <col min="5" max="5" width="9" style="39"/>
+    <col min="6" max="6" width="18.5" style="9" customWidth="1"/>
+    <col min="7" max="7" width="10" style="9" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="9" style="12"/>
+    <col min="10" max="10" width="13.5" style="20"/>
+    <col min="11" max="11" width="9" style="19"/>
+    <col min="12" max="13" width="9.1640625" style="9"/>
+    <col min="14" max="1021" width="9.1640625" style="20"/>
+    <col min="1022" max="1024" width="8.5"/>
+    <col min="1025" max="1030" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="12.75">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7465,25 +7509,28 @@
         <v>270</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>273</v>
       </c>
@@ -7496,18 +7543,21 @@
       <c r="D2" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="K2" s="11"/>
       <c r="L2" s="11"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1">
+      <c r="M2" s="11"/>
+      <c r="N2" s="9"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>276</v>
       </c>
@@ -7520,18 +7570,21 @@
       <c r="D3" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="9"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="M3" s="11"/>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>279</v>
       </c>
@@ -7544,17 +7597,20 @@
       <c r="D4" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>487</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>282</v>
       </c>
@@ -7567,18 +7623,21 @@
       <c r="D5" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="G5" s="39" t="s">
         <v>487</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>376</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H849"/>
+  <autoFilter ref="A1:I849" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -7589,25 +7648,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -7636,7 +7695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>310</v>
       </c>
@@ -7654,7 +7713,7 @@
       </c>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>313</v>
       </c>
@@ -7672,7 +7731,7 @@
       </c>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>315</v>
       </c>
@@ -7696,29 +7755,29 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AMI37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="82"/>
+    <col min="1" max="1" width="17.5" style="82"/>
     <col min="2" max="3" width="9" style="82"/>
-    <col min="4" max="4" width="10.42578125" style="82" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="82" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="82"/>
-    <col min="7" max="9" width="13.42578125" style="82"/>
-    <col min="10" max="11" width="20.7109375" style="81" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="85" customWidth="1"/>
-    <col min="13" max="1023" width="32.42578125" style="81"/>
-    <col min="1024" max="1025" width="8.42578125" style="86"/>
+    <col min="4" max="4" width="10.5" style="82" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="82" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="82"/>
+    <col min="7" max="9" width="13.5" style="82"/>
+    <col min="10" max="11" width="20.6640625" style="81" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" style="85" customWidth="1"/>
+    <col min="13" max="1023" width="32.5" style="81"/>
+    <col min="1024" max="1025" width="8.5" style="86"/>
     <col min="1026" max="16384" width="9" style="86"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" s="79" customFormat="1" ht="12.75">
+    <row r="1" spans="1:1023" s="79" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
@@ -7762,7 +7821,7 @@
       <c r="AMH1" s="81"/>
       <c r="AMI1" s="81"/>
     </row>
-    <row r="2" spans="1:1023">
+    <row r="2" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A2" s="82" t="s">
         <v>79</v>
       </c>
@@ -7786,7 +7845,7 @@
         <v>20651511</v>
       </c>
     </row>
-    <row r="3" spans="1:1023">
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A3" s="82" t="s">
         <v>82</v>
       </c>
@@ -7810,7 +7869,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="4" spans="1:1023">
+    <row r="4" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A4" s="82" t="s">
         <v>85</v>
       </c>
@@ -7834,7 +7893,7 @@
         <v>69387254</v>
       </c>
     </row>
-    <row r="5" spans="1:1023">
+    <row r="5" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A5" s="82" t="s">
         <v>88</v>
       </c>
@@ -7858,7 +7917,7 @@
         <v>40574685</v>
       </c>
     </row>
-    <row r="6" spans="1:1023">
+    <row r="6" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A6" s="82" t="s">
         <v>91</v>
       </c>
@@ -7882,7 +7941,7 @@
         <v>112649530</v>
       </c>
     </row>
-    <row r="7" spans="1:1023">
+    <row r="7" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A7" s="82" t="s">
         <v>94</v>
       </c>
@@ -7906,7 +7965,7 @@
         <v>83605875</v>
       </c>
     </row>
-    <row r="8" spans="1:1023">
+    <row r="8" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A8" s="82" t="s">
         <v>97</v>
       </c>
@@ -7930,7 +7989,7 @@
         <v>127899195</v>
       </c>
     </row>
-    <row r="9" spans="1:1023">
+    <row r="9" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A9" s="82" t="s">
         <v>100</v>
       </c>
@@ -7954,7 +8013,7 @@
         <v>160421711</v>
       </c>
     </row>
-    <row r="10" spans="1:1023">
+    <row r="10" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A10" s="82" t="s">
         <v>103</v>
       </c>
@@ -7978,7 +8037,7 @@
         <v>152129619</v>
       </c>
     </row>
-    <row r="11" spans="1:1023">
+    <row r="11" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A11" s="82" t="s">
         <v>106</v>
       </c>
@@ -8002,7 +8061,7 @@
         <v>56051604</v>
       </c>
     </row>
-    <row r="12" spans="1:1023">
+    <row r="12" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A12" s="82" t="s">
         <v>109</v>
       </c>
@@ -8026,7 +8085,7 @@
         <v>18084998</v>
       </c>
     </row>
-    <row r="13" spans="1:1023">
+    <row r="13" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A13" s="82" t="s">
         <v>112</v>
       </c>
@@ -8050,7 +8109,7 @@
         <v>19967258</v>
       </c>
     </row>
-    <row r="14" spans="1:1023" ht="15" customHeight="1">
+    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="82" t="s">
         <v>115</v>
       </c>
@@ -8074,7 +8133,7 @@
         <v>136423761</v>
       </c>
     </row>
-    <row r="15" spans="1:1023">
+    <row r="15" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A15" s="82" t="s">
         <v>118</v>
       </c>
@@ -8098,7 +8157,7 @@
         <v>7787981</v>
       </c>
     </row>
-    <row r="16" spans="1:1023">
+    <row r="16" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A16" s="82" t="s">
         <v>121</v>
       </c>
@@ -8122,7 +8181,7 @@
         <v>133421307</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="82" t="s">
         <v>124</v>
       </c>
@@ -8146,7 +8205,7 @@
         <v>13732346</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="82" t="s">
         <v>127</v>
       </c>
@@ -8170,7 +8229,7 @@
         <v>114450279</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="82" t="s">
         <v>130</v>
       </c>
@@ -8194,7 +8253,7 @@
         <v>77065580</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="82" t="s">
         <v>133</v>
       </c>
@@ -8218,7 +8277,7 @@
         <v>113359493</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="82" t="s">
         <v>136</v>
       </c>
@@ -8242,7 +8301,7 @@
         <v>52476628</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="82" t="s">
         <v>139</v>
       </c>
@@ -8266,7 +8325,7 @@
         <v>103057462</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="82" t="s">
         <v>142</v>
       </c>
@@ -8290,7 +8349,7 @@
         <v>65578352</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="82" t="s">
         <v>145</v>
       </c>
@@ -8314,7 +8373,7 @@
         <v>101251932</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="82" t="s">
         <v>148</v>
       </c>
@@ -8338,7 +8397,7 @@
         <v>89155846</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="82" t="s">
         <v>151</v>
       </c>
@@ -8362,7 +8421,7 @@
         <v>49223225</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="82" t="s">
         <v>154</v>
       </c>
@@ -8386,7 +8445,7 @@
         <v>50988121</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="82" t="s">
         <v>157</v>
       </c>
@@ -8410,7 +8469,7 @@
         <v>41440717</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="82" t="s">
         <v>160</v>
       </c>
@@ -8434,7 +8493,7 @@
         <v>47784686</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="82" t="s">
         <v>163</v>
       </c>
@@ -8458,7 +8517,7 @@
         <v>13638940</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="82" t="s">
         <v>166</v>
       </c>
@@ -8482,7 +8541,7 @@
         <v>44652233</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="82" t="s">
         <v>169</v>
       </c>
@@ -8506,7 +8565,7 @@
         <v>31668931</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="82" t="s">
         <v>172</v>
       </c>
@@ -8530,7 +8589,7 @@
         <v>20859417</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="82" t="s">
         <v>175</v>
       </c>
@@ -8554,7 +8613,7 @@
         <v>38738299</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="82" t="s">
         <v>178</v>
       </c>
@@ -8578,7 +8637,7 @@
         <v>119605895</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="82" t="s">
         <v>181</v>
       </c>
@@ -8602,7 +8661,7 @@
         <v>23005465</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="82" t="s">
         <v>184</v>
       </c>
@@ -8627,7 +8686,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:I1064"/>
+  <autoFilter ref="F1:I1064" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -8638,23 +8697,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMG9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" style="28" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="48" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="28" customWidth="1"/>
-    <col min="8" max="1021" width="9.140625" style="4"/>
+    <col min="1" max="3" width="20.6640625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="48" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="28" customWidth="1"/>
+    <col min="8" max="1021" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="12.75">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8677,7 +8736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -8685,7 +8744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -8693,7 +8752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -8701,7 +8760,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -8709,7 +8768,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>34</v>
       </c>
@@ -8717,7 +8776,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
         <v>37</v>
       </c>
@@ -8725,7 +8784,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
         <v>40</v>
       </c>
@@ -8733,7 +8792,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Minor edit of names
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20295" windowHeight="6780" tabRatio="993" firstSheet="1" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="24975" windowHeight="10860" tabRatio="993" firstSheet="2" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -16,11 +16,11 @@
     <sheet name="Ptm site" sheetId="22" r:id="rId7"/>
     <sheet name="Genes" sheetId="6" r:id="rId8"/>
     <sheet name="Metabolites" sheetId="4" r:id="rId9"/>
-    <sheet name="Transcript species types" sheetId="10" r:id="rId10"/>
+    <sheet name="Transcripts" sheetId="10" r:id="rId10"/>
     <sheet name="Proteins" sheetId="12" r:id="rId11"/>
     <sheet name="Complexes" sheetId="13" r:id="rId12"/>
     <sheet name="Concentrations" sheetId="14" r:id="rId13"/>
-    <sheet name="SpeciesType properties" sheetId="23" r:id="rId14"/>
+    <sheet name="Species type properties" sheetId="23" r:id="rId14"/>
     <sheet name="Observables" sheetId="15" r:id="rId15"/>
     <sheet name="Reactions" sheetId="16" r:id="rId16"/>
     <sheet name="Rate laws" sheetId="17" r:id="rId17"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="494">
   <si>
     <t>Id</t>
   </si>
@@ -1558,6 +1558,9 @@
   </si>
   <si>
     <t>Enzymes</t>
+  </si>
+  <si>
+    <t>backward</t>
   </si>
 </sst>
 </file>
@@ -2591,7 +2594,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3283,7 +3286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -3541,7 +3544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -3800,7 +3803,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4966,7 +4969,7 @@
         <v>31</v>
       </c>
       <c r="C7" s="88" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="D7" s="49" t="s">
         <v>390</v>
@@ -5028,7 +5031,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8642,7 +8645,7 @@
   <dimension ref="A1:AMG9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
track complexes - fix subunit complications
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="494">
   <si>
     <t>Id</t>
   </si>
@@ -1557,16 +1557,10 @@
     <t>Species properties</t>
   </si>
   <si>
-    <t>[c]: (2) ENSP00000234111 ==&gt; Complex_1</t>
-  </si>
-  <si>
-    <t>[c]: (2) ENSP00000385333 ==&gt; Complex_2</t>
-  </si>
-  <si>
-    <t>[c]: ENSP00000234111 + ENSP00000385333 ==&gt; Complex_3</t>
-  </si>
-  <si>
-    <t>[c]: (2) ENSP00000390691 ==&gt; Complex_4</t>
+    <t>ENSP00000234111 + ENSP00000385333</t>
+  </si>
+  <si>
+    <t>(2) ENSP00000390691</t>
   </si>
 </sst>
 </file>
@@ -3091,7 +3085,7 @@
   <dimension ref="A1:AMF5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3154,7 +3148,7 @@
         <v>481</v>
       </c>
       <c r="F2" s="94" t="s">
-        <v>492</v>
+        <v>223</v>
       </c>
       <c r="J2" s="89" t="s">
         <v>322</v>
@@ -3174,7 +3168,7 @@
         <v>481</v>
       </c>
       <c r="F3" s="94" t="s">
-        <v>493</v>
+        <v>303</v>
       </c>
       <c r="J3" s="89"/>
       <c r="K3" s="89"/>
@@ -3192,7 +3186,7 @@
         <v>481</v>
       </c>
       <c r="F4" s="94" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="J4" s="89"/>
       <c r="K4" s="89"/>
@@ -3209,7 +3203,7 @@
         <v>481</v>
       </c>
       <c r="F5" s="94" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="J5" s="89"/>
       <c r="K5" s="89"/>

</xml_diff>

<commit_message>
change name regulatory_element to promoter
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chebaro/WC/wc_kb/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DCF944D-4FB8-FA41-86CA-4E7B4D94A6AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A93673E-6B98-D241-A8C4-342BC90756A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5440" yWindow="4920" windowWidth="24980" windowHeight="5320" tabRatio="993" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -666,9 +666,6 @@
     <t>Gene</t>
   </si>
   <si>
-    <t>Regulatory Element</t>
-  </si>
-  <si>
     <t>Binding factor</t>
   </si>
   <si>
@@ -1318,6 +1315,9 @@
   </si>
   <si>
     <t>(2) ENSP00000390691</t>
+  </si>
+  <si>
+    <t>Promoter</t>
   </si>
 </sst>
 </file>
@@ -2557,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2565,7 +2565,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2581,7 +2581,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2615,7 +2615,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2655,13 +2655,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
@@ -2678,50 +2678,50 @@
         <v>193</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>226</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2773,28 +2773,28 @@
   <sheetData>
     <row r="1" spans="1:11" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D1" s="57" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" s="57" t="s">
         <v>243</v>
       </c>
-      <c r="F1" s="57" t="s">
-        <v>244</v>
-      </c>
       <c r="G1" s="89" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H1" s="89" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I1" s="57" t="s">
         <v>13</v>
@@ -2808,73 +2808,73 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="85" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" s="85" t="s">
         <v>245</v>
-      </c>
-      <c r="B2" s="85" t="s">
-        <v>246</v>
       </c>
       <c r="C2" s="85"/>
       <c r="D2" s="85"/>
       <c r="E2" s="88" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F2" s="90" t="s">
         <v>193</v>
       </c>
       <c r="J2" s="85" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K2" s="85"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="85" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B3" s="85" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C3" s="85"/>
       <c r="D3" s="85"/>
       <c r="E3" s="88" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F3" s="90" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J3" s="85"/>
       <c r="K3" s="85"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="85" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4" s="85" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" s="85"/>
       <c r="D4" s="85"/>
       <c r="E4" s="88" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F4" s="90" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J4" s="85"/>
       <c r="K4" s="85"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="85" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D5" s="85"/>
       <c r="E5" s="88" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F5" s="90" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J5" s="85"/>
       <c r="K5" s="85"/>
@@ -2911,16 +2911,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="57" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="D1" s="57" t="s">
         <v>252</v>
       </c>
-      <c r="D1" s="57" t="s">
-        <v>253</v>
-      </c>
       <c r="E1" s="57" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F1" s="57" t="s">
         <v>13</v>
@@ -2934,56 +2934,56 @@
     </row>
     <row r="2" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="69" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C2" s="30">
         <v>1</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="68" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C3" s="30">
         <v>1</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
       <c r="G3" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C4" s="30">
         <v>1</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
@@ -2992,16 +2992,16 @@
     </row>
     <row r="5" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="68" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C5" s="30">
         <v>1</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
@@ -3010,16 +3010,16 @@
     </row>
     <row r="6" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="68" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" s="30">
         <v>0.25</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
@@ -3028,16 +3028,16 @@
     </row>
     <row r="7" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C7" s="30">
         <v>0.25</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -3046,16 +3046,16 @@
     </row>
     <row r="8" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="68" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C8" s="30">
         <v>0.25</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -3064,16 +3064,16 @@
     </row>
     <row r="9" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="68" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C9" s="30">
         <v>0.25</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
@@ -3082,16 +3082,16 @@
     </row>
     <row r="10" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="68" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C10" s="30">
         <v>0.5</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
@@ -3100,16 +3100,16 @@
     </row>
     <row r="11" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="68" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C11" s="30">
         <v>0.5</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
@@ -3118,16 +3118,16 @@
     </row>
     <row r="12" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="68" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B12" s="70" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C12" s="30">
         <v>0.5</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
@@ -3136,16 +3136,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="68" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C13" s="30">
         <v>0.1</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>
@@ -3154,16 +3154,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="68" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C14" s="30">
         <v>0.36</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
@@ -3172,16 +3172,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="68" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C15" s="30">
         <v>0.5</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
@@ -3190,16 +3190,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="68" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C16" s="30">
         <v>0.25</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
@@ -3234,22 +3234,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="47" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1" s="47" t="s">
         <v>357</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="D1" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="47" t="s">
         <v>358</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="F1" s="47" t="s">
         <v>252</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="G1" s="46" t="s">
         <v>359</v>
-      </c>
-      <c r="F1" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="G1" s="46" t="s">
-        <v>360</v>
       </c>
       <c r="H1" s="46" t="s">
         <v>13</v>
@@ -3263,22 +3263,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B2" s="45" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
@@ -3288,22 +3288,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
@@ -3312,22 +3312,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B4" s="40" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>39</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
@@ -3336,22 +3336,22 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B5" s="40" t="s">
         <v>42</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="32"/>
@@ -3434,10 +3434,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
@@ -3451,10 +3451,10 @@
     </row>
     <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>275</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -3496,31 +3496,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D1" s="55" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="54" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>406</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>380</v>
+      </c>
+      <c r="H1" s="55" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="54" t="s">
-        <v>407</v>
-      </c>
-      <c r="G1" s="54" t="s">
-        <v>381</v>
-      </c>
-      <c r="H1" s="55" t="s">
-        <v>277</v>
-      </c>
       <c r="I1" s="55" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J1" s="54" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K1" s="55" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L1" s="55" t="s">
         <v>13</v>
@@ -3534,15 +3534,15 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>278</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>279</v>
       </c>
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
       <c r="E2" s="42" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
@@ -3560,15 +3560,15 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="42" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>281</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>282</v>
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
       <c r="E3" s="42" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -3586,15 +3586,15 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="42" t="s">
+        <v>283</v>
+      </c>
+      <c r="B4" s="42" t="s">
         <v>284</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>285</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="42"/>
       <c r="E4" s="42" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
@@ -3612,15 +3612,15 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="B5" s="42" t="s">
         <v>287</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>288</v>
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="42"/>
       <c r="E5" s="42" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
@@ -3646,7 +3646,7 @@
       <c r="C6" s="42"/>
       <c r="D6" s="42"/>
       <c r="E6" s="42" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42"/>
@@ -3664,15 +3664,15 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="42" t="s">
+        <v>290</v>
+      </c>
+      <c r="B7" s="42" t="s">
         <v>291</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>292</v>
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="42"/>
       <c r="E7" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
@@ -3690,15 +3690,15 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="42" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
       <c r="E8" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F8" s="42"/>
       <c r="G8" s="42"/>
@@ -3748,19 +3748,19 @@
   <sheetData>
     <row r="1" spans="1:1024" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="48" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C1" s="79" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F1" s="49" t="s">
         <v>13</v>
@@ -4790,16 +4790,16 @@
     </row>
     <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>277</v>
+      </c>
+      <c r="C2" s="80" t="s">
         <v>296</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="C2" s="80" t="s">
+      <c r="D2" s="41" t="s">
         <v>297</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>298</v>
       </c>
       <c r="E2" s="27">
         <v>1</v>
@@ -4809,100 +4809,100 @@
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="80" t="s">
+        <v>296</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>299</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>281</v>
-      </c>
-      <c r="C3" s="80" t="s">
-        <v>297</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>300</v>
       </c>
       <c r="E3" s="27">
         <v>1</v>
       </c>
       <c r="F3" s="33"/>
       <c r="H3" s="41" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="80" t="s">
+        <v>296</v>
+      </c>
+      <c r="D4" s="41" t="s">
         <v>302</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>284</v>
-      </c>
-      <c r="C4" s="80" t="s">
-        <v>297</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>303</v>
       </c>
       <c r="E4" s="27">
         <v>1</v>
       </c>
       <c r="F4" s="33"/>
       <c r="H4" s="41" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C5" s="80" t="s">
+        <v>296</v>
+      </c>
+      <c r="D5" s="41" t="s">
         <v>297</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>298</v>
       </c>
       <c r="E5" s="27">
         <v>1</v>
       </c>
       <c r="F5" s="33"/>
       <c r="H5" s="41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B6" s="41" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="80" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E6" s="27">
         <v>1</v>
       </c>
       <c r="F6" s="33"/>
       <c r="H6" s="41" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B7" s="41" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="80" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E7" s="27">
         <v>1</v>
@@ -4911,42 +4911,42 @@
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="C8" s="80" t="s">
+        <v>296</v>
+      </c>
+      <c r="D8" s="41" t="s">
         <v>312</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>291</v>
-      </c>
-      <c r="C8" s="80" t="s">
-        <v>297</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>313</v>
       </c>
       <c r="E8" s="27">
         <v>1</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>293</v>
+      </c>
+      <c r="C9" s="80" t="s">
+        <v>296</v>
+      </c>
+      <c r="D9" s="41" t="s">
         <v>315</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>294</v>
-      </c>
-      <c r="C9" s="80" t="s">
-        <v>297</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>316</v>
       </c>
       <c r="E9" s="27">
         <v>1</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -4980,16 +4980,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D1" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>253</v>
-      </c>
       <c r="F1" s="37" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>13</v>
@@ -5003,140 +5003,140 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>318</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>319</v>
       </c>
       <c r="D2" s="27">
         <v>20.5</v>
       </c>
       <c r="E2" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="G2" s="33" t="s">
         <v>320</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>322</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>323</v>
       </c>
       <c r="D3" s="27">
         <v>1.35</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B4" s="33" t="s">
         <v>325</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>326</v>
       </c>
       <c r="D4" s="27">
         <v>0.46</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="B5" s="33" t="s">
         <v>327</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>328</v>
       </c>
       <c r="D5" s="27">
         <v>1.2</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D6" s="27">
         <v>2.1</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" t="s">
         <v>331</v>
-      </c>
-      <c r="B7" t="s">
-        <v>332</v>
       </c>
       <c r="D7" s="53">
         <v>3.0000000000000001E-12</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B8" t="s">
         <v>334</v>
-      </c>
-      <c r="B8" t="s">
-        <v>335</v>
       </c>
       <c r="D8" s="53">
         <v>10000000</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>336</v>
+      </c>
+      <c r="B9" t="s">
         <v>337</v>
-      </c>
-      <c r="B9" t="s">
-        <v>338</v>
       </c>
       <c r="D9" s="29">
         <v>0.7</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>339</v>
+      </c>
+      <c r="B10" t="s">
         <v>340</v>
-      </c>
-      <c r="B10" t="s">
-        <v>341</v>
       </c>
       <c r="D10" s="29">
         <v>71280</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5170,22 +5170,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="60" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C1" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>252</v>
+      </c>
+      <c r="G1" s="60" t="s">
         <v>365</v>
-      </c>
-      <c r="D1" s="60" t="s">
-        <v>358</v>
-      </c>
-      <c r="E1" s="60" t="s">
-        <v>252</v>
-      </c>
-      <c r="F1" s="60" t="s">
-        <v>253</v>
-      </c>
-      <c r="G1" s="60" t="s">
-        <v>366</v>
       </c>
       <c r="H1" s="61" t="s">
         <v>13</v>
@@ -5222,34 +5222,34 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B1" s="59" t="s">
+        <v>366</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>404</v>
+      </c>
+      <c r="D1" s="59" t="s">
         <v>367</v>
       </c>
-      <c r="C1" s="59" t="s">
-        <v>405</v>
-      </c>
-      <c r="D1" s="59" t="s">
+      <c r="E1" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="F1" s="59" t="s">
         <v>368</v>
       </c>
-      <c r="E1" s="59" t="s">
-        <v>251</v>
-      </c>
-      <c r="F1" s="59" t="s">
+      <c r="G1" s="59" t="s">
         <v>369</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="H1" s="59" t="s">
         <v>370</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="I1" s="59" t="s">
         <v>371</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="J1" s="59" t="s">
         <v>372</v>
-      </c>
-      <c r="J1" s="59" t="s">
-        <v>373</v>
       </c>
       <c r="K1" s="59" t="s">
         <v>13</v>
@@ -5292,7 +5292,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -5300,7 +5300,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5316,7 +5316,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -5354,25 +5354,25 @@
         <v>75</v>
       </c>
       <c r="D1" s="62" t="s">
+        <v>373</v>
+      </c>
+      <c r="E1" s="64" t="s">
         <v>374</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="F1" s="62" t="s">
         <v>375</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="G1" s="64" t="s">
         <v>376</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="H1" s="64" t="s">
         <v>377</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="I1" s="65" t="s">
         <v>378</v>
       </c>
-      <c r="I1" s="65" t="s">
+      <c r="J1" s="62" t="s">
         <v>379</v>
-      </c>
-      <c r="J1" s="62" t="s">
-        <v>380</v>
       </c>
       <c r="K1" s="63" t="s">
         <v>13</v>
@@ -5383,26 +5383,26 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -5966,10 +5966,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D26" s="6">
         <v>0</v>
@@ -5996,7 +5996,7 @@
   <dimension ref="A1:AMG5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6029,19 +6029,19 @@
         <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>195</v>
+        <v>412</v>
       </c>
       <c r="E1" s="81" t="s">
         <v>187</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>75</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>13</v>
@@ -6055,10 +6055,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>82</v>
@@ -6071,10 +6071,10 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -6082,10 +6082,10 @@
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>97</v>
@@ -6098,10 +6098,10 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -6109,10 +6109,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>204</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>205</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>97</v>
@@ -6124,21 +6124,21 @@
         <v>188</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>94</v>
@@ -6150,13 +6150,13 @@
         <v>188</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -6197,16 +6197,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
@@ -6220,16 +6220,16 @@
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="C2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>236</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="F2">
         <v>0.5</v>
@@ -6238,16 +6238,16 @@
     </row>
     <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>238</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>239</v>
       </c>
       <c r="F3">
         <v>0.8</v>
@@ -6256,16 +6256,16 @@
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>241</v>
       </c>
       <c r="F4">
         <v>0.02</v>
@@ -6308,13 +6308,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D1" s="71" t="s">
         <v>74</v>
       </c>
       <c r="E1" s="72" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F1" s="71" t="s">
         <v>73</v>
@@ -6359,7 +6359,7 @@
         <v>49</v>
       </c>
       <c r="G2" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H2" s="76">
         <v>20633455</v>
@@ -6383,7 +6383,7 @@
         <v>50</v>
       </c>
       <c r="G3" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H3" s="76">
         <v>10439968</v>
@@ -6407,7 +6407,7 @@
         <v>50</v>
       </c>
       <c r="G4" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H4" s="76">
         <v>69319769</v>
@@ -6431,7 +6431,7 @@
         <v>51</v>
       </c>
       <c r="G5" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H5" s="76">
         <v>40524878</v>
@@ -6455,7 +6455,7 @@
         <v>51</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H6" s="76">
         <v>112596794</v>
@@ -6479,7 +6479,7 @@
         <v>52</v>
       </c>
       <c r="G7" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H7" s="76">
         <v>83535914</v>
@@ -6503,7 +6503,7 @@
         <v>52</v>
       </c>
       <c r="G8" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H8" s="76">
         <v>127880861</v>
@@ -6527,7 +6527,7 @@
         <v>53</v>
       </c>
       <c r="G9" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H9" s="76">
         <v>160401641</v>
@@ -6551,7 +6551,7 @@
         <v>54</v>
       </c>
       <c r="G10" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H10" s="76">
         <v>151656691</v>
@@ -6575,7 +6575,7 @@
         <v>55</v>
       </c>
       <c r="G11" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H11" s="76">
         <v>56011051</v>
@@ -6599,7 +6599,7 @@
         <v>56</v>
       </c>
       <c r="G12" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H12" s="76">
         <v>18055992</v>
@@ -6623,7 +6623,7 @@
         <v>56</v>
       </c>
       <c r="G13" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H13" s="76">
         <v>19901717</v>
@@ -6647,7 +6647,7 @@
         <v>57</v>
       </c>
       <c r="G14" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H14" s="76">
         <v>136410570</v>
@@ -6671,7 +6671,7 @@
         <v>58</v>
       </c>
       <c r="G15" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H15" s="76">
         <v>7750962</v>
@@ -6695,7 +6695,7 @@
         <v>58</v>
       </c>
       <c r="G16" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H16" s="76">
         <v>133394094</v>
@@ -6719,7 +6719,7 @@
         <v>59</v>
       </c>
       <c r="G17" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H17" s="76">
         <v>13668670</v>
@@ -6743,7 +6743,7 @@
         <v>59</v>
       </c>
       <c r="G18" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H18" s="76">
         <v>114439386</v>
@@ -6767,7 +6767,7 @@
         <v>60</v>
       </c>
       <c r="G19" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H19" s="76">
         <v>77021247</v>
@@ -6791,7 +6791,7 @@
         <v>60</v>
       </c>
       <c r="G20" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H20" s="76">
         <v>113298759</v>
@@ -6815,7 +6815,7 @@
         <v>61</v>
       </c>
       <c r="G21" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H21" s="76">
         <v>52455429</v>
@@ -6839,7 +6839,7 @@
         <v>62</v>
       </c>
       <c r="G22" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H22" s="76">
         <v>102932379</v>
@@ -6863,7 +6863,7 @@
         <v>63</v>
       </c>
       <c r="G23" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H23" s="76">
         <v>65530418</v>
@@ -6887,7 +6887,7 @@
         <v>63</v>
       </c>
       <c r="G24" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H24" s="76">
         <v>101175723</v>
@@ -6911,7 +6911,7 @@
         <v>64</v>
       </c>
       <c r="G25" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H25" s="76">
         <v>89088375</v>
@@ -6935,7 +6935,7 @@
         <v>65</v>
       </c>
       <c r="G26" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H26" s="76">
         <v>49210227</v>
@@ -6959,7 +6959,7 @@
         <v>66</v>
       </c>
       <c r="G27" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H27" s="76">
         <v>50967991</v>
@@ -6983,7 +6983,7 @@
         <v>67</v>
       </c>
       <c r="G28" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H28" s="76">
         <v>41431318</v>
@@ -7007,7 +7007,7 @@
         <v>67</v>
       </c>
       <c r="G29" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H29" s="76">
         <v>47778572</v>
@@ -7031,7 +7031,7 @@
         <v>68</v>
       </c>
       <c r="G30" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H30" s="76">
         <v>13389392</v>
@@ -7055,7 +7055,7 @@
         <v>68</v>
       </c>
       <c r="G31" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H31" s="76">
         <v>44619522</v>
@@ -7079,7 +7079,7 @@
         <v>69</v>
       </c>
       <c r="G32" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H32" s="76">
         <v>31659622</v>
@@ -7103,7 +7103,7 @@
         <v>70</v>
       </c>
       <c r="G33" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H33" s="76">
         <v>20707691</v>
@@ -7127,7 +7127,7 @@
         <v>70</v>
       </c>
       <c r="G34" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H34" s="76">
         <v>38705723</v>
@@ -7151,7 +7151,7 @@
         <v>71</v>
       </c>
       <c r="G35" s="75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H35" s="76">
         <v>119588337</v>
@@ -7175,7 +7175,7 @@
         <v>72</v>
       </c>
       <c r="G36" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H36" s="76">
         <v>22973819</v>
@@ -7196,10 +7196,10 @@
         <v>186</v>
       </c>
       <c r="F37" s="74" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G37" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H37" s="76">
         <v>5904</v>
@@ -7244,16 +7244,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="84" t="s">
+        <v>408</v>
+      </c>
+      <c r="F1" s="84" t="s">
         <v>409</v>
-      </c>
-      <c r="F1" s="84" t="s">
-        <v>410</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
@@ -7370,7 +7370,7 @@
         <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
@@ -7384,58 +7384,58 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" t="s">
         <v>210</v>
-      </c>
-      <c r="B2" t="s">
-        <v>211</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" t="s">
         <v>213</v>
-      </c>
-      <c r="B3" t="s">
-        <v>214</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" t="s">
         <v>216</v>
-      </c>
-      <c r="B4" t="s">
-        <v>217</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" t="s">
         <v>219</v>
-      </c>
-      <c r="B5" t="s">
-        <v>220</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Reverting to enumeration classes for regulation type, direction and activity
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chebaro/WC/wc_kb/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A93673E-6B98-D241-A8C4-342BC90756A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0207D554-3BED-0240-8BF7-8A20471E2946}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="4920" windowWidth="24980" windowHeight="5320" tabRatio="993" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="4820" windowWidth="24980" windowHeight="5320" tabRatio="993" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="412">
   <si>
     <t>Id</t>
   </si>
@@ -1278,18 +1278,9 @@
     <t>book</t>
   </si>
   <si>
-    <t>reverse</t>
-  </si>
-  <si>
     <t>MacromolecularComplexation</t>
   </si>
   <si>
-    <t>Proximal</t>
-  </si>
-  <si>
-    <t>Distal</t>
-  </si>
-  <si>
     <t>chromosomeM</t>
   </si>
   <si>
@@ -1318,6 +1309,12 @@
   </si>
   <si>
     <t>Promoter</t>
+  </si>
+  <si>
+    <t>proximal</t>
+  </si>
+  <si>
+    <t>distal</t>
   </si>
 </sst>
 </file>
@@ -2791,10 +2788,10 @@
         <v>243</v>
       </c>
       <c r="G1" s="89" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H1" s="89" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="I1" s="57" t="s">
         <v>13</v>
@@ -2816,7 +2813,7 @@
       <c r="C2" s="85"/>
       <c r="D2" s="85"/>
       <c r="E2" s="88" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F2" s="90" t="s">
         <v>193</v>
@@ -2836,7 +2833,7 @@
       <c r="C3" s="85"/>
       <c r="D3" s="85"/>
       <c r="E3" s="88" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F3" s="90" t="s">
         <v>227</v>
@@ -2854,10 +2851,10 @@
       <c r="C4" s="85"/>
       <c r="D4" s="85"/>
       <c r="E4" s="88" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F4" s="90" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="J4" s="85"/>
       <c r="K4" s="85"/>
@@ -2871,10 +2868,10 @@
       </c>
       <c r="D5" s="85"/>
       <c r="E5" s="88" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F5" s="90" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="J5" s="85"/>
       <c r="K5" s="85"/>
@@ -3505,7 +3502,7 @@
         <v>275</v>
       </c>
       <c r="F1" s="54" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G1" s="54" t="s">
         <v>380</v>
@@ -3514,7 +3511,7 @@
         <v>276</v>
       </c>
       <c r="I1" s="55" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="J1" s="54" t="s">
         <v>363</v>
@@ -4899,7 +4896,7 @@
         <v>31</v>
       </c>
       <c r="C7" s="80" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D7" s="41" t="s">
         <v>310</v>
@@ -5228,7 +5225,7 @@
         <v>366</v>
       </c>
       <c r="C1" s="59" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D1" s="59" t="s">
         <v>367</v>
@@ -5966,10 +5963,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D26" s="6">
         <v>0</v>
@@ -6029,7 +6026,7 @@
         <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E1" s="81" t="s">
         <v>187</v>
@@ -6071,10 +6068,10 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>296</v>
+        <v>199</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -6098,10 +6095,10 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>399</v>
+        <v>202</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -6127,10 +6124,10 @@
         <v>205</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>399</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -6153,10 +6150,10 @@
         <v>205</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>296</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -7196,7 +7193,7 @@
         <v>186</v>
       </c>
       <c r="F37" s="74" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G37" s="75" t="s">
         <v>199</v>
@@ -7250,10 +7247,10 @@
         <v>75</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F1" s="84" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Change strand back to enumeration type; Fix error-prone cross-attributing in Concentration and SpeciesTypeProperty
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chebaro/WC/wc_kb/tests/fixtures/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0207D554-3BED-0240-8BF7-8A20471E2946}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="4820" windowWidth="24980" windowHeight="5320" tabRatio="993" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="4815" windowWidth="24975" windowHeight="5325" tabRatio="993" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -36,7 +30,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cell!$A$1:$B$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Complexes!$A$1:$K$221</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Complexes!$A$1:$I$221</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Genes!$F$1:$I$1064</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KB!$A$1:$B$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Proteins!$A$1:$H$719</definedName>
@@ -79,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="410">
   <si>
     <t>Id</t>
   </si>
@@ -1294,12 +1288,6 @@
   </si>
   <si>
     <t>backward</t>
-  </si>
-  <si>
-    <t>Concentration</t>
-  </si>
-  <si>
-    <t>Species properties</t>
   </si>
   <si>
     <t>ENSP00000234111 + ENSP00000385333</t>
@@ -1320,7 +1308,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1718,7 +1706,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1941,9 +1929,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1956,9 +1941,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1966,170 +1948,170 @@
   <cellStyles count="166">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="13" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 10 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 10 2 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 10 2 2 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 10 2 2 3" xfId="156" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 10 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 10 2 4" xfId="134" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 10 3" xfId="41" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 10 3 2" xfId="86" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 10 3 3" xfId="145" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 10 4" xfId="64" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 10 4 2" xfId="121" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Normal 10 5" xfId="108" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Normal 11" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Normal 11 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Normal 11 2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Normal 11 2 2 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Normal 11 2 2 3" xfId="157" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Normal 11 2 3" xfId="76" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Normal 11 2 4" xfId="135" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Normal 11 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Normal 11 3 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Normal 11 3 3" xfId="146" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Normal 11 4" xfId="65" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Normal 11 4 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Normal 11 5" xfId="109" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Normal 12" xfId="17" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Normal 12 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Normal 12 2 2" xfId="55" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Normal 12 2 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Normal 12 2 2 3" xfId="159" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Normal 12 2 3" xfId="78" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Normal 12 2 4" xfId="137" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Normal 12 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Normal 12 3 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Normal 12 3 3" xfId="148" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal 12 4" xfId="67" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Normal 12 4 2" xfId="125" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Normal 12 5" xfId="111" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Normal 13" xfId="57" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Normal 14" xfId="161" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Normal 15" xfId="164" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Normal 3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="119" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Normal 3 3" xfId="15" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="123" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Normal 3 4" xfId="18" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Normal 3 4 3" xfId="126" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Normal 3 5" xfId="21" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Normal 3 6" xfId="114" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Normal 3 7" xfId="162" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Normal 5" xfId="6" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Normal 6" xfId="7" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Normal 6 10" xfId="165" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Normal 6 11" xfId="103" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Normal 6 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Normal 6 2 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3" xfId="153" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Normal 6 2 2 3" xfId="72" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Normal 6 2 2 4" xfId="131" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Normal 6 2 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Normal 6 2 3 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Normal 6 2 3 3" xfId="142" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Normal 6 2 4" xfId="61" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Normal 6 2 4 2" xfId="117" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 6 2 5" xfId="105" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 6 3" xfId="12" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 6 3 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 6 3 2 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 6 3 2 2 3" xfId="155" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 6 3 2 3" xfId="74" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 6 3 2 4" xfId="133" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 6 3 3" xfId="40" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 6 3 3 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 6 3 3 3" xfId="144" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 6 3 4" xfId="63" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 6 3 4 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 6 3 5" xfId="107" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 6 4" xfId="16" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 6 4 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 6 4 2 2 2" xfId="99" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 6 4 2 2 3" xfId="158" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 6 4 2 3" xfId="77" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 6 4 2 4" xfId="136" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 6 4 3" xfId="43" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 6 4 3 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 6 4 3 3" xfId="147" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 6 4 4" xfId="66" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 6 4 4 2" xfId="124" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 6 4 5" xfId="110" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 6 5" xfId="19" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 6 5 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 6 5 2 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 6 5 2 2 3" xfId="160" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 6 5 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 6 5 2 4" xfId="138" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 6 5 3" xfId="45" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6 5 3 2" xfId="90" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 6 5 3 3" xfId="149" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 6 5 4" xfId="68" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 6 5 4 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Normal 6 5 5" xfId="112" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Normal 6 6" xfId="22" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Normal 6 6 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Normal 6 6 2 2" xfId="92" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Normal 6 6 2 3" xfId="151" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Normal 6 6 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Normal 6 6 4" xfId="129" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Normal 6 7" xfId="36" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Normal 6 7 2" xfId="81" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Normal 6 7 3" xfId="140" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Normal 6 8" xfId="59" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Normal 6 8 2" xfId="115" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Normal 6 9" xfId="163" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Normal 7" xfId="2" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Normal 7 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Normal 7 2 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Normal 7 2 2 2" xfId="91" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Normal 7 2 2 3" xfId="150" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Normal 7 2 3" xfId="69" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Normal 7 2 4" xfId="128" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Normal 7 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Normal 7 3 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Normal 7 3 3" xfId="139" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Normal 7 4" xfId="58" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Normal 7 4 2" xfId="113" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Normal 7 5" xfId="102" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Normal 8" xfId="8" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Normal 8 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Normal 8 2 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Normal 8 2 2 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Normal 8 2 2 3" xfId="152" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Normal 8 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Normal 8 2 4" xfId="130" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Normal 8 3" xfId="37" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Normal 8 3 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Normal 8 3 3" xfId="141" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Normal 8 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Normal 8 4 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Normal 8 5" xfId="104" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Normal 9" xfId="10" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="Normal 9 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="Normal 9 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="Normal 9 2 2 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="Normal 9 2 2 3" xfId="154" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="Normal 9 2 3" xfId="73" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="Normal 9 2 4" xfId="132" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="Normal 9 3" xfId="39" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="Normal 9 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="Normal 9 3 3" xfId="143" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="Normal 9 4" xfId="62" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="Normal 9 4 2" xfId="118" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="Normal 9 5" xfId="106" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Normal 10" xfId="13"/>
+    <cellStyle name="Normal 10 2" xfId="28"/>
+    <cellStyle name="Normal 10 2 2" xfId="52"/>
+    <cellStyle name="Normal 10 2 2 2" xfId="97"/>
+    <cellStyle name="Normal 10 2 2 3" xfId="156"/>
+    <cellStyle name="Normal 10 2 3" xfId="75"/>
+    <cellStyle name="Normal 10 2 4" xfId="134"/>
+    <cellStyle name="Normal 10 3" xfId="41"/>
+    <cellStyle name="Normal 10 3 2" xfId="86"/>
+    <cellStyle name="Normal 10 3 3" xfId="145"/>
+    <cellStyle name="Normal 10 4" xfId="64"/>
+    <cellStyle name="Normal 10 4 2" xfId="121"/>
+    <cellStyle name="Normal 10 5" xfId="108"/>
+    <cellStyle name="Normal 11" xfId="14"/>
+    <cellStyle name="Normal 11 2" xfId="29"/>
+    <cellStyle name="Normal 11 2 2" xfId="53"/>
+    <cellStyle name="Normal 11 2 2 2" xfId="98"/>
+    <cellStyle name="Normal 11 2 2 3" xfId="157"/>
+    <cellStyle name="Normal 11 2 3" xfId="76"/>
+    <cellStyle name="Normal 11 2 4" xfId="135"/>
+    <cellStyle name="Normal 11 3" xfId="42"/>
+    <cellStyle name="Normal 11 3 2" xfId="87"/>
+    <cellStyle name="Normal 11 3 3" xfId="146"/>
+    <cellStyle name="Normal 11 4" xfId="65"/>
+    <cellStyle name="Normal 11 4 2" xfId="122"/>
+    <cellStyle name="Normal 11 5" xfId="109"/>
+    <cellStyle name="Normal 12" xfId="17"/>
+    <cellStyle name="Normal 12 2" xfId="32"/>
+    <cellStyle name="Normal 12 2 2" xfId="55"/>
+    <cellStyle name="Normal 12 2 2 2" xfId="100"/>
+    <cellStyle name="Normal 12 2 2 3" xfId="159"/>
+    <cellStyle name="Normal 12 2 3" xfId="78"/>
+    <cellStyle name="Normal 12 2 4" xfId="137"/>
+    <cellStyle name="Normal 12 3" xfId="44"/>
+    <cellStyle name="Normal 12 3 2" xfId="89"/>
+    <cellStyle name="Normal 12 3 3" xfId="148"/>
+    <cellStyle name="Normal 12 4" xfId="67"/>
+    <cellStyle name="Normal 12 4 2" xfId="125"/>
+    <cellStyle name="Normal 12 5" xfId="111"/>
+    <cellStyle name="Normal 13" xfId="57"/>
+    <cellStyle name="Normal 14" xfId="161"/>
+    <cellStyle name="Normal 15" xfId="164"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 3" xfId="4"/>
+    <cellStyle name="Normal 3 2" xfId="11"/>
+    <cellStyle name="Normal 3 2 2" xfId="26"/>
+    <cellStyle name="Normal 3 2 3" xfId="119"/>
+    <cellStyle name="Normal 3 3" xfId="15"/>
+    <cellStyle name="Normal 3 3 2" xfId="30"/>
+    <cellStyle name="Normal 3 3 3" xfId="123"/>
+    <cellStyle name="Normal 3 4" xfId="18"/>
+    <cellStyle name="Normal 3 4 2" xfId="33"/>
+    <cellStyle name="Normal 3 4 3" xfId="126"/>
+    <cellStyle name="Normal 3 5" xfId="21"/>
+    <cellStyle name="Normal 3 6" xfId="114"/>
+    <cellStyle name="Normal 3 7" xfId="162"/>
+    <cellStyle name="Normal 4" xfId="5"/>
+    <cellStyle name="Normal 5" xfId="6"/>
+    <cellStyle name="Normal 6" xfId="7"/>
+    <cellStyle name="Normal 6 10" xfId="165"/>
+    <cellStyle name="Normal 6 11" xfId="103"/>
+    <cellStyle name="Normal 6 2" xfId="9"/>
+    <cellStyle name="Normal 6 2 2" xfId="24"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="49"/>
+    <cellStyle name="Normal 6 2 2 2 2" xfId="94"/>
+    <cellStyle name="Normal 6 2 2 2 3" xfId="153"/>
+    <cellStyle name="Normal 6 2 2 3" xfId="72"/>
+    <cellStyle name="Normal 6 2 2 4" xfId="131"/>
+    <cellStyle name="Normal 6 2 3" xfId="38"/>
+    <cellStyle name="Normal 6 2 3 2" xfId="83"/>
+    <cellStyle name="Normal 6 2 3 3" xfId="142"/>
+    <cellStyle name="Normal 6 2 4" xfId="61"/>
+    <cellStyle name="Normal 6 2 4 2" xfId="117"/>
+    <cellStyle name="Normal 6 2 5" xfId="105"/>
+    <cellStyle name="Normal 6 3" xfId="12"/>
+    <cellStyle name="Normal 6 3 2" xfId="27"/>
+    <cellStyle name="Normal 6 3 2 2" xfId="51"/>
+    <cellStyle name="Normal 6 3 2 2 2" xfId="96"/>
+    <cellStyle name="Normal 6 3 2 2 3" xfId="155"/>
+    <cellStyle name="Normal 6 3 2 3" xfId="74"/>
+    <cellStyle name="Normal 6 3 2 4" xfId="133"/>
+    <cellStyle name="Normal 6 3 3" xfId="40"/>
+    <cellStyle name="Normal 6 3 3 2" xfId="85"/>
+    <cellStyle name="Normal 6 3 3 3" xfId="144"/>
+    <cellStyle name="Normal 6 3 4" xfId="63"/>
+    <cellStyle name="Normal 6 3 4 2" xfId="120"/>
+    <cellStyle name="Normal 6 3 5" xfId="107"/>
+    <cellStyle name="Normal 6 4" xfId="16"/>
+    <cellStyle name="Normal 6 4 2" xfId="31"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="54"/>
+    <cellStyle name="Normal 6 4 2 2 2" xfId="99"/>
+    <cellStyle name="Normal 6 4 2 2 3" xfId="158"/>
+    <cellStyle name="Normal 6 4 2 3" xfId="77"/>
+    <cellStyle name="Normal 6 4 2 4" xfId="136"/>
+    <cellStyle name="Normal 6 4 3" xfId="43"/>
+    <cellStyle name="Normal 6 4 3 2" xfId="88"/>
+    <cellStyle name="Normal 6 4 3 3" xfId="147"/>
+    <cellStyle name="Normal 6 4 4" xfId="66"/>
+    <cellStyle name="Normal 6 4 4 2" xfId="124"/>
+    <cellStyle name="Normal 6 4 5" xfId="110"/>
+    <cellStyle name="Normal 6 5" xfId="19"/>
+    <cellStyle name="Normal 6 5 2" xfId="34"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="56"/>
+    <cellStyle name="Normal 6 5 2 2 2" xfId="101"/>
+    <cellStyle name="Normal 6 5 2 2 3" xfId="160"/>
+    <cellStyle name="Normal 6 5 2 3" xfId="79"/>
+    <cellStyle name="Normal 6 5 2 4" xfId="138"/>
+    <cellStyle name="Normal 6 5 3" xfId="45"/>
+    <cellStyle name="Normal 6 5 3 2" xfId="90"/>
+    <cellStyle name="Normal 6 5 3 3" xfId="149"/>
+    <cellStyle name="Normal 6 5 4" xfId="68"/>
+    <cellStyle name="Normal 6 5 4 2" xfId="127"/>
+    <cellStyle name="Normal 6 5 5" xfId="112"/>
+    <cellStyle name="Normal 6 6" xfId="22"/>
+    <cellStyle name="Normal 6 6 2" xfId="47"/>
+    <cellStyle name="Normal 6 6 2 2" xfId="92"/>
+    <cellStyle name="Normal 6 6 2 3" xfId="151"/>
+    <cellStyle name="Normal 6 6 3" xfId="70"/>
+    <cellStyle name="Normal 6 6 4" xfId="129"/>
+    <cellStyle name="Normal 6 7" xfId="36"/>
+    <cellStyle name="Normal 6 7 2" xfId="81"/>
+    <cellStyle name="Normal 6 7 3" xfId="140"/>
+    <cellStyle name="Normal 6 8" xfId="59"/>
+    <cellStyle name="Normal 6 8 2" xfId="115"/>
+    <cellStyle name="Normal 6 9" xfId="163"/>
+    <cellStyle name="Normal 7" xfId="2"/>
+    <cellStyle name="Normal 7 2" xfId="20"/>
+    <cellStyle name="Normal 7 2 2" xfId="46"/>
+    <cellStyle name="Normal 7 2 2 2" xfId="91"/>
+    <cellStyle name="Normal 7 2 2 3" xfId="150"/>
+    <cellStyle name="Normal 7 2 3" xfId="69"/>
+    <cellStyle name="Normal 7 2 4" xfId="128"/>
+    <cellStyle name="Normal 7 3" xfId="35"/>
+    <cellStyle name="Normal 7 3 2" xfId="80"/>
+    <cellStyle name="Normal 7 3 3" xfId="139"/>
+    <cellStyle name="Normal 7 4" xfId="58"/>
+    <cellStyle name="Normal 7 4 2" xfId="113"/>
+    <cellStyle name="Normal 7 5" xfId="102"/>
+    <cellStyle name="Normal 8" xfId="8"/>
+    <cellStyle name="Normal 8 2" xfId="23"/>
+    <cellStyle name="Normal 8 2 2" xfId="48"/>
+    <cellStyle name="Normal 8 2 2 2" xfId="93"/>
+    <cellStyle name="Normal 8 2 2 3" xfId="152"/>
+    <cellStyle name="Normal 8 2 3" xfId="71"/>
+    <cellStyle name="Normal 8 2 4" xfId="130"/>
+    <cellStyle name="Normal 8 3" xfId="37"/>
+    <cellStyle name="Normal 8 3 2" xfId="82"/>
+    <cellStyle name="Normal 8 3 3" xfId="141"/>
+    <cellStyle name="Normal 8 4" xfId="60"/>
+    <cellStyle name="Normal 8 4 2" xfId="116"/>
+    <cellStyle name="Normal 8 5" xfId="104"/>
+    <cellStyle name="Normal 9" xfId="10"/>
+    <cellStyle name="Normal 9 2" xfId="25"/>
+    <cellStyle name="Normal 9 2 2" xfId="50"/>
+    <cellStyle name="Normal 9 2 2 2" xfId="95"/>
+    <cellStyle name="Normal 9 2 2 3" xfId="154"/>
+    <cellStyle name="Normal 9 2 3" xfId="73"/>
+    <cellStyle name="Normal 9 2 4" xfId="132"/>
+    <cellStyle name="Normal 9 3" xfId="39"/>
+    <cellStyle name="Normal 9 3 2" xfId="84"/>
+    <cellStyle name="Normal 9 3 3" xfId="143"/>
+    <cellStyle name="Normal 9 4" xfId="62"/>
+    <cellStyle name="Normal 9 4 2" xfId="118"/>
+    <cellStyle name="Normal 9 5" xfId="106"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2255,7 +2237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2288,26 +2270,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2340,23 +2305,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2532,7 +2480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2542,14 +2490,14 @@
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="19"/>
-    <col min="2" max="2" width="43.5" style="3"/>
-    <col min="3" max="1025" width="8.5"/>
+    <col min="1" max="1" width="21.42578125" style="19"/>
+    <col min="2" max="2" width="43.42578125" style="3"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -2557,7 +2505,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
@@ -2565,7 +2513,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>2</v>
       </c>
@@ -2573,7 +2521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
@@ -2581,25 +2529,25 @@
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
@@ -2607,7 +2555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>9</v>
       </c>
@@ -2616,35 +2564,35 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:B9"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AME15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="4"/>
-    <col min="2" max="2" width="33.83203125" style="4"/>
-    <col min="3" max="3" width="16.5" style="9"/>
+    <col min="1" max="1" width="20.28515625" style="4"/>
+    <col min="2" max="2" width="33.85546875" style="4"/>
+    <col min="3" max="3" width="16.42578125" style="9"/>
     <col min="4" max="4" width="17" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="1019" width="9.1640625" style="3"/>
-    <col min="1022" max="1024" width="8.6640625"/>
+    <col min="5" max="5" width="25.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="1019" width="9.140625" style="3"/>
+    <col min="1022" max="1024" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2670,7 +2618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>193</v>
       </c>
@@ -2687,7 +2635,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>227</v>
       </c>
@@ -2704,7 +2652,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>205</v>
       </c>
@@ -2721,24 +2669,24 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F719" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
+  <autoFilter ref="A1:F719"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -2749,26 +2697,26 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:AMF5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMD5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" style="87" customWidth="1"/>
-    <col min="3" max="4" width="9" style="87"/>
-    <col min="5" max="5" width="30.6640625" style="87" customWidth="1"/>
-    <col min="6" max="8" width="30.6640625" style="68" customWidth="1"/>
-    <col min="9" max="11" width="15.6640625" style="87" customWidth="1"/>
-    <col min="12" max="1020" width="8.5" style="87"/>
-    <col min="1021" max="1023" width="8.5" style="86"/>
-    <col min="1024" max="16384" width="9" style="86"/>
+    <col min="1" max="2" width="20.7109375" style="86" customWidth="1"/>
+    <col min="3" max="4" width="9" style="86"/>
+    <col min="5" max="5" width="30.7109375" style="86" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="68" customWidth="1"/>
+    <col min="7" max="9" width="15.7109375" style="86" customWidth="1"/>
+    <col min="10" max="1018" width="8.42578125" style="86"/>
+    <col min="1019" max="1021" width="8.42578125" style="85"/>
+    <col min="1022" max="16384" width="9" style="85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
         <v>241</v>
       </c>
@@ -2787,104 +2735,98 @@
       <c r="F1" s="57" t="s">
         <v>243</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="84" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="87" t="s">
+        <v>399</v>
+      </c>
+      <c r="F2" s="88" t="s">
+        <v>193</v>
+      </c>
+      <c r="H2" s="84" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" s="84"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="84" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="84" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="87" t="s">
+        <v>399</v>
+      </c>
+      <c r="F3" s="88" t="s">
+        <v>227</v>
+      </c>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="84" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" s="84" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="87" t="s">
+        <v>399</v>
+      </c>
+      <c r="F4" s="88" t="s">
+        <v>405</v>
+      </c>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="84" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="84" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="84"/>
+      <c r="E5" s="87" t="s">
+        <v>399</v>
+      </c>
+      <c r="F5" s="88" t="s">
         <v>406</v>
       </c>
-      <c r="H1" s="89" t="s">
-        <v>405</v>
-      </c>
-      <c r="I1" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
-        <v>244</v>
-      </c>
-      <c r="B2" s="85" t="s">
-        <v>245</v>
-      </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="88" t="s">
-        <v>399</v>
-      </c>
-      <c r="F2" s="90" t="s">
-        <v>193</v>
-      </c>
-      <c r="J2" s="85" t="s">
-        <v>246</v>
-      </c>
-      <c r="K2" s="85"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="85" t="s">
-        <v>247</v>
-      </c>
-      <c r="B3" s="85" t="s">
-        <v>245</v>
-      </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="88" t="s">
-        <v>399</v>
-      </c>
-      <c r="F3" s="90" t="s">
-        <v>227</v>
-      </c>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="85" t="s">
-        <v>248</v>
-      </c>
-      <c r="B4" s="85" t="s">
-        <v>245</v>
-      </c>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="88" t="s">
-        <v>399</v>
-      </c>
-      <c r="F4" s="90" t="s">
-        <v>407</v>
-      </c>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="B5" s="85" t="s">
-        <v>245</v>
-      </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="88" t="s">
-        <v>399</v>
-      </c>
-      <c r="F5" s="90" t="s">
-        <v>408</v>
-      </c>
-      <c r="J5" s="85"/>
-      <c r="K5" s="85"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I221" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>
+  <autoFilter ref="A1:G221"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2894,16 +2836,16 @@
       <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="5" customWidth="1"/>
-    <col min="3" max="4" width="15.6640625" style="5" customWidth="1"/>
-    <col min="5" max="8" width="20.6640625" style="5" customWidth="1"/>
-    <col min="9" max="1026" width="8.5" style="5"/>
+    <col min="1" max="1" width="20.7109375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="5" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" style="5" customWidth="1"/>
+    <col min="5" max="8" width="20.7109375" style="5" customWidth="1"/>
+    <col min="9" max="1026" width="8.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="67" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="67" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
@@ -2929,7 +2871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
         <v>381</v>
       </c>
@@ -2949,7 +2891,7 @@
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
     </row>
-    <row r="3" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
         <v>382</v>
       </c>
@@ -2969,7 +2911,7 @@
       </c>
       <c r="H3" s="30"/>
     </row>
-    <row r="4" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="68" t="s">
         <v>383</v>
       </c>
@@ -2987,7 +2929,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
     </row>
-    <row r="5" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>384</v>
       </c>
@@ -3005,7 +2947,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
     </row>
-    <row r="6" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="68" t="s">
         <v>385</v>
       </c>
@@ -3023,7 +2965,7 @@
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
     </row>
-    <row r="7" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="68" t="s">
         <v>386</v>
       </c>
@@ -3041,7 +2983,7 @@
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
     </row>
-    <row r="8" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="68" t="s">
         <v>387</v>
       </c>
@@ -3059,7 +3001,7 @@
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
     </row>
-    <row r="9" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="68" t="s">
         <v>388</v>
       </c>
@@ -3077,7 +3019,7 @@
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
     </row>
-    <row r="10" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="68" t="s">
         <v>389</v>
       </c>
@@ -3095,7 +3037,7 @@
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
     </row>
-    <row r="11" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="68" t="s">
         <v>390</v>
       </c>
@@ -3113,7 +3055,7 @@
       <c r="G11" s="30"/>
       <c r="H11" s="30"/>
     </row>
-    <row r="12" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="68" t="s">
         <v>391</v>
       </c>
@@ -3131,7 +3073,7 @@
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="68" t="s">
         <v>392</v>
       </c>
@@ -3149,7 +3091,7 @@
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="68" t="s">
         <v>393</v>
       </c>
@@ -3167,7 +3109,7 @@
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="68" t="s">
         <v>394</v>
       </c>
@@ -3185,7 +3127,7 @@
       <c r="G15" s="30"/>
       <c r="H15" s="30"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="68" t="s">
         <v>395</v>
       </c>
@@ -3210,23 +3152,23 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="3" width="20.6640625" style="29" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="6" width="20.6640625" style="29" customWidth="1"/>
-    <col min="7" max="10" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" style="29" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="29" customWidth="1"/>
+    <col min="7" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -3258,7 +3200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>352</v>
       </c>
@@ -3283,7 +3225,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>353</v>
       </c>
@@ -3307,7 +3249,7 @@
       <c r="J3" s="22"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>354</v>
       </c>
@@ -3331,7 +3273,7 @@
       <c r="J4" s="22"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>355</v>
       </c>
@@ -3355,7 +3297,7 @@
       <c r="J5" s="22"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="40"/>
       <c r="D6" s="22"/>
       <c r="E6" s="40"/>
@@ -3365,7 +3307,7 @@
       <c r="J6" s="22"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40"/>
@@ -3378,7 +3320,7 @@
       <c r="J7" s="22"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
@@ -3391,7 +3333,7 @@
       <c r="J8" s="22"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
@@ -3409,21 +3351,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16"/>
-    <col min="3" max="3" width="15.5"/>
-    <col min="6" max="6" width="11.1640625"/>
+    <col min="3" max="3" width="15.42578125"/>
+    <col min="6" max="6" width="11.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3446,7 +3388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -3468,24 +3410,24 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="20.6640625" style="33" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" style="33" customWidth="1"/>
-    <col min="6" max="11" width="15.6640625" style="33" customWidth="1"/>
-    <col min="12" max="14" width="20.6640625" style="33" customWidth="1"/>
-    <col min="15" max="16384" width="18.6640625" style="33"/>
+    <col min="1" max="3" width="20.7109375" style="33" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="33" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="33" customWidth="1"/>
+    <col min="6" max="11" width="15.7109375" style="33" customWidth="1"/>
+    <col min="12" max="14" width="20.7109375" style="33" customWidth="1"/>
+    <col min="15" max="16384" width="18.7109375" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -3529,7 +3471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
         <v>277</v>
       </c>
@@ -3555,7 +3497,7 @@
       <c r="M2" s="42"/>
       <c r="N2" s="42"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
         <v>280</v>
       </c>
@@ -3581,7 +3523,7 @@
       <c r="M3" s="42"/>
       <c r="N3" s="42"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>283</v>
       </c>
@@ -3607,7 +3549,7 @@
       <c r="M4" s="42"/>
       <c r="N4" s="42"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="42" t="s">
         <v>286</v>
       </c>
@@ -3633,7 +3575,7 @@
       <c r="M5" s="42"/>
       <c r="N5" s="42"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
         <v>31</v>
       </c>
@@ -3659,7 +3601,7 @@
       <c r="M6" s="42"/>
       <c r="N6" s="42"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>290</v>
       </c>
@@ -3685,7 +3627,7 @@
       <c r="M7" s="42"/>
       <c r="N7" s="42"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="42" t="s">
         <v>293</v>
       </c>
@@ -3712,7 +3654,7 @@
       <c r="N8" s="42"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L220" xr:uid="{00000000-0009-0000-0000-00000F000000}"/>
+  <autoFilter ref="A1:L220"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -3723,27 +3665,27 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" style="41" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="80" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="41" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="52" customWidth="1"/>
-    <col min="6" max="8" width="20.6640625" style="41" customWidth="1"/>
-    <col min="9" max="1024" width="8.6640625" style="2"/>
+    <col min="1" max="2" width="20.7109375" style="41" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="80" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="41" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="52" customWidth="1"/>
+    <col min="6" max="8" width="20.7109375" style="41" customWidth="1"/>
+    <col min="9" max="1024" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>241</v>
       </c>
@@ -4785,7 +4727,7 @@
       <c r="AMI1" s="50"/>
       <c r="AMJ1" s="50"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>295</v>
       </c>
@@ -4804,7 +4746,7 @@
       <c r="F2" s="33"/>
       <c r="H2" s="33"/>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>298</v>
       </c>
@@ -4825,7 +4767,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>301</v>
       </c>
@@ -4846,7 +4788,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>304</v>
       </c>
@@ -4867,7 +4809,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>306</v>
       </c>
@@ -4888,7 +4830,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>309</v>
       </c>
@@ -4906,7 +4848,7 @@
       </c>
       <c r="F7" s="33"/>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>311</v>
       </c>
@@ -4926,7 +4868,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>314</v>
       </c>
@@ -4947,29 +4889,29 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F9" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
+  <autoFilter ref="A1:F9"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="20.6640625" style="33" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" style="27" customWidth="1"/>
-    <col min="6" max="9" width="20.6640625" style="33" customWidth="1"/>
-    <col min="10" max="1025" width="8.5"/>
+    <col min="1" max="3" width="20.7109375" style="33" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" style="27" customWidth="1"/>
+    <col min="6" max="9" width="20.7109375" style="33" customWidth="1"/>
+    <col min="10" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -4998,7 +4940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>317</v>
       </c>
@@ -5015,7 +4957,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>321</v>
       </c>
@@ -5032,7 +4974,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>324</v>
       </c>
@@ -5049,7 +4991,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>326</v>
       </c>
@@ -5066,7 +5008,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>297</v>
       </c>
@@ -5080,7 +5022,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>330</v>
       </c>
@@ -5094,7 +5036,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>333</v>
       </c>
@@ -5108,7 +5050,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>336</v>
       </c>
@@ -5122,7 +5064,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>339</v>
       </c>
@@ -5136,7 +5078,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -5149,20 +5091,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="20.6640625" customWidth="1"/>
-    <col min="1020" max="1024" width="8.6640625"/>
+    <col min="1" max="10" width="20.7109375" customWidth="1"/>
+    <col min="1020" max="1024" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
@@ -5205,19 +5147,19 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="20.6640625" customWidth="1"/>
+    <col min="1" max="13" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
         <v>241</v>
       </c>
@@ -5258,7 +5200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F15" s="34"/>
     </row>
   </sheetData>
@@ -5267,7 +5209,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5277,14 +5219,14 @@
       <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="56" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="26" customWidth="1"/>
-    <col min="3" max="1025" width="8.5"/>
+    <col min="1" max="1" width="30.7109375" style="56" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="26" customWidth="1"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -5292,7 +5234,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>1</v>
       </c>
@@ -5300,7 +5242,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>10</v>
       </c>
@@ -5308,7 +5250,7 @@
         <v>9606</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>9</v>
       </c>
@@ -5317,30 +5259,30 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:B4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="27" customWidth="1"/>
-    <col min="4" max="12" width="20.6640625" style="33" customWidth="1"/>
-    <col min="13" max="1025" width="8.5" style="33"/>
+    <col min="1" max="2" width="20.7109375" style="33" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="27" customWidth="1"/>
+    <col min="4" max="12" width="20.7109375" style="33" customWidth="1"/>
+    <col min="13" max="1025" width="8.42578125" style="33"/>
     <col min="1026" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
@@ -5378,7 +5320,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
         <v>246</v>
       </c>
@@ -5386,7 +5328,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
         <v>258</v>
       </c>
@@ -5394,7 +5336,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
         <v>342</v>
       </c>
@@ -5409,22 +5351,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="20" customWidth="1"/>
-    <col min="2" max="6" width="20.6640625" style="3" customWidth="1"/>
-    <col min="8" max="1020" width="9.1640625" style="3"/>
-    <col min="1024" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="20.7109375" style="20" customWidth="1"/>
+    <col min="2" max="6" width="20.7109375" style="3" customWidth="1"/>
+    <col min="8" max="1020" width="9.140625" style="3"/>
+    <col min="1024" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5444,7 +5386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>14</v>
       </c>
@@ -5461,7 +5403,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>18</v>
       </c>
@@ -5473,7 +5415,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
@@ -5487,7 +5429,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>23</v>
       </c>
@@ -5506,24 +5448,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="6" customWidth="1"/>
-    <col min="3" max="6" width="20.6640625" style="3" customWidth="1"/>
-    <col min="7" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.5"/>
+    <col min="1" max="1" width="20.7109375" style="20" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="6" customWidth="1"/>
+    <col min="3" max="6" width="20.7109375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5552,7 +5494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
@@ -5570,7 +5512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>50</v>
       </c>
@@ -5587,7 +5529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>51</v>
       </c>
@@ -5604,7 +5546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>52</v>
       </c>
@@ -5621,7 +5563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>53</v>
       </c>
@@ -5638,7 +5580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>54</v>
       </c>
@@ -5655,7 +5597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>55</v>
       </c>
@@ -5672,7 +5614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>56</v>
       </c>
@@ -5689,7 +5631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>57</v>
       </c>
@@ -5706,7 +5648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>58</v>
       </c>
@@ -5723,7 +5665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>59</v>
       </c>
@@ -5740,7 +5682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>60</v>
       </c>
@@ -5757,7 +5699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>61</v>
       </c>
@@ -5774,7 +5716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>62</v>
       </c>
@@ -5791,7 +5733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>63</v>
       </c>
@@ -5808,7 +5750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>64</v>
       </c>
@@ -5825,7 +5767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>65</v>
       </c>
@@ -5842,7 +5784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>66</v>
       </c>
@@ -5859,7 +5801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>67</v>
       </c>
@@ -5876,7 +5818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>68</v>
       </c>
@@ -5893,7 +5835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>69</v>
       </c>
@@ -5910,7 +5852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>70</v>
       </c>
@@ -5927,7 +5869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>71</v>
       </c>
@@ -5944,7 +5886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>72</v>
       </c>
@@ -5961,7 +5903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>400</v>
       </c>
@@ -5989,33 +5931,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="50.5" style="6"/>
+    <col min="1" max="1" width="9.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" style="6"/>
     <col min="5" max="5" width="9" style="31"/>
-    <col min="6" max="6" width="18.5" style="6" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="6" customWidth="1"/>
     <col min="7" max="7" width="10" style="6" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="6" customWidth="1"/>
     <col min="9" max="9" width="9" style="9"/>
-    <col min="10" max="10" width="13.5" style="17"/>
+    <col min="10" max="10" width="13.42578125" style="17"/>
     <col min="11" max="11" width="9" style="16"/>
-    <col min="12" max="13" width="9.1640625" style="6"/>
-    <col min="14" max="1021" width="9.1640625" style="17"/>
-    <col min="1022" max="1024" width="8.5"/>
-    <col min="1025" max="1030" width="8.6640625"/>
+    <col min="12" max="13" width="9.140625" style="6"/>
+    <col min="14" max="1021" width="9.140625" style="17"/>
+    <col min="1022" max="1024" width="8.42578125"/>
+    <col min="1025" max="1030" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6026,7 +5968,7 @@
         <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E1" s="81" t="s">
         <v>187</v>
@@ -6050,7 +5992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>197</v>
       </c>
@@ -6068,7 +6010,7 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>199</v>
@@ -6077,7 +6019,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>200</v>
       </c>
@@ -6095,7 +6037,7 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>202</v>
@@ -6104,7 +6046,7 @@
       <c r="M3" s="8"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>203</v>
       </c>
@@ -6124,13 +6066,13 @@
         <v>205</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>206</v>
       </c>
@@ -6150,14 +6092,14 @@
         <v>205</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I849" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <autoFilter ref="A1:I849"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -6168,25 +6110,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="8" max="8" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -6215,7 +6157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>234</v>
       </c>
@@ -6233,7 +6175,7 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>237</v>
       </c>
@@ -6251,7 +6193,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>239</v>
       </c>
@@ -6275,29 +6217,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="74"/>
+    <col min="1" max="1" width="17.42578125" style="74"/>
     <col min="2" max="3" width="9" style="74"/>
-    <col min="4" max="4" width="10.5" style="74" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="74" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="74"/>
-    <col min="7" max="9" width="13.5" style="74"/>
-    <col min="10" max="11" width="20.6640625" style="73" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" style="77" customWidth="1"/>
-    <col min="13" max="1023" width="32.5" style="73"/>
-    <col min="1024" max="1025" width="8.5" style="78"/>
+    <col min="4" max="4" width="10.42578125" style="74" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="74" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="74"/>
+    <col min="7" max="9" width="13.42578125" style="74"/>
+    <col min="10" max="11" width="20.7109375" style="73" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="77" customWidth="1"/>
+    <col min="13" max="1023" width="32.42578125" style="73"/>
+    <col min="1024" max="1025" width="8.42578125" style="78"/>
     <col min="1026" max="16384" width="9" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" s="71" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1023" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
@@ -6341,7 +6283,7 @@
       <c r="AMH1" s="73"/>
       <c r="AMI1" s="73"/>
     </row>
-    <row r="2" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
         <v>79</v>
       </c>
@@ -6365,7 +6307,7 @@
         <v>20651511</v>
       </c>
     </row>
-    <row r="3" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>82</v>
       </c>
@@ -6389,7 +6331,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="4" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
         <v>85</v>
       </c>
@@ -6413,7 +6355,7 @@
         <v>69387254</v>
       </c>
     </row>
-    <row r="5" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A5" s="74" t="s">
         <v>88</v>
       </c>
@@ -6437,7 +6379,7 @@
         <v>40574685</v>
       </c>
     </row>
-    <row r="6" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
         <v>91</v>
       </c>
@@ -6461,7 +6403,7 @@
         <v>112649530</v>
       </c>
     </row>
-    <row r="7" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
         <v>94</v>
       </c>
@@ -6485,7 +6427,7 @@
         <v>83605875</v>
       </c>
     </row>
-    <row r="8" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
         <v>97</v>
       </c>
@@ -6509,7 +6451,7 @@
         <v>127899195</v>
       </c>
     </row>
-    <row r="9" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
         <v>100</v>
       </c>
@@ -6533,7 +6475,7 @@
         <v>160421711</v>
       </c>
     </row>
-    <row r="10" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
         <v>103</v>
       </c>
@@ -6557,7 +6499,7 @@
         <v>152129619</v>
       </c>
     </row>
-    <row r="11" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
         <v>106</v>
       </c>
@@ -6581,7 +6523,7 @@
         <v>56051604</v>
       </c>
     </row>
-    <row r="12" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>109</v>
       </c>
@@ -6605,7 +6547,7 @@
         <v>18084998</v>
       </c>
     </row>
-    <row r="13" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
         <v>112</v>
       </c>
@@ -6629,7 +6571,7 @@
         <v>19967258</v>
       </c>
     </row>
-    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
         <v>115</v>
       </c>
@@ -6653,7 +6595,7 @@
         <v>136423761</v>
       </c>
     </row>
-    <row r="15" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
         <v>118</v>
       </c>
@@ -6677,7 +6619,7 @@
         <v>7787981</v>
       </c>
     </row>
-    <row r="16" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
         <v>121</v>
       </c>
@@ -6701,7 +6643,7 @@
         <v>133421307</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
         <v>124</v>
       </c>
@@ -6725,7 +6667,7 @@
         <v>13732346</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
         <v>127</v>
       </c>
@@ -6749,7 +6691,7 @@
         <v>114450279</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
         <v>130</v>
       </c>
@@ -6773,7 +6715,7 @@
         <v>77065580</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
         <v>133</v>
       </c>
@@ -6797,7 +6739,7 @@
         <v>113359493</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
         <v>136</v>
       </c>
@@ -6821,7 +6763,7 @@
         <v>52476628</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="74" t="s">
         <v>139</v>
       </c>
@@ -6845,7 +6787,7 @@
         <v>103057462</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="74" t="s">
         <v>142</v>
       </c>
@@ -6869,7 +6811,7 @@
         <v>65578352</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="74" t="s">
         <v>145</v>
       </c>
@@ -6893,7 +6835,7 @@
         <v>101251932</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="74" t="s">
         <v>148</v>
       </c>
@@ -6917,7 +6859,7 @@
         <v>89155846</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="74" t="s">
         <v>151</v>
       </c>
@@ -6941,7 +6883,7 @@
         <v>49223225</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="74" t="s">
         <v>154</v>
       </c>
@@ -6965,7 +6907,7 @@
         <v>50988121</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="74" t="s">
         <v>157</v>
       </c>
@@ -6989,7 +6931,7 @@
         <v>41440717</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="74" t="s">
         <v>160</v>
       </c>
@@ -7013,7 +6955,7 @@
         <v>47784686</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
         <v>163</v>
       </c>
@@ -7037,7 +6979,7 @@
         <v>13638940</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="s">
         <v>166</v>
       </c>
@@ -7061,7 +7003,7 @@
         <v>44652233</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="74" t="s">
         <v>169</v>
       </c>
@@ -7085,7 +7027,7 @@
         <v>31668931</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="74" t="s">
         <v>172</v>
       </c>
@@ -7109,7 +7051,7 @@
         <v>20859417</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
         <v>175</v>
       </c>
@@ -7133,7 +7075,7 @@
         <v>38738299</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="74" t="s">
         <v>178</v>
       </c>
@@ -7157,7 +7099,7 @@
         <v>119605895</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="74" t="s">
         <v>181</v>
       </c>
@@ -7181,7 +7123,7 @@
         <v>23005465</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="74" t="s">
         <v>184</v>
       </c>
@@ -7206,7 +7148,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:I1064" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="F1:I1064"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -7217,23 +7159,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMI9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMG9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+      <selection activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="20.6640625" style="22" customWidth="1"/>
-    <col min="4" max="6" width="20.6640625" style="40" customWidth="1"/>
-    <col min="7" max="8" width="20.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="22" customWidth="1"/>
-    <col min="10" max="1023" width="9.1640625" style="3"/>
+    <col min="1" max="3" width="20.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="40" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="22" customWidth="1"/>
+    <col min="8" max="1021" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7246,23 +7188,17 @@
       <c r="D1" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="84" t="s">
-        <v>405</v>
-      </c>
-      <c r="F1" s="84" t="s">
-        <v>406</v>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -7270,7 +7206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -7278,7 +7214,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -7286,7 +7222,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -7294,7 +7230,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>34</v>
       </c>
@@ -7302,7 +7238,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>37</v>
       </c>
@@ -7310,7 +7246,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>40</v>
       </c>
@@ -7318,7 +7254,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>42</v>
       </c>
@@ -7337,26 +7273,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="1023" width="8.5"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="1023" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -7379,7 +7315,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>209</v>
       </c>
@@ -7393,7 +7329,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -7407,7 +7343,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -7421,7 +7357,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>218</v>
       </c>
@@ -7435,10 +7371,10 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="14"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E20" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing regulation direction values to activation/repression
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chebaro/WC/wc_kb/tests/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C681338F-59DE-9647-B1A8-6508371A65AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="4815" windowWidth="24975" windowHeight="5325" tabRatio="993" firstSheet="2" activeTab="12"/>
+    <workbookView xWindow="1360" yWindow="4820" windowWidth="24980" windowHeight="5320" tabRatio="993" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -73,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="412">
   <si>
     <t>Id</t>
   </si>
@@ -1303,12 +1309,18 @@
   </si>
   <si>
     <t>distal</t>
+  </si>
+  <si>
+    <t>activation</t>
+  </si>
+  <si>
+    <t>repression</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1948,170 +1960,170 @@
   <cellStyles count="166">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="13"/>
-    <cellStyle name="Normal 10 2" xfId="28"/>
-    <cellStyle name="Normal 10 2 2" xfId="52"/>
-    <cellStyle name="Normal 10 2 2 2" xfId="97"/>
-    <cellStyle name="Normal 10 2 2 3" xfId="156"/>
-    <cellStyle name="Normal 10 2 3" xfId="75"/>
-    <cellStyle name="Normal 10 2 4" xfId="134"/>
-    <cellStyle name="Normal 10 3" xfId="41"/>
-    <cellStyle name="Normal 10 3 2" xfId="86"/>
-    <cellStyle name="Normal 10 3 3" xfId="145"/>
-    <cellStyle name="Normal 10 4" xfId="64"/>
-    <cellStyle name="Normal 10 4 2" xfId="121"/>
-    <cellStyle name="Normal 10 5" xfId="108"/>
-    <cellStyle name="Normal 11" xfId="14"/>
-    <cellStyle name="Normal 11 2" xfId="29"/>
-    <cellStyle name="Normal 11 2 2" xfId="53"/>
-    <cellStyle name="Normal 11 2 2 2" xfId="98"/>
-    <cellStyle name="Normal 11 2 2 3" xfId="157"/>
-    <cellStyle name="Normal 11 2 3" xfId="76"/>
-    <cellStyle name="Normal 11 2 4" xfId="135"/>
-    <cellStyle name="Normal 11 3" xfId="42"/>
-    <cellStyle name="Normal 11 3 2" xfId="87"/>
-    <cellStyle name="Normal 11 3 3" xfId="146"/>
-    <cellStyle name="Normal 11 4" xfId="65"/>
-    <cellStyle name="Normal 11 4 2" xfId="122"/>
-    <cellStyle name="Normal 11 5" xfId="109"/>
-    <cellStyle name="Normal 12" xfId="17"/>
-    <cellStyle name="Normal 12 2" xfId="32"/>
-    <cellStyle name="Normal 12 2 2" xfId="55"/>
-    <cellStyle name="Normal 12 2 2 2" xfId="100"/>
-    <cellStyle name="Normal 12 2 2 3" xfId="159"/>
-    <cellStyle name="Normal 12 2 3" xfId="78"/>
-    <cellStyle name="Normal 12 2 4" xfId="137"/>
-    <cellStyle name="Normal 12 3" xfId="44"/>
-    <cellStyle name="Normal 12 3 2" xfId="89"/>
-    <cellStyle name="Normal 12 3 3" xfId="148"/>
-    <cellStyle name="Normal 12 4" xfId="67"/>
-    <cellStyle name="Normal 12 4 2" xfId="125"/>
-    <cellStyle name="Normal 12 5" xfId="111"/>
-    <cellStyle name="Normal 13" xfId="57"/>
-    <cellStyle name="Normal 14" xfId="161"/>
-    <cellStyle name="Normal 15" xfId="164"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 3 2" xfId="11"/>
-    <cellStyle name="Normal 3 2 2" xfId="26"/>
-    <cellStyle name="Normal 3 2 3" xfId="119"/>
-    <cellStyle name="Normal 3 3" xfId="15"/>
-    <cellStyle name="Normal 3 3 2" xfId="30"/>
-    <cellStyle name="Normal 3 3 3" xfId="123"/>
-    <cellStyle name="Normal 3 4" xfId="18"/>
-    <cellStyle name="Normal 3 4 2" xfId="33"/>
-    <cellStyle name="Normal 3 4 3" xfId="126"/>
-    <cellStyle name="Normal 3 5" xfId="21"/>
-    <cellStyle name="Normal 3 6" xfId="114"/>
-    <cellStyle name="Normal 3 7" xfId="162"/>
-    <cellStyle name="Normal 4" xfId="5"/>
-    <cellStyle name="Normal 5" xfId="6"/>
-    <cellStyle name="Normal 6" xfId="7"/>
-    <cellStyle name="Normal 6 10" xfId="165"/>
-    <cellStyle name="Normal 6 11" xfId="103"/>
-    <cellStyle name="Normal 6 2" xfId="9"/>
-    <cellStyle name="Normal 6 2 2" xfId="24"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="49"/>
-    <cellStyle name="Normal 6 2 2 2 2" xfId="94"/>
-    <cellStyle name="Normal 6 2 2 2 3" xfId="153"/>
-    <cellStyle name="Normal 6 2 2 3" xfId="72"/>
-    <cellStyle name="Normal 6 2 2 4" xfId="131"/>
-    <cellStyle name="Normal 6 2 3" xfId="38"/>
-    <cellStyle name="Normal 6 2 3 2" xfId="83"/>
-    <cellStyle name="Normal 6 2 3 3" xfId="142"/>
-    <cellStyle name="Normal 6 2 4" xfId="61"/>
-    <cellStyle name="Normal 6 2 4 2" xfId="117"/>
-    <cellStyle name="Normal 6 2 5" xfId="105"/>
-    <cellStyle name="Normal 6 3" xfId="12"/>
-    <cellStyle name="Normal 6 3 2" xfId="27"/>
-    <cellStyle name="Normal 6 3 2 2" xfId="51"/>
-    <cellStyle name="Normal 6 3 2 2 2" xfId="96"/>
-    <cellStyle name="Normal 6 3 2 2 3" xfId="155"/>
-    <cellStyle name="Normal 6 3 2 3" xfId="74"/>
-    <cellStyle name="Normal 6 3 2 4" xfId="133"/>
-    <cellStyle name="Normal 6 3 3" xfId="40"/>
-    <cellStyle name="Normal 6 3 3 2" xfId="85"/>
-    <cellStyle name="Normal 6 3 3 3" xfId="144"/>
-    <cellStyle name="Normal 6 3 4" xfId="63"/>
-    <cellStyle name="Normal 6 3 4 2" xfId="120"/>
-    <cellStyle name="Normal 6 3 5" xfId="107"/>
-    <cellStyle name="Normal 6 4" xfId="16"/>
-    <cellStyle name="Normal 6 4 2" xfId="31"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="54"/>
-    <cellStyle name="Normal 6 4 2 2 2" xfId="99"/>
-    <cellStyle name="Normal 6 4 2 2 3" xfId="158"/>
-    <cellStyle name="Normal 6 4 2 3" xfId="77"/>
-    <cellStyle name="Normal 6 4 2 4" xfId="136"/>
-    <cellStyle name="Normal 6 4 3" xfId="43"/>
-    <cellStyle name="Normal 6 4 3 2" xfId="88"/>
-    <cellStyle name="Normal 6 4 3 3" xfId="147"/>
-    <cellStyle name="Normal 6 4 4" xfId="66"/>
-    <cellStyle name="Normal 6 4 4 2" xfId="124"/>
-    <cellStyle name="Normal 6 4 5" xfId="110"/>
-    <cellStyle name="Normal 6 5" xfId="19"/>
-    <cellStyle name="Normal 6 5 2" xfId="34"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="56"/>
-    <cellStyle name="Normal 6 5 2 2 2" xfId="101"/>
-    <cellStyle name="Normal 6 5 2 2 3" xfId="160"/>
-    <cellStyle name="Normal 6 5 2 3" xfId="79"/>
-    <cellStyle name="Normal 6 5 2 4" xfId="138"/>
-    <cellStyle name="Normal 6 5 3" xfId="45"/>
-    <cellStyle name="Normal 6 5 3 2" xfId="90"/>
-    <cellStyle name="Normal 6 5 3 3" xfId="149"/>
-    <cellStyle name="Normal 6 5 4" xfId="68"/>
-    <cellStyle name="Normal 6 5 4 2" xfId="127"/>
-    <cellStyle name="Normal 6 5 5" xfId="112"/>
-    <cellStyle name="Normal 6 6" xfId="22"/>
-    <cellStyle name="Normal 6 6 2" xfId="47"/>
-    <cellStyle name="Normal 6 6 2 2" xfId="92"/>
-    <cellStyle name="Normal 6 6 2 3" xfId="151"/>
-    <cellStyle name="Normal 6 6 3" xfId="70"/>
-    <cellStyle name="Normal 6 6 4" xfId="129"/>
-    <cellStyle name="Normal 6 7" xfId="36"/>
-    <cellStyle name="Normal 6 7 2" xfId="81"/>
-    <cellStyle name="Normal 6 7 3" xfId="140"/>
-    <cellStyle name="Normal 6 8" xfId="59"/>
-    <cellStyle name="Normal 6 8 2" xfId="115"/>
-    <cellStyle name="Normal 6 9" xfId="163"/>
-    <cellStyle name="Normal 7" xfId="2"/>
-    <cellStyle name="Normal 7 2" xfId="20"/>
-    <cellStyle name="Normal 7 2 2" xfId="46"/>
-    <cellStyle name="Normal 7 2 2 2" xfId="91"/>
-    <cellStyle name="Normal 7 2 2 3" xfId="150"/>
-    <cellStyle name="Normal 7 2 3" xfId="69"/>
-    <cellStyle name="Normal 7 2 4" xfId="128"/>
-    <cellStyle name="Normal 7 3" xfId="35"/>
-    <cellStyle name="Normal 7 3 2" xfId="80"/>
-    <cellStyle name="Normal 7 3 3" xfId="139"/>
-    <cellStyle name="Normal 7 4" xfId="58"/>
-    <cellStyle name="Normal 7 4 2" xfId="113"/>
-    <cellStyle name="Normal 7 5" xfId="102"/>
-    <cellStyle name="Normal 8" xfId="8"/>
-    <cellStyle name="Normal 8 2" xfId="23"/>
-    <cellStyle name="Normal 8 2 2" xfId="48"/>
-    <cellStyle name="Normal 8 2 2 2" xfId="93"/>
-    <cellStyle name="Normal 8 2 2 3" xfId="152"/>
-    <cellStyle name="Normal 8 2 3" xfId="71"/>
-    <cellStyle name="Normal 8 2 4" xfId="130"/>
-    <cellStyle name="Normal 8 3" xfId="37"/>
-    <cellStyle name="Normal 8 3 2" xfId="82"/>
-    <cellStyle name="Normal 8 3 3" xfId="141"/>
-    <cellStyle name="Normal 8 4" xfId="60"/>
-    <cellStyle name="Normal 8 4 2" xfId="116"/>
-    <cellStyle name="Normal 8 5" xfId="104"/>
-    <cellStyle name="Normal 9" xfId="10"/>
-    <cellStyle name="Normal 9 2" xfId="25"/>
-    <cellStyle name="Normal 9 2 2" xfId="50"/>
-    <cellStyle name="Normal 9 2 2 2" xfId="95"/>
-    <cellStyle name="Normal 9 2 2 3" xfId="154"/>
-    <cellStyle name="Normal 9 2 3" xfId="73"/>
-    <cellStyle name="Normal 9 2 4" xfId="132"/>
-    <cellStyle name="Normal 9 3" xfId="39"/>
-    <cellStyle name="Normal 9 3 2" xfId="84"/>
-    <cellStyle name="Normal 9 3 3" xfId="143"/>
-    <cellStyle name="Normal 9 4" xfId="62"/>
-    <cellStyle name="Normal 9 4 2" xfId="118"/>
-    <cellStyle name="Normal 9 5" xfId="106"/>
+    <cellStyle name="Normal 10" xfId="13" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 10 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 10 2 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 10 2 2 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 10 2 2 3" xfId="156" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 10 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 10 2 4" xfId="134" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 10 3" xfId="41" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 10 3 2" xfId="86" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 10 3 3" xfId="145" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 10 4" xfId="64" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 10 4 2" xfId="121" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 10 5" xfId="108" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 11" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 11 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 11 2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 11 2 2 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 11 2 2 3" xfId="157" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 11 2 3" xfId="76" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 11 2 4" xfId="135" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 11 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 11 3 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 11 3 3" xfId="146" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 11 4" xfId="65" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 11 4 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 11 5" xfId="109" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 12" xfId="17" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 12 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 12 2 2" xfId="55" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 12 2 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 12 2 2 3" xfId="159" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 12 2 3" xfId="78" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normal 12 2 4" xfId="137" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normal 12 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normal 12 3 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 12 3 3" xfId="148" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 12 4" xfId="67" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 12 4 2" xfId="125" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 12 5" xfId="111" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 13" xfId="57" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 14" xfId="161" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 15" xfId="164" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Normal 3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 3 2 3" xfId="119" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal 3 3" xfId="15" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 3 3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 3 3 3" xfId="123" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 3 4" xfId="18" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Normal 3 4 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 3 4 3" xfId="126" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Normal 3 5" xfId="21" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Normal 3 6" xfId="114" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Normal 3 7" xfId="162" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Normal 5" xfId="6" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Normal 6" xfId="7" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Normal 6 10" xfId="165" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Normal 6 11" xfId="103" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Normal 6 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Normal 6 2 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3" xfId="153" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Normal 6 2 2 3" xfId="72" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 6 2 2 4" xfId="131" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Normal 6 2 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Normal 6 2 3 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Normal 6 2 3 3" xfId="142" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Normal 6 2 4" xfId="61" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Normal 6 2 4 2" xfId="117" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 6 2 5" xfId="105" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 6 3" xfId="12" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 6 3 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 6 3 2 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3" xfId="155" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 6 3 2 3" xfId="74" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 6 3 2 4" xfId="133" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 6 3 3" xfId="40" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 6 3 3 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 6 3 3 3" xfId="144" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 6 3 4" xfId="63" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 6 3 4 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 6 3 5" xfId="107" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 6 4" xfId="16" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 6 4 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 6 4 2 2 2" xfId="99" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 6 4 2 2 3" xfId="158" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 6 4 2 3" xfId="77" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 6 4 2 4" xfId="136" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 6 4 3" xfId="43" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 6 4 3 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 6 4 3 3" xfId="147" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 6 4 4" xfId="66" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 6 4 4 2" xfId="124" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 6 4 5" xfId="110" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 6 5" xfId="19" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 6 5 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 6 5 2 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 6 5 2 2 3" xfId="160" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 6 5 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 6 5 2 4" xfId="138" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 6 5 3" xfId="45" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 6 5 3 2" xfId="90" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 6 5 3 3" xfId="149" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 6 5 4" xfId="68" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 6 5 4 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 6 5 5" xfId="112" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 6 6" xfId="22" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Normal 6 6 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Normal 6 6 2 2" xfId="92" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Normal 6 6 2 3" xfId="151" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Normal 6 6 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Normal 6 6 4" xfId="129" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Normal 6 7" xfId="36" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Normal 6 7 2" xfId="81" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Normal 6 7 3" xfId="140" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Normal 6 8" xfId="59" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Normal 6 8 2" xfId="115" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Normal 6 9" xfId="163" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Normal 7" xfId="2" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Normal 7 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Normal 7 2 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Normal 7 2 2 2" xfId="91" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Normal 7 2 2 3" xfId="150" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Normal 7 2 3" xfId="69" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Normal 7 2 4" xfId="128" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Normal 7 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Normal 7 3 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Normal 7 3 3" xfId="139" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Normal 7 4" xfId="58" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Normal 7 4 2" xfId="113" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Normal 7 5" xfId="102" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Normal 8" xfId="8" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Normal 8 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Normal 8 2 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Normal 8 2 2 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Normal 8 2 2 3" xfId="152" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Normal 8 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Normal 8 2 4" xfId="130" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Normal 8 3" xfId="37" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Normal 8 3 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Normal 8 3 3" xfId="141" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Normal 8 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Normal 8 4 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Normal 8 5" xfId="104" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Normal 9" xfId="10" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Normal 9 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Normal 9 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Normal 9 2 2 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Normal 9 2 2 3" xfId="154" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Normal 9 2 3" xfId="73" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Normal 9 2 4" xfId="132" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Normal 9 3" xfId="39" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Normal 9 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Normal 9 3 3" xfId="143" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Normal 9 4" xfId="62" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Normal 9 4 2" xfId="118" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Normal 9 5" xfId="106" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2237,7 +2249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2270,9 +2282,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2305,6 +2334,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2480,7 +2526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2490,14 +2536,14 @@
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="19"/>
-    <col min="2" max="2" width="43.42578125" style="3"/>
-    <col min="3" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="21.5" style="19"/>
+    <col min="2" max="2" width="43.5" style="3"/>
+    <col min="3" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -2505,7 +2551,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
@@ -2513,7 +2559,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>2</v>
       </c>
@@ -2521,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
@@ -2529,25 +2575,25 @@
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
@@ -2555,7 +2601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>9</v>
       </c>
@@ -2564,35 +2610,35 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9"/>
+  <autoFilter ref="A1:B9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AME15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="4"/>
-    <col min="2" max="2" width="33.85546875" style="4"/>
-    <col min="3" max="3" width="16.42578125" style="9"/>
+    <col min="1" max="1" width="20.33203125" style="4"/>
+    <col min="2" max="2" width="33.83203125" style="4"/>
+    <col min="3" max="3" width="16.5" style="9"/>
     <col min="4" max="4" width="17" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="1019" width="9.140625" style="3"/>
-    <col min="1022" max="1024" width="8.7109375"/>
+    <col min="5" max="5" width="25.5" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="1019" width="9.1640625" style="3"/>
+    <col min="1022" max="1024" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2618,7 +2664,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>193</v>
       </c>
@@ -2635,7 +2681,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>227</v>
       </c>
@@ -2652,7 +2698,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>205</v>
       </c>
@@ -2669,24 +2715,24 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F719"/>
+  <autoFilter ref="A1:F719" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -2697,26 +2743,26 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMD5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" style="86" customWidth="1"/>
+    <col min="1" max="2" width="20.6640625" style="86" customWidth="1"/>
     <col min="3" max="4" width="9" style="86"/>
-    <col min="5" max="5" width="30.7109375" style="86" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="68" customWidth="1"/>
-    <col min="7" max="9" width="15.7109375" style="86" customWidth="1"/>
-    <col min="10" max="1018" width="8.42578125" style="86"/>
-    <col min="1019" max="1021" width="8.42578125" style="85"/>
+    <col min="5" max="5" width="30.6640625" style="86" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="68" customWidth="1"/>
+    <col min="7" max="9" width="15.6640625" style="86" customWidth="1"/>
+    <col min="10" max="1018" width="8.5" style="86"/>
+    <col min="1019" max="1021" width="8.5" style="85"/>
     <col min="1022" max="16384" width="9" style="85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="57" t="s">
         <v>241</v>
       </c>
@@ -2745,7 +2791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="84" t="s">
         <v>244</v>
       </c>
@@ -2765,7 +2811,7 @@
       </c>
       <c r="I2" s="84"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="84" t="s">
         <v>247</v>
       </c>
@@ -2783,7 +2829,7 @@
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="84" t="s">
         <v>248</v>
       </c>
@@ -2801,7 +2847,7 @@
       <c r="H4" s="84"/>
       <c r="I4" s="84"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="84" t="s">
         <v>249</v>
       </c>
@@ -2819,14 +2865,14 @@
       <c r="I5" s="84"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G221"/>
+  <autoFilter ref="A1:G221" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AML16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2836,16 +2882,16 @@
       <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="25" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="5" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" style="5" customWidth="1"/>
-    <col min="5" max="8" width="20.7109375" style="5" customWidth="1"/>
-    <col min="9" max="1026" width="8.42578125" style="5"/>
+    <col min="1" max="1" width="20.6640625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="5" customWidth="1"/>
+    <col min="3" max="4" width="15.6640625" style="5" customWidth="1"/>
+    <col min="5" max="8" width="20.6640625" style="5" customWidth="1"/>
+    <col min="9" max="1026" width="8.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="67" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="67" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
@@ -2871,7 +2917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="69" t="s">
         <v>381</v>
       </c>
@@ -2891,7 +2937,7 @@
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
     </row>
-    <row r="3" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="68" t="s">
         <v>382</v>
       </c>
@@ -2911,7 +2957,7 @@
       </c>
       <c r="H3" s="30"/>
     </row>
-    <row r="4" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
         <v>383</v>
       </c>
@@ -2929,7 +2975,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
     </row>
-    <row r="5" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="68" t="s">
         <v>384</v>
       </c>
@@ -2947,7 +2993,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
     </row>
-    <row r="6" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="68" t="s">
         <v>385</v>
       </c>
@@ -2965,7 +3011,7 @@
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
     </row>
-    <row r="7" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="s">
         <v>386</v>
       </c>
@@ -2983,7 +3029,7 @@
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
     </row>
-    <row r="8" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="68" t="s">
         <v>387</v>
       </c>
@@ -3001,7 +3047,7 @@
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
     </row>
-    <row r="9" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="68" t="s">
         <v>388</v>
       </c>
@@ -3019,7 +3065,7 @@
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
     </row>
-    <row r="10" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="68" t="s">
         <v>389</v>
       </c>
@@ -3037,7 +3083,7 @@
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
     </row>
-    <row r="11" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="68" t="s">
         <v>390</v>
       </c>
@@ -3055,7 +3101,7 @@
       <c r="G11" s="30"/>
       <c r="H11" s="30"/>
     </row>
-    <row r="12" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="68" t="s">
         <v>391</v>
       </c>
@@ -3073,7 +3119,7 @@
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="68" t="s">
         <v>392</v>
       </c>
@@ -3091,7 +3137,7 @@
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="68" t="s">
         <v>393</v>
       </c>
@@ -3109,7 +3155,7 @@
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="68" t="s">
         <v>394</v>
       </c>
@@ -3127,7 +3173,7 @@
       <c r="G15" s="30"/>
       <c r="H15" s="30"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="68" t="s">
         <v>395</v>
       </c>
@@ -3152,23 +3198,23 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="29" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="29" customWidth="1"/>
-    <col min="7" max="10" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="29" customWidth="1"/>
+    <col min="7" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -3200,7 +3246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>352</v>
       </c>
@@ -3225,7 +3271,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>353</v>
       </c>
@@ -3249,7 +3295,7 @@
       <c r="J3" s="22"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>354</v>
       </c>
@@ -3273,7 +3319,7 @@
       <c r="J4" s="22"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
         <v>355</v>
       </c>
@@ -3297,7 +3343,7 @@
       <c r="J5" s="22"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C6" s="40"/>
       <c r="D6" s="22"/>
       <c r="E6" s="40"/>
@@ -3307,7 +3353,7 @@
       <c r="J6" s="22"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40"/>
@@ -3320,7 +3366,7 @@
       <c r="J7" s="22"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
@@ -3333,7 +3379,7 @@
       <c r="J8" s="22"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
@@ -3351,21 +3397,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16"/>
-    <col min="3" max="3" width="15.42578125"/>
-    <col min="6" max="6" width="11.140625"/>
+    <col min="3" max="3" width="15.5"/>
+    <col min="6" max="6" width="11.1640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3388,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -3410,24 +3456,24 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" style="33" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="33" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" style="33" customWidth="1"/>
-    <col min="6" max="11" width="15.7109375" style="33" customWidth="1"/>
-    <col min="12" max="14" width="20.7109375" style="33" customWidth="1"/>
-    <col min="15" max="16384" width="18.7109375" style="33"/>
+    <col min="1" max="3" width="20.6640625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="33" customWidth="1"/>
+    <col min="6" max="11" width="15.6640625" style="33" customWidth="1"/>
+    <col min="12" max="14" width="20.6640625" style="33" customWidth="1"/>
+    <col min="15" max="16384" width="18.6640625" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -3471,7 +3517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="42" t="s">
         <v>277</v>
       </c>
@@ -3497,7 +3543,7 @@
       <c r="M2" s="42"/>
       <c r="N2" s="42"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="42" t="s">
         <v>280</v>
       </c>
@@ -3523,7 +3569,7 @@
       <c r="M3" s="42"/>
       <c r="N3" s="42"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="42" t="s">
         <v>283</v>
       </c>
@@ -3549,7 +3595,7 @@
       <c r="M4" s="42"/>
       <c r="N4" s="42"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="42" t="s">
         <v>286</v>
       </c>
@@ -3575,7 +3621,7 @@
       <c r="M5" s="42"/>
       <c r="N5" s="42"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="42" t="s">
         <v>31</v>
       </c>
@@ -3601,7 +3647,7 @@
       <c r="M6" s="42"/>
       <c r="N6" s="42"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="42" t="s">
         <v>290</v>
       </c>
@@ -3627,7 +3673,7 @@
       <c r="M7" s="42"/>
       <c r="N7" s="42"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="42" t="s">
         <v>293</v>
       </c>
@@ -3654,7 +3700,7 @@
       <c r="N8" s="42"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L220"/>
+  <autoFilter ref="A1:L220" xr:uid="{00000000-0009-0000-0000-00000E000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -3665,7 +3711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3675,17 +3721,17 @@
       <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" style="41" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="80" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="41" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="52" customWidth="1"/>
-    <col min="6" max="8" width="20.7109375" style="41" customWidth="1"/>
-    <col min="9" max="1024" width="8.7109375" style="2"/>
+    <col min="1" max="2" width="20.6640625" style="41" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="80" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="52" customWidth="1"/>
+    <col min="6" max="8" width="20.6640625" style="41" customWidth="1"/>
+    <col min="9" max="1024" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1024" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="48" t="s">
         <v>241</v>
       </c>
@@ -4727,7 +4773,7 @@
       <c r="AMI1" s="50"/>
       <c r="AMJ1" s="50"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>295</v>
       </c>
@@ -4746,7 +4792,7 @@
       <c r="F2" s="33"/>
       <c r="H2" s="33"/>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>298</v>
       </c>
@@ -4767,7 +4813,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
         <v>301</v>
       </c>
@@ -4788,7 +4834,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
         <v>304</v>
       </c>
@@ -4809,7 +4855,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
         <v>306</v>
       </c>
@@ -4830,7 +4876,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>309</v>
       </c>
@@ -4848,7 +4894,7 @@
       </c>
       <c r="F7" s="33"/>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>311</v>
       </c>
@@ -4868,7 +4914,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
         <v>314</v>
       </c>
@@ -4889,29 +4935,29 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F9"/>
+  <autoFilter ref="A1:F9" xr:uid="{00000000-0009-0000-0000-00000F000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" style="33" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" style="27" customWidth="1"/>
-    <col min="6" max="9" width="20.7109375" style="33" customWidth="1"/>
-    <col min="10" max="1025" width="8.42578125"/>
+    <col min="1" max="3" width="20.6640625" style="33" customWidth="1"/>
+    <col min="4" max="5" width="15.6640625" style="27" customWidth="1"/>
+    <col min="6" max="9" width="20.6640625" style="33" customWidth="1"/>
+    <col min="10" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -4940,7 +4986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
         <v>317</v>
       </c>
@@ -4957,7 +5003,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
         <v>321</v>
       </c>
@@ -4974,7 +5020,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
         <v>324</v>
       </c>
@@ -4991,7 +5037,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>326</v>
       </c>
@@ -5008,7 +5054,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="33" t="s">
         <v>297</v>
       </c>
@@ -5022,7 +5068,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>330</v>
       </c>
@@ -5036,7 +5082,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>333</v>
       </c>
@@ -5050,7 +5096,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>336</v>
       </c>
@@ -5064,7 +5110,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>339</v>
       </c>
@@ -5078,7 +5124,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -5091,20 +5137,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="20.7109375" customWidth="1"/>
-    <col min="1020" max="1024" width="8.7109375"/>
+    <col min="1" max="10" width="20.6640625" customWidth="1"/>
+    <col min="1020" max="1024" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
@@ -5147,19 +5193,19 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="20.7109375" customWidth="1"/>
+    <col min="1" max="13" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
         <v>241</v>
       </c>
@@ -5200,7 +5246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F15" s="34"/>
     </row>
   </sheetData>
@@ -5209,7 +5255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5219,14 +5265,14 @@
       <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="56" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="26" customWidth="1"/>
-    <col min="3" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="30.6640625" style="56" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="26" customWidth="1"/>
+    <col min="3" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -5234,7 +5280,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="56" t="s">
         <v>1</v>
       </c>
@@ -5242,7 +5288,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
         <v>10</v>
       </c>
@@ -5250,7 +5296,7 @@
         <v>9606</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="56" t="s">
         <v>9</v>
       </c>
@@ -5259,30 +5305,30 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B4"/>
+  <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" style="33" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="27" customWidth="1"/>
-    <col min="4" max="12" width="20.7109375" style="33" customWidth="1"/>
-    <col min="13" max="1025" width="8.42578125" style="33"/>
+    <col min="1" max="2" width="20.6640625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="27" customWidth="1"/>
+    <col min="4" max="12" width="20.6640625" style="33" customWidth="1"/>
+    <col min="13" max="1025" width="8.5" style="33"/>
     <col min="1026" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
@@ -5320,7 +5366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>246</v>
       </c>
@@ -5328,7 +5374,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>258</v>
       </c>
@@ -5336,7 +5382,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="33" t="s">
         <v>342</v>
       </c>
@@ -5351,22 +5397,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="20" customWidth="1"/>
-    <col min="2" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="8" max="1020" width="9.140625" style="3"/>
-    <col min="1024" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="20.6640625" style="20" customWidth="1"/>
+    <col min="2" max="6" width="20.6640625" style="3" customWidth="1"/>
+    <col min="8" max="1020" width="9.1640625" style="3"/>
+    <col min="1024" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5386,7 +5432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>14</v>
       </c>
@@ -5403,7 +5449,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>18</v>
       </c>
@@ -5415,7 +5461,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
@@ -5429,7 +5475,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>23</v>
       </c>
@@ -5448,24 +5494,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="20" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="6" customWidth="1"/>
-    <col min="3" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125"/>
+    <col min="1" max="1" width="20.6640625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="6" customWidth="1"/>
+    <col min="3" max="6" width="20.6640625" style="3" customWidth="1"/>
+    <col min="7" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5494,7 +5540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
@@ -5512,7 +5558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>50</v>
       </c>
@@ -5529,7 +5575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>51</v>
       </c>
@@ -5546,7 +5592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>52</v>
       </c>
@@ -5563,7 +5609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>53</v>
       </c>
@@ -5580,7 +5626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>54</v>
       </c>
@@ -5597,7 +5643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>55</v>
       </c>
@@ -5614,7 +5660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>56</v>
       </c>
@@ -5631,7 +5677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>57</v>
       </c>
@@ -5648,7 +5694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>58</v>
       </c>
@@ -5665,7 +5711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>59</v>
       </c>
@@ -5682,7 +5728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>60</v>
       </c>
@@ -5699,7 +5745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>61</v>
       </c>
@@ -5716,7 +5762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>62</v>
       </c>
@@ -5733,7 +5779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>63</v>
       </c>
@@ -5750,7 +5796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>64</v>
       </c>
@@ -5767,7 +5813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>65</v>
       </c>
@@ -5784,7 +5830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>66</v>
       </c>
@@ -5801,7 +5847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>67</v>
       </c>
@@ -5818,7 +5864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>68</v>
       </c>
@@ -5835,7 +5881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>69</v>
       </c>
@@ -5852,7 +5898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>70</v>
       </c>
@@ -5869,7 +5915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>71</v>
       </c>
@@ -5886,7 +5932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>72</v>
       </c>
@@ -5903,7 +5949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
         <v>400</v>
       </c>
@@ -5931,33 +5977,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMG5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" style="6"/>
+    <col min="1" max="1" width="9.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="50.5" style="6"/>
     <col min="5" max="5" width="9" style="31"/>
-    <col min="6" max="6" width="18.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="6" customWidth="1"/>
     <col min="7" max="7" width="10" style="6" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="6" customWidth="1"/>
     <col min="9" max="9" width="9" style="9"/>
-    <col min="10" max="10" width="13.42578125" style="17"/>
+    <col min="10" max="10" width="13.5" style="17"/>
     <col min="11" max="11" width="9" style="16"/>
-    <col min="12" max="13" width="9.140625" style="6"/>
-    <col min="14" max="1021" width="9.140625" style="17"/>
-    <col min="1022" max="1024" width="8.42578125"/>
-    <col min="1025" max="1030" width="8.7109375"/>
+    <col min="12" max="13" width="9.1640625" style="6"/>
+    <col min="14" max="1021" width="9.1640625" style="17"/>
+    <col min="1022" max="1024" width="8.5"/>
+    <col min="1025" max="1030" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5992,7 +6038,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>197</v>
       </c>
@@ -6013,13 +6059,13 @@
         <v>408</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>199</v>
+        <v>410</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>200</v>
       </c>
@@ -6040,13 +6086,13 @@
         <v>408</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>203</v>
       </c>
@@ -6069,10 +6115,10 @@
         <v>409</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>206</v>
       </c>
@@ -6095,11 +6141,11 @@
         <v>409</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>199</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I849"/>
+  <autoFilter ref="A1:I849" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -6110,25 +6156,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -6157,7 +6203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>234</v>
       </c>
@@ -6175,7 +6221,7 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>237</v>
       </c>
@@ -6193,7 +6239,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>239</v>
       </c>
@@ -6217,29 +6263,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMI37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="74"/>
+    <col min="1" max="1" width="17.5" style="74"/>
     <col min="2" max="3" width="9" style="74"/>
-    <col min="4" max="4" width="10.42578125" style="74" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="74" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="74"/>
-    <col min="7" max="9" width="13.42578125" style="74"/>
-    <col min="10" max="11" width="20.7109375" style="73" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="77" customWidth="1"/>
-    <col min="13" max="1023" width="32.42578125" style="73"/>
-    <col min="1024" max="1025" width="8.42578125" style="78"/>
+    <col min="4" max="4" width="10.5" style="74" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="74" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="74"/>
+    <col min="7" max="9" width="13.5" style="74"/>
+    <col min="10" max="11" width="20.6640625" style="73" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" style="77" customWidth="1"/>
+    <col min="13" max="1023" width="32.5" style="73"/>
+    <col min="1024" max="1025" width="8.5" style="78"/>
     <col min="1026" max="16384" width="9" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1023" s="71" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
@@ -6283,7 +6329,7 @@
       <c r="AMH1" s="73"/>
       <c r="AMI1" s="73"/>
     </row>
-    <row r="2" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A2" s="74" t="s">
         <v>79</v>
       </c>
@@ -6307,7 +6353,7 @@
         <v>20651511</v>
       </c>
     </row>
-    <row r="3" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A3" s="74" t="s">
         <v>82</v>
       </c>
@@ -6331,7 +6377,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="4" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A4" s="74" t="s">
         <v>85</v>
       </c>
@@ -6355,7 +6401,7 @@
         <v>69387254</v>
       </c>
     </row>
-    <row r="5" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A5" s="74" t="s">
         <v>88</v>
       </c>
@@ -6379,7 +6425,7 @@
         <v>40574685</v>
       </c>
     </row>
-    <row r="6" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A6" s="74" t="s">
         <v>91</v>
       </c>
@@ -6403,7 +6449,7 @@
         <v>112649530</v>
       </c>
     </row>
-    <row r="7" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A7" s="74" t="s">
         <v>94</v>
       </c>
@@ -6427,7 +6473,7 @@
         <v>83605875</v>
       </c>
     </row>
-    <row r="8" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A8" s="74" t="s">
         <v>97</v>
       </c>
@@ -6451,7 +6497,7 @@
         <v>127899195</v>
       </c>
     </row>
-    <row r="9" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A9" s="74" t="s">
         <v>100</v>
       </c>
@@ -6475,7 +6521,7 @@
         <v>160421711</v>
       </c>
     </row>
-    <row r="10" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A10" s="74" t="s">
         <v>103</v>
       </c>
@@ -6499,7 +6545,7 @@
         <v>152129619</v>
       </c>
     </row>
-    <row r="11" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A11" s="74" t="s">
         <v>106</v>
       </c>
@@ -6523,7 +6569,7 @@
         <v>56051604</v>
       </c>
     </row>
-    <row r="12" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A12" s="74" t="s">
         <v>109</v>
       </c>
@@ -6547,7 +6593,7 @@
         <v>18084998</v>
       </c>
     </row>
-    <row r="13" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A13" s="74" t="s">
         <v>112</v>
       </c>
@@ -6571,7 +6617,7 @@
         <v>19967258</v>
       </c>
     </row>
-    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="74" t="s">
         <v>115</v>
       </c>
@@ -6595,7 +6641,7 @@
         <v>136423761</v>
       </c>
     </row>
-    <row r="15" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A15" s="74" t="s">
         <v>118</v>
       </c>
@@ -6619,7 +6665,7 @@
         <v>7787981</v>
       </c>
     </row>
-    <row r="16" spans="1:1023" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A16" s="74" t="s">
         <v>121</v>
       </c>
@@ -6643,7 +6689,7 @@
         <v>133421307</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="74" t="s">
         <v>124</v>
       </c>
@@ -6667,7 +6713,7 @@
         <v>13732346</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="74" t="s">
         <v>127</v>
       </c>
@@ -6691,7 +6737,7 @@
         <v>114450279</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="74" t="s">
         <v>130</v>
       </c>
@@ -6715,7 +6761,7 @@
         <v>77065580</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="74" t="s">
         <v>133</v>
       </c>
@@ -6739,7 +6785,7 @@
         <v>113359493</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="74" t="s">
         <v>136</v>
       </c>
@@ -6763,7 +6809,7 @@
         <v>52476628</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="74" t="s">
         <v>139</v>
       </c>
@@ -6787,7 +6833,7 @@
         <v>103057462</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="74" t="s">
         <v>142</v>
       </c>
@@ -6811,7 +6857,7 @@
         <v>65578352</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="74" t="s">
         <v>145</v>
       </c>
@@ -6835,7 +6881,7 @@
         <v>101251932</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="74" t="s">
         <v>148</v>
       </c>
@@ -6859,7 +6905,7 @@
         <v>89155846</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="74" t="s">
         <v>151</v>
       </c>
@@ -6883,7 +6929,7 @@
         <v>49223225</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="74" t="s">
         <v>154</v>
       </c>
@@ -6907,7 +6953,7 @@
         <v>50988121</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="74" t="s">
         <v>157</v>
       </c>
@@ -6931,7 +6977,7 @@
         <v>41440717</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="74" t="s">
         <v>160</v>
       </c>
@@ -6955,7 +7001,7 @@
         <v>47784686</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="74" t="s">
         <v>163</v>
       </c>
@@ -6979,7 +7025,7 @@
         <v>13638940</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="74" t="s">
         <v>166</v>
       </c>
@@ -7003,7 +7049,7 @@
         <v>44652233</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="74" t="s">
         <v>169</v>
       </c>
@@ -7027,7 +7073,7 @@
         <v>31668931</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="74" t="s">
         <v>172</v>
       </c>
@@ -7051,7 +7097,7 @@
         <v>20859417</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="74" t="s">
         <v>175</v>
       </c>
@@ -7075,7 +7121,7 @@
         <v>38738299</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="74" t="s">
         <v>178</v>
       </c>
@@ -7099,7 +7145,7 @@
         <v>119605895</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="74" t="s">
         <v>181</v>
       </c>
@@ -7123,7 +7169,7 @@
         <v>23005465</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="74" t="s">
         <v>184</v>
       </c>
@@ -7148,7 +7194,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:I1064"/>
+  <autoFilter ref="F1:I1064" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -7159,23 +7205,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AMG9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" style="22" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="40" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="22" customWidth="1"/>
-    <col min="8" max="1021" width="9.140625" style="3"/>
+    <col min="1" max="3" width="20.6640625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="40" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="22" customWidth="1"/>
+    <col min="8" max="1021" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7198,7 +7244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -7206,7 +7252,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -7214,7 +7260,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -7222,7 +7268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -7230,7 +7276,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>34</v>
       </c>
@@ -7238,7 +7284,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>37</v>
       </c>
@@ -7246,7 +7292,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>40</v>
       </c>
@@ -7254,7 +7300,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>42</v>
       </c>
@@ -7273,26 +7319,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="1023" width="8.42578125"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="1023" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -7315,7 +7361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>209</v>
       </c>
@@ -7329,7 +7375,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -7343,7 +7389,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -7357,7 +7403,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>218</v>
       </c>
@@ -7371,10 +7417,10 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="14"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E20" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add transcript type to eukaryote_schema
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chebaro/WC/wc_kb/tests/fixtures/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C681338F-59DE-9647-B1A8-6508371A65AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="4820" windowWidth="24980" windowHeight="5320" tabRatio="993" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="4815" windowWidth="24975" windowHeight="5325" tabRatio="993" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -79,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="414">
   <si>
     <t>Id</t>
   </si>
@@ -1315,12 +1309,18 @@
   </si>
   <si>
     <t>repression</t>
+  </si>
+  <si>
+    <t>mRna</t>
+  </si>
+  <si>
+    <t>rRna</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1960,170 +1960,170 @@
   <cellStyles count="166">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="13" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 10 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 10 2 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 10 2 2 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 10 2 2 3" xfId="156" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 10 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 10 2 4" xfId="134" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 10 3" xfId="41" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 10 3 2" xfId="86" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 10 3 3" xfId="145" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 10 4" xfId="64" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 10 4 2" xfId="121" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Normal 10 5" xfId="108" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Normal 11" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Normal 11 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Normal 11 2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Normal 11 2 2 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Normal 11 2 2 3" xfId="157" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Normal 11 2 3" xfId="76" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Normal 11 2 4" xfId="135" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Normal 11 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Normal 11 3 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Normal 11 3 3" xfId="146" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Normal 11 4" xfId="65" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Normal 11 4 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Normal 11 5" xfId="109" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Normal 12" xfId="17" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Normal 12 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Normal 12 2 2" xfId="55" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Normal 12 2 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Normal 12 2 2 3" xfId="159" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Normal 12 2 3" xfId="78" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Normal 12 2 4" xfId="137" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Normal 12 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Normal 12 3 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Normal 12 3 3" xfId="148" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal 12 4" xfId="67" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Normal 12 4 2" xfId="125" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Normal 12 5" xfId="111" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Normal 13" xfId="57" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Normal 14" xfId="161" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Normal 15" xfId="164" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Normal 3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="119" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Normal 3 3" xfId="15" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="123" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Normal 3 4" xfId="18" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Normal 3 4 3" xfId="126" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Normal 3 5" xfId="21" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Normal 3 6" xfId="114" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Normal 3 7" xfId="162" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Normal 5" xfId="6" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Normal 6" xfId="7" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Normal 6 10" xfId="165" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Normal 6 11" xfId="103" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Normal 6 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Normal 6 2 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3" xfId="153" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Normal 6 2 2 3" xfId="72" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Normal 6 2 2 4" xfId="131" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Normal 6 2 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Normal 6 2 3 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Normal 6 2 3 3" xfId="142" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Normal 6 2 4" xfId="61" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Normal 6 2 4 2" xfId="117" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 6 2 5" xfId="105" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 6 3" xfId="12" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 6 3 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 6 3 2 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 6 3 2 2 3" xfId="155" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 6 3 2 3" xfId="74" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 6 3 2 4" xfId="133" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 6 3 3" xfId="40" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 6 3 3 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 6 3 3 3" xfId="144" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 6 3 4" xfId="63" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 6 3 4 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 6 3 5" xfId="107" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 6 4" xfId="16" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 6 4 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 6 4 2 2 2" xfId="99" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 6 4 2 2 3" xfId="158" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 6 4 2 3" xfId="77" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 6 4 2 4" xfId="136" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 6 4 3" xfId="43" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 6 4 3 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 6 4 3 3" xfId="147" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 6 4 4" xfId="66" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 6 4 4 2" xfId="124" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 6 4 5" xfId="110" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 6 5" xfId="19" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 6 5 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 6 5 2 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 6 5 2 2 3" xfId="160" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 6 5 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 6 5 2 4" xfId="138" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 6 5 3" xfId="45" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6 5 3 2" xfId="90" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 6 5 3 3" xfId="149" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 6 5 4" xfId="68" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 6 5 4 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Normal 6 5 5" xfId="112" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Normal 6 6" xfId="22" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Normal 6 6 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Normal 6 6 2 2" xfId="92" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Normal 6 6 2 3" xfId="151" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Normal 6 6 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Normal 6 6 4" xfId="129" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Normal 6 7" xfId="36" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Normal 6 7 2" xfId="81" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Normal 6 7 3" xfId="140" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Normal 6 8" xfId="59" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Normal 6 8 2" xfId="115" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Normal 6 9" xfId="163" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Normal 7" xfId="2" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Normal 7 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Normal 7 2 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Normal 7 2 2 2" xfId="91" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Normal 7 2 2 3" xfId="150" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Normal 7 2 3" xfId="69" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Normal 7 2 4" xfId="128" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Normal 7 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Normal 7 3 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Normal 7 3 3" xfId="139" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Normal 7 4" xfId="58" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Normal 7 4 2" xfId="113" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Normal 7 5" xfId="102" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Normal 8" xfId="8" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Normal 8 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Normal 8 2 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Normal 8 2 2 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Normal 8 2 2 3" xfId="152" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Normal 8 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Normal 8 2 4" xfId="130" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Normal 8 3" xfId="37" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Normal 8 3 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Normal 8 3 3" xfId="141" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Normal 8 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Normal 8 4 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Normal 8 5" xfId="104" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Normal 9" xfId="10" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="Normal 9 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="Normal 9 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="Normal 9 2 2 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="Normal 9 2 2 3" xfId="154" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="Normal 9 2 3" xfId="73" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="Normal 9 2 4" xfId="132" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="Normal 9 3" xfId="39" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="Normal 9 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="Normal 9 3 3" xfId="143" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="Normal 9 4" xfId="62" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="Normal 9 4 2" xfId="118" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="Normal 9 5" xfId="106" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Normal 10" xfId="13"/>
+    <cellStyle name="Normal 10 2" xfId="28"/>
+    <cellStyle name="Normal 10 2 2" xfId="52"/>
+    <cellStyle name="Normal 10 2 2 2" xfId="97"/>
+    <cellStyle name="Normal 10 2 2 3" xfId="156"/>
+    <cellStyle name="Normal 10 2 3" xfId="75"/>
+    <cellStyle name="Normal 10 2 4" xfId="134"/>
+    <cellStyle name="Normal 10 3" xfId="41"/>
+    <cellStyle name="Normal 10 3 2" xfId="86"/>
+    <cellStyle name="Normal 10 3 3" xfId="145"/>
+    <cellStyle name="Normal 10 4" xfId="64"/>
+    <cellStyle name="Normal 10 4 2" xfId="121"/>
+    <cellStyle name="Normal 10 5" xfId="108"/>
+    <cellStyle name="Normal 11" xfId="14"/>
+    <cellStyle name="Normal 11 2" xfId="29"/>
+    <cellStyle name="Normal 11 2 2" xfId="53"/>
+    <cellStyle name="Normal 11 2 2 2" xfId="98"/>
+    <cellStyle name="Normal 11 2 2 3" xfId="157"/>
+    <cellStyle name="Normal 11 2 3" xfId="76"/>
+    <cellStyle name="Normal 11 2 4" xfId="135"/>
+    <cellStyle name="Normal 11 3" xfId="42"/>
+    <cellStyle name="Normal 11 3 2" xfId="87"/>
+    <cellStyle name="Normal 11 3 3" xfId="146"/>
+    <cellStyle name="Normal 11 4" xfId="65"/>
+    <cellStyle name="Normal 11 4 2" xfId="122"/>
+    <cellStyle name="Normal 11 5" xfId="109"/>
+    <cellStyle name="Normal 12" xfId="17"/>
+    <cellStyle name="Normal 12 2" xfId="32"/>
+    <cellStyle name="Normal 12 2 2" xfId="55"/>
+    <cellStyle name="Normal 12 2 2 2" xfId="100"/>
+    <cellStyle name="Normal 12 2 2 3" xfId="159"/>
+    <cellStyle name="Normal 12 2 3" xfId="78"/>
+    <cellStyle name="Normal 12 2 4" xfId="137"/>
+    <cellStyle name="Normal 12 3" xfId="44"/>
+    <cellStyle name="Normal 12 3 2" xfId="89"/>
+    <cellStyle name="Normal 12 3 3" xfId="148"/>
+    <cellStyle name="Normal 12 4" xfId="67"/>
+    <cellStyle name="Normal 12 4 2" xfId="125"/>
+    <cellStyle name="Normal 12 5" xfId="111"/>
+    <cellStyle name="Normal 13" xfId="57"/>
+    <cellStyle name="Normal 14" xfId="161"/>
+    <cellStyle name="Normal 15" xfId="164"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 3" xfId="4"/>
+    <cellStyle name="Normal 3 2" xfId="11"/>
+    <cellStyle name="Normal 3 2 2" xfId="26"/>
+    <cellStyle name="Normal 3 2 3" xfId="119"/>
+    <cellStyle name="Normal 3 3" xfId="15"/>
+    <cellStyle name="Normal 3 3 2" xfId="30"/>
+    <cellStyle name="Normal 3 3 3" xfId="123"/>
+    <cellStyle name="Normal 3 4" xfId="18"/>
+    <cellStyle name="Normal 3 4 2" xfId="33"/>
+    <cellStyle name="Normal 3 4 3" xfId="126"/>
+    <cellStyle name="Normal 3 5" xfId="21"/>
+    <cellStyle name="Normal 3 6" xfId="114"/>
+    <cellStyle name="Normal 3 7" xfId="162"/>
+    <cellStyle name="Normal 4" xfId="5"/>
+    <cellStyle name="Normal 5" xfId="6"/>
+    <cellStyle name="Normal 6" xfId="7"/>
+    <cellStyle name="Normal 6 10" xfId="165"/>
+    <cellStyle name="Normal 6 11" xfId="103"/>
+    <cellStyle name="Normal 6 2" xfId="9"/>
+    <cellStyle name="Normal 6 2 2" xfId="24"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="49"/>
+    <cellStyle name="Normal 6 2 2 2 2" xfId="94"/>
+    <cellStyle name="Normal 6 2 2 2 3" xfId="153"/>
+    <cellStyle name="Normal 6 2 2 3" xfId="72"/>
+    <cellStyle name="Normal 6 2 2 4" xfId="131"/>
+    <cellStyle name="Normal 6 2 3" xfId="38"/>
+    <cellStyle name="Normal 6 2 3 2" xfId="83"/>
+    <cellStyle name="Normal 6 2 3 3" xfId="142"/>
+    <cellStyle name="Normal 6 2 4" xfId="61"/>
+    <cellStyle name="Normal 6 2 4 2" xfId="117"/>
+    <cellStyle name="Normal 6 2 5" xfId="105"/>
+    <cellStyle name="Normal 6 3" xfId="12"/>
+    <cellStyle name="Normal 6 3 2" xfId="27"/>
+    <cellStyle name="Normal 6 3 2 2" xfId="51"/>
+    <cellStyle name="Normal 6 3 2 2 2" xfId="96"/>
+    <cellStyle name="Normal 6 3 2 2 3" xfId="155"/>
+    <cellStyle name="Normal 6 3 2 3" xfId="74"/>
+    <cellStyle name="Normal 6 3 2 4" xfId="133"/>
+    <cellStyle name="Normal 6 3 3" xfId="40"/>
+    <cellStyle name="Normal 6 3 3 2" xfId="85"/>
+    <cellStyle name="Normal 6 3 3 3" xfId="144"/>
+    <cellStyle name="Normal 6 3 4" xfId="63"/>
+    <cellStyle name="Normal 6 3 4 2" xfId="120"/>
+    <cellStyle name="Normal 6 3 5" xfId="107"/>
+    <cellStyle name="Normal 6 4" xfId="16"/>
+    <cellStyle name="Normal 6 4 2" xfId="31"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="54"/>
+    <cellStyle name="Normal 6 4 2 2 2" xfId="99"/>
+    <cellStyle name="Normal 6 4 2 2 3" xfId="158"/>
+    <cellStyle name="Normal 6 4 2 3" xfId="77"/>
+    <cellStyle name="Normal 6 4 2 4" xfId="136"/>
+    <cellStyle name="Normal 6 4 3" xfId="43"/>
+    <cellStyle name="Normal 6 4 3 2" xfId="88"/>
+    <cellStyle name="Normal 6 4 3 3" xfId="147"/>
+    <cellStyle name="Normal 6 4 4" xfId="66"/>
+    <cellStyle name="Normal 6 4 4 2" xfId="124"/>
+    <cellStyle name="Normal 6 4 5" xfId="110"/>
+    <cellStyle name="Normal 6 5" xfId="19"/>
+    <cellStyle name="Normal 6 5 2" xfId="34"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="56"/>
+    <cellStyle name="Normal 6 5 2 2 2" xfId="101"/>
+    <cellStyle name="Normal 6 5 2 2 3" xfId="160"/>
+    <cellStyle name="Normal 6 5 2 3" xfId="79"/>
+    <cellStyle name="Normal 6 5 2 4" xfId="138"/>
+    <cellStyle name="Normal 6 5 3" xfId="45"/>
+    <cellStyle name="Normal 6 5 3 2" xfId="90"/>
+    <cellStyle name="Normal 6 5 3 3" xfId="149"/>
+    <cellStyle name="Normal 6 5 4" xfId="68"/>
+    <cellStyle name="Normal 6 5 4 2" xfId="127"/>
+    <cellStyle name="Normal 6 5 5" xfId="112"/>
+    <cellStyle name="Normal 6 6" xfId="22"/>
+    <cellStyle name="Normal 6 6 2" xfId="47"/>
+    <cellStyle name="Normal 6 6 2 2" xfId="92"/>
+    <cellStyle name="Normal 6 6 2 3" xfId="151"/>
+    <cellStyle name="Normal 6 6 3" xfId="70"/>
+    <cellStyle name="Normal 6 6 4" xfId="129"/>
+    <cellStyle name="Normal 6 7" xfId="36"/>
+    <cellStyle name="Normal 6 7 2" xfId="81"/>
+    <cellStyle name="Normal 6 7 3" xfId="140"/>
+    <cellStyle name="Normal 6 8" xfId="59"/>
+    <cellStyle name="Normal 6 8 2" xfId="115"/>
+    <cellStyle name="Normal 6 9" xfId="163"/>
+    <cellStyle name="Normal 7" xfId="2"/>
+    <cellStyle name="Normal 7 2" xfId="20"/>
+    <cellStyle name="Normal 7 2 2" xfId="46"/>
+    <cellStyle name="Normal 7 2 2 2" xfId="91"/>
+    <cellStyle name="Normal 7 2 2 3" xfId="150"/>
+    <cellStyle name="Normal 7 2 3" xfId="69"/>
+    <cellStyle name="Normal 7 2 4" xfId="128"/>
+    <cellStyle name="Normal 7 3" xfId="35"/>
+    <cellStyle name="Normal 7 3 2" xfId="80"/>
+    <cellStyle name="Normal 7 3 3" xfId="139"/>
+    <cellStyle name="Normal 7 4" xfId="58"/>
+    <cellStyle name="Normal 7 4 2" xfId="113"/>
+    <cellStyle name="Normal 7 5" xfId="102"/>
+    <cellStyle name="Normal 8" xfId="8"/>
+    <cellStyle name="Normal 8 2" xfId="23"/>
+    <cellStyle name="Normal 8 2 2" xfId="48"/>
+    <cellStyle name="Normal 8 2 2 2" xfId="93"/>
+    <cellStyle name="Normal 8 2 2 3" xfId="152"/>
+    <cellStyle name="Normal 8 2 3" xfId="71"/>
+    <cellStyle name="Normal 8 2 4" xfId="130"/>
+    <cellStyle name="Normal 8 3" xfId="37"/>
+    <cellStyle name="Normal 8 3 2" xfId="82"/>
+    <cellStyle name="Normal 8 3 3" xfId="141"/>
+    <cellStyle name="Normal 8 4" xfId="60"/>
+    <cellStyle name="Normal 8 4 2" xfId="116"/>
+    <cellStyle name="Normal 8 5" xfId="104"/>
+    <cellStyle name="Normal 9" xfId="10"/>
+    <cellStyle name="Normal 9 2" xfId="25"/>
+    <cellStyle name="Normal 9 2 2" xfId="50"/>
+    <cellStyle name="Normal 9 2 2 2" xfId="95"/>
+    <cellStyle name="Normal 9 2 2 3" xfId="154"/>
+    <cellStyle name="Normal 9 2 3" xfId="73"/>
+    <cellStyle name="Normal 9 2 4" xfId="132"/>
+    <cellStyle name="Normal 9 3" xfId="39"/>
+    <cellStyle name="Normal 9 3 2" xfId="84"/>
+    <cellStyle name="Normal 9 3 3" xfId="143"/>
+    <cellStyle name="Normal 9 4" xfId="62"/>
+    <cellStyle name="Normal 9 4 2" xfId="118"/>
+    <cellStyle name="Normal 9 5" xfId="106"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2249,7 +2249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2282,26 +2282,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2334,23 +2317,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2526,7 +2492,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2536,14 +2502,14 @@
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="19"/>
-    <col min="2" max="2" width="43.5" style="3"/>
-    <col min="3" max="1025" width="8.5"/>
+    <col min="1" max="1" width="21.42578125" style="19"/>
+    <col min="2" max="2" width="43.42578125" style="3"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -2551,7 +2517,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
@@ -2559,7 +2525,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>2</v>
       </c>
@@ -2567,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
@@ -2575,25 +2541,25 @@
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
@@ -2601,7 +2567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>9</v>
       </c>
@@ -2610,35 +2576,35 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:B9"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AME15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="4"/>
-    <col min="2" max="2" width="33.83203125" style="4"/>
-    <col min="3" max="3" width="16.5" style="9"/>
+    <col min="1" max="1" width="20.28515625" style="4"/>
+    <col min="2" max="2" width="33.85546875" style="4"/>
+    <col min="3" max="3" width="16.42578125" style="9"/>
     <col min="4" max="4" width="17" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="1019" width="9.1640625" style="3"/>
-    <col min="1022" max="1024" width="8.6640625"/>
+    <col min="5" max="5" width="25.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="1019" width="9.140625" style="3"/>
+    <col min="1022" max="1024" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2664,7 +2630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>193</v>
       </c>
@@ -2681,7 +2647,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>227</v>
       </c>
@@ -2698,7 +2664,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>205</v>
       </c>
@@ -2715,24 +2681,24 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F719" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
+  <autoFilter ref="A1:F719"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -2743,26 +2709,26 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMD5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" style="86" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" style="86" customWidth="1"/>
     <col min="3" max="4" width="9" style="86"/>
-    <col min="5" max="5" width="30.6640625" style="86" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" style="68" customWidth="1"/>
-    <col min="7" max="9" width="15.6640625" style="86" customWidth="1"/>
-    <col min="10" max="1018" width="8.5" style="86"/>
-    <col min="1019" max="1021" width="8.5" style="85"/>
+    <col min="5" max="5" width="30.7109375" style="86" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="68" customWidth="1"/>
+    <col min="7" max="9" width="15.7109375" style="86" customWidth="1"/>
+    <col min="10" max="1018" width="8.42578125" style="86"/>
+    <col min="1019" max="1021" width="8.42578125" style="85"/>
     <col min="1022" max="16384" width="9" style="85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
         <v>241</v>
       </c>
@@ -2791,7 +2757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="84" t="s">
         <v>244</v>
       </c>
@@ -2811,7 +2777,7 @@
       </c>
       <c r="I2" s="84"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="84" t="s">
         <v>247</v>
       </c>
@@ -2829,7 +2795,7 @@
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="84" t="s">
         <v>248</v>
       </c>
@@ -2847,7 +2813,7 @@
       <c r="H4" s="84"/>
       <c r="I4" s="84"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="84" t="s">
         <v>249</v>
       </c>
@@ -2865,14 +2831,14 @@
       <c r="I5" s="84"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G221" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
+  <autoFilter ref="A1:G221"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2882,16 +2848,16 @@
       <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="5" customWidth="1"/>
-    <col min="3" max="4" width="15.6640625" style="5" customWidth="1"/>
-    <col min="5" max="8" width="20.6640625" style="5" customWidth="1"/>
-    <col min="9" max="1026" width="8.5" style="5"/>
+    <col min="1" max="1" width="20.7109375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="5" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" style="5" customWidth="1"/>
+    <col min="5" max="8" width="20.7109375" style="5" customWidth="1"/>
+    <col min="9" max="1026" width="8.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="67" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="67" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
@@ -2917,7 +2883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
         <v>381</v>
       </c>
@@ -2937,7 +2903,7 @@
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
     </row>
-    <row r="3" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
         <v>382</v>
       </c>
@@ -2957,7 +2923,7 @@
       </c>
       <c r="H3" s="30"/>
     </row>
-    <row r="4" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="68" t="s">
         <v>383</v>
       </c>
@@ -2975,7 +2941,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
     </row>
-    <row r="5" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>384</v>
       </c>
@@ -2993,7 +2959,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
     </row>
-    <row r="6" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="68" t="s">
         <v>385</v>
       </c>
@@ -3011,7 +2977,7 @@
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
     </row>
-    <row r="7" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="68" t="s">
         <v>386</v>
       </c>
@@ -3029,7 +2995,7 @@
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
     </row>
-    <row r="8" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="68" t="s">
         <v>387</v>
       </c>
@@ -3047,7 +3013,7 @@
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
     </row>
-    <row r="9" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="68" t="s">
         <v>388</v>
       </c>
@@ -3065,7 +3031,7 @@
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
     </row>
-    <row r="10" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="68" t="s">
         <v>389</v>
       </c>
@@ -3083,7 +3049,7 @@
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
     </row>
-    <row r="11" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="68" t="s">
         <v>390</v>
       </c>
@@ -3101,7 +3067,7 @@
       <c r="G11" s="30"/>
       <c r="H11" s="30"/>
     </row>
-    <row r="12" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="68" t="s">
         <v>391</v>
       </c>
@@ -3119,7 +3085,7 @@
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="68" t="s">
         <v>392</v>
       </c>
@@ -3137,7 +3103,7 @@
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="68" t="s">
         <v>393</v>
       </c>
@@ -3155,7 +3121,7 @@
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="68" t="s">
         <v>394</v>
       </c>
@@ -3173,7 +3139,7 @@
       <c r="G15" s="30"/>
       <c r="H15" s="30"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="68" t="s">
         <v>395</v>
       </c>
@@ -3198,23 +3164,23 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="3" width="20.6640625" style="29" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="6" width="20.6640625" style="29" customWidth="1"/>
-    <col min="7" max="10" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" style="29" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="29" customWidth="1"/>
+    <col min="7" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -3246,7 +3212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>352</v>
       </c>
@@ -3271,7 +3237,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>353</v>
       </c>
@@ -3295,7 +3261,7 @@
       <c r="J3" s="22"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>354</v>
       </c>
@@ -3319,7 +3285,7 @@
       <c r="J4" s="22"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>355</v>
       </c>
@@ -3343,7 +3309,7 @@
       <c r="J5" s="22"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="40"/>
       <c r="D6" s="22"/>
       <c r="E6" s="40"/>
@@ -3353,7 +3319,7 @@
       <c r="J6" s="22"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40"/>
@@ -3366,7 +3332,7 @@
       <c r="J7" s="22"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
@@ -3379,7 +3345,7 @@
       <c r="J8" s="22"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
@@ -3397,21 +3363,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16"/>
-    <col min="3" max="3" width="15.5"/>
-    <col min="6" max="6" width="11.1640625"/>
+    <col min="3" max="3" width="15.42578125"/>
+    <col min="6" max="6" width="11.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3434,7 +3400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -3456,24 +3422,24 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="20.6640625" style="33" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" style="33" customWidth="1"/>
-    <col min="6" max="11" width="15.6640625" style="33" customWidth="1"/>
-    <col min="12" max="14" width="20.6640625" style="33" customWidth="1"/>
-    <col min="15" max="16384" width="18.6640625" style="33"/>
+    <col min="1" max="3" width="20.7109375" style="33" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="33" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="33" customWidth="1"/>
+    <col min="6" max="11" width="15.7109375" style="33" customWidth="1"/>
+    <col min="12" max="14" width="20.7109375" style="33" customWidth="1"/>
+    <col min="15" max="16384" width="18.7109375" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -3517,7 +3483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
         <v>277</v>
       </c>
@@ -3543,7 +3509,7 @@
       <c r="M2" s="42"/>
       <c r="N2" s="42"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
         <v>280</v>
       </c>
@@ -3569,7 +3535,7 @@
       <c r="M3" s="42"/>
       <c r="N3" s="42"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>283</v>
       </c>
@@ -3595,7 +3561,7 @@
       <c r="M4" s="42"/>
       <c r="N4" s="42"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="42" t="s">
         <v>286</v>
       </c>
@@ -3621,7 +3587,7 @@
       <c r="M5" s="42"/>
       <c r="N5" s="42"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
         <v>31</v>
       </c>
@@ -3647,7 +3613,7 @@
       <c r="M6" s="42"/>
       <c r="N6" s="42"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>290</v>
       </c>
@@ -3673,7 +3639,7 @@
       <c r="M7" s="42"/>
       <c r="N7" s="42"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="42" t="s">
         <v>293</v>
       </c>
@@ -3700,7 +3666,7 @@
       <c r="N8" s="42"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L220" xr:uid="{00000000-0009-0000-0000-00000E000000}"/>
+  <autoFilter ref="A1:L220"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -3711,7 +3677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3721,17 +3687,17 @@
       <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" style="41" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="80" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="41" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="52" customWidth="1"/>
-    <col min="6" max="8" width="20.6640625" style="41" customWidth="1"/>
-    <col min="9" max="1024" width="8.6640625" style="2"/>
+    <col min="1" max="2" width="20.7109375" style="41" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="80" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="41" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="52" customWidth="1"/>
+    <col min="6" max="8" width="20.7109375" style="41" customWidth="1"/>
+    <col min="9" max="1024" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>241</v>
       </c>
@@ -4773,7 +4739,7 @@
       <c r="AMI1" s="50"/>
       <c r="AMJ1" s="50"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>295</v>
       </c>
@@ -4792,7 +4758,7 @@
       <c r="F2" s="33"/>
       <c r="H2" s="33"/>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>298</v>
       </c>
@@ -4813,7 +4779,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>301</v>
       </c>
@@ -4834,7 +4800,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>304</v>
       </c>
@@ -4855,7 +4821,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>306</v>
       </c>
@@ -4876,7 +4842,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>309</v>
       </c>
@@ -4894,7 +4860,7 @@
       </c>
       <c r="F7" s="33"/>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>311</v>
       </c>
@@ -4914,7 +4880,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>314</v>
       </c>
@@ -4935,29 +4901,29 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F9" xr:uid="{00000000-0009-0000-0000-00000F000000}"/>
+  <autoFilter ref="A1:F9"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="20.6640625" style="33" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" style="27" customWidth="1"/>
-    <col min="6" max="9" width="20.6640625" style="33" customWidth="1"/>
-    <col min="10" max="1025" width="8.5"/>
+    <col min="1" max="3" width="20.7109375" style="33" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" style="27" customWidth="1"/>
+    <col min="6" max="9" width="20.7109375" style="33" customWidth="1"/>
+    <col min="10" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -4986,7 +4952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>317</v>
       </c>
@@ -5003,7 +4969,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>321</v>
       </c>
@@ -5020,7 +4986,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>324</v>
       </c>
@@ -5037,7 +5003,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>326</v>
       </c>
@@ -5054,7 +5020,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>297</v>
       </c>
@@ -5068,7 +5034,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>330</v>
       </c>
@@ -5082,7 +5048,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>333</v>
       </c>
@@ -5096,7 +5062,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>336</v>
       </c>
@@ -5110,7 +5076,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>339</v>
       </c>
@@ -5124,7 +5090,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -5137,20 +5103,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="20.6640625" customWidth="1"/>
-    <col min="1020" max="1024" width="8.6640625"/>
+    <col min="1" max="10" width="20.7109375" customWidth="1"/>
+    <col min="1020" max="1024" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
@@ -5193,19 +5159,19 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="20.6640625" customWidth="1"/>
+    <col min="1" max="13" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
         <v>241</v>
       </c>
@@ -5246,7 +5212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F15" s="34"/>
     </row>
   </sheetData>
@@ -5255,7 +5221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5265,14 +5231,14 @@
       <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="56" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="26" customWidth="1"/>
-    <col min="3" max="1025" width="8.5"/>
+    <col min="1" max="1" width="30.7109375" style="56" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="26" customWidth="1"/>
+    <col min="3" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -5280,7 +5246,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>1</v>
       </c>
@@ -5288,7 +5254,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>10</v>
       </c>
@@ -5296,7 +5262,7 @@
         <v>9606</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>9</v>
       </c>
@@ -5305,30 +5271,30 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:B4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="27" customWidth="1"/>
-    <col min="4" max="12" width="20.6640625" style="33" customWidth="1"/>
-    <col min="13" max="1025" width="8.5" style="33"/>
+    <col min="1" max="2" width="20.7109375" style="33" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="27" customWidth="1"/>
+    <col min="4" max="12" width="20.7109375" style="33" customWidth="1"/>
+    <col min="13" max="1025" width="8.42578125" style="33"/>
     <col min="1026" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
@@ -5366,7 +5332,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
         <v>246</v>
       </c>
@@ -5374,7 +5340,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
         <v>258</v>
       </c>
@@ -5382,7 +5348,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
         <v>342</v>
       </c>
@@ -5397,22 +5363,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="20" customWidth="1"/>
-    <col min="2" max="6" width="20.6640625" style="3" customWidth="1"/>
-    <col min="8" max="1020" width="9.1640625" style="3"/>
-    <col min="1024" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="20.7109375" style="20" customWidth="1"/>
+    <col min="2" max="6" width="20.7109375" style="3" customWidth="1"/>
+    <col min="8" max="1020" width="9.140625" style="3"/>
+    <col min="1024" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5432,7 +5398,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>14</v>
       </c>
@@ -5449,7 +5415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>18</v>
       </c>
@@ -5461,7 +5427,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
@@ -5475,7 +5441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>23</v>
       </c>
@@ -5494,24 +5460,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="6" customWidth="1"/>
-    <col min="3" max="6" width="20.6640625" style="3" customWidth="1"/>
-    <col min="7" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.5"/>
+    <col min="1" max="1" width="20.7109375" style="20" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="6" customWidth="1"/>
+    <col min="3" max="6" width="20.7109375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5540,7 +5506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
@@ -5558,7 +5524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>50</v>
       </c>
@@ -5575,7 +5541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>51</v>
       </c>
@@ -5592,7 +5558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>52</v>
       </c>
@@ -5609,7 +5575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>53</v>
       </c>
@@ -5626,7 +5592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>54</v>
       </c>
@@ -5643,7 +5609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>55</v>
       </c>
@@ -5660,7 +5626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>56</v>
       </c>
@@ -5677,7 +5643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>57</v>
       </c>
@@ -5694,7 +5660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>58</v>
       </c>
@@ -5711,7 +5677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>59</v>
       </c>
@@ -5728,7 +5694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>60</v>
       </c>
@@ -5745,7 +5711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>61</v>
       </c>
@@ -5762,7 +5728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>62</v>
       </c>
@@ -5779,7 +5745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>63</v>
       </c>
@@ -5796,7 +5762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>64</v>
       </c>
@@ -5813,7 +5779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>65</v>
       </c>
@@ -5830,7 +5796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>66</v>
       </c>
@@ -5847,7 +5813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>67</v>
       </c>
@@ -5864,7 +5830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>68</v>
       </c>
@@ -5881,7 +5847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>69</v>
       </c>
@@ -5898,7 +5864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>70</v>
       </c>
@@ -5915,7 +5881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>71</v>
       </c>
@@ -5932,7 +5898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>72</v>
       </c>
@@ -5949,7 +5915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>400</v>
       </c>
@@ -5977,33 +5943,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="50.5" style="6"/>
+    <col min="1" max="1" width="9.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" style="6"/>
     <col min="5" max="5" width="9" style="31"/>
-    <col min="6" max="6" width="18.5" style="6" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="6" customWidth="1"/>
     <col min="7" max="7" width="10" style="6" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="6" customWidth="1"/>
     <col min="9" max="9" width="9" style="9"/>
-    <col min="10" max="10" width="13.5" style="17"/>
+    <col min="10" max="10" width="13.42578125" style="17"/>
     <col min="11" max="11" width="9" style="16"/>
-    <col min="12" max="13" width="9.1640625" style="6"/>
-    <col min="14" max="1021" width="9.1640625" style="17"/>
-    <col min="1022" max="1024" width="8.5"/>
-    <col min="1025" max="1030" width="8.6640625"/>
+    <col min="12" max="13" width="9.140625" style="6"/>
+    <col min="14" max="1021" width="9.140625" style="17"/>
+    <col min="1022" max="1024" width="8.42578125"/>
+    <col min="1025" max="1030" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6038,7 +6004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>197</v>
       </c>
@@ -6065,7 +6031,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>200</v>
       </c>
@@ -6092,7 +6058,7 @@
       <c r="M3" s="8"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>203</v>
       </c>
@@ -6118,7 +6084,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>206</v>
       </c>
@@ -6145,7 +6111,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I849" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:I849"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -6156,25 +6122,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="8" max="8" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -6203,7 +6169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>234</v>
       </c>
@@ -6221,7 +6187,7 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>237</v>
       </c>
@@ -6239,7 +6205,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>239</v>
       </c>
@@ -6263,29 +6229,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="74"/>
+    <col min="1" max="1" width="17.42578125" style="74"/>
     <col min="2" max="3" width="9" style="74"/>
-    <col min="4" max="4" width="10.5" style="74" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="74" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="74"/>
-    <col min="7" max="9" width="13.5" style="74"/>
-    <col min="10" max="11" width="20.6640625" style="73" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" style="77" customWidth="1"/>
-    <col min="13" max="1023" width="32.5" style="73"/>
-    <col min="1024" max="1025" width="8.5" style="78"/>
+    <col min="4" max="4" width="10.42578125" style="74" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="74" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="74"/>
+    <col min="7" max="9" width="13.42578125" style="74"/>
+    <col min="10" max="11" width="20.7109375" style="73" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="77" customWidth="1"/>
+    <col min="13" max="1023" width="32.42578125" style="73"/>
+    <col min="1024" max="1025" width="8.42578125" style="78"/>
     <col min="1026" max="16384" width="9" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" s="71" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1023" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
@@ -6329,7 +6295,7 @@
       <c r="AMH1" s="73"/>
       <c r="AMI1" s="73"/>
     </row>
-    <row r="2" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
         <v>79</v>
       </c>
@@ -6353,7 +6319,7 @@
         <v>20651511</v>
       </c>
     </row>
-    <row r="3" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>82</v>
       </c>
@@ -6377,7 +6343,7 @@
         <v>10448504</v>
       </c>
     </row>
-    <row r="4" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
         <v>85</v>
       </c>
@@ -6401,7 +6367,7 @@
         <v>69387254</v>
       </c>
     </row>
-    <row r="5" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A5" s="74" t="s">
         <v>88</v>
       </c>
@@ -6425,7 +6391,7 @@
         <v>40574685</v>
       </c>
     </row>
-    <row r="6" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
         <v>91</v>
       </c>
@@ -6449,7 +6415,7 @@
         <v>112649530</v>
       </c>
     </row>
-    <row r="7" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
         <v>94</v>
       </c>
@@ -6473,7 +6439,7 @@
         <v>83605875</v>
       </c>
     </row>
-    <row r="8" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
         <v>97</v>
       </c>
@@ -6497,7 +6463,7 @@
         <v>127899195</v>
       </c>
     </row>
-    <row r="9" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
         <v>100</v>
       </c>
@@ -6521,7 +6487,7 @@
         <v>160421711</v>
       </c>
     </row>
-    <row r="10" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
         <v>103</v>
       </c>
@@ -6545,7 +6511,7 @@
         <v>152129619</v>
       </c>
     </row>
-    <row r="11" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
         <v>106</v>
       </c>
@@ -6569,7 +6535,7 @@
         <v>56051604</v>
       </c>
     </row>
-    <row r="12" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>109</v>
       </c>
@@ -6593,7 +6559,7 @@
         <v>18084998</v>
       </c>
     </row>
-    <row r="13" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
         <v>112</v>
       </c>
@@ -6617,7 +6583,7 @@
         <v>19967258</v>
       </c>
     </row>
-    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1023" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
         <v>115</v>
       </c>
@@ -6641,7 +6607,7 @@
         <v>136423761</v>
       </c>
     </row>
-    <row r="15" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
         <v>118</v>
       </c>
@@ -6665,7 +6631,7 @@
         <v>7787981</v>
       </c>
     </row>
-    <row r="16" spans="1:1023" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1023" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
         <v>121</v>
       </c>
@@ -6689,7 +6655,7 @@
         <v>133421307</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
         <v>124</v>
       </c>
@@ -6713,7 +6679,7 @@
         <v>13732346</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
         <v>127</v>
       </c>
@@ -6737,7 +6703,7 @@
         <v>114450279</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
         <v>130</v>
       </c>
@@ -6761,7 +6727,7 @@
         <v>77065580</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
         <v>133</v>
       </c>
@@ -6785,7 +6751,7 @@
         <v>113359493</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
         <v>136</v>
       </c>
@@ -6809,7 +6775,7 @@
         <v>52476628</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="74" t="s">
         <v>139</v>
       </c>
@@ -6833,7 +6799,7 @@
         <v>103057462</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="74" t="s">
         <v>142</v>
       </c>
@@ -6857,7 +6823,7 @@
         <v>65578352</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="74" t="s">
         <v>145</v>
       </c>
@@ -6881,7 +6847,7 @@
         <v>101251932</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="74" t="s">
         <v>148</v>
       </c>
@@ -6905,7 +6871,7 @@
         <v>89155846</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="74" t="s">
         <v>151</v>
       </c>
@@ -6929,7 +6895,7 @@
         <v>49223225</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="74" t="s">
         <v>154</v>
       </c>
@@ -6953,7 +6919,7 @@
         <v>50988121</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="74" t="s">
         <v>157</v>
       </c>
@@ -6977,7 +6943,7 @@
         <v>41440717</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="74" t="s">
         <v>160</v>
       </c>
@@ -7001,7 +6967,7 @@
         <v>47784686</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
         <v>163</v>
       </c>
@@ -7025,7 +6991,7 @@
         <v>13638940</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="s">
         <v>166</v>
       </c>
@@ -7049,7 +7015,7 @@
         <v>44652233</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="74" t="s">
         <v>169</v>
       </c>
@@ -7073,7 +7039,7 @@
         <v>31668931</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="74" t="s">
         <v>172</v>
       </c>
@@ -7097,7 +7063,7 @@
         <v>20859417</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
         <v>175</v>
       </c>
@@ -7121,7 +7087,7 @@
         <v>38738299</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="74" t="s">
         <v>178</v>
       </c>
@@ -7145,7 +7111,7 @@
         <v>119605895</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="74" t="s">
         <v>181</v>
       </c>
@@ -7169,7 +7135,7 @@
         <v>23005465</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="74" t="s">
         <v>184</v>
       </c>
@@ -7194,7 +7160,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:I1064" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
+  <autoFilter ref="F1:I1064"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -7205,23 +7171,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMG9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="20.6640625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="40" customWidth="1"/>
-    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="22" customWidth="1"/>
-    <col min="8" max="1021" width="9.1640625" style="3"/>
+    <col min="1" max="3" width="20.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="40" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="22" customWidth="1"/>
+    <col min="8" max="1021" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7244,7 +7210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -7252,7 +7218,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -7260,7 +7226,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -7268,7 +7234,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -7276,7 +7242,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>34</v>
       </c>
@@ -7284,7 +7250,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>37</v>
       </c>
@@ -7292,7 +7258,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>40</v>
       </c>
@@ -7300,7 +7266,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>42</v>
       </c>
@@ -7319,26 +7285,27 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="1023" width="8.5"/>
+    <col min="5" max="5" width="16.5703125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="1024" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -7351,17 +7318,20 @@
       <c r="D1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="81" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>209</v>
       </c>
@@ -7374,8 +7344,11 @@
       <c r="D2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E2" s="25" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -7388,8 +7361,11 @@
       <c r="D3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E3" s="25" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -7402,8 +7378,11 @@
       <c r="D4" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4" s="25" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>218</v>
       </c>
@@ -7416,12 +7395,15 @@
       <c r="D5" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E20" s="14"/>
+      <c r="E5" s="25" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Rename abundance_ratio attribute in PTM to fractional_abundance
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="4815" windowWidth="24975" windowHeight="5325" tabRatio="993" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="1365" yWindow="4815" windowWidth="24975" windowHeight="5325" tabRatio="993" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -774,9 +774,6 @@
     <t>Modified residue</t>
   </si>
   <si>
-    <t>Abundance ratio</t>
-  </si>
-  <si>
     <t>ENSP00000355428_1</t>
   </si>
   <si>
@@ -1315,6 +1312,9 @@
   </si>
   <si>
     <t>WC:string</t>
+  </si>
+  <si>
+    <t>Fractional abundance</t>
   </si>
 </sst>
 </file>
@@ -2511,7 +2511,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2519,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2569,7 +2569,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -2601,22 +2601,22 @@
   <sheetData>
     <row r="1" spans="1:9" s="56" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="86" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B1" s="86" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="86" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D1" s="86" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="86" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="86" t="s">
         <v>242</v>
-      </c>
-      <c r="F1" s="86" t="s">
-        <v>243</v>
       </c>
       <c r="G1" s="86" t="s">
         <v>13</v>
@@ -2630,36 +2630,36 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="87" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="87" t="s">
         <v>244</v>
-      </c>
-      <c r="B2" s="87" t="s">
-        <v>245</v>
       </c>
       <c r="C2" s="87"/>
       <c r="D2" s="87"/>
       <c r="E2" s="84" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F2" s="83" t="s">
         <v>193</v>
       </c>
       <c r="G2" s="71"/>
       <c r="H2" s="87" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I2" s="87"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="87" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B3" s="87" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C3" s="87"/>
       <c r="D3" s="87"/>
       <c r="E3" s="84" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F3" s="83" t="s">
         <v>227</v>
@@ -2670,18 +2670,18 @@
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="87" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C4" s="87"/>
       <c r="D4" s="87"/>
       <c r="E4" s="84" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F4" s="83" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G4" s="71"/>
       <c r="H4" s="87"/>
@@ -2689,18 +2689,18 @@
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="87" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B5" s="87" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C5" s="71"/>
       <c r="D5" s="87"/>
       <c r="E5" s="84" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F5" s="83" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G5" s="71"/>
       <c r="H5" s="87"/>
@@ -2738,7 +2738,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>75</v>
@@ -2849,22 +2849,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>351</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>352</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="46" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="46" t="s">
         <v>353</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="F1" s="46" t="s">
         <v>251</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>354</v>
-      </c>
-      <c r="F1" s="46" t="s">
-        <v>252</v>
-      </c>
-      <c r="G1" s="45" t="s">
-        <v>355</v>
       </c>
       <c r="H1" s="45" t="s">
         <v>13</v>
@@ -2878,22 +2878,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="80" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
@@ -2903,22 +2903,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="80" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
@@ -2927,22 +2927,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B4" s="39" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>39</v>
       </c>
       <c r="E4" s="80" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
@@ -2951,22 +2951,22 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B5" s="39" t="s">
         <v>42</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="80" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="32"/>
@@ -3051,16 +3051,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="56" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="D1" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="D1" s="56" t="s">
-        <v>252</v>
-      </c>
       <c r="E1" s="56" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F1" s="56" t="s">
         <v>13</v>
@@ -3074,56 +3074,56 @@
     </row>
     <row r="2" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2" s="30">
         <v>1</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="67" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C3" s="30">
         <v>1</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
       <c r="G3" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C4" s="30">
         <v>1</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
@@ -3132,16 +3132,16 @@
     </row>
     <row r="5" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C5" s="30">
         <v>1</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
@@ -3150,16 +3150,16 @@
     </row>
     <row r="6" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="67" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C6" s="30">
         <v>0.25</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
@@ -3168,16 +3168,16 @@
     </row>
     <row r="7" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="67" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C7" s="30">
         <v>0.25</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -3186,16 +3186,16 @@
     </row>
     <row r="8" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="67" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C8" s="30">
         <v>0.25</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -3204,16 +3204,16 @@
     </row>
     <row r="9" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="67" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C9" s="30">
         <v>0.25</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
@@ -3222,16 +3222,16 @@
     </row>
     <row r="10" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B10" s="69" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C10" s="30">
         <v>0.5</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
@@ -3240,16 +3240,16 @@
     </row>
     <row r="11" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="67" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B11" s="69" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C11" s="30">
         <v>0.5</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
@@ -3258,16 +3258,16 @@
     </row>
     <row r="12" spans="1:8" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="67" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C12" s="30">
         <v>0.5</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
@@ -3276,16 +3276,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="67" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C13" s="30">
         <v>0.1</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>
@@ -3294,16 +3294,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="67" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C14" s="30">
         <v>0.36</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
@@ -3312,16 +3312,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C15" s="30">
         <v>0.5</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
@@ -3330,16 +3330,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="67" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C16" s="30">
         <v>0.25</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
@@ -3375,10 +3375,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
@@ -3392,10 +3392,10 @@
     </row>
     <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>273</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>274</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -3437,31 +3437,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D1" s="54" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="53" t="s">
+        <v>274</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>393</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>374</v>
+      </c>
+      <c r="H1" s="54" t="s">
         <v>275</v>
       </c>
-      <c r="F1" s="53" t="s">
-        <v>394</v>
-      </c>
-      <c r="G1" s="53" t="s">
-        <v>375</v>
-      </c>
-      <c r="H1" s="54" t="s">
-        <v>276</v>
-      </c>
       <c r="I1" s="54" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J1" s="53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K1" s="54" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L1" s="54" t="s">
         <v>13</v>
@@ -3475,15 +3475,15 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>277</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>278</v>
       </c>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
       <c r="E2" s="41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
@@ -3501,15 +3501,15 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>280</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>281</v>
       </c>
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
       <c r="E3" s="41" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
@@ -3527,15 +3527,15 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>283</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>284</v>
       </c>
       <c r="C4" s="41"/>
       <c r="D4" s="41"/>
       <c r="E4" s="41" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
@@ -3553,15 +3553,15 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>286</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>287</v>
       </c>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
       <c r="E5" s="41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
@@ -3587,7 +3587,7 @@
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
       <c r="E6" s="41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
@@ -3605,15 +3605,15 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>290</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>291</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
       <c r="E7" s="41" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="41"/>
@@ -3631,15 +3631,15 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F8" s="41"/>
       <c r="G8" s="41"/>
@@ -3689,19 +3689,19 @@
   <sheetData>
     <row r="1" spans="1:1024" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C1" s="76" t="s">
         <v>196</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F1" s="48" t="s">
         <v>13</v>
@@ -4731,16 +4731,16 @@
     </row>
     <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" s="77" t="s">
         <v>295</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="C2" s="77" t="s">
+      <c r="D2" s="40" t="s">
         <v>296</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>297</v>
       </c>
       <c r="E2" s="27">
         <v>1</v>
@@ -4750,100 +4750,100 @@
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>295</v>
+      </c>
+      <c r="D3" s="43" t="s">
         <v>298</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>280</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>296</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>299</v>
       </c>
       <c r="E3" s="27">
         <v>1</v>
       </c>
       <c r="F3" s="33"/>
       <c r="H3" s="40" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="C4" s="77" t="s">
+        <v>295</v>
+      </c>
+      <c r="D4" s="40" t="s">
         <v>301</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>283</v>
-      </c>
-      <c r="C4" s="77" t="s">
-        <v>296</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>302</v>
       </c>
       <c r="E4" s="27">
         <v>1</v>
       </c>
       <c r="F4" s="33"/>
       <c r="H4" s="40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C5" s="77" t="s">
+        <v>295</v>
+      </c>
+      <c r="D5" s="40" t="s">
         <v>296</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>297</v>
       </c>
       <c r="E5" s="27">
         <v>1</v>
       </c>
       <c r="F5" s="33"/>
       <c r="H5" s="40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B6" s="40" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="77" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E6" s="27">
         <v>1</v>
       </c>
       <c r="F6" s="33"/>
       <c r="H6" s="40" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="77" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E7" s="27">
         <v>1</v>
@@ -4852,42 +4852,42 @@
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
+        <v>310</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="C8" s="77" t="s">
+        <v>295</v>
+      </c>
+      <c r="D8" s="40" t="s">
         <v>311</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>290</v>
-      </c>
-      <c r="C8" s="77" t="s">
-        <v>296</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>312</v>
       </c>
       <c r="E8" s="27">
         <v>1</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
+        <v>313</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" s="77" t="s">
+        <v>295</v>
+      </c>
+      <c r="D9" s="40" t="s">
         <v>314</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>293</v>
-      </c>
-      <c r="C9" s="77" t="s">
-        <v>296</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>315</v>
       </c>
       <c r="E9" s="27">
         <v>1</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -4921,16 +4921,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D1" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>251</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>252</v>
-      </c>
       <c r="F1" s="37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>13</v>
@@ -4944,140 +4944,140 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>317</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>318</v>
       </c>
       <c r="D2" s="27">
         <v>20.5</v>
       </c>
       <c r="E2" s="27" t="s">
+        <v>318</v>
+      </c>
+      <c r="G2" s="33" t="s">
         <v>319</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>321</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>322</v>
       </c>
       <c r="D3" s="27">
         <v>1.35</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="B4" s="33" t="s">
         <v>324</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>325</v>
       </c>
       <c r="D4" s="27">
         <v>0.46</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="B5" s="33" t="s">
         <v>326</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>327</v>
       </c>
       <c r="D5" s="27">
         <v>1.2</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D6" s="27">
         <v>2.1</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>329</v>
+      </c>
+      <c r="B7" t="s">
         <v>330</v>
-      </c>
-      <c r="B7" t="s">
-        <v>331</v>
       </c>
       <c r="D7" s="52">
         <v>3.0000000000000001E-12</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>332</v>
+      </c>
+      <c r="B8" t="s">
         <v>333</v>
-      </c>
-      <c r="B8" t="s">
-        <v>334</v>
       </c>
       <c r="D8" s="52">
         <v>10000000</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>335</v>
+      </c>
+      <c r="B9" t="s">
         <v>336</v>
-      </c>
-      <c r="B9" t="s">
-        <v>337</v>
       </c>
       <c r="D9" s="29">
         <v>0.7</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>338</v>
+      </c>
+      <c r="B10" t="s">
         <v>339</v>
-      </c>
-      <c r="B10" t="s">
-        <v>340</v>
       </c>
       <c r="D10" s="29">
         <v>71280</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -5111,22 +5111,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C1" s="59" t="s">
+        <v>358</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="F1" s="59" t="s">
+        <v>251</v>
+      </c>
+      <c r="G1" s="59" t="s">
         <v>359</v>
-      </c>
-      <c r="D1" s="59" t="s">
-        <v>353</v>
-      </c>
-      <c r="E1" s="59" t="s">
-        <v>251</v>
-      </c>
-      <c r="F1" s="59" t="s">
-        <v>252</v>
-      </c>
-      <c r="G1" s="59" t="s">
-        <v>360</v>
       </c>
       <c r="H1" s="60" t="s">
         <v>13</v>
@@ -5163,34 +5163,34 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B1" s="58" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1" s="58" t="s">
         <v>361</v>
       </c>
-      <c r="C1" s="58" t="s">
-        <v>392</v>
-      </c>
-      <c r="D1" s="58" t="s">
+      <c r="E1" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1" s="58" t="s">
         <v>362</v>
       </c>
-      <c r="E1" s="58" t="s">
-        <v>250</v>
-      </c>
-      <c r="F1" s="58" t="s">
+      <c r="G1" s="58" t="s">
         <v>363</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="H1" s="58" t="s">
         <v>364</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="I1" s="58" t="s">
         <v>365</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="J1" s="58" t="s">
         <v>366</v>
-      </c>
-      <c r="J1" s="58" t="s">
-        <v>367</v>
       </c>
       <c r="K1" s="58" t="s">
         <v>13</v>
@@ -5233,7 +5233,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5257,7 +5257,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -5295,25 +5295,25 @@
         <v>75</v>
       </c>
       <c r="D1" s="61" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1" s="63" t="s">
         <v>368</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="F1" s="61" t="s">
         <v>369</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="G1" s="63" t="s">
         <v>370</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="H1" s="63" t="s">
         <v>371</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="I1" s="64" t="s">
         <v>372</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="J1" s="61" t="s">
         <v>373</v>
-      </c>
-      <c r="J1" s="61" t="s">
-        <v>374</v>
       </c>
       <c r="K1" s="62" t="s">
         <v>13</v>
@@ -5324,26 +5324,26 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C2" s="79" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -5907,10 +5907,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D26" s="6">
         <v>0</v>
@@ -5963,13 +5963,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D1" s="70" t="s">
         <v>74</v>
       </c>
       <c r="E1" s="70" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F1" s="70" t="s">
         <v>73</v>
@@ -6886,7 +6886,7 @@
         <v>186</v>
       </c>
       <c r="F37" s="72" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G37" s="85" t="s">
         <v>199</v>
@@ -6914,7 +6914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -6948,7 +6948,7 @@
         <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E1" s="78" t="s">
         <v>187</v>
@@ -6990,10 +6990,10 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -7017,10 +7017,10 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -7046,10 +7046,10 @@
         <v>205</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -7072,10 +7072,10 @@
         <v>205</v>
       </c>
       <c r="G5" s="31" t="s">
+        <v>399</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>400</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -7150,7 +7150,7 @@
         <v>211</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -7167,7 +7167,7 @@
         <v>214</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -7184,7 +7184,7 @@
         <v>217</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -7201,7 +7201,7 @@
         <v>220</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">
@@ -7346,8 +7346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7357,7 +7357,7 @@
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7378,7 +7378,7 @@
         <v>232</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>233</v>
+        <v>413</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
@@ -7392,16 +7392,16 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C2" t="s">
         <v>227</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>235</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>236</v>
       </c>
       <c r="F2">
         <v>0.5</v>
@@ -7410,16 +7410,16 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>227</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F3">
         <v>0.8</v>
@@ -7428,16 +7428,16 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>227</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F4">
         <v>0.02</v>

</xml_diff>

<commit_message>
Fix units to pass obj_model unit validation
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="4815" windowWidth="24975" windowHeight="5325" tabRatio="993" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="1365" yWindow="4815" windowWidth="24975" windowHeight="5325" tabRatio="993" firstSheet="2" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="415">
   <si>
     <t>Id</t>
   </si>
@@ -1315,6 +1315,9 @@
   </si>
   <si>
     <t>Fractional abundance</t>
+  </si>
+  <si>
+    <t>M s-1</t>
   </si>
 </sst>
 </file>
@@ -3034,7 +3037,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3356,8 +3359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3397,8 +3400,8 @@
       <c r="C2" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
+      <c r="D2" s="72" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3674,7 +3677,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4742,8 +4745,8 @@
       <c r="D2" s="40" t="s">
         <v>296</v>
       </c>
-      <c r="E2" s="27">
-        <v>1</v>
+      <c r="E2" s="79" t="s">
+        <v>414</v>
       </c>
       <c r="F2" s="33"/>
       <c r="H2" s="33"/>
@@ -4761,8 +4764,8 @@
       <c r="D3" s="43" t="s">
         <v>298</v>
       </c>
-      <c r="E3" s="27">
-        <v>1</v>
+      <c r="E3" s="79" t="s">
+        <v>414</v>
       </c>
       <c r="F3" s="33"/>
       <c r="H3" s="40" t="s">
@@ -4782,8 +4785,8 @@
       <c r="D4" s="40" t="s">
         <v>301</v>
       </c>
-      <c r="E4" s="27">
-        <v>1</v>
+      <c r="E4" s="79" t="s">
+        <v>414</v>
       </c>
       <c r="F4" s="33"/>
       <c r="H4" s="40" t="s">
@@ -4803,8 +4806,8 @@
       <c r="D5" s="40" t="s">
         <v>296</v>
       </c>
-      <c r="E5" s="27">
-        <v>1</v>
+      <c r="E5" s="79" t="s">
+        <v>414</v>
       </c>
       <c r="F5" s="33"/>
       <c r="H5" s="40" t="s">
@@ -4824,8 +4827,8 @@
       <c r="D6" s="40" t="s">
         <v>306</v>
       </c>
-      <c r="E6" s="27">
-        <v>1</v>
+      <c r="E6" s="79" t="s">
+        <v>414</v>
       </c>
       <c r="F6" s="33"/>
       <c r="H6" s="40" t="s">
@@ -4845,8 +4848,8 @@
       <c r="D7" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="E7" s="27">
-        <v>1</v>
+      <c r="E7" s="79" t="s">
+        <v>414</v>
       </c>
       <c r="F7" s="33"/>
     </row>
@@ -4863,8 +4866,8 @@
       <c r="D8" s="40" t="s">
         <v>311</v>
       </c>
-      <c r="E8" s="27">
-        <v>1</v>
+      <c r="E8" s="79" t="s">
+        <v>414</v>
       </c>
       <c r="F8" s="40" t="s">
         <v>312</v>
@@ -4883,8 +4886,8 @@
       <c r="D9" s="40" t="s">
         <v>314</v>
       </c>
-      <c r="E9" s="27">
-        <v>1</v>
+      <c r="E9" s="79" t="s">
+        <v>414</v>
       </c>
       <c r="F9" s="40" t="s">
         <v>315</v>
@@ -7346,7 +7349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Allow only one of inchi and smiles to represent structure'
</commit_message>
<xml_diff>
--- a/tests/fixtures/eukaryote_core.xlsx
+++ b/tests/fixtures/eukaryote_core.xlsx
@@ -1392,7 +1392,7 @@
     <t>WC:book</t>
   </si>
   <si>
-    <t>inchi_structure</t>
+    <t>structure</t>
   </si>
 </sst>
 </file>
@@ -2196,7 +2196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2231,7 +2231,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2790,7 +2790,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>